<commit_message>
fixed download filepath for template excel
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/static/input_files/acfrs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908DFE4B-89B3-384D-853E-FBC5105F040A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1CCF02-A629-104E-861B-3299B168D1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="500" windowWidth="24180" windowHeight="17500" tabRatio="834" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="500" windowWidth="24180" windowHeight="17500" tabRatio="834" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Label Dropdowns" sheetId="8" r:id="rId1"/>
@@ -5978,31 +5978,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="31">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -6134,6 +6110,14 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -15398,8 +15382,8 @@
   </sheetPr>
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H83" sqref="H83"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -16845,18 +16829,18 @@
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <conditionalFormatting sqref="C101:F101">
-    <cfRule type="cellIs" dxfId="32" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="18" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="19" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="20" operator="notEqual">
+    <cfRule type="cellIs" dxfId="28" priority="20" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F101 C23 C37 C50 C65 C76:C77 C89 C101">
-    <cfRule type="expression" dxfId="29" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="2" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16898,7 +16882,7 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -18525,74 +18509,64 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
-  <conditionalFormatting sqref="C23 C37 C50 D53:G63 D74:H77 J74:J77 I74 I78:I99">
-    <cfRule type="expression" dxfId="28" priority="49" stopIfTrue="1">
+  <conditionalFormatting sqref="C23 C37 C50 D53:G63 D74:H77 J74:J77">
+    <cfRule type="expression" dxfId="26" priority="49" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:J64">
-    <cfRule type="expression" dxfId="27" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="34" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:J72">
-    <cfRule type="expression" dxfId="26" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="10" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F6 D52:F52">
-    <cfRule type="expression" dxfId="25" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="46" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:G51">
-    <cfRule type="expression" dxfId="24" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="6" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D65:J65 D66:H70 J66:J70">
-    <cfRule type="expression" dxfId="23" priority="16" stopIfTrue="1">
+  <conditionalFormatting sqref="D65:J70">
+    <cfRule type="expression" dxfId="21" priority="2" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39:H50">
-    <cfRule type="expression" dxfId="22" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="5" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38:I38">
-    <cfRule type="expression" dxfId="21" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="43" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:J6 D7:I37 I39:I51">
-    <cfRule type="expression" dxfId="20" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="39" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H52:J53 H54:H63 J54:J63">
-    <cfRule type="expression" dxfId="19" priority="23" stopIfTrue="1">
+  <conditionalFormatting sqref="H52:J63">
+    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7:J50">
-    <cfRule type="expression" dxfId="18" priority="4" stopIfTrue="1">
-      <formula>J$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I54:I63">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="I74:I99">
+    <cfRule type="expression" dxfId="16" priority="1" stopIfTrue="1">
       <formula>I$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I66:I70">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>I$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I75:I77">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>I$6=""</formula>
+  <conditionalFormatting sqref="J7:J50">
+    <cfRule type="expression" dxfId="15" priority="4" stopIfTrue="1">
+      <formula>J$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -18619,7 +18593,7 @@
   <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -19974,7 +19948,7 @@
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="D7:I7 D8:J23 C23 D25:J36 C36 C37:J37 D38:J71 C60:J60 C70">
-    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21324,31 +21298,31 @@
     <mergeCell ref="B25:E25"/>
   </mergeCells>
   <conditionalFormatting sqref="C102">
-    <cfRule type="cellIs" dxfId="16" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="equal">
       <formula>$C$102</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>$C$102</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C102:E102">
-    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D102">
-    <cfRule type="cellIs" dxfId="13" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" stopIfTrue="1" operator="equal">
       <formula>$D$102</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="notEqual">
       <formula>$D$102</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E102">
-    <cfRule type="cellIs" dxfId="11" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>$E$102</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>$E$102</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22682,31 +22656,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C101">
-    <cfRule type="cellIs" dxfId="9" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="equal">
       <formula>$C$101</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>$C$101</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:E101">
-    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D101">
-    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
       <formula>$D$101</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="notEqual">
       <formula>$D$101</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E101">
-    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>$E$101</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
       <formula>$E$101</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
governmental fund balance sheet template draft
followed the Clayton page 40 example
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/static/input_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/byflow/Documents/Research/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1CCF02-A629-104E-861B-3299B168D1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE15D284-3CAD-C943-A8B7-B3909F0F3BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="500" windowWidth="24180" windowHeight="17500" tabRatio="834" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="15000" windowHeight="18900" tabRatio="834" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Label Dropdowns" sheetId="8" r:id="rId1"/>
@@ -18,12 +18,13 @@
     <sheet name="Master Info" sheetId="13" r:id="rId3"/>
     <sheet name="Statement of Net Position" sheetId="9" r:id="rId4"/>
     <sheet name="Statement of Activities" sheetId="19" r:id="rId5"/>
-    <sheet name="GovFund Stmt of Rev Exp and Chg" sheetId="15" r:id="rId6"/>
-    <sheet name="Prop Fund Stmt of Net Position" sheetId="11" state="hidden" r:id="rId7"/>
-    <sheet name="Prop Fund Stmt of Rev Exp Bal" sheetId="12" state="hidden" r:id="rId8"/>
+    <sheet name="GovFund Balance Sheet" sheetId="22" r:id="rId6"/>
+    <sheet name="GovFund Stmt of Rev Exp and Chg" sheetId="15" r:id="rId7"/>
+    <sheet name="Prop Fund Stmt of Net Position" sheetId="11" state="hidden" r:id="rId8"/>
+    <sheet name="Prop Fund Stmt of Rev Exp Bal" sheetId="12" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'GovFund Stmt of Rev Exp and Chg'!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'GovFund Stmt of Rev Exp and Chg'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Label Dropdowns'!$A$1:$C$522</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Statement of Activities'!$B$25:$B$36</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Statement of Net Position'!$B$25:$B$36</definedName>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2593" uniqueCount="1744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2622" uniqueCount="1756">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -5310,6 +5311,42 @@
   </si>
   <si>
     <t>acfr:ProgramRevenues,acfr:Expenses,acfr:NetExpenseRevenue</t>
+  </si>
+  <si>
+    <t>Balance Sheet</t>
+  </si>
+  <si>
+    <t>Landscape Maintenance District</t>
+  </si>
+  <si>
+    <t>Successor Housing Agency</t>
+  </si>
+  <si>
+    <t>LIABILITIES, DEFERRED INFLOWS OF RESOURCES AND FUND BALANCES</t>
+  </si>
+  <si>
+    <t>Liabilities:</t>
+  </si>
+  <si>
+    <t>Deferred Inflows of Resources:</t>
+  </si>
+  <si>
+    <t>Fund Balance:</t>
+  </si>
+  <si>
+    <t>acfr:</t>
+  </si>
+  <si>
+    <t>Total Liabilities, Deferred Inflows of Resources and Fund Balances</t>
+  </si>
+  <si>
+    <t>American Rescue Plan Act</t>
+  </si>
+  <si>
+    <t>Capital Improvement Program</t>
+  </si>
+  <si>
+    <t>Other Governmental Funds</t>
   </si>
 </sst>
 </file>
@@ -5320,7 +5357,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -5450,8 +5487,32 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5527,6 +5588,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA6A6A6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF595959"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF262626"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -5775,7 +5866,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5972,13 +6063,62 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="44" fontId="13" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="23" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="24" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="23" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="23" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="23" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="23" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="55">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -6110,6 +6250,198 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6555,7 +6887,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C522"/>
   <sheetViews>
-    <sheetView topLeftCell="A316" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -12322,8 +12654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF490C29-31E1-3E46-B6B7-83D944E71A74}">
   <dimension ref="A1:H218"/>
   <sheetViews>
-    <sheetView topLeftCell="A165" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B177" sqref="B177"/>
+    <sheetView topLeftCell="A65" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -15382,8 +15714,8 @@
   </sheetPr>
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A29" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -16829,18 +17161,18 @@
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <conditionalFormatting sqref="C101:F101">
-    <cfRule type="cellIs" dxfId="30" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="18" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="19" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="20" operator="notEqual">
+    <cfRule type="cellIs" dxfId="52" priority="20" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F101 C23 C37 C50 C65 C76:C77 C89 C101">
-    <cfRule type="expression" dxfId="27" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="2" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18510,62 +18842,62 @@
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <conditionalFormatting sqref="C23 C37 C50 D53:G63 D74:H77 J74:J77">
-    <cfRule type="expression" dxfId="26" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="49" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:J64">
-    <cfRule type="expression" dxfId="25" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="34" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:J72">
-    <cfRule type="expression" dxfId="24" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="10" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F6 D52:F52">
-    <cfRule type="expression" dxfId="23" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="46" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:G51">
-    <cfRule type="expression" dxfId="22" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="6" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:J70">
-    <cfRule type="expression" dxfId="21" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="2" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39:H50">
-    <cfRule type="expression" dxfId="20" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="5" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38:I38">
-    <cfRule type="expression" dxfId="19" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="43" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:J6 D7:I37 I39:I51">
-    <cfRule type="expression" dxfId="18" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="39" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52:J63">
-    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="3" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I74:I99">
-    <cfRule type="expression" dxfId="16" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="1" stopIfTrue="1">
       <formula>I$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:J50">
-    <cfRule type="expression" dxfId="15" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="4" stopIfTrue="1">
       <formula>J$6=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18586,14 +18918,773 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62560919-E4A0-3A4F-9164-3F35B35B852C}">
+  <dimension ref="A1:I36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="29.5" style="121" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="17">
+      <c r="A1" s="45" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B1" s="113" t="str">
+        <f>_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3)</f>
+        <v>City of Clayton, California</v>
+      </c>
+      <c r="C1" s="55"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+    </row>
+    <row r="2" spans="1:9" ht="17">
+      <c r="A2" s="46" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B2" s="61" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C2" s="55"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+    </row>
+    <row r="3" spans="1:9" ht="17">
+      <c r="A3" s="46" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+    </row>
+    <row r="4" spans="1:9" ht="17" thickBot="1">
+      <c r="A4" s="48" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B4" s="114">
+        <f>'Master Info'!C4</f>
+        <v>44742</v>
+      </c>
+      <c r="C4" s="55"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+    </row>
+    <row r="5" spans="1:9" ht="16">
+      <c r="A5" s="56"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+    </row>
+    <row r="6" spans="1:9" ht="48">
+      <c r="A6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="115"/>
+      <c r="C6" s="12" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>1745</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>1753</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>1754</v>
+      </c>
+      <c r="H6" s="105" t="s">
+        <v>1755</v>
+      </c>
+      <c r="I6" s="105" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16">
+      <c r="A7" s="7"/>
+      <c r="B7" s="116" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="106"/>
+    </row>
+    <row r="8" spans="1:9" ht="15">
+      <c r="A8" s="8" t="str">
+        <f>IF(B8="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B8,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B8" s="117"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="107"/>
+      <c r="I8" s="107">
+        <f>SUM(C8:H8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15">
+      <c r="A9" s="8" t="str">
+        <f>IF(B9="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B9,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B9" s="117"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="107"/>
+      <c r="I9" s="107">
+        <f>SUM(C9:H9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15">
+      <c r="A10" s="8" t="str">
+        <f>IF(B10="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B10,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B10" s="117"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="107"/>
+      <c r="I10" s="107">
+        <f>SUM(C10:H10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15">
+      <c r="A11" s="8" t="str">
+        <f>IF(B11="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B11,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B11" s="117"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="107"/>
+      <c r="I11" s="107">
+        <f>SUM(C11:H11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15">
+      <c r="A12" s="8" t="str">
+        <f>IF(B12="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B12,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B12" s="117"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="107"/>
+      <c r="I12" s="107">
+        <f>SUM(C12:H12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15">
+      <c r="A13" s="8" t="str">
+        <f>IF(B13="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B13,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B13" s="117"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="107"/>
+      <c r="I13" s="107">
+        <f>SUM(C13:H13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15">
+      <c r="A14" s="8" t="str">
+        <f>IF(B14="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B14,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B14" s="117"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="107"/>
+      <c r="I14" s="107">
+        <f t="shared" ref="I14:I15" si="0">SUM(C14:H14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15">
+      <c r="A15" s="8" t="str">
+        <f>IF(B15="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B15,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B15" s="117"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="107"/>
+      <c r="I15" s="107">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15">
+      <c r="A16" s="8" t="str">
+        <f>IF(B16="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B16,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B16" s="117"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="107"/>
+      <c r="I16" s="107">
+        <f>SUM(C16:H16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="16">
+      <c r="A17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="118" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="23">
+        <f>SUM(C8:C16)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="23">
+        <f>SUM(D8:D16)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="23">
+        <f t="shared" ref="E17:H17" si="1">SUM(E8:E16)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="108">
+        <f>SUM(C17:H17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="32">
+      <c r="B18" s="116" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="106"/>
+      <c r="I18" s="106"/>
+    </row>
+    <row r="19" spans="1:9" ht="16">
+      <c r="B19" s="119" t="s">
+        <v>1748</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" ht="15">
+      <c r="A20" s="8" t="str">
+        <f>IF(B20="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B20,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B20" s="117"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="109">
+        <f>SUM(C20:H20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15">
+      <c r="A21" s="8" t="str">
+        <f>IF(B21="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B21,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B21" s="117"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="110"/>
+      <c r="I21" s="109">
+        <f t="shared" ref="I21:I24" si="2">SUM(C21:H21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15">
+      <c r="A22" s="8" t="str">
+        <f>IF(B22="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B22,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B22" s="117"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="107"/>
+      <c r="I22" s="109">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15">
+      <c r="A23" s="8" t="str">
+        <f>IF(B23="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B23,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B23" s="117"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="107"/>
+      <c r="I23" s="109">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15">
+      <c r="A24" s="8" t="str">
+        <f>IF(B24="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B24,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B24" s="117"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="107"/>
+      <c r="I24" s="109">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="16">
+      <c r="A25" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="120" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="104">
+        <f>SUM(C20:C24)</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="104">
+        <f t="shared" ref="D25:H25" si="3">SUM(D20:D24)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="104">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="104">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="104">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="104">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="111">
+        <f>SUM(C25:H25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="16">
+      <c r="B26" s="119" t="s">
+        <v>1749</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" ht="15">
+      <c r="A27" s="8" t="str">
+        <f>IF(B27="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B27,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B27" s="117"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="112"/>
+      <c r="I27" s="112"/>
+    </row>
+    <row r="28" spans="1:9" ht="16">
+      <c r="A28" s="8" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B28" s="120" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="17">
+        <f>SUM(C27)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="17">
+        <f>SUM(D27)</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="17">
+        <f t="shared" ref="E28:H28" si="4">SUM(E27)</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="17">
+        <f>SUM(I27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="16">
+      <c r="B29" s="119" t="s">
+        <v>1750</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" ht="15">
+      <c r="A30" s="8" t="str">
+        <f>IF(B30="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B30,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B30" s="117"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="109"/>
+      <c r="I30" s="109">
+        <f>SUM(C30:H30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15">
+      <c r="A31" s="8" t="str">
+        <f>IF(B31="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B31,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B31" s="117"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="110"/>
+      <c r="I31" s="110">
+        <f>SUM(C31:H31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15">
+      <c r="A32" s="8" t="str">
+        <f>IF(B32="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B32,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B32" s="117"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="107"/>
+      <c r="I32" s="107">
+        <f>SUM(C32:H32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15">
+      <c r="A33" s="8" t="str">
+        <f>IF(B33="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B33,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B33" s="117"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="107"/>
+      <c r="I33" s="107">
+        <f>SUM(C33:H33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15">
+      <c r="A34" s="8" t="str">
+        <f>IF(B34="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B34,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B34" s="117"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="107"/>
+      <c r="I34" s="107">
+        <f>SUM(C34:H34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="16">
+      <c r="A35" s="8" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B35" s="120" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="17">
+        <f>SUM(C30:C34)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="17">
+        <f>SUM(D30:D34)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="17">
+        <f>SUM(E30:E34)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="17">
+        <f>SUM(F30:F34)</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="17">
+        <f>SUM(G30:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="111">
+        <f>SUM(H30:H34)</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="111">
+        <f>SUM(C35:H35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="32">
+      <c r="A36" s="9" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B36" s="118" t="s">
+        <v>1752</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="108"/>
+      <c r="I36" s="108"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D6:E7">
+    <cfRule type="expression" dxfId="38" priority="23" stopIfTrue="1">
+      <formula>D$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D16">
+    <cfRule type="expression" dxfId="37" priority="22" stopIfTrue="1">
+      <formula>D$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8:E16">
+    <cfRule type="expression" dxfId="36" priority="21" stopIfTrue="1">
+      <formula>E$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:G18">
+    <cfRule type="expression" dxfId="35" priority="20" stopIfTrue="1">
+      <formula>D$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20:D24">
+    <cfRule type="expression" dxfId="32" priority="18" stopIfTrue="1">
+      <formula>D$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:E24">
+    <cfRule type="expression" dxfId="31" priority="17" stopIfTrue="1">
+      <formula>E$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:H25">
+    <cfRule type="expression" dxfId="30" priority="16" stopIfTrue="1">
+      <formula>C$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="expression" dxfId="29" priority="15" stopIfTrue="1">
+      <formula>D$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27:G27">
+    <cfRule type="expression" dxfId="28" priority="14" stopIfTrue="1">
+      <formula>E$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30:D34">
+    <cfRule type="expression" dxfId="27" priority="13" stopIfTrue="1">
+      <formula>D$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30:E34">
+    <cfRule type="expression" dxfId="26" priority="12" stopIfTrue="1">
+      <formula>E$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:I28">
+    <cfRule type="expression" dxfId="25" priority="11" stopIfTrue="1">
+      <formula>C$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:G35">
+    <cfRule type="expression" dxfId="24" priority="10" stopIfTrue="1">
+      <formula>C$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="expression" dxfId="23" priority="9" stopIfTrue="1">
+      <formula>D$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:F7">
+    <cfRule type="expression" dxfId="22" priority="8" stopIfTrue="1">
+      <formula>F$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:F16">
+    <cfRule type="expression" dxfId="21" priority="7" stopIfTrue="1">
+      <formula>F$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20:F24">
+    <cfRule type="expression" dxfId="20" priority="6" stopIfTrue="1">
+      <formula>F$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F30:F34">
+    <cfRule type="expression" dxfId="19" priority="5" stopIfTrue="1">
+      <formula>F$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6:G7">
+    <cfRule type="expression" dxfId="18" priority="4" stopIfTrue="1">
+      <formula>G$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:G16">
+    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
+      <formula>G$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20:G24">
+    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
+      <formula>G$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G30:G34">
+    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
+      <formula>G$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B16 B27" xr:uid="{C05164A8-FCB4-D447-A641-AF82C1FC0132}">
+      <formula1>current_assets</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20:B24 B30:B34" xr:uid="{E7758463-A14F-B541-9130-AEC634E9AF3C}">
+      <formula1>current_liabilities</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A741F4-D4C9-9A45-AFFB-14EF6B58F69B}">
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -19980,7 +21071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788A9A8B-CD70-4E43-B731-FB7C17794303}">
   <dimension ref="A1:E102"/>
   <sheetViews>
@@ -21353,7 +22444,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A27AB5-4C32-7545-9FCB-B1E2421FAC8B}">
   <dimension ref="A1:E101"/>
   <sheetViews>

</xml_diff>

<commit_message>
chanegd to governmental funds
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/byflow/Documents/Research/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE15D284-3CAD-C943-A8B7-B3909F0F3BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF7CA85-55E7-7740-A446-D1B9505F8085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15000" windowHeight="18900" tabRatio="834" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11700" yWindow="760" windowWidth="15000" windowHeight="18880" tabRatio="834" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Label Dropdowns" sheetId="8" r:id="rId1"/>
@@ -6054,15 +6054,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="44" fontId="13" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="21" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -6112,13 +6103,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="40">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -6250,126 +6250,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -17161,18 +17041,18 @@
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <conditionalFormatting sqref="C101:F101">
-    <cfRule type="cellIs" dxfId="54" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="18" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="19" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="20" operator="notEqual">
+    <cfRule type="cellIs" dxfId="37" priority="20" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F101 C23 C37 C50 C65 C76:C77 C89 C101">
-    <cfRule type="expression" dxfId="51" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="2" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18842,62 +18722,62 @@
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <conditionalFormatting sqref="C23 C37 C50 D53:G63 D74:H77 J74:J77">
-    <cfRule type="expression" dxfId="50" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="49" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:J64">
-    <cfRule type="expression" dxfId="49" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="34" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:J72">
-    <cfRule type="expression" dxfId="48" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="10" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F6 D52:F52">
-    <cfRule type="expression" dxfId="47" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="46" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:G51">
-    <cfRule type="expression" dxfId="46" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="6" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:J70">
-    <cfRule type="expression" dxfId="45" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="2" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39:H50">
-    <cfRule type="expression" dxfId="44" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="5" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38:I38">
-    <cfRule type="expression" dxfId="43" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="43" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:J6 D7:I37 I39:I51">
-    <cfRule type="expression" dxfId="42" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="39" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52:J63">
-    <cfRule type="expression" dxfId="41" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="3" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I74:I99">
-    <cfRule type="expression" dxfId="40" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="1" stopIfTrue="1">
       <formula>I$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:J50">
-    <cfRule type="expression" dxfId="39" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="4" stopIfTrue="1">
       <formula>J$6=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18921,21 +18801,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62560919-E4A0-3A4F-9164-3F35B35B852C}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="29.5" style="121" customWidth="1"/>
+    <col min="2" max="2" width="29.5" style="118" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17">
       <c r="A1" s="45" t="s">
         <v>1074</v>
       </c>
-      <c r="B1" s="113" t="str">
+      <c r="B1" s="110" t="str">
         <f>_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3)</f>
         <v>City of Clayton, California</v>
       </c>
@@ -18948,7 +18828,7 @@
         <v>1105</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>1106</v>
+        <v>1081</v>
       </c>
       <c r="C2" s="55"/>
       <c r="D2" s="49"/>
@@ -18969,7 +18849,7 @@
       <c r="A4" s="48" t="s">
         <v>1076</v>
       </c>
-      <c r="B4" s="114">
+      <c r="B4" s="111">
         <f>'Master Info'!C4</f>
         <v>44742</v>
       </c>
@@ -18988,7 +18868,7 @@
       <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="115"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="12" t="s">
         <v>1083</v>
       </c>
@@ -19004,16 +18884,16 @@
       <c r="G6" s="12" t="s">
         <v>1754</v>
       </c>
-      <c r="H6" s="105" t="s">
+      <c r="H6" s="102" t="s">
         <v>1755</v>
       </c>
-      <c r="I6" s="105" t="s">
+      <c r="I6" s="102" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16">
       <c r="A7" s="7"/>
-      <c r="B7" s="116" t="s">
+      <c r="B7" s="113" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="14"/>
@@ -19021,23 +18901,23 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="106"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
     </row>
     <row r="8" spans="1:9" ht="15">
       <c r="A8" s="8" t="str">
         <f>IF(B8="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B8,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B8" s="117"/>
+      <c r="B8" s="114"/>
       <c r="C8" s="19"/>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
-      <c r="H8" s="107"/>
-      <c r="I8" s="107">
-        <f>SUM(C8:H8)</f>
+      <c r="H8" s="104"/>
+      <c r="I8" s="104">
+        <f t="shared" ref="I8:I13" si="0">SUM(C8:H8)</f>
         <v>0</v>
       </c>
     </row>
@@ -19046,15 +18926,15 @@
         <f>IF(B9="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B9,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B9" s="117"/>
+      <c r="B9" s="114"/>
       <c r="C9" s="19"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
-      <c r="H9" s="107"/>
-      <c r="I9" s="107">
-        <f>SUM(C9:H9)</f>
+      <c r="H9" s="104"/>
+      <c r="I9" s="104">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -19063,15 +18943,15 @@
         <f>IF(B10="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B10,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B10" s="117"/>
+      <c r="B10" s="114"/>
       <c r="C10" s="19"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="107"/>
-      <c r="I10" s="107">
-        <f>SUM(C10:H10)</f>
+      <c r="H10" s="104"/>
+      <c r="I10" s="104">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -19080,15 +18960,15 @@
         <f>IF(B11="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B11,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B11" s="117"/>
+      <c r="B11" s="114"/>
       <c r="C11" s="19"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="107">
-        <f>SUM(C11:H11)</f>
+      <c r="H11" s="104"/>
+      <c r="I11" s="104">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -19097,15 +18977,15 @@
         <f>IF(B12="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B12,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B12" s="117"/>
+      <c r="B12" s="114"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="107"/>
-      <c r="I12" s="107">
-        <f>SUM(C12:H12)</f>
+      <c r="H12" s="104"/>
+      <c r="I12" s="104">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -19114,15 +18994,15 @@
         <f>IF(B13="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B13,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B13" s="117"/>
+      <c r="B13" s="114"/>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
-      <c r="H13" s="107"/>
-      <c r="I13" s="107">
-        <f>SUM(C13:H13)</f>
+      <c r="H13" s="104"/>
+      <c r="I13" s="104">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -19131,15 +19011,15 @@
         <f>IF(B14="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B14,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B14" s="117"/>
+      <c r="B14" s="114"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
-      <c r="H14" s="107"/>
-      <c r="I14" s="107">
-        <f t="shared" ref="I14:I15" si="0">SUM(C14:H14)</f>
+      <c r="H14" s="104"/>
+      <c r="I14" s="104">
+        <f t="shared" ref="I14:I15" si="1">SUM(C14:H14)</f>
         <v>0</v>
       </c>
     </row>
@@ -19148,15 +19028,15 @@
         <f>IF(B15="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B15,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B15" s="117"/>
+      <c r="B15" s="114"/>
       <c r="C15" s="19"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
-      <c r="H15" s="107"/>
-      <c r="I15" s="107">
-        <f t="shared" si="0"/>
+      <c r="H15" s="104"/>
+      <c r="I15" s="104">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -19165,14 +19045,14 @@
         <f>IF(B16="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B16,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B16" s="117"/>
+      <c r="B16" s="114"/>
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
-      <c r="H16" s="107"/>
-      <c r="I16" s="107">
+      <c r="H16" s="104"/>
+      <c r="I16" s="104">
         <f>SUM(C16:H16)</f>
         <v>0</v>
       </c>
@@ -19181,7 +19061,7 @@
       <c r="A17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="118" t="s">
+      <c r="B17" s="115" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="23">
@@ -19193,28 +19073,28 @@
         <v>0</v>
       </c>
       <c r="E17" s="23">
-        <f t="shared" ref="E17:H17" si="1">SUM(E8:E16)</f>
+        <f t="shared" ref="E17:H17" si="2">SUM(E8:E16)</f>
         <v>0</v>
       </c>
       <c r="F17" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G17" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H17" s="23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="108">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="105">
         <f>SUM(C17:H17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="32">
-      <c r="B18" s="116" t="s">
+      <c r="B18" s="113" t="s">
         <v>1747</v>
       </c>
       <c r="C18" s="14"/>
@@ -19222,11 +19102,11 @@
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="106"/>
+      <c r="H18" s="103"/>
+      <c r="I18" s="103"/>
     </row>
     <row r="19" spans="1:9" ht="16">
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="116" t="s">
         <v>1748</v>
       </c>
       <c r="H19" s="2"/>
@@ -19237,14 +19117,14 @@
         <f>IF(B20="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B20,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B20" s="117"/>
+      <c r="B20" s="114"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
-      <c r="H20" s="109"/>
-      <c r="I20" s="109">
+      <c r="H20" s="106"/>
+      <c r="I20" s="106">
         <f>SUM(C20:H20)</f>
         <v>0</v>
       </c>
@@ -19254,15 +19134,15 @@
         <f>IF(B21="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B21,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B21" s="117"/>
+      <c r="B21" s="114"/>
       <c r="C21" s="20"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
-      <c r="H21" s="110"/>
-      <c r="I21" s="109">
-        <f t="shared" ref="I21:I24" si="2">SUM(C21:H21)</f>
+      <c r="H21" s="107"/>
+      <c r="I21" s="106">
+        <f t="shared" ref="I21:I24" si="3">SUM(C21:H21)</f>
         <v>0</v>
       </c>
     </row>
@@ -19271,15 +19151,15 @@
         <f>IF(B22="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B22,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B22" s="117"/>
+      <c r="B22" s="114"/>
       <c r="C22" s="19"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
-      <c r="H22" s="107"/>
-      <c r="I22" s="109">
-        <f t="shared" si="2"/>
+      <c r="H22" s="104"/>
+      <c r="I22" s="106">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -19288,15 +19168,15 @@
         <f>IF(B23="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B23,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B23" s="117"/>
+      <c r="B23" s="114"/>
       <c r="C23" s="19"/>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
-      <c r="H23" s="107"/>
-      <c r="I23" s="109">
-        <f t="shared" si="2"/>
+      <c r="H23" s="104"/>
+      <c r="I23" s="106">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -19305,15 +19185,15 @@
         <f>IF(B24="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B24,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B24" s="117"/>
+      <c r="B24" s="114"/>
       <c r="C24" s="19"/>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
-      <c r="H24" s="107"/>
-      <c r="I24" s="109">
-        <f t="shared" si="2"/>
+      <c r="H24" s="104"/>
+      <c r="I24" s="106">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -19321,40 +19201,40 @@
       <c r="A25" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="120" t="s">
+      <c r="B25" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="104">
+      <c r="C25" s="101">
         <f>SUM(C20:C24)</f>
         <v>0</v>
       </c>
-      <c r="D25" s="104">
-        <f t="shared" ref="D25:H25" si="3">SUM(D20:D24)</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="104">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="104">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="104">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="104">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="111">
+      <c r="D25" s="101">
+        <f t="shared" ref="D25:H25" si="4">SUM(D20:D24)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="101">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="101">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="101">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="101">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="108">
         <f>SUM(C25:H25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="16">
-      <c r="B26" s="119" t="s">
+      <c r="B26" s="116" t="s">
         <v>1749</v>
       </c>
       <c r="H26" s="2"/>
@@ -19365,20 +19245,20 @@
         <f>IF(B27="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B27,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B27" s="117"/>
+      <c r="B27" s="114"/>
       <c r="C27" s="19"/>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
-      <c r="H27" s="112"/>
-      <c r="I27" s="112"/>
+      <c r="H27" s="109"/>
+      <c r="I27" s="109"/>
     </row>
     <row r="28" spans="1:9" ht="16">
       <c r="A28" s="8" t="s">
         <v>1751</v>
       </c>
-      <c r="B28" s="120" t="s">
+      <c r="B28" s="117" t="s">
         <v>46</v>
       </c>
       <c r="C28" s="17">
@@ -19390,19 +19270,19 @@
         <v>0</v>
       </c>
       <c r="E28" s="17">
-        <f t="shared" ref="E28:H28" si="4">SUM(E27)</f>
+        <f t="shared" ref="E28:H28" si="5">SUM(E27)</f>
         <v>0</v>
       </c>
       <c r="F28" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G28" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H28" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I28" s="17">
@@ -19411,7 +19291,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="16">
-      <c r="B29" s="119" t="s">
+      <c r="B29" s="116" t="s">
         <v>1750</v>
       </c>
       <c r="H29" s="2"/>
@@ -19422,15 +19302,15 @@
         <f>IF(B30="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B30,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B30" s="117"/>
+      <c r="B30" s="114"/>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
-      <c r="H30" s="109"/>
-      <c r="I30" s="109">
-        <f>SUM(C30:H30)</f>
+      <c r="H30" s="106"/>
+      <c r="I30" s="106">
+        <f t="shared" ref="I30:I35" si="6">SUM(C30:H30)</f>
         <v>0</v>
       </c>
     </row>
@@ -19439,15 +19319,15 @@
         <f>IF(B31="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B31,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B31" s="117"/>
+      <c r="B31" s="114"/>
       <c r="C31" s="20"/>
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
-      <c r="H31" s="110"/>
-      <c r="I31" s="110">
-        <f>SUM(C31:H31)</f>
+      <c r="H31" s="107"/>
+      <c r="I31" s="107">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -19456,15 +19336,15 @@
         <f>IF(B32="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B32,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B32" s="117"/>
+      <c r="B32" s="114"/>
       <c r="C32" s="19"/>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20"/>
-      <c r="H32" s="107"/>
-      <c r="I32" s="107">
-        <f>SUM(C32:H32)</f>
+      <c r="H32" s="104"/>
+      <c r="I32" s="104">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -19473,15 +19353,15 @@
         <f>IF(B33="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B33,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B33" s="117"/>
+      <c r="B33" s="114"/>
       <c r="C33" s="19"/>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
       <c r="G33" s="20"/>
-      <c r="H33" s="107"/>
-      <c r="I33" s="107">
-        <f>SUM(C33:H33)</f>
+      <c r="H33" s="104"/>
+      <c r="I33" s="104">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -19490,15 +19370,15 @@
         <f>IF(B34="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B34,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B34" s="117"/>
+      <c r="B34" s="114"/>
       <c r="C34" s="19"/>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
       <c r="G34" s="20"/>
-      <c r="H34" s="107"/>
-      <c r="I34" s="107">
-        <f>SUM(C34:H34)</f>
+      <c r="H34" s="104"/>
+      <c r="I34" s="104">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -19506,35 +19386,35 @@
       <c r="A35" s="8" t="s">
         <v>1751</v>
       </c>
-      <c r="B35" s="120" t="s">
+      <c r="B35" s="117" t="s">
         <v>46</v>
       </c>
       <c r="C35" s="17">
-        <f>SUM(C30:C34)</f>
+        <f t="shared" ref="C35:H35" si="7">SUM(C30:C34)</f>
         <v>0</v>
       </c>
       <c r="D35" s="17">
-        <f>SUM(D30:D34)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E35" s="17">
-        <f>SUM(E30:E34)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F35" s="17">
-        <f>SUM(F30:F34)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G35" s="17">
-        <f>SUM(G30:G34)</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="111">
-        <f>SUM(H30:H34)</f>
-        <v>0</v>
-      </c>
-      <c r="I35" s="111">
-        <f>SUM(C35:H35)</f>
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H35" s="108">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="108">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -19542,7 +19422,7 @@
       <c r="A36" s="9" t="s">
         <v>1751</v>
       </c>
-      <c r="B36" s="118" t="s">
+      <c r="B36" s="115" t="s">
         <v>1752</v>
       </c>
       <c r="C36" s="23"/>
@@ -19550,118 +19430,53 @@
       <c r="E36" s="23"/>
       <c r="F36" s="23"/>
       <c r="G36" s="23"/>
-      <c r="H36" s="108"/>
-      <c r="I36" s="108"/>
+      <c r="H36" s="105"/>
+      <c r="I36" s="105"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D6:E7">
-    <cfRule type="expression" dxfId="38" priority="23" stopIfTrue="1">
-      <formula>D$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D16">
-    <cfRule type="expression" dxfId="37" priority="22" stopIfTrue="1">
-      <formula>D$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8:E16">
-    <cfRule type="expression" dxfId="36" priority="21" stopIfTrue="1">
-      <formula>E$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18:G18">
-    <cfRule type="expression" dxfId="35" priority="20" stopIfTrue="1">
-      <formula>D$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20:D24">
-    <cfRule type="expression" dxfId="32" priority="18" stopIfTrue="1">
-      <formula>D$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20:E24">
-    <cfRule type="expression" dxfId="31" priority="17" stopIfTrue="1">
-      <formula>E$6=""</formula>
+  <conditionalFormatting sqref="C35:G35">
+    <cfRule type="expression" dxfId="23" priority="10" stopIfTrue="1">
+      <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:H25">
-    <cfRule type="expression" dxfId="30" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="16" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="29" priority="15" stopIfTrue="1">
-      <formula>D$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27:G27">
-    <cfRule type="expression" dxfId="28" priority="14" stopIfTrue="1">
-      <formula>E$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30:D34">
-    <cfRule type="expression" dxfId="27" priority="13" stopIfTrue="1">
-      <formula>D$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30:E34">
-    <cfRule type="expression" dxfId="26" priority="12" stopIfTrue="1">
-      <formula>E$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C28:I28">
-    <cfRule type="expression" dxfId="25" priority="11" stopIfTrue="1">
-      <formula>C$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35:G35">
-    <cfRule type="expression" dxfId="24" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="11" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="23" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="9" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6:F7">
-    <cfRule type="expression" dxfId="22" priority="8" stopIfTrue="1">
-      <formula>F$6=""</formula>
+  <conditionalFormatting sqref="D6:G16">
+    <cfRule type="expression" dxfId="19" priority="3" stopIfTrue="1">
+      <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8:F16">
-    <cfRule type="expression" dxfId="21" priority="7" stopIfTrue="1">
-      <formula>F$6=""</formula>
+  <conditionalFormatting sqref="D18:G18">
+    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
+      <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F24">
-    <cfRule type="expression" dxfId="20" priority="6" stopIfTrue="1">
-      <formula>F$6=""</formula>
+  <conditionalFormatting sqref="D20:G24">
+    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
+      <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F30:F34">
-    <cfRule type="expression" dxfId="19" priority="5" stopIfTrue="1">
-      <formula>F$6=""</formula>
+  <conditionalFormatting sqref="D27:G27">
+    <cfRule type="expression" dxfId="16" priority="14" stopIfTrue="1">
+      <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G7">
-    <cfRule type="expression" dxfId="18" priority="4" stopIfTrue="1">
-      <formula>G$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G16">
-    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
-      <formula>G$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G20:G24">
-    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
-      <formula>G$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G30:G34">
+  <conditionalFormatting sqref="D30:G34">
     <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
-      <formula>G$6=""</formula>
+      <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -21367,12 +21182,12 @@
     </row>
     <row r="25" spans="1:5" ht="15">
       <c r="A25" s="7"/>
-      <c r="B25" s="101" t="s">
+      <c r="B25" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="102"/>
-      <c r="D25" s="102"/>
-      <c r="E25" s="103"/>
+      <c r="C25" s="120"/>
+      <c r="D25" s="120"/>
+      <c r="E25" s="121"/>
     </row>
     <row r="26" spans="1:5" ht="15">
       <c r="A26" s="8" t="str">

</xml_diff>

<commit_message>
updated gov fund balance
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/byflow/Documents/Research/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF7CA85-55E7-7740-A446-D1B9505F8085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C61D5B-432A-EC44-8BB8-338F754C0CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11700" yWindow="760" windowWidth="15000" windowHeight="18880" tabRatio="834" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11720" yWindow="740" windowWidth="18520" windowHeight="18900" tabRatio="834" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Label Dropdowns" sheetId="8" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2622" uniqueCount="1756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2630" uniqueCount="1755">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -5316,12 +5316,6 @@
     <t>Balance Sheet</t>
   </si>
   <si>
-    <t>Landscape Maintenance District</t>
-  </si>
-  <si>
-    <t>Successor Housing Agency</t>
-  </si>
-  <si>
     <t>LIABILITIES, DEFERRED INFLOWS OF RESOURCES AND FUND BALANCES</t>
   </si>
   <si>
@@ -5334,19 +5328,22 @@
     <t>Fund Balance:</t>
   </si>
   <si>
-    <t>acfr:</t>
-  </si>
-  <si>
     <t>Total Liabilities, Deferred Inflows of Resources and Fund Balances</t>
   </si>
   <si>
-    <t>American Rescue Plan Act</t>
-  </si>
-  <si>
-    <t>Capital Improvement Program</t>
-  </si>
-  <si>
-    <t>Other Governmental Funds</t>
+    <t>Total Fund Balances</t>
+  </si>
+  <si>
+    <t>acfr:LiabilitiesAndDeferredInflowsOfResourcesAndFundBalancesModifiedAccrual</t>
+  </si>
+  <si>
+    <t>acfr:DeferredInflowsOfResourcesModifiedAccrual</t>
+  </si>
+  <si>
+    <t>acfr:LiabilitiesModifiedAccrual</t>
+  </si>
+  <si>
+    <t>acfr:AssetsModifiedAccrual</t>
   </si>
 </sst>
 </file>
@@ -5357,7 +5354,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -5488,13 +5485,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -5512,7 +5502,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5588,12 +5578,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA6A6A6"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF595959"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -5866,7 +5850,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6055,23 +6039,19 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="13" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="23" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="22" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="24" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="23" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="44" fontId="23" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="22" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="23" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="44" fontId="22" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="23" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="23" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="22" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
@@ -6112,13 +6092,26 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="23" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="23" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="23" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="23" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="23" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="23" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="34">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -6250,54 +6243,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -17041,18 +16986,18 @@
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <conditionalFormatting sqref="C101:F101">
-    <cfRule type="cellIs" dxfId="39" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="18" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="19" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="20" operator="notEqual">
+    <cfRule type="cellIs" dxfId="31" priority="20" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F101 C23 C37 C50 C65 C76:C77 C89 C101">
-    <cfRule type="expression" dxfId="36" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="2" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18722,62 +18667,62 @@
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <conditionalFormatting sqref="C23 C37 C50 D53:G63 D74:H77 J74:J77">
-    <cfRule type="expression" dxfId="35" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="49" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:J64">
-    <cfRule type="expression" dxfId="34" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="34" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:J72">
-    <cfRule type="expression" dxfId="33" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="10" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F6 D52:F52">
-    <cfRule type="expression" dxfId="32" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="46" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:G51">
-    <cfRule type="expression" dxfId="31" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="6" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:J70">
-    <cfRule type="expression" dxfId="30" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="2" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39:H50">
-    <cfRule type="expression" dxfId="29" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="5" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38:I38">
-    <cfRule type="expression" dxfId="28" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="43" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:J6 D7:I37 I39:I51">
-    <cfRule type="expression" dxfId="27" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="39" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52:J63">
-    <cfRule type="expression" dxfId="26" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="3" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I74:I99">
-    <cfRule type="expression" dxfId="25" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="1" stopIfTrue="1">
       <formula>I$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:J50">
-    <cfRule type="expression" dxfId="24" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="4" stopIfTrue="1">
       <formula>J$6=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18799,23 +18744,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62560919-E4A0-3A4F-9164-3F35B35B852C}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="29.5" style="118" customWidth="1"/>
+    <col min="2" max="2" width="29.5" style="116" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17">
+    <row r="1" spans="1:10" ht="17">
       <c r="A1" s="45" t="s">
         <v>1074</v>
       </c>
-      <c r="B1" s="110" t="str">
+      <c r="B1" s="108" t="str">
         <f>_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3)</f>
         <v>City of Clayton, California</v>
       </c>
@@ -18823,7 +18768,7 @@
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
     </row>
-    <row r="2" spans="1:9" ht="17">
+    <row r="2" spans="1:10" ht="17">
       <c r="A2" s="46" t="s">
         <v>1105</v>
       </c>
@@ -18834,7 +18779,7 @@
       <c r="D2" s="49"/>
       <c r="E2" s="49"/>
     </row>
-    <row r="3" spans="1:9" ht="17">
+    <row r="3" spans="1:10" ht="17">
       <c r="A3" s="46" t="s">
         <v>1075</v>
       </c>
@@ -18845,11 +18790,11 @@
       <c r="D3" s="49"/>
       <c r="E3" s="49"/>
     </row>
-    <row r="4" spans="1:9" ht="17" thickBot="1">
+    <row r="4" spans="1:10" ht="17" thickBot="1">
       <c r="A4" s="48" t="s">
         <v>1076</v>
       </c>
-      <c r="B4" s="111">
+      <c r="B4" s="109">
         <f>'Master Info'!C4</f>
         <v>44742</v>
       </c>
@@ -18857,634 +18802,1061 @@
       <c r="D4" s="49"/>
       <c r="E4" s="49"/>
     </row>
-    <row r="5" spans="1:9" ht="16">
+    <row r="5" spans="1:10" ht="16">
       <c r="A5" s="56"/>
       <c r="B5" s="87"/>
       <c r="C5" s="51"/>
       <c r="D5" s="51"/>
       <c r="E5" s="51"/>
     </row>
-    <row r="6" spans="1:9" ht="48">
+    <row r="6" spans="1:10" ht="57">
       <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="112"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="110"/>
+      <c r="C6" s="68" t="s">
         <v>1083</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>1745</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>1746</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>1753</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>1754</v>
-      </c>
-      <c r="H6" s="102" t="s">
-        <v>1755</v>
-      </c>
-      <c r="I6" s="102" t="s">
+      <c r="D6" s="70" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E6" s="70" t="s">
+        <v>1115</v>
+      </c>
+      <c r="F6" s="70" t="s">
+        <v>1115</v>
+      </c>
+      <c r="G6" s="70" t="s">
+        <v>1115</v>
+      </c>
+      <c r="H6" s="70" t="s">
+        <v>1115</v>
+      </c>
+      <c r="I6" s="70" t="s">
+        <v>1115</v>
+      </c>
+      <c r="J6" s="120"/>
+    </row>
+    <row r="7" spans="1:10" ht="32">
+      <c r="B7" s="11"/>
+      <c r="C7" s="62" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D7" s="71" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E7" s="71" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F7" s="71" t="s">
+        <v>1116</v>
+      </c>
+      <c r="G7" s="71" t="s">
+        <v>1116</v>
+      </c>
+      <c r="H7" s="71" t="s">
+        <v>1116</v>
+      </c>
+      <c r="I7" s="71" t="s">
+        <v>1116</v>
+      </c>
+      <c r="J7" s="63" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="16">
-      <c r="A7" s="7"/>
-      <c r="B7" s="113" t="s">
+    <row r="8" spans="1:10" ht="16">
+      <c r="A8" s="7"/>
+      <c r="B8" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="103"/>
-      <c r="I7" s="103"/>
-    </row>
-    <row r="8" spans="1:9" ht="15">
-      <c r="A8" s="8" t="str">
-        <f>IF(B8="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B8,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B8" s="114"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="104"/>
-      <c r="I8" s="104">
-        <f t="shared" ref="I8:I13" si="0">SUM(C8:H8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+    </row>
+    <row r="9" spans="1:10" ht="15">
       <c r="A9" s="8" t="str">
         <f>IF(B9="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B9,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B9" s="114"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="19"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15">
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="124">
+        <f>SUM(C9:I9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15">
       <c r="A10" s="8" t="str">
         <f>IF(B10="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B10,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B10" s="114"/>
+      <c r="B10" s="112"/>
       <c r="C10" s="19"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="104">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15">
+      <c r="H10" s="103"/>
+      <c r="I10" s="103"/>
+      <c r="J10" s="124">
+        <f t="shared" ref="J10:J18" si="0">SUM(C10:I10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15">
       <c r="A11" s="8" t="str">
         <f>IF(B11="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B11,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B11" s="114"/>
+      <c r="B11" s="112"/>
       <c r="C11" s="19"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
-      <c r="H11" s="104"/>
-      <c r="I11" s="104">
+      <c r="H11" s="103"/>
+      <c r="I11" s="103"/>
+      <c r="J11" s="124">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15">
+    <row r="12" spans="1:10" ht="15">
       <c r="A12" s="8" t="str">
         <f>IF(B12="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B12,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B12" s="114"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="104"/>
-      <c r="I12" s="104">
+      <c r="H12" s="103"/>
+      <c r="I12" s="103"/>
+      <c r="J12" s="124">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15">
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" s="8" t="str">
         <f>IF(B13="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B13,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B13" s="114"/>
+      <c r="B13" s="112"/>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
-      <c r="H13" s="104"/>
-      <c r="I13" s="104">
+      <c r="H13" s="103"/>
+      <c r="I13" s="103"/>
+      <c r="J13" s="124">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15">
+    <row r="14" spans="1:10" ht="15">
       <c r="A14" s="8" t="str">
         <f>IF(B14="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B14,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B14" s="114"/>
+      <c r="B14" s="112"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
-      <c r="H14" s="104"/>
-      <c r="I14" s="104">
-        <f t="shared" ref="I14:I15" si="1">SUM(C14:H14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15">
+      <c r="H14" s="103"/>
+      <c r="I14" s="103"/>
+      <c r="J14" s="124">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15">
       <c r="A15" s="8" t="str">
         <f>IF(B15="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B15,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B15" s="114"/>
+      <c r="B15" s="112"/>
       <c r="C15" s="19"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
-      <c r="H15" s="104"/>
-      <c r="I15" s="104">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15">
+      <c r="H15" s="103"/>
+      <c r="I15" s="103"/>
+      <c r="J15" s="124">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="8" t="str">
         <f>IF(B16="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B16,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B16" s="114"/>
+      <c r="B16" s="112"/>
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
-      <c r="H16" s="104"/>
-      <c r="I16" s="104">
-        <f>SUM(C16:H16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="16">
-      <c r="A17" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="115" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="23">
-        <f>SUM(C8:C16)</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="23">
-        <f>SUM(D8:D16)</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="23">
-        <f t="shared" ref="E17:H17" si="2">SUM(E8:E16)</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="105">
-        <f>SUM(C17:H17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="32">
-      <c r="B18" s="113" t="s">
-        <v>1747</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="H16" s="103"/>
+      <c r="I16" s="103"/>
+      <c r="J16" s="124">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15">
+      <c r="A17" s="8" t="str">
+        <f>IF(B17="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B17,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B17" s="112"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="103"/>
+      <c r="I17" s="103"/>
+      <c r="J17" s="124">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15">
+      <c r="A18" s="8" t="str">
+        <f>IF(B18="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B18,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B18" s="112"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="103"/>
       <c r="I18" s="103"/>
-    </row>
-    <row r="19" spans="1:9" ht="16">
-      <c r="B19" s="116" t="s">
-        <v>1748</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" ht="15">
-      <c r="A20" s="8" t="str">
-        <f>IF(B20="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B20,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B20" s="114"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="106"/>
-      <c r="I20" s="106">
-        <f>SUM(C20:H20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15">
-      <c r="A21" s="8" t="str">
-        <f>IF(B21="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B21,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B21" s="114"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="107"/>
-      <c r="I21" s="106">
-        <f t="shared" ref="I21:I24" si="3">SUM(C21:H21)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15">
+      <c r="J18" s="124">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="16">
+      <c r="A19" s="9" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B19" s="113" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="23">
+        <f>SUM(C9:C18)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="23">
+        <f>SUM(D9:D18)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="23">
+        <f t="shared" ref="E19:H19" si="1">SUM(E9:E18)</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="23">
+        <f t="shared" ref="I19" si="2">SUM(I9:I18)</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="121">
+        <f>SUM(C19:I19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="32">
+      <c r="B20" s="111" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="102"/>
+      <c r="I20" s="102"/>
+      <c r="J20" s="102"/>
+    </row>
+    <row r="21" spans="1:10" ht="16">
+      <c r="B21" s="114" t="s">
+        <v>1746</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" ht="15">
       <c r="A22" s="8" t="str">
         <f>IF(B22="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B22,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B22" s="114"/>
+      <c r="B22" s="112"/>
       <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="104"/>
-      <c r="I22" s="106">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15">
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="105"/>
+      <c r="I22" s="105"/>
+      <c r="J22" s="122">
+        <f>SUM(C22:I22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15">
       <c r="A23" s="8" t="str">
         <f>IF(B23="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B23,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B23" s="114"/>
+      <c r="B23" s="112"/>
       <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="104"/>
-      <c r="I23" s="106">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15">
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="106"/>
+      <c r="I23" s="106"/>
+      <c r="J23" s="122">
+        <f t="shared" ref="J23:J27" si="3">SUM(C23:I23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15">
       <c r="A24" s="8" t="str">
         <f>IF(B24="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B24,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B24" s="114"/>
+      <c r="B24" s="112"/>
       <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="104"/>
-      <c r="I24" s="106">
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="106"/>
+      <c r="I24" s="106"/>
+      <c r="J24" s="122">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="16">
-      <c r="A25" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="117" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="101">
-        <f>SUM(C20:C24)</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="101">
-        <f t="shared" ref="D25:H25" si="4">SUM(D20:D24)</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="101">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="101">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="101">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="101">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="108">
-        <f>SUM(C25:H25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="16">
-      <c r="B26" s="116" t="s">
-        <v>1749</v>
-      </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" ht="15">
+    <row r="25" spans="1:10" ht="15">
+      <c r="A25" s="8" t="str">
+        <f>IF(B25="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B25,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B25" s="112"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="106"/>
+      <c r="I25" s="106"/>
+      <c r="J25" s="122">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15">
+      <c r="A26" s="8" t="str">
+        <f>IF(B26="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B26,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B26" s="112"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="106"/>
+      <c r="I26" s="106"/>
+      <c r="J26" s="122">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15">
       <c r="A27" s="8" t="str">
         <f>IF(B27="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B27,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B27" s="114"/>
+      <c r="B27" s="112"/>
       <c r="C27" s="19"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="109"/>
-      <c r="I27" s="109"/>
-    </row>
-    <row r="28" spans="1:9" ht="16">
-      <c r="A28" s="8" t="s">
-        <v>1751</v>
-      </c>
-      <c r="B28" s="117" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="17">
-        <f>SUM(C27)</f>
-        <v>0</v>
-      </c>
-      <c r="D28" s="17">
-        <f>SUM(D27)</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="17">
-        <f t="shared" ref="E28:H28" si="5">SUM(E27)</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G28" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H28" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="17">
-        <f>SUM(I27)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="16">
-      <c r="B29" s="116" t="s">
-        <v>1750</v>
-      </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" ht="15">
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="106"/>
+      <c r="I27" s="106"/>
+      <c r="J27" s="122">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15">
+      <c r="A28" s="8" t="str">
+        <f>IF(B28="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B28,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B28" s="112"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="106"/>
+      <c r="I28" s="106"/>
+      <c r="J28" s="122">
+        <f t="shared" ref="J28:J31" si="4">SUM(C28:I28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15">
+      <c r="A29" s="8" t="str">
+        <f>IF(B29="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B29,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B29" s="112"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="103"/>
+      <c r="I29" s="103"/>
+      <c r="J29" s="122">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15">
       <c r="A30" s="8" t="str">
         <f>IF(B30="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B30,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B30" s="114"/>
+      <c r="B30" s="112"/>
       <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="106"/>
-      <c r="I30" s="106">
-        <f t="shared" ref="I30:I35" si="6">SUM(C30:H30)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15">
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="103"/>
+      <c r="I30" s="103"/>
+      <c r="J30" s="122">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15">
       <c r="A31" s="8" t="str">
         <f>IF(B31="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B31,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B31" s="114"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="107"/>
-      <c r="I31" s="107">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15">
-      <c r="A32" s="8" t="str">
-        <f>IF(B32="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B32,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B32" s="114"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="104"/>
-      <c r="I32" s="104">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="15">
-      <c r="A33" s="8" t="str">
-        <f>IF(B33="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B33,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B33" s="114"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="104"/>
-      <c r="I33" s="104">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="15">
+      <c r="B31" s="112"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="103"/>
+      <c r="I31" s="103"/>
+      <c r="J31" s="122">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="16">
+      <c r="A32" s="8" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B32" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="101">
+        <f>SUM(C22:C31)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="101">
+        <f t="shared" ref="D32:H32" si="5">SUM(D22:D31)</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="101">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="101">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="101">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="101">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="101">
+        <f t="shared" ref="I32" si="6">SUM(I22:I31)</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="123">
+        <f>SUM(C32:I32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="16">
+      <c r="B33" s="114" t="s">
+        <v>1747</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:10" ht="15">
       <c r="A34" s="8" t="str">
         <f>IF(B34="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B34,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
-      <c r="B34" s="114"/>
+      <c r="B34" s="112"/>
       <c r="C34" s="19"/>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
       <c r="G34" s="20"/>
-      <c r="H34" s="104"/>
-      <c r="I34" s="104">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="16">
-      <c r="A35" s="8" t="s">
+      <c r="H34" s="107"/>
+      <c r="I34" s="107"/>
+      <c r="J34" s="126">
+        <f>SUM(C34:I34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15">
+      <c r="A35" s="8" t="str">
+        <f>IF(B35="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B35,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B35" s="112"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="107"/>
+      <c r="I35" s="107"/>
+      <c r="J35" s="126">
+        <f>SUM(C35:I35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15">
+      <c r="A36" s="8" t="str">
+        <f>IF(B36="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B36,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B36" s="112"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="107"/>
+      <c r="I36" s="107"/>
+      <c r="J36" s="126">
+        <f t="shared" ref="J36:J43" si="7">SUM(C36:I36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15">
+      <c r="A37" s="8" t="str">
+        <f>IF(B37="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B37,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B37" s="112"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="107"/>
+      <c r="I37" s="107"/>
+      <c r="J37" s="126">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15">
+      <c r="A38" s="8" t="str">
+        <f>IF(B38="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B38,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B38" s="112"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="107"/>
+      <c r="I38" s="107"/>
+      <c r="J38" s="126">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15">
+      <c r="A39" s="8" t="str">
+        <f>IF(B39="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B39,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B39" s="112"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="107"/>
+      <c r="I39" s="107"/>
+      <c r="J39" s="126">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15">
+      <c r="A40" s="8" t="str">
+        <f>IF(B40="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B40,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B40" s="112"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="107"/>
+      <c r="I40" s="107"/>
+      <c r="J40" s="126">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15">
+      <c r="A41" s="8" t="str">
+        <f>IF(B41="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B41,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B41" s="112"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="107"/>
+      <c r="I41" s="107"/>
+      <c r="J41" s="126">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15">
+      <c r="A42" s="8" t="str">
+        <f>IF(B42="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B42,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B42" s="112"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="107"/>
+      <c r="I42" s="107"/>
+      <c r="J42" s="126">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15">
+      <c r="A43" s="8" t="str">
+        <f>IF(B43="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B43,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B43" s="112"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="107"/>
+      <c r="I43" s="107"/>
+      <c r="J43" s="126">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="16">
+      <c r="A44" s="8" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B44" s="115" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="101">
+        <f>SUM(C34:C43)</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="101">
+        <f>SUM(D34:D43)</f>
+        <v>0</v>
+      </c>
+      <c r="E44" s="101">
+        <f>SUM(E34:E43)</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="101">
+        <f>SUM(F34:F43)</f>
+        <v>0</v>
+      </c>
+      <c r="G44" s="101">
+        <f>SUM(G34:G43)</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="101">
+        <f>SUM(H34:H43)</f>
+        <v>0</v>
+      </c>
+      <c r="I44" s="101">
+        <f>SUM(I34:I43)</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="101">
+        <f>SUM(C44:I44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="16">
+      <c r="B45" s="114" t="s">
+        <v>1748</v>
+      </c>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="1:10" ht="15">
+      <c r="A46" s="8" t="str">
+        <f>IF(B46="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B46,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B46" s="112"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="105"/>
+      <c r="I46" s="105"/>
+      <c r="J46" s="122">
+        <f>SUM(C46:I46)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15">
+      <c r="A47" s="8" t="str">
+        <f>IF(B47="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B47,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B47" s="112"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="106"/>
+      <c r="I47" s="106"/>
+      <c r="J47" s="122">
+        <f t="shared" ref="J47:J56" si="8">SUM(C47:I47)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="15">
+      <c r="A48" s="8" t="str">
+        <f>IF(B48="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B48,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B48" s="112"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="103"/>
+      <c r="I48" s="103"/>
+      <c r="J48" s="122">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="15">
+      <c r="A49" s="8" t="str">
+        <f>IF(B49="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B49,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B49" s="112"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="103"/>
+      <c r="I49" s="103"/>
+      <c r="J49" s="122">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15">
+      <c r="A50" s="8" t="str">
+        <f>IF(B50="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B50,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B50" s="112"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="103"/>
+      <c r="I50" s="103"/>
+      <c r="J50" s="122">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15">
+      <c r="A51" s="8" t="str">
+        <f>IF(B51="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B51,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B51" s="112"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="103"/>
+      <c r="I51" s="103"/>
+      <c r="J51" s="122">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15">
+      <c r="A52" s="8" t="str">
+        <f>IF(B52="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B52,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B52" s="112"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="103"/>
+      <c r="I52" s="103"/>
+      <c r="J52" s="122">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15">
+      <c r="A53" s="8" t="str">
+        <f>IF(B53="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B53,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B53" s="112"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="103"/>
+      <c r="I53" s="103"/>
+      <c r="J53" s="122">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15">
+      <c r="A54" s="8" t="str">
+        <f>IF(B54="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B54,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B54" s="112"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="103"/>
+      <c r="I54" s="103"/>
+      <c r="J54" s="122">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15">
+      <c r="A55" s="8" t="str">
+        <f>IF(B55="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B55,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B55" s="112"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="103"/>
+      <c r="I55" s="103"/>
+      <c r="J55" s="122">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15">
+      <c r="A56" s="8" t="str">
+        <f>IF(B56="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B56,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B56" s="112"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="103"/>
+      <c r="I56" s="103"/>
+      <c r="J56" s="122">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="16">
+      <c r="A57" s="8" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B57" s="115" t="s">
+        <v>1750</v>
+      </c>
+      <c r="C57" s="101">
+        <f t="shared" ref="C57:H57" si="9">SUM(C46:C56)</f>
+        <v>0</v>
+      </c>
+      <c r="D57" s="101">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E57" s="101">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="101">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G57" s="101">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H57" s="125">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I57" s="125">
+        <f t="shared" ref="I57" si="10">SUM(I46:I56)</f>
+        <v>0</v>
+      </c>
+      <c r="J57" s="123">
+        <f>SUM(C57:I57)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="32">
+      <c r="A58" s="9" t="s">
         <v>1751</v>
       </c>
-      <c r="B35" s="117" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="17">
-        <f t="shared" ref="C35:H35" si="7">SUM(C30:C34)</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="E35" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G35" s="17">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="H35" s="108">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="108">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="32">
-      <c r="A36" s="9" t="s">
-        <v>1751</v>
-      </c>
-      <c r="B36" s="115" t="s">
-        <v>1752</v>
-      </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="105"/>
-      <c r="I36" s="105"/>
+      <c r="B58" s="113" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="104"/>
+      <c r="I58" s="104"/>
+      <c r="J58" s="104"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C35:G35">
-    <cfRule type="expression" dxfId="23" priority="10" stopIfTrue="1">
+  <conditionalFormatting sqref="C57:G57 D58 D8:G18 D20:G20 D22:G31 D34:G43 D46:G56 C32:I32 C44:I44">
+    <cfRule type="expression" dxfId="17" priority="51" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:H25">
-    <cfRule type="expression" dxfId="22" priority="16" stopIfTrue="1">
-      <formula>C$6=""</formula>
+  <conditionalFormatting sqref="D7:I7">
+    <cfRule type="expression" dxfId="16" priority="1" stopIfTrue="1">
+      <formula>D$7=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:I28">
-    <cfRule type="expression" dxfId="21" priority="11" stopIfTrue="1">
-      <formula>C$6=""</formula>
+  <conditionalFormatting sqref="J44">
+    <cfRule type="expression" dxfId="15" priority="53" stopIfTrue="1">
+      <formula>I$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="20" priority="9" stopIfTrue="1">
-      <formula>D$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6:G16">
-    <cfRule type="expression" dxfId="19" priority="3" stopIfTrue="1">
-      <formula>D$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18:G18">
-    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
-      <formula>D$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20:G24">
-    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
-      <formula>D$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27:G27">
-    <cfRule type="expression" dxfId="16" priority="14" stopIfTrue="1">
-      <formula>D$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30:G34">
-    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
-      <formula>D$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B16 B27" xr:uid="{C05164A8-FCB4-D447-A641-AF82C1FC0132}">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B18 B34:B43" xr:uid="{C05164A8-FCB4-D447-A641-AF82C1FC0132}">
       <formula1>current_assets</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20:B24 B30:B34" xr:uid="{E7758463-A14F-B541-9130-AEC634E9AF3C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22:B31 B46:B56" xr:uid="{E7758463-A14F-B541-9130-AEC634E9AF3C}">
       <formula1>current_liabilities</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:J6" xr:uid="{B34980F1-F3F1-3843-BC5A-2A296C0C0599}">
+      <formula1>"Select fund type or delete column, General Fund, Special Revenue Fund, Capital Project, Debt Service, Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{F6E02613-D880-4D46-8748-5B833C7CAEEC}">
+      <formula1>"General Fund, Special Revenue Fund, Capital Project, Debt Service, Other"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19498,8 +19870,8 @@
   </sheetPr>
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView topLeftCell="A25" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -19916,7 +20288,7 @@
         <v>1086</v>
       </c>
       <c r="C23" s="26">
-        <f t="shared" ref="C23:J23" si="1">IF(C7="","",SUM(C9:C22))</f>
+        <f t="shared" ref="C23:I23" si="1">IF(C7="","",SUM(C9:C22))</f>
         <v>0</v>
       </c>
       <c r="D23" s="26">
@@ -19944,7 +20316,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="26">
-        <f t="shared" si="1"/>
+        <f>IF(J7="","",SUM(J9:J22))</f>
         <v>0</v>
       </c>
     </row>
@@ -21182,12 +21554,12 @@
     </row>
     <row r="25" spans="1:5" ht="15">
       <c r="A25" s="7"/>
-      <c r="B25" s="119" t="s">
+      <c r="B25" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="120"/>
-      <c r="D25" s="120"/>
-      <c r="E25" s="121"/>
+      <c r="C25" s="118"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="119"/>
     </row>
     <row r="26" spans="1:5" ht="15">
       <c r="A26" s="8" t="str">

</xml_diff>

<commit_message>
initial skeleton of reconciliation table
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/byflow/Documents/Research/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C61D5B-432A-EC44-8BB8-338F754C0CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB8607D-4C2E-F541-9C2C-40FA22542E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11720" yWindow="740" windowWidth="18520" windowHeight="18900" tabRatio="834" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" tabRatio="834" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Label Dropdowns" sheetId="8" r:id="rId1"/>
@@ -19,12 +19,13 @@
     <sheet name="Statement of Net Position" sheetId="9" r:id="rId4"/>
     <sheet name="Statement of Activities" sheetId="19" r:id="rId5"/>
     <sheet name="GovFund Balance Sheet" sheetId="22" r:id="rId6"/>
-    <sheet name="GovFund Stmt of Rev Exp and Chg" sheetId="15" r:id="rId7"/>
-    <sheet name="Prop Fund Stmt of Net Position" sheetId="11" state="hidden" r:id="rId8"/>
-    <sheet name="Prop Fund Stmt of Rev Exp Bal" sheetId="12" state="hidden" r:id="rId9"/>
+    <sheet name="Reconciliation Table" sheetId="23" r:id="rId7"/>
+    <sheet name="GovFund Stmt of Rev Exp and Chg" sheetId="15" r:id="rId8"/>
+    <sheet name="Prop Fund Stmt of Net Position" sheetId="11" state="hidden" r:id="rId9"/>
+    <sheet name="Prop Fund Stmt of Rev Exp Bal" sheetId="12" state="hidden" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'GovFund Stmt of Rev Exp and Chg'!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'GovFund Stmt of Rev Exp and Chg'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Label Dropdowns'!$A$1:$C$522</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Statement of Activities'!$B$25:$B$36</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Statement of Net Position'!$B$25:$B$36</definedName>
@@ -79,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2630" uniqueCount="1755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2653" uniqueCount="1772">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -5344,6 +5345,59 @@
   </si>
   <si>
     <t>acfr:AssetsModifiedAccrual</t>
+  </si>
+  <si>
+    <t>Reconciliation of Governmental Funds Balance Sheet to the Statement of Net Position</t>
+  </si>
+  <si>
+    <t>CAPITAL ASSETS</t>
+  </si>
+  <si>
+    <t>Non-depreciable capital assets</t>
+  </si>
+  <si>
+    <t>Depreciable capital assets</t>
+  </si>
+  <si>
+    <t>ACCRUAL OF NON-CURRENT REVENEUS AND EXPENSES</t>
+  </si>
+  <si>
+    <t>Net OPEB liability not reported on the Governmental Funds Balance Sheet</t>
+  </si>
+  <si>
+    <t>Compensated absences payable</t>
+  </si>
+  <si>
+    <t>Lease liability not reported on the Governmental Funds Balance Sheet</t>
+  </si>
+  <si>
+    <t>Net pension liability not reported on the Governmental Funds Balance Sheet</t>
+  </si>
+  <si>
+    <t>DEFERRED INFLOWS AND OUTFLOWS</t>
+  </si>
+  <si>
+    <t>Deferred outflows of resources for net pension liability</t>
+  </si>
+  <si>
+    <t>Deferred inflows of resources for net pension liability</t>
+  </si>
+  <si>
+    <t>Deferred outflows of resources for net OPEB liability</t>
+  </si>
+  <si>
+    <t>Deferred inflows of resources for net OPEB liability</t>
+  </si>
+  <si>
+    <t>ALLOCATION OF INTERNAL SERVICE FUND NET POSITION</t>
+  </si>
+  <si>
+    <t>Internal service funds are used by management to charge the costs of certain activities to
+individual funds. The assets and liabilities of the internal service funds are included in the
+governmental activities in the Government-wide Statement of Net Position.</t>
+  </si>
+  <si>
+    <t>Net Position of Governmental Activities</t>
   </si>
 </sst>
 </file>
@@ -12475,6 +12529,1364 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A27AB5-4C32-7545-9FCB-B1E2421FAC8B}">
+  <dimension ref="A1:E101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="35.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16">
+      <c r="A1" s="4" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" ht="16">
+      <c r="A2" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+    </row>
+    <row r="3" spans="1:5" ht="34" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+    </row>
+    <row r="4" spans="1:5" ht="16">
+      <c r="A4" s="5" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+    </row>
+    <row r="5" spans="1:5" ht="15">
+      <c r="A5" s="36"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="37"/>
+    </row>
+    <row r="6" spans="1:5" ht="32">
+      <c r="A6" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="35" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15">
+      <c r="A8" s="7"/>
+      <c r="B8" s="13" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="1:5" ht="15">
+      <c r="A9" s="8" t="str">
+        <f>IF(B9="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B9,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="17">
+        <f>SUM(C9:D9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15">
+      <c r="A10" s="8" t="str">
+        <f>IF(B10="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B10,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="17">
+        <f t="shared" ref="E10:E22" si="0">SUM(C10:D10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15">
+      <c r="A11" s="8" t="str">
+        <f>IF(B11="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B11,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15">
+      <c r="A12" s="8" t="str">
+        <f>IF(B12="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B12,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15">
+      <c r="A13" s="8" t="str">
+        <f>IF(B13="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B13,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15">
+      <c r="A14" s="8" t="str">
+        <f>IF(B14="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B14,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15">
+      <c r="A15" s="8" t="str">
+        <f>IF(B15="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B15,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15">
+      <c r="A16" s="8" t="str">
+        <f>IF(B16="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B16,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15">
+      <c r="A17" s="8" t="str">
+        <f>IF(B17="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B17,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15">
+      <c r="A18" s="8" t="str">
+        <f>IF(B18="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B18,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15">
+      <c r="A19" s="8" t="str">
+        <f>IF(B19="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B19,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15">
+      <c r="A20" s="8" t="str">
+        <f>IF(B20="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B20,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15">
+      <c r="A21" s="8" t="str">
+        <f>IF(B21="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B21,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15">
+      <c r="A22" s="8" t="str">
+        <f>IF(B22="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B22,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C23" s="17" cm="1">
+        <f t="array" aca="1" ref="C23" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Current Assets:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="17" cm="1">
+        <f t="array" aca="1" ref="D23" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Current Assets:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="17">
+        <f ca="1">SUM(C23:D23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15">
+      <c r="A24" s="7"/>
+      <c r="B24" s="13" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" spans="1:5" ht="15">
+      <c r="A25" s="8" t="str">
+        <f>IF(B25="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B25,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="17">
+        <f t="shared" ref="E25:E38" si="1">SUM(C25:D25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15">
+      <c r="A26" s="8" t="str">
+        <f>IF(B26="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B26,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15">
+      <c r="A27" s="8" t="str">
+        <f>IF(B27="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B27,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15">
+      <c r="A28" s="8" t="str">
+        <f>IF(B28="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B28,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15">
+      <c r="A29" s="8" t="str">
+        <f>IF(B29="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B29,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15">
+      <c r="A30" s="8" t="str">
+        <f>IF(B30="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B30,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B30" s="18"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15">
+      <c r="A31" s="8" t="str">
+        <f>IF(B31="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B31,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B31" s="18"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15">
+      <c r="A32" s="8" t="str">
+        <f>IF(B32="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B32,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B32" s="18"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15">
+      <c r="A33" s="8" t="str">
+        <f>IF(B33="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B33,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15">
+      <c r="A34" s="8" t="str">
+        <f>IF(B34="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B34,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B34" s="18"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15">
+      <c r="A35" s="8" t="str">
+        <f>IF(B35="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B35,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B35" s="18"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15">
+      <c r="A36" s="8" t="str">
+        <f>IF(B36="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B36,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B36" s="18"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15">
+      <c r="A37" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="17" cm="1">
+        <f t="array" aca="1" ref="C37" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Noncurrent Assets:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="17" cm="1">
+        <f t="array" aca="1" ref="D37" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Noncurrent Assets:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15">
+      <c r="A38" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="23" t="e">
+        <f>SUM(_xlfn.XLOOKUP("Total Current Assets",$B:$B,C:C),(_xlfn.XLOOKUP("Total Noncurrent Assets",$B:$B,C:C)))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D38" s="23" t="e">
+        <f>SUM(_xlfn.XLOOKUP("Total Current Assets",$B:$B,D:D),(_xlfn.XLOOKUP("Total Noncurrent Assets",$B:$B,D:D)))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E38" s="23" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+    </row>
+    <row r="40" spans="1:5" ht="15">
+      <c r="A40" s="7"/>
+      <c r="B40" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+    </row>
+    <row r="41" spans="1:5" ht="15">
+      <c r="A41" s="8" t="str">
+        <f>IF(B41="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B41,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B41" s="18"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="17">
+        <f t="shared" ref="E41:E50" si="2">SUM(C41:D41)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15">
+      <c r="A42" s="8" t="str">
+        <f>IF(B42="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B42,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B42" s="18"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15">
+      <c r="A43" s="8" t="str">
+        <f>IF(B43="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B43,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B43" s="18"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15">
+      <c r="A44" s="8" t="str">
+        <f>IF(B44="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B44,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B44" s="18"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15">
+      <c r="A45" s="8" t="str">
+        <f>IF(B45="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B45,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B45" s="18"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15">
+      <c r="A46" s="8" t="str">
+        <f>IF(B46="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B46,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B46" s="18"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15">
+      <c r="A47" s="8" t="str">
+        <f>IF(B47="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B47,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B47" s="18"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15">
+      <c r="A48" s="8" t="str">
+        <f>IF(B48="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B48,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B48" s="18"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15">
+      <c r="A49" s="8" t="str">
+        <f>IF(B49="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B49,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B49" s="18"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15">
+      <c r="A50" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="25" cm="1">
+        <f t="array" aca="1" ref="C50" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("DEFERRED OUTFLOW OF RESOURCES",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+      <c r="D50" s="25" cm="1">
+        <f t="array" aca="1" ref="D50" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("DEFERRED OUTFLOW OF RESOURCES",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+      <c r="E50" s="26">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="24"/>
+    </row>
+    <row r="52" spans="1:5" ht="15">
+      <c r="A52" s="7"/>
+      <c r="B52" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+    </row>
+    <row r="53" spans="1:5" ht="15">
+      <c r="A53" s="7"/>
+      <c r="B53" s="15" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+    </row>
+    <row r="54" spans="1:5" ht="15">
+      <c r="A54" s="8" t="str">
+        <f>IF(B54="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B54,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B54" s="18"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="17">
+        <f t="shared" ref="E54:E77" si="3">SUM(C54:D54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15">
+      <c r="A55" s="8" t="str">
+        <f>IF(B55="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B55,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B55" s="18"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15">
+      <c r="A56" s="8" t="str">
+        <f>IF(B56="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B56,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B56" s="18"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15">
+      <c r="A57" s="8" t="str">
+        <f>IF(B57="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B57,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B57" s="18"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15">
+      <c r="A58" s="8" t="str">
+        <f>IF(B58="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B58,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B58" s="18"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15">
+      <c r="A59" s="8" t="str">
+        <f>IF(B59="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B59,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B59" s="18"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15">
+      <c r="A60" s="8" t="str">
+        <f>IF(B60="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B60,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B60" s="18"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15">
+      <c r="A61" s="8" t="str">
+        <f>IF(B61="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B61,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B61" s="18"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15">
+      <c r="A62" s="8" t="str">
+        <f>IF(B62="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B62,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B62" s="18"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15">
+      <c r="A63" s="8" t="str">
+        <f>IF(B63="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B63,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B63" s="18"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15">
+      <c r="A64" s="8" t="str">
+        <f>IF(B64="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B64,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B64" s="18"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15">
+      <c r="A65" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65" s="17" cm="1">
+        <f t="array" aca="1" ref="C65" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Current Liabilities:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+      <c r="D65" s="17" cm="1">
+        <f t="array" aca="1" ref="D65" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Current Liabilities:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+      <c r="E65" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15">
+      <c r="A66" s="7"/>
+      <c r="B66" s="15" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+    </row>
+    <row r="67" spans="1:5" ht="15">
+      <c r="A67" s="8" t="str">
+        <f>IF(B67="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B67,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B67" s="18"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15">
+      <c r="A68" s="8" t="str">
+        <f>IF(B68="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B68,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B68" s="18"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15">
+      <c r="A69" s="8" t="str">
+        <f>IF(B69="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B69,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B69" s="18"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15">
+      <c r="A70" s="8" t="str">
+        <f>IF(B70="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B70,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B70" s="18"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15">
+      <c r="A71" s="8" t="str">
+        <f>IF(B71="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B71,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B71" s="18"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15">
+      <c r="A72" s="8" t="str">
+        <f>IF(B72="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B72,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B72" s="18"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15">
+      <c r="A73" s="8" t="str">
+        <f>IF(B73="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B73,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B73" s="18"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15">
+      <c r="A74" s="8" t="str">
+        <f>IF(B74="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B74,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B74" s="18"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15">
+      <c r="A75" s="8" t="str">
+        <f>IF(B75="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B75,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B75" s="18"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15">
+      <c r="A76" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C76" s="17" cm="1">
+        <f t="array" aca="1" ref="C76" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Noncurrent Liabilities:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+      <c r="D76" s="17" cm="1">
+        <f t="array" aca="1" ref="D76" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Noncurrent Liabilities:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+      <c r="E76" s="17">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15">
+      <c r="A77" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C77" s="23">
+        <f ca="1">SUM(_xlfn.XLOOKUP("Total Current Liabilities",$B:$B,C:C),(_xlfn.XLOOKUP("Total Noncurrent Liabilities",$B:$B,C:C)))</f>
+        <v>0</v>
+      </c>
+      <c r="D77" s="23">
+        <f ca="1">SUM(_xlfn.XLOOKUP("Total Current Liabilities",$B:$B,D:D),(_xlfn.XLOOKUP("Total Noncurrent Liabilities",$B:$B,D:D)))</f>
+        <v>0</v>
+      </c>
+      <c r="E77" s="23">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15">
+      <c r="A78" s="7"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+    </row>
+    <row r="79" spans="1:5" ht="15">
+      <c r="A79" s="7"/>
+      <c r="B79" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+    </row>
+    <row r="80" spans="1:5" ht="15">
+      <c r="A80" s="8" t="str">
+        <f>IF(B80="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B80,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B80" s="18"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="28">
+        <f t="shared" ref="E80:E89" si="4">SUM(C80:D80)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15">
+      <c r="A81" s="8" t="str">
+        <f>IF(B81="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B81,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B81" s="18"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15">
+      <c r="A82" s="8" t="str">
+        <f>IF(B82="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B82,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B82" s="18"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15">
+      <c r="A83" s="8" t="str">
+        <f>IF(B83="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B83,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B83" s="18"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="20"/>
+      <c r="E83" s="28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15">
+      <c r="A84" s="8" t="str">
+        <f>IF(B84="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B84,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B84" s="18"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15">
+      <c r="A85" s="8" t="str">
+        <f>IF(B85="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B85,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B85" s="18"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="20"/>
+      <c r="E85" s="28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15">
+      <c r="A86" s="8" t="str">
+        <f>IF(B86="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B86,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B86" s="18"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="20"/>
+      <c r="E86" s="28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15">
+      <c r="A87" s="8" t="str">
+        <f>IF(B87="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B87,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B87" s="18"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="20"/>
+      <c r="E87" s="28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15">
+      <c r="A88" s="8" t="str">
+        <f>IF(B88="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B88,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B88" s="18"/>
+      <c r="C88" s="20"/>
+      <c r="D88" s="20"/>
+      <c r="E88" s="28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="15">
+      <c r="A89" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C89" s="26" cm="1">
+        <f t="array" aca="1" ref="C89" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("DEFERRED INFLOWS OF RESOURCES",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+      <c r="D89" s="26" cm="1">
+        <f t="array" aca="1" ref="D89" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("DEFERRED INFLOWS OF RESOURCES",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+      <c r="E89" s="26">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15">
+      <c r="A90" s="7"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29"/>
+    </row>
+    <row r="91" spans="1:5" ht="15">
+      <c r="A91" s="7"/>
+      <c r="B91" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="13"/>
+    </row>
+    <row r="92" spans="1:5" ht="15">
+      <c r="A92" s="8" t="str">
+        <f>IF(B92="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B92,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B92" s="18"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="19"/>
+      <c r="E92" s="17">
+        <f t="shared" ref="E92:E100" si="5">SUM(C92:D92)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15">
+      <c r="A93" s="8" t="str">
+        <f>IF(B93="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B93,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B93" s="18"/>
+      <c r="C93" s="19"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15">
+      <c r="A94" s="8" t="str">
+        <f>IF(B94="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B94,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B94" s="18"/>
+      <c r="C94" s="19"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="15">
+      <c r="A95" s="8" t="str">
+        <f>IF(B95="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B95,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B95" s="18"/>
+      <c r="C95" s="19"/>
+      <c r="D95" s="19"/>
+      <c r="E95" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15">
+      <c r="A96" s="8" t="str">
+        <f>IF(B96="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B96,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B96" s="18"/>
+      <c r="C96" s="19"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="15">
+      <c r="A97" s="8" t="str">
+        <f>IF(B97="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B97,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B97" s="18"/>
+      <c r="C97" s="19"/>
+      <c r="D97" s="19"/>
+      <c r="E97" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="15">
+      <c r="A98" s="8" t="str">
+        <f>IF(B98="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B98,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B98" s="18"/>
+      <c r="C98" s="19"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="15">
+      <c r="A99" s="8" t="str">
+        <f>IF(B99="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B99,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B99" s="18"/>
+      <c r="C99" s="19"/>
+      <c r="D99" s="20"/>
+      <c r="E99" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="15">
+      <c r="A100" s="8" t="str">
+        <f>IF(B100="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B100,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B100" s="18"/>
+      <c r="C100" s="19"/>
+      <c r="D100" s="19"/>
+      <c r="E100" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="15">
+      <c r="A101" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B101" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C101" s="23" cm="1">
+        <f t="array" aca="1" ref="C101" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("NET POSITION",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+      <c r="D101" s="23" cm="1">
+        <f t="array" aca="1" ref="D101" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("NET POSITION",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+      <c r="E101" s="23" cm="1">
+        <f t="array" aca="1" ref="E101" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("NET POSITION",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C101">
+    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="equal">
+      <formula>$C$101</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="notEqual">
+      <formula>$C$101</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C101:E101">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D101">
+    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
+      <formula>$D$101</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="notEqual">
+      <formula>$D$101</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E101">
+    <cfRule type="cellIs" dxfId="1" priority="6" stopIfTrue="1" operator="notEqual">
+      <formula>$E$101</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+      <formula>$E$101</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41:B49" xr:uid="{9BC0AF47-8E6A-144C-B8AC-ED095E97A81D}">
+      <formula1>deferred_outflows</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54:B64" xr:uid="{5C058698-9073-DC49-8BB5-F4FB5112E246}">
+      <formula1>current_liabilities</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B67:B75" xr:uid="{3F616EBA-A90E-4541-9183-0F01CFC3F5F8}">
+      <formula1>noncurrent_liabilities</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B80:B88" xr:uid="{EBEC4932-F8CB-1846-89BE-0CC169CA7F33}">
+      <formula1>deferred_inflows</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B92:B100" xr:uid="{8A04D23E-8118-1A4B-8A84-8F6AD5B16721}">
+      <formula1>net_position</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25:B36" xr:uid="{FA5EF3AC-325A-BC4B-874B-CA2CF2946D73}">
+      <formula1>noncurrent_assets</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B22" xr:uid="{5C4A5840-DD0A-C841-8FFC-758CD4B37D08}">
+      <formula1>current_assets</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF490C29-31E1-3E46-B6B7-83D944E71A74}">
   <dimension ref="A1:H218"/>
@@ -15539,7 +16951,7 @@
   </sheetPr>
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
@@ -18746,8 +20158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62560919-E4A0-3A4F-9164-3F35B35B852C}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -19864,6 +21276,153 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAF299C-3D3B-8F47-AA92-8FD95A662E81}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="34">
+      <c r="A1" s="45" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B1" s="108" t="str">
+        <f>_xlfn.CONCAT('Master Info'!C2, ", ", 'Master Info'!$C$3)</f>
+        <v>City of Clayton, California</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17">
+      <c r="A2" s="46" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B2" s="61" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="85">
+      <c r="A3" s="46" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17" thickBot="1">
+      <c r="A4" s="48" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B4" s="109">
+        <f>'Master Info'!C4</f>
+        <v>44742</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15">
+      <c r="A6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="110"/>
+    </row>
+    <row r="7" spans="1:2" ht="16">
+      <c r="A7" s="111" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B7" s="111"/>
+    </row>
+    <row r="8" spans="1:2" ht="34">
+      <c r="A8" s="61" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="34">
+      <c r="A9" s="61" t="s">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="48">
+      <c r="A10" s="111" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B10" s="111"/>
+    </row>
+    <row r="11" spans="1:2" ht="68">
+      <c r="A11" s="61" t="s">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="34">
+      <c r="A12" s="61" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="68">
+      <c r="A13" s="61" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="68">
+      <c r="A14" s="61" t="s">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="32">
+      <c r="A15" s="111" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B15" s="111"/>
+    </row>
+    <row r="16" spans="1:2" ht="51">
+      <c r="A16" s="61" t="s">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="51">
+      <c r="A17" s="61" t="s">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="51">
+      <c r="A18" s="61" t="s">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="51">
+      <c r="A19" s="61" t="s">
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="48">
+      <c r="A20" s="111" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B20" s="111"/>
+    </row>
+    <row r="21" spans="1:2" ht="221">
+      <c r="A21" s="61" t="s">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="32">
+      <c r="A22" s="111" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B22">
+        <f>SUM(B21, B16:B19, B11:B14, B8:B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A741F4-D4C9-9A45-AFFB-14EF6B58F69B}">
   <sheetPr>
     <tabColor theme="6"/>
@@ -21258,7 +22817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788A9A8B-CD70-4E43-B731-FB7C17794303}">
   <dimension ref="A1:E102"/>
   <sheetViews>
@@ -22629,1362 +24188,4 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A27AB5-4C32-7545-9FCB-B1E2421FAC8B}">
-  <dimension ref="A1:E101"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="1" width="35.1640625" customWidth="1"/>
-    <col min="2" max="2" width="29.1640625" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="16">
-      <c r="A1" s="4" t="s">
-        <v>1074</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-    </row>
-    <row r="2" spans="1:5" ht="16">
-      <c r="A2" s="4" t="s">
-        <v>1077</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>1102</v>
-      </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-    </row>
-    <row r="3" spans="1:5" ht="34" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>1075</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>1107</v>
-      </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-    </row>
-    <row r="4" spans="1:5" ht="16">
-      <c r="A4" s="5" t="s">
-        <v>1076</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-    </row>
-    <row r="5" spans="1:5" ht="15">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="37"/>
-    </row>
-    <row r="6" spans="1:5" ht="32">
-      <c r="A6" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="35" t="s">
-        <v>1103</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>1104</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15">
-      <c r="A8" s="7"/>
-      <c r="B8" s="13" t="s">
-        <v>1108</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="1:5" ht="15">
-      <c r="A9" s="8" t="str">
-        <f>IF(B9="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B9,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="17">
-        <f>SUM(C9:D9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15">
-      <c r="A10" s="8" t="str">
-        <f>IF(B10="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B10,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="17">
-        <f t="shared" ref="E10:E22" si="0">SUM(C10:D10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15">
-      <c r="A11" s="8" t="str">
-        <f>IF(B11="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B11,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15">
-      <c r="A12" s="8" t="str">
-        <f>IF(B12="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B12,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15">
-      <c r="A13" s="8" t="str">
-        <f>IF(B13="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B13,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15">
-      <c r="A14" s="8" t="str">
-        <f>IF(B14="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B14,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15">
-      <c r="A15" s="8" t="str">
-        <f>IF(B15="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B15,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15">
-      <c r="A16" s="8" t="str">
-        <f>IF(B16="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B16,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15">
-      <c r="A17" s="8" t="str">
-        <f>IF(B17="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B17,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15">
-      <c r="A18" s="8" t="str">
-        <f>IF(B18="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B18,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15">
-      <c r="A19" s="8" t="str">
-        <f>IF(B19="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B19,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15">
-      <c r="A20" s="8" t="str">
-        <f>IF(B20="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B20,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15">
-      <c r="A21" s="8" t="str">
-        <f>IF(B21="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B21,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15">
-      <c r="A22" s="8" t="str">
-        <f>IF(B22="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B22,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8" t="s">
-        <v>1109</v>
-      </c>
-      <c r="C23" s="17" cm="1">
-        <f t="array" aca="1" ref="C23" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Current Assets:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="17" cm="1">
-        <f t="array" aca="1" ref="D23" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Current Assets:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="17">
-        <f ca="1">SUM(C23:D23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15">
-      <c r="A24" s="7"/>
-      <c r="B24" s="13" t="s">
-        <v>1110</v>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="13"/>
-    </row>
-    <row r="25" spans="1:5" ht="15">
-      <c r="A25" s="8" t="str">
-        <f>IF(B25="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B25,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="17">
-        <f t="shared" ref="E25:E38" si="1">SUM(C25:D25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15">
-      <c r="A26" s="8" t="str">
-        <f>IF(B26="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B26,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15">
-      <c r="A27" s="8" t="str">
-        <f>IF(B27="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B27,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15">
-      <c r="A28" s="8" t="str">
-        <f>IF(B28="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B28,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15">
-      <c r="A29" s="8" t="str">
-        <f>IF(B29="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B29,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15">
-      <c r="A30" s="8" t="str">
-        <f>IF(B30="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B30,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15">
-      <c r="A31" s="8" t="str">
-        <f>IF(B31="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B31,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15">
-      <c r="A32" s="8" t="str">
-        <f>IF(B32="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B32,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15">
-      <c r="A33" s="8" t="str">
-        <f>IF(B33="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B33,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15">
-      <c r="A34" s="8" t="str">
-        <f>IF(B34="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B34,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15">
-      <c r="A35" s="8" t="str">
-        <f>IF(B35="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B35,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15">
-      <c r="A36" s="8" t="str">
-        <f>IF(B36="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B36,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15">
-      <c r="A37" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="17" cm="1">
-        <f t="array" aca="1" ref="C37" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Noncurrent Assets:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-      <c r="D37" s="17" cm="1">
-        <f t="array" aca="1" ref="D37" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Noncurrent Assets:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="17">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15">
-      <c r="A38" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="23" t="e">
-        <f>SUM(_xlfn.XLOOKUP("Total Current Assets",$B:$B,C:C),(_xlfn.XLOOKUP("Total Noncurrent Assets",$B:$B,C:C)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D38" s="23" t="e">
-        <f>SUM(_xlfn.XLOOKUP("Total Current Assets",$B:$B,D:D),(_xlfn.XLOOKUP("Total Noncurrent Assets",$B:$B,D:D)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E38" s="23" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-    </row>
-    <row r="40" spans="1:5" ht="15">
-      <c r="A40" s="7"/>
-      <c r="B40" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-    </row>
-    <row r="41" spans="1:5" ht="15">
-      <c r="A41" s="8" t="str">
-        <f>IF(B41="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B41,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="17">
-        <f t="shared" ref="E41:E50" si="2">SUM(C41:D41)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15">
-      <c r="A42" s="8" t="str">
-        <f>IF(B42="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B42,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15">
-      <c r="A43" s="8" t="str">
-        <f>IF(B43="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B43,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15">
-      <c r="A44" s="8" t="str">
-        <f>IF(B44="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B44,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15">
-      <c r="A45" s="8" t="str">
-        <f>IF(B45="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B45,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15">
-      <c r="A46" s="8" t="str">
-        <f>IF(B46="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B46,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15">
-      <c r="A47" s="8" t="str">
-        <f>IF(B47="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B47,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="15">
-      <c r="A48" s="8" t="str">
-        <f>IF(B48="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B48,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="15">
-      <c r="A49" s="8" t="str">
-        <f>IF(B49="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B49,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="15">
-      <c r="A50" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C50" s="25" cm="1">
-        <f t="array" aca="1" ref="C50" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("DEFERRED OUTFLOW OF RESOURCES",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-      <c r="D50" s="25" cm="1">
-        <f t="array" aca="1" ref="D50" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("DEFERRED OUTFLOW OF RESOURCES",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-      <c r="E50" s="26">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="15">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="24"/>
-    </row>
-    <row r="52" spans="1:5" ht="15">
-      <c r="A52" s="7"/>
-      <c r="B52" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-    </row>
-    <row r="53" spans="1:5" ht="15">
-      <c r="A53" s="7"/>
-      <c r="B53" s="15" t="s">
-        <v>1078</v>
-      </c>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-    </row>
-    <row r="54" spans="1:5" ht="15">
-      <c r="A54" s="8" t="str">
-        <f>IF(B54="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B54,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B54" s="18"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="17">
-        <f t="shared" ref="E54:E77" si="3">SUM(C54:D54)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="15">
-      <c r="A55" s="8" t="str">
-        <f>IF(B55="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B55,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B55" s="18"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="15">
-      <c r="A56" s="8" t="str">
-        <f>IF(B56="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B56,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B56" s="18"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="15">
-      <c r="A57" s="8" t="str">
-        <f>IF(B57="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B57,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B57" s="18"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15">
-      <c r="A58" s="8" t="str">
-        <f>IF(B58="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B58,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B58" s="18"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="15">
-      <c r="A59" s="8" t="str">
-        <f>IF(B59="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B59,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B59" s="18"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="15">
-      <c r="A60" s="8" t="str">
-        <f>IF(B60="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B60,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B60" s="18"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="15">
-      <c r="A61" s="8" t="str">
-        <f>IF(B61="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B61,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B61" s="18"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="15">
-      <c r="A62" s="8" t="str">
-        <f>IF(B62="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B62,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B62" s="18"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="15">
-      <c r="A63" s="8" t="str">
-        <f>IF(B63="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B63,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B63" s="18"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="15">
-      <c r="A64" s="8" t="str">
-        <f>IF(B64="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B64,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B64" s="18"/>
-      <c r="C64" s="19"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="15">
-      <c r="A65" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C65" s="17" cm="1">
-        <f t="array" aca="1" ref="C65" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Current Liabilities:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-      <c r="D65" s="17" cm="1">
-        <f t="array" aca="1" ref="D65" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Current Liabilities:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-      <c r="E65" s="17">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="15">
-      <c r="A66" s="7"/>
-      <c r="B66" s="15" t="s">
-        <v>1079</v>
-      </c>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15"/>
-    </row>
-    <row r="67" spans="1:5" ht="15">
-      <c r="A67" s="8" t="str">
-        <f>IF(B67="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B67,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B67" s="18"/>
-      <c r="C67" s="19"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="15">
-      <c r="A68" s="8" t="str">
-        <f>IF(B68="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B68,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B68" s="18"/>
-      <c r="C68" s="19"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="15">
-      <c r="A69" s="8" t="str">
-        <f>IF(B69="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B69,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="15">
-      <c r="A70" s="8" t="str">
-        <f>IF(B70="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B70,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B70" s="18"/>
-      <c r="C70" s="19"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="15">
-      <c r="A71" s="8" t="str">
-        <f>IF(B71="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B71,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B71" s="18"/>
-      <c r="C71" s="19"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="15">
-      <c r="A72" s="8" t="str">
-        <f>IF(B72="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B72,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B72" s="18"/>
-      <c r="C72" s="19"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="15">
-      <c r="A73" s="8" t="str">
-        <f>IF(B73="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B73,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B73" s="18"/>
-      <c r="C73" s="19"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="15">
-      <c r="A74" s="8" t="str">
-        <f>IF(B74="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B74,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B74" s="18"/>
-      <c r="C74" s="19"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="15">
-      <c r="A75" s="8" t="str">
-        <f>IF(B75="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B75,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B75" s="18"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="15">
-      <c r="A76" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C76" s="17" cm="1">
-        <f t="array" aca="1" ref="C76" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Noncurrent Liabilities:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-      <c r="D76" s="17" cm="1">
-        <f t="array" aca="1" ref="D76" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("Noncurrent Liabilities:",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-      <c r="E76" s="17">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="15">
-      <c r="A77" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C77" s="23">
-        <f ca="1">SUM(_xlfn.XLOOKUP("Total Current Liabilities",$B:$B,C:C),(_xlfn.XLOOKUP("Total Noncurrent Liabilities",$B:$B,C:C)))</f>
-        <v>0</v>
-      </c>
-      <c r="D77" s="23">
-        <f ca="1">SUM(_xlfn.XLOOKUP("Total Current Liabilities",$B:$B,D:D),(_xlfn.XLOOKUP("Total Noncurrent Liabilities",$B:$B,D:D)))</f>
-        <v>0</v>
-      </c>
-      <c r="E77" s="23">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="15">
-      <c r="A78" s="7"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="24"/>
-      <c r="D78" s="24"/>
-      <c r="E78" s="24"/>
-    </row>
-    <row r="79" spans="1:5" ht="15">
-      <c r="A79" s="7"/>
-      <c r="B79" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="13"/>
-    </row>
-    <row r="80" spans="1:5" ht="15">
-      <c r="A80" s="8" t="str">
-        <f>IF(B80="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B80,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B80" s="18"/>
-      <c r="C80" s="19"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="28">
-        <f t="shared" ref="E80:E89" si="4">SUM(C80:D80)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="15">
-      <c r="A81" s="8" t="str">
-        <f>IF(B81="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B81,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B81" s="18"/>
-      <c r="C81" s="19"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="15">
-      <c r="A82" s="8" t="str">
-        <f>IF(B82="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B82,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B82" s="18"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="15">
-      <c r="A83" s="8" t="str">
-        <f>IF(B83="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B83,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B83" s="18"/>
-      <c r="C83" s="19"/>
-      <c r="D83" s="20"/>
-      <c r="E83" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="15">
-      <c r="A84" s="8" t="str">
-        <f>IF(B84="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B84,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B84" s="18"/>
-      <c r="C84" s="19"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="15">
-      <c r="A85" s="8" t="str">
-        <f>IF(B85="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B85,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B85" s="18"/>
-      <c r="C85" s="19"/>
-      <c r="D85" s="20"/>
-      <c r="E85" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="15">
-      <c r="A86" s="8" t="str">
-        <f>IF(B86="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B86,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B86" s="18"/>
-      <c r="C86" s="19"/>
-      <c r="D86" s="20"/>
-      <c r="E86" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="15">
-      <c r="A87" s="8" t="str">
-        <f>IF(B87="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B87,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B87" s="18"/>
-      <c r="C87" s="19"/>
-      <c r="D87" s="20"/>
-      <c r="E87" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="15">
-      <c r="A88" s="8" t="str">
-        <f>IF(B88="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B88,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B88" s="18"/>
-      <c r="C88" s="20"/>
-      <c r="D88" s="20"/>
-      <c r="E88" s="28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="15">
-      <c r="A89" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B89" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C89" s="26" cm="1">
-        <f t="array" aca="1" ref="C89" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("DEFERRED INFLOWS OF RESOURCES",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-      <c r="D89" s="26" cm="1">
-        <f t="array" aca="1" ref="D89" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("DEFERRED INFLOWS OF RESOURCES",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-      <c r="E89" s="26">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="15">
-      <c r="A90" s="7"/>
-      <c r="B90" s="29"/>
-      <c r="C90" s="29"/>
-      <c r="D90" s="29"/>
-      <c r="E90" s="29"/>
-    </row>
-    <row r="91" spans="1:5" ht="15">
-      <c r="A91" s="7"/>
-      <c r="B91" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C91" s="13"/>
-      <c r="D91" s="13"/>
-      <c r="E91" s="13"/>
-    </row>
-    <row r="92" spans="1:5" ht="15">
-      <c r="A92" s="8" t="str">
-        <f>IF(B92="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B92,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B92" s="18"/>
-      <c r="C92" s="19"/>
-      <c r="D92" s="19"/>
-      <c r="E92" s="17">
-        <f t="shared" ref="E92:E100" si="5">SUM(C92:D92)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="15">
-      <c r="A93" s="8" t="str">
-        <f>IF(B93="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B93,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B93" s="18"/>
-      <c r="C93" s="19"/>
-      <c r="D93" s="19"/>
-      <c r="E93" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="15">
-      <c r="A94" s="8" t="str">
-        <f>IF(B94="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B94,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B94" s="18"/>
-      <c r="C94" s="19"/>
-      <c r="D94" s="19"/>
-      <c r="E94" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="15">
-      <c r="A95" s="8" t="str">
-        <f>IF(B95="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B95,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B95" s="18"/>
-      <c r="C95" s="19"/>
-      <c r="D95" s="19"/>
-      <c r="E95" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="15">
-      <c r="A96" s="8" t="str">
-        <f>IF(B96="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B96,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B96" s="18"/>
-      <c r="C96" s="19"/>
-      <c r="D96" s="19"/>
-      <c r="E96" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="15">
-      <c r="A97" s="8" t="str">
-        <f>IF(B97="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B97,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B97" s="18"/>
-      <c r="C97" s="19"/>
-      <c r="D97" s="19"/>
-      <c r="E97" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="15">
-      <c r="A98" s="8" t="str">
-        <f>IF(B98="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B98,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B98" s="18"/>
-      <c r="C98" s="19"/>
-      <c r="D98" s="19"/>
-      <c r="E98" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="15">
-      <c r="A99" s="8" t="str">
-        <f>IF(B99="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B99,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B99" s="18"/>
-      <c r="C99" s="19"/>
-      <c r="D99" s="20"/>
-      <c r="E99" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="15">
-      <c r="A100" s="8" t="str">
-        <f>IF(B100="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B100,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B100" s="18"/>
-      <c r="C100" s="19"/>
-      <c r="D100" s="19"/>
-      <c r="E100" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="15">
-      <c r="A101" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B101" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C101" s="23" cm="1">
-        <f t="array" aca="1" ref="C101" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("NET POSITION",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-      <c r="D101" s="23" cm="1">
-        <f t="array" aca="1" ref="D101" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("NET POSITION",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-      <c r="E101" s="23" cm="1">
-        <f t="array" aca="1" ref="E101" ca="1">SUM(INDIRECT(ADDRESS(CELL("row",INDEX($B:$B,_xlfn.XMATCH("NET POSITION",$B:$B,1)))+1,COLUMN())&amp;":"&amp;ADDRESS(ROW()-1,COLUMN())))</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C101">
-    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="equal">
-      <formula>$C$101</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="notEqual">
-      <formula>$C$101</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C101:E101">
-    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D101">
-    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
-      <formula>$D$101</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="notEqual">
-      <formula>$D$101</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E101">
-    <cfRule type="cellIs" dxfId="1" priority="6" stopIfTrue="1" operator="notEqual">
-      <formula>$E$101</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
-      <formula>$E$101</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41:B49" xr:uid="{9BC0AF47-8E6A-144C-B8AC-ED095E97A81D}">
-      <formula1>deferred_outflows</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54:B64" xr:uid="{5C058698-9073-DC49-8BB5-F4FB5112E246}">
-      <formula1>current_liabilities</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B67:B75" xr:uid="{3F616EBA-A90E-4541-9183-0F01CFC3F5F8}">
-      <formula1>noncurrent_liabilities</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B80:B88" xr:uid="{EBEC4932-F8CB-1846-89BE-0CC169CA7F33}">
-      <formula1>deferred_inflows</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B92:B100" xr:uid="{8A04D23E-8118-1A4B-8A84-8F6AD5B16721}">
-      <formula1>net_position</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25:B36" xr:uid="{FA5EF3AC-325A-BC4B-874B-CA2CF2946D73}">
-      <formula1>noncurrent_assets</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B22" xr:uid="{5C4A5840-DD0A-C841-8FFC-758CD4B37D08}">
-      <formula1>current_assets</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added editable fields into reconciliation table
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/byflow/Documents/Research/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB8607D-4C2E-F541-9C2C-40FA22542E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E77C92A-9CCE-E849-9CC9-142D71CB248F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" tabRatio="834" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19400" yWindow="0" windowWidth="19000" windowHeight="21600" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Label Dropdowns" sheetId="8" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2653" uniqueCount="1772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2645" uniqueCount="1764">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -5353,51 +5353,25 @@
     <t>CAPITAL ASSETS</t>
   </si>
   <si>
-    <t>Non-depreciable capital assets</t>
-  </si>
-  <si>
-    <t>Depreciable capital assets</t>
-  </si>
-  <si>
     <t>ACCRUAL OF NON-CURRENT REVENEUS AND EXPENSES</t>
   </si>
   <si>
-    <t>Net OPEB liability not reported on the Governmental Funds Balance Sheet</t>
-  </si>
-  <si>
-    <t>Compensated absences payable</t>
-  </si>
-  <si>
-    <t>Lease liability not reported on the Governmental Funds Balance Sheet</t>
-  </si>
-  <si>
-    <t>Net pension liability not reported on the Governmental Funds Balance Sheet</t>
-  </si>
-  <si>
     <t>DEFERRED INFLOWS AND OUTFLOWS</t>
   </si>
   <si>
-    <t>Deferred outflows of resources for net pension liability</t>
-  </si>
-  <si>
-    <t>Deferred inflows of resources for net pension liability</t>
-  </si>
-  <si>
-    <t>Deferred outflows of resources for net OPEB liability</t>
-  </si>
-  <si>
-    <t>Deferred inflows of resources for net OPEB liability</t>
-  </si>
-  <si>
     <t>ALLOCATION OF INTERNAL SERVICE FUND NET POSITION</t>
   </si>
   <si>
-    <t>Internal service funds are used by management to charge the costs of certain activities to
-individual funds. The assets and liabilities of the internal service funds are included in the
-governmental activities in the Government-wide Statement of Net Position.</t>
-  </si>
-  <si>
     <t>Net Position of Governmental Activities</t>
+  </si>
+  <si>
+    <t>Fund balances for governmental funds</t>
+  </si>
+  <si>
+    <t>acfr:AccountsReceivableModifiedAccrual</t>
+  </si>
+  <si>
+    <t>XBRL Modified Label</t>
   </si>
 </sst>
 </file>
@@ -5904,7 +5878,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6137,6 +6111,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="23" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="23" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="23" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="23" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6145,19 +6130,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="23" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="23" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="23" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="23" fillId="15" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="23" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="23" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6764,10 +6736,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE09D81-CE0E-407C-B6C2-C3432BAC9950}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C522"/>
+  <dimension ref="A1:D522"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -6777,7 +6749,7 @@
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="1" t="s">
         <v>58</v>
       </c>
@@ -6787,19 +6759,25 @@
       <c r="C1" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>314</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="2" t="s">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -6810,7 +6788,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -6821,7 +6799,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -6832,7 +6810,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -6843,7 +6821,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -6854,7 +6832,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -6865,7 +6843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -6876,7 +6854,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -6887,7 +6865,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -6898,7 +6876,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -6909,7 +6887,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -6920,7 +6898,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -6931,7 +6909,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -6942,7 +6920,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -12520,7 +12498,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C522">
     <sortCondition ref="A2:A522"/>
     <sortCondition ref="B2:B522"/>
@@ -16951,7 +16928,7 @@
   </sheetPr>
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
@@ -20158,8 +20135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62560919-E4A0-3A4F-9164-3F35B35B852C}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -20247,7 +20224,7 @@
       <c r="I6" s="70" t="s">
         <v>1115</v>
       </c>
-      <c r="J6" s="120"/>
+      <c r="J6" s="117"/>
     </row>
     <row r="7" spans="1:10" ht="32">
       <c r="B7" s="11"/>
@@ -20303,7 +20280,7 @@
       <c r="G9" s="20"/>
       <c r="H9" s="103"/>
       <c r="I9" s="103"/>
-      <c r="J9" s="124">
+      <c r="J9" s="120">
         <f>SUM(C9:I9)</f>
         <v>0</v>
       </c>
@@ -20321,7 +20298,7 @@
       <c r="G10" s="20"/>
       <c r="H10" s="103"/>
       <c r="I10" s="103"/>
-      <c r="J10" s="124">
+      <c r="J10" s="120">
         <f t="shared" ref="J10:J18" si="0">SUM(C10:I10)</f>
         <v>0</v>
       </c>
@@ -20339,7 +20316,7 @@
       <c r="G11" s="20"/>
       <c r="H11" s="103"/>
       <c r="I11" s="103"/>
-      <c r="J11" s="124">
+      <c r="J11" s="120">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -20357,7 +20334,7 @@
       <c r="G12" s="20"/>
       <c r="H12" s="103"/>
       <c r="I12" s="103"/>
-      <c r="J12" s="124">
+      <c r="J12" s="120">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -20375,7 +20352,7 @@
       <c r="G13" s="20"/>
       <c r="H13" s="103"/>
       <c r="I13" s="103"/>
-      <c r="J13" s="124">
+      <c r="J13" s="120">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -20393,7 +20370,7 @@
       <c r="G14" s="20"/>
       <c r="H14" s="103"/>
       <c r="I14" s="103"/>
-      <c r="J14" s="124">
+      <c r="J14" s="120">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -20411,7 +20388,7 @@
       <c r="G15" s="20"/>
       <c r="H15" s="103"/>
       <c r="I15" s="103"/>
-      <c r="J15" s="124">
+      <c r="J15" s="120">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -20429,7 +20406,7 @@
       <c r="G16" s="20"/>
       <c r="H16" s="103"/>
       <c r="I16" s="103"/>
-      <c r="J16" s="124">
+      <c r="J16" s="120">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -20447,7 +20424,7 @@
       <c r="G17" s="20"/>
       <c r="H17" s="103"/>
       <c r="I17" s="103"/>
-      <c r="J17" s="124">
+      <c r="J17" s="120">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -20465,7 +20442,7 @@
       <c r="G18" s="20"/>
       <c r="H18" s="103"/>
       <c r="I18" s="103"/>
-      <c r="J18" s="124">
+      <c r="J18" s="120">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -20505,7 +20482,7 @@
         <f t="shared" ref="I19" si="2">SUM(I9:I18)</f>
         <v>0</v>
       </c>
-      <c r="J19" s="121">
+      <c r="J19" s="104">
         <f>SUM(C19:I19)</f>
         <v>0</v>
       </c>
@@ -20544,7 +20521,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="105"/>
       <c r="I22" s="105"/>
-      <c r="J22" s="122">
+      <c r="J22" s="118">
         <f>SUM(C22:I22)</f>
         <v>0</v>
       </c>
@@ -20562,7 +20539,7 @@
       <c r="G23" s="19"/>
       <c r="H23" s="106"/>
       <c r="I23" s="106"/>
-      <c r="J23" s="122">
+      <c r="J23" s="118">
         <f t="shared" ref="J23:J27" si="3">SUM(C23:I23)</f>
         <v>0</v>
       </c>
@@ -20580,7 +20557,7 @@
       <c r="G24" s="19"/>
       <c r="H24" s="106"/>
       <c r="I24" s="106"/>
-      <c r="J24" s="122">
+      <c r="J24" s="118">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -20598,7 +20575,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="106"/>
       <c r="I25" s="106"/>
-      <c r="J25" s="122">
+      <c r="J25" s="118">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -20616,7 +20593,7 @@
       <c r="G26" s="19"/>
       <c r="H26" s="106"/>
       <c r="I26" s="106"/>
-      <c r="J26" s="122">
+      <c r="J26" s="118">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -20634,7 +20611,7 @@
       <c r="G27" s="19"/>
       <c r="H27" s="106"/>
       <c r="I27" s="106"/>
-      <c r="J27" s="122">
+      <c r="J27" s="118">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -20652,7 +20629,7 @@
       <c r="G28" s="19"/>
       <c r="H28" s="106"/>
       <c r="I28" s="106"/>
-      <c r="J28" s="122">
+      <c r="J28" s="118">
         <f t="shared" ref="J28:J31" si="4">SUM(C28:I28)</f>
         <v>0</v>
       </c>
@@ -20670,7 +20647,7 @@
       <c r="G29" s="20"/>
       <c r="H29" s="103"/>
       <c r="I29" s="103"/>
-      <c r="J29" s="122">
+      <c r="J29" s="118">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -20688,7 +20665,7 @@
       <c r="G30" s="20"/>
       <c r="H30" s="103"/>
       <c r="I30" s="103"/>
-      <c r="J30" s="122">
+      <c r="J30" s="118">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -20706,7 +20683,7 @@
       <c r="G31" s="20"/>
       <c r="H31" s="103"/>
       <c r="I31" s="103"/>
-      <c r="J31" s="122">
+      <c r="J31" s="118">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -20746,7 +20723,7 @@
         <f t="shared" ref="I32" si="6">SUM(I22:I31)</f>
         <v>0</v>
       </c>
-      <c r="J32" s="123">
+      <c r="J32" s="119">
         <f>SUM(C32:I32)</f>
         <v>0</v>
       </c>
@@ -20772,7 +20749,7 @@
       <c r="G34" s="20"/>
       <c r="H34" s="107"/>
       <c r="I34" s="107"/>
-      <c r="J34" s="126">
+      <c r="J34" s="121">
         <f>SUM(C34:I34)</f>
         <v>0</v>
       </c>
@@ -20790,7 +20767,7 @@
       <c r="G35" s="20"/>
       <c r="H35" s="107"/>
       <c r="I35" s="107"/>
-      <c r="J35" s="126">
+      <c r="J35" s="121">
         <f>SUM(C35:I35)</f>
         <v>0</v>
       </c>
@@ -20808,7 +20785,7 @@
       <c r="G36" s="20"/>
       <c r="H36" s="107"/>
       <c r="I36" s="107"/>
-      <c r="J36" s="126">
+      <c r="J36" s="121">
         <f t="shared" ref="J36:J43" si="7">SUM(C36:I36)</f>
         <v>0</v>
       </c>
@@ -20826,7 +20803,7 @@
       <c r="G37" s="20"/>
       <c r="H37" s="107"/>
       <c r="I37" s="107"/>
-      <c r="J37" s="126">
+      <c r="J37" s="121">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -20844,7 +20821,7 @@
       <c r="G38" s="20"/>
       <c r="H38" s="107"/>
       <c r="I38" s="107"/>
-      <c r="J38" s="126">
+      <c r="J38" s="121">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -20862,7 +20839,7 @@
       <c r="G39" s="20"/>
       <c r="H39" s="107"/>
       <c r="I39" s="107"/>
-      <c r="J39" s="126">
+      <c r="J39" s="121">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -20880,7 +20857,7 @@
       <c r="G40" s="20"/>
       <c r="H40" s="107"/>
       <c r="I40" s="107"/>
-      <c r="J40" s="126">
+      <c r="J40" s="121">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -20898,7 +20875,7 @@
       <c r="G41" s="20"/>
       <c r="H41" s="107"/>
       <c r="I41" s="107"/>
-      <c r="J41" s="126">
+      <c r="J41" s="121">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -20916,7 +20893,7 @@
       <c r="G42" s="20"/>
       <c r="H42" s="107"/>
       <c r="I42" s="107"/>
-      <c r="J42" s="126">
+      <c r="J42" s="121">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -20934,7 +20911,7 @@
       <c r="G43" s="20"/>
       <c r="H43" s="107"/>
       <c r="I43" s="107"/>
-      <c r="J43" s="126">
+      <c r="J43" s="121">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -20947,31 +20924,31 @@
         <v>46</v>
       </c>
       <c r="C44" s="101">
-        <f>SUM(C34:C43)</f>
+        <f t="shared" ref="C44:I44" si="8">SUM(C34:C43)</f>
         <v>0</v>
       </c>
       <c r="D44" s="101">
-        <f>SUM(D34:D43)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E44" s="101">
-        <f>SUM(E34:E43)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F44" s="101">
-        <f>SUM(F34:F43)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G44" s="101">
-        <f>SUM(G34:G43)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H44" s="101">
-        <f>SUM(H34:H43)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I44" s="101">
-        <f>SUM(I34:I43)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J44" s="101">
@@ -21000,7 +20977,7 @@
       <c r="G46" s="19"/>
       <c r="H46" s="105"/>
       <c r="I46" s="105"/>
-      <c r="J46" s="122">
+      <c r="J46" s="118">
         <f>SUM(C46:I46)</f>
         <v>0</v>
       </c>
@@ -21018,8 +20995,8 @@
       <c r="G47" s="19"/>
       <c r="H47" s="106"/>
       <c r="I47" s="106"/>
-      <c r="J47" s="122">
-        <f t="shared" ref="J47:J56" si="8">SUM(C47:I47)</f>
+      <c r="J47" s="118">
+        <f t="shared" ref="J47:J56" si="9">SUM(C47:I47)</f>
         <v>0</v>
       </c>
     </row>
@@ -21036,8 +21013,8 @@
       <c r="G48" s="20"/>
       <c r="H48" s="103"/>
       <c r="I48" s="103"/>
-      <c r="J48" s="122">
-        <f t="shared" si="8"/>
+      <c r="J48" s="118">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -21054,17 +21031,19 @@
       <c r="G49" s="20"/>
       <c r="H49" s="103"/>
       <c r="I49" s="103"/>
-      <c r="J49" s="122">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="15">
+      <c r="J49" s="118">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="16">
       <c r="A50" s="8" t="str">
         <f>IF(B50="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B50,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>Choose from drop-down --&gt;</v>
-      </c>
-      <c r="B50" s="112"/>
+        <v>acfr:AccruedConnectionFees</v>
+      </c>
+      <c r="B50" s="112" t="s">
+        <v>571</v>
+      </c>
       <c r="C50" s="19"/>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
@@ -21072,8 +21051,8 @@
       <c r="G50" s="20"/>
       <c r="H50" s="103"/>
       <c r="I50" s="103"/>
-      <c r="J50" s="122">
-        <f t="shared" si="8"/>
+      <c r="J50" s="118">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -21090,8 +21069,8 @@
       <c r="G51" s="20"/>
       <c r="H51" s="103"/>
       <c r="I51" s="103"/>
-      <c r="J51" s="122">
-        <f t="shared" si="8"/>
+      <c r="J51" s="118">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -21108,8 +21087,8 @@
       <c r="G52" s="20"/>
       <c r="H52" s="103"/>
       <c r="I52" s="103"/>
-      <c r="J52" s="122">
-        <f t="shared" si="8"/>
+      <c r="J52" s="118">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -21126,8 +21105,8 @@
       <c r="G53" s="20"/>
       <c r="H53" s="103"/>
       <c r="I53" s="103"/>
-      <c r="J53" s="122">
-        <f t="shared" si="8"/>
+      <c r="J53" s="118">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -21144,8 +21123,8 @@
       <c r="G54" s="20"/>
       <c r="H54" s="103"/>
       <c r="I54" s="103"/>
-      <c r="J54" s="122">
-        <f t="shared" si="8"/>
+      <c r="J54" s="118">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -21162,8 +21141,8 @@
       <c r="G55" s="20"/>
       <c r="H55" s="103"/>
       <c r="I55" s="103"/>
-      <c r="J55" s="122">
-        <f t="shared" si="8"/>
+      <c r="J55" s="118">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -21180,8 +21159,8 @@
       <c r="G56" s="20"/>
       <c r="H56" s="103"/>
       <c r="I56" s="103"/>
-      <c r="J56" s="122">
-        <f t="shared" si="8"/>
+      <c r="J56" s="118">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -21193,34 +21172,34 @@
         <v>1750</v>
       </c>
       <c r="C57" s="101">
-        <f t="shared" ref="C57:H57" si="9">SUM(C46:C56)</f>
+        <f t="shared" ref="C57:H57" si="10">SUM(C46:C56)</f>
         <v>0</v>
       </c>
       <c r="D57" s="101">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="E57" s="101">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F57" s="101">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G57" s="101">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="H57" s="125">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="I57" s="125">
-        <f t="shared" ref="I57" si="10">SUM(I46:I56)</f>
-        <v>0</v>
-      </c>
-      <c r="J57" s="123">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H57" s="119">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I57" s="119">
+        <f t="shared" ref="I57" si="11">SUM(I46:I56)</f>
+        <v>0</v>
+      </c>
+      <c r="J57" s="119">
         <f>SUM(C57:I57)</f>
         <v>0</v>
       </c>
@@ -21242,7 +21221,7 @@
       <c r="J58" s="104"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C57:G57 D58 D8:G18 D20:G20 D22:G31 D34:G43 D46:G56 C32:I32 C44:I44">
+  <conditionalFormatting sqref="D8:G18 D20:G20 D22:G31 C32:I32 D34:G43 C44:I44 D46:G56 C57:G57 D58">
     <cfRule type="expression" dxfId="17" priority="51" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
@@ -21277,10 +21256,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAF299C-3D3B-8F47-AA92-8FD95A662E81}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -21323,101 +21302,127 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15">
-      <c r="A6" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="110"/>
-    </row>
-    <row r="7" spans="1:2" ht="16">
-      <c r="A7" s="111" t="s">
+    <row r="6" spans="1:2" ht="32">
+      <c r="A6" s="111" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B6" s="111"/>
+    </row>
+    <row r="7" spans="1:2" ht="15">
+      <c r="A7" s="112"/>
+      <c r="B7" s="112"/>
+    </row>
+    <row r="8" spans="1:2" ht="16">
+      <c r="A8" s="111" t="s">
         <v>1756</v>
       </c>
-      <c r="B7" s="111"/>
-    </row>
-    <row r="8" spans="1:2" ht="34">
-      <c r="A8" s="61" t="s">
+      <c r="B8" s="111"/>
+    </row>
+    <row r="9" spans="1:2" ht="15">
+      <c r="A9" s="112"/>
+      <c r="B9" s="112"/>
+    </row>
+    <row r="10" spans="1:2" ht="15">
+      <c r="A10" s="112"/>
+      <c r="B10" s="112"/>
+    </row>
+    <row r="11" spans="1:2" ht="15">
+      <c r="A11" s="112"/>
+      <c r="B11" s="112"/>
+    </row>
+    <row r="12" spans="1:2" ht="15">
+      <c r="A12" s="112"/>
+      <c r="B12" s="112"/>
+    </row>
+    <row r="13" spans="1:2" ht="15">
+      <c r="A13" s="112"/>
+      <c r="B13" s="112"/>
+    </row>
+    <row r="14" spans="1:2" ht="48">
+      <c r="A14" s="111" t="s">
         <v>1757</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="34">
-      <c r="A9" s="61" t="s">
+      <c r="B14" s="111"/>
+    </row>
+    <row r="15" spans="1:2" ht="15">
+      <c r="A15" s="112"/>
+      <c r="B15" s="112"/>
+    </row>
+    <row r="16" spans="1:2" ht="15">
+      <c r="A16" s="112"/>
+      <c r="B16" s="112"/>
+    </row>
+    <row r="17" spans="1:2" ht="15">
+      <c r="A17" s="112"/>
+      <c r="B17" s="112"/>
+    </row>
+    <row r="18" spans="1:2" ht="15">
+      <c r="A18" s="112"/>
+      <c r="B18" s="112"/>
+    </row>
+    <row r="19" spans="1:2" ht="15">
+      <c r="A19" s="112"/>
+      <c r="B19" s="112"/>
+    </row>
+    <row r="20" spans="1:2" ht="32">
+      <c r="A20" s="111" t="s">
         <v>1758</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="48">
-      <c r="A10" s="111" t="s">
+      <c r="B20" s="111"/>
+    </row>
+    <row r="21" spans="1:2" ht="15">
+      <c r="A21" s="112"/>
+      <c r="B21" s="112"/>
+    </row>
+    <row r="22" spans="1:2" ht="15">
+      <c r="A22" s="112"/>
+      <c r="B22" s="112"/>
+    </row>
+    <row r="23" spans="1:2" ht="15">
+      <c r="A23" s="112"/>
+      <c r="B23" s="112"/>
+    </row>
+    <row r="24" spans="1:2" ht="15">
+      <c r="A24" s="112"/>
+      <c r="B24" s="112"/>
+    </row>
+    <row r="25" spans="1:2" ht="15">
+      <c r="A25" s="112"/>
+      <c r="B25" s="112"/>
+    </row>
+    <row r="26" spans="1:2" ht="48">
+      <c r="A26" s="111" t="s">
         <v>1759</v>
       </c>
-      <c r="B10" s="111"/>
-    </row>
-    <row r="11" spans="1:2" ht="68">
-      <c r="A11" s="61" t="s">
+      <c r="B26" s="111"/>
+    </row>
+    <row r="27" spans="1:2" ht="15">
+      <c r="A27" s="112"/>
+      <c r="B27" s="112"/>
+    </row>
+    <row r="28" spans="1:2" ht="15">
+      <c r="A28" s="112"/>
+      <c r="B28" s="112"/>
+    </row>
+    <row r="29" spans="1:2" ht="15">
+      <c r="A29" s="112"/>
+      <c r="B29" s="112"/>
+    </row>
+    <row r="30" spans="1:2" ht="15">
+      <c r="A30" s="112"/>
+      <c r="B30" s="112"/>
+    </row>
+    <row r="31" spans="1:2" ht="32">
+      <c r="A31" s="111" t="s">
         <v>1760</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="34">
-      <c r="A12" s="61" t="s">
-        <v>1761</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="68">
-      <c r="A13" s="61" t="s">
-        <v>1763</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="68">
-      <c r="A14" s="61" t="s">
-        <v>1762</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="32">
-      <c r="A15" s="111" t="s">
-        <v>1764</v>
-      </c>
-      <c r="B15" s="111"/>
-    </row>
-    <row r="16" spans="1:2" ht="51">
-      <c r="A16" s="61" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="51">
-      <c r="A17" s="61" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="51">
-      <c r="A18" s="61" t="s">
-        <v>1767</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="51">
-      <c r="A19" s="61" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="48">
-      <c r="A20" s="111" t="s">
-        <v>1769</v>
-      </c>
-      <c r="B20" s="111"/>
-    </row>
-    <row r="21" spans="1:2" ht="221">
-      <c r="A21" s="61" t="s">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="32">
-      <c r="A22" s="111" t="s">
-        <v>1771</v>
-      </c>
-      <c r="B22">
-        <f>SUM(B21, B16:B19, B11:B14, B8:B9)</f>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A15:B19 A9:B13 A21:B25 A27:B30 A7:B7" xr:uid="{A0810FF0-C7CF-774D-8C40-611438650983}">
+      <formula1>current_liabilities</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -23113,12 +23118,12 @@
     </row>
     <row r="25" spans="1:5" ht="15">
       <c r="A25" s="7"/>
-      <c r="B25" s="117" t="s">
+      <c r="B25" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="118"/>
-      <c r="D25" s="118"/>
-      <c r="E25" s="119"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="123"/>
+      <c r="E25" s="124"/>
     </row>
     <row r="26" spans="1:5" ht="15">
       <c r="A26" s="8" t="str">

</xml_diff>

<commit_message>
pulled in total fund balance from other tab
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/byflow/Documents/Research/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0365E7B6-84E2-AC46-8A1E-4420972A1F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA10A89B-365A-7648-893C-3F968B47DA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="834" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Label Dropdowns" sheetId="8" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2645" uniqueCount="1764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2644" uniqueCount="1764">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -5878,7 +5878,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6131,6 +6131,11 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="44" fontId="22" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -6738,7 +6743,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D522"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B335" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G523" sqref="G523"/>
     </sheetView>
   </sheetViews>
@@ -22216,8 +22221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62560919-E4A0-3A4F-9164-3F35B35B852C}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -23117,14 +23122,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="16">
+    <row r="50" spans="1:10" ht="15">
       <c r="A50" s="8" t="str">
         <f>IF(B50="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B50,'Label Dropdowns'!$B$2:$B$522,'Label Dropdowns'!$C$2:$C$522))</f>
-        <v>acfr:AccruedConnectionFees</v>
-      </c>
-      <c r="B50" s="112" t="s">
-        <v>571</v>
-      </c>
+        <v>Choose from drop-down --&gt;</v>
+      </c>
+      <c r="B50" s="112"/>
       <c r="C50" s="19"/>
       <c r="D50" s="20"/>
       <c r="E50" s="20"/>
@@ -23337,10 +23340,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAF299C-3D3B-8F47-AA92-8FD95A662E81}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -23390,8 +23393,11 @@
       <c r="B6" s="111"/>
     </row>
     <row r="7" spans="1:2" ht="15">
-      <c r="A7" s="112"/>
-      <c r="B7" s="112"/>
+      <c r="A7" s="103"/>
+      <c r="B7" s="103">
+        <f>'GovFund Balance Sheet'!J57</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="16">
       <c r="A8" s="111" t="s">
@@ -23400,24 +23406,24 @@
       <c r="B8" s="111"/>
     </row>
     <row r="9" spans="1:2" ht="15">
-      <c r="A9" s="112"/>
-      <c r="B9" s="112"/>
+      <c r="A9" s="103"/>
+      <c r="B9" s="103"/>
     </row>
     <row r="10" spans="1:2" ht="15">
-      <c r="A10" s="112"/>
-      <c r="B10" s="112"/>
+      <c r="A10" s="103"/>
+      <c r="B10" s="103"/>
     </row>
     <row r="11" spans="1:2" ht="15">
-      <c r="A11" s="112"/>
-      <c r="B11" s="112"/>
+      <c r="A11" s="103"/>
+      <c r="B11" s="103"/>
     </row>
     <row r="12" spans="1:2" ht="15">
-      <c r="A12" s="112"/>
-      <c r="B12" s="112"/>
+      <c r="A12" s="103"/>
+      <c r="B12" s="103"/>
     </row>
     <row r="13" spans="1:2" ht="15">
-      <c r="A13" s="112"/>
-      <c r="B13" s="112"/>
+      <c r="A13" s="103"/>
+      <c r="B13" s="103"/>
     </row>
     <row r="14" spans="1:2" ht="48">
       <c r="A14" s="111" t="s">
@@ -23426,24 +23432,24 @@
       <c r="B14" s="111"/>
     </row>
     <row r="15" spans="1:2" ht="15">
-      <c r="A15" s="112"/>
-      <c r="B15" s="112"/>
+      <c r="A15" s="103"/>
+      <c r="B15" s="103"/>
     </row>
     <row r="16" spans="1:2" ht="15">
-      <c r="A16" s="112"/>
-      <c r="B16" s="112"/>
+      <c r="A16" s="103"/>
+      <c r="B16" s="103"/>
     </row>
     <row r="17" spans="1:2" ht="15">
-      <c r="A17" s="112"/>
-      <c r="B17" s="112"/>
+      <c r="A17" s="103"/>
+      <c r="B17" s="103"/>
     </row>
     <row r="18" spans="1:2" ht="15">
-      <c r="A18" s="112"/>
-      <c r="B18" s="112"/>
+      <c r="A18" s="103"/>
+      <c r="B18" s="103"/>
     </row>
     <row r="19" spans="1:2" ht="15">
-      <c r="A19" s="112"/>
-      <c r="B19" s="112"/>
+      <c r="A19" s="103"/>
+      <c r="B19" s="103"/>
     </row>
     <row r="20" spans="1:2" ht="32">
       <c r="A20" s="111" t="s">
@@ -23452,24 +23458,24 @@
       <c r="B20" s="111"/>
     </row>
     <row r="21" spans="1:2" ht="15">
-      <c r="A21" s="112"/>
-      <c r="B21" s="112"/>
+      <c r="A21" s="103"/>
+      <c r="B21" s="103"/>
     </row>
     <row r="22" spans="1:2" ht="15">
-      <c r="A22" s="112"/>
-      <c r="B22" s="112"/>
+      <c r="A22" s="103"/>
+      <c r="B22" s="103"/>
     </row>
     <row r="23" spans="1:2" ht="15">
-      <c r="A23" s="112"/>
-      <c r="B23" s="112"/>
+      <c r="A23" s="103"/>
+      <c r="B23" s="103"/>
     </row>
     <row r="24" spans="1:2" ht="15">
-      <c r="A24" s="112"/>
-      <c r="B24" s="112"/>
+      <c r="A24" s="103"/>
+      <c r="B24" s="103"/>
     </row>
     <row r="25" spans="1:2" ht="15">
-      <c r="A25" s="112"/>
-      <c r="B25" s="112"/>
+      <c r="A25" s="103"/>
+      <c r="B25" s="103"/>
     </row>
     <row r="26" spans="1:2" ht="48">
       <c r="A26" s="111" t="s">
@@ -23478,32 +23484,35 @@
       <c r="B26" s="111"/>
     </row>
     <row r="27" spans="1:2" ht="15">
-      <c r="A27" s="112"/>
-      <c r="B27" s="112"/>
+      <c r="A27" s="103"/>
+      <c r="B27" s="103"/>
     </row>
     <row r="28" spans="1:2" ht="15">
-      <c r="A28" s="112"/>
-      <c r="B28" s="112"/>
+      <c r="A28" s="103"/>
+      <c r="B28" s="103"/>
     </row>
     <row r="29" spans="1:2" ht="15">
-      <c r="A29" s="112"/>
-      <c r="B29" s="112"/>
+      <c r="A29" s="103"/>
+      <c r="B29" s="103"/>
     </row>
     <row r="30" spans="1:2" ht="15">
-      <c r="A30" s="112"/>
-      <c r="B30" s="112"/>
-    </row>
-    <row r="31" spans="1:2" ht="32">
-      <c r="A31" s="111" t="s">
+      <c r="A30" s="103"/>
+      <c r="B30" s="103"/>
+    </row>
+    <row r="31" spans="1:2" ht="15">
+      <c r="A31" s="103"/>
+      <c r="B31" s="125"/>
+    </row>
+    <row r="32" spans="1:2" ht="32">
+      <c r="A32" s="111" t="s">
         <v>1760</v>
       </c>
+      <c r="B32" s="126">
+        <f>SUM(B27:B31, B21:B25, B15:B19, B9:B13, B7)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A15:B19 A9:B13 A21:B25 A27:B30 A7:B7" xr:uid="{A0810FF0-C7CF-774D-8C40-611438650983}">
-      <formula1>current_liabilities</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
summed govfund balance sheet
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/byflow/Documents/Research/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA10A89B-365A-7648-893C-3F968B47DA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346C2F90-1591-CD4B-97FD-E8A157BC0E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="834" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5530,7 +5530,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5630,6 +5630,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -5878,7 +5884,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6136,6 +6142,12 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="23" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -22221,8 +22233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62560919-E4A0-3A4F-9164-3F35B35B852C}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -22534,41 +22546,41 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="16">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="127" t="s">
         <v>1754</v>
       </c>
-      <c r="B19" s="113" t="s">
+      <c r="B19" s="128" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C19" s="129">
         <f>SUM(C9:C18)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="129">
         <f>SUM(D9:D18)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="129">
         <f t="shared" ref="E19:H19" si="1">SUM(E9:E18)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="129">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="129">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="129">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I19" s="23">
+      <c r="I19" s="129">
         <f t="shared" ref="I19" si="2">SUM(I9:I18)</f>
         <v>0</v>
       </c>
-      <c r="J19" s="104">
+      <c r="J19" s="130">
         <f>SUM(C19:I19)</f>
         <v>0</v>
       </c>
@@ -23295,14 +23307,38 @@
       <c r="B58" s="113" t="s">
         <v>1749</v>
       </c>
-      <c r="C58" s="23"/>
-      <c r="D58" s="23"/>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23"/>
-      <c r="H58" s="104"/>
-      <c r="I58" s="104"/>
-      <c r="J58" s="104"/>
+      <c r="C58" s="23">
+        <f>SUM(C57, C44, C32, C19)</f>
+        <v>0</v>
+      </c>
+      <c r="D58" s="23">
+        <f>SUM(D57, D44, D32, D19)</f>
+        <v>0</v>
+      </c>
+      <c r="E58" s="23">
+        <f>SUM(E57, E44, E32, E19)</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="23">
+        <f>SUM(F57, F44, F32, F19)</f>
+        <v>0</v>
+      </c>
+      <c r="G58" s="23">
+        <f>SUM(G57, G44, G32, G19)</f>
+        <v>0</v>
+      </c>
+      <c r="H58" s="104">
+        <f>SUM(H57, H44, H32, H19)</f>
+        <v>0</v>
+      </c>
+      <c r="I58" s="104">
+        <f>SUM(I57, I44, I32, I19)</f>
+        <v>0</v>
+      </c>
+      <c r="J58" s="104">
+        <f>SUM(J57, J44, J32, J19)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D8:G18 D20:G20 D22:G31 C32:I32 D34:G43 C44:I44 D46:G56 C57:G57 D58">

</xml_diff>

<commit_message>
fixed error in stmt of activities lookup table
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADA7EA2-8226-244D-90C0-A1AD1788D139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963E8334-8A71-9C45-8AAE-F52DE9212834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="834" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="834" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Label Dropdowns" sheetId="8" r:id="rId1"/>
@@ -5269,7 +5269,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -5372,12 +5372,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Söhne Mono"/>
-      <family val="3"/>
     </font>
     <font>
       <b/>
@@ -5711,7 +5705,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5832,7 +5826,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5857,14 +5850,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -5873,7 +5866,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12099,22 +12092,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF490C29-31E1-3E46-B6B7-83D944E71A74}">
-  <dimension ref="A1:H218"/>
+  <dimension ref="A1:E218"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="37.83203125" customWidth="1"/>
-    <col min="3" max="3" width="33.83203125" customWidth="1"/>
-    <col min="4" max="4" width="38" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
+    <col min="4" max="4" width="33.83203125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" customHeight="1">
+    <row r="1" spans="1:5" ht="17" customHeight="1">
       <c r="A1" s="69" t="s">
         <v>57</v>
       </c>
@@ -12122,16 +12115,16 @@
         <v>1668</v>
       </c>
       <c r="C1" s="68" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D1" s="68" t="s">
         <v>1321</v>
-      </c>
-      <c r="D1" s="68" t="s">
-        <v>1322</v>
       </c>
       <c r="E1" s="69" t="s">
         <v>1438</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12139,17 +12132,16 @@
         <v>1439</v>
       </c>
       <c r="C2" s="65" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D2" s="65" t="s">
         <v>1134</v>
-      </c>
-      <c r="D2" s="65" t="s">
-        <v>1244</v>
       </c>
       <c r="E2" s="65" t="s">
         <v>1330</v>
       </c>
-      <c r="H2" s="71"/>
-    </row>
-    <row r="3" spans="1:8" ht="15">
+    </row>
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12157,16 +12149,16 @@
         <v>1440</v>
       </c>
       <c r="C3" s="65" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D3" s="65" t="s">
         <v>1135</v>
-      </c>
-      <c r="D3" s="65" t="s">
-        <v>1245</v>
       </c>
       <c r="E3" s="65" t="s">
         <v>1331</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:5" ht="15">
       <c r="A4" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12174,16 +12166,16 @@
         <v>1441</v>
       </c>
       <c r="C4" s="65" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D4" s="65" t="s">
         <v>1136</v>
-      </c>
-      <c r="D4" s="65" t="s">
-        <v>1246</v>
       </c>
       <c r="E4" s="65" t="s">
         <v>1332</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12191,16 +12183,16 @@
         <v>1442</v>
       </c>
       <c r="C5" s="65" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D5" s="65" t="s">
         <v>1137</v>
-      </c>
-      <c r="D5" s="65" t="s">
-        <v>1247</v>
       </c>
       <c r="E5" s="65" t="s">
         <v>1333</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:5" ht="15">
       <c r="A6" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12208,16 +12200,16 @@
         <v>1443</v>
       </c>
       <c r="C6" s="65" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D6" s="65" t="s">
         <v>1138</v>
-      </c>
-      <c r="D6" s="65" t="s">
-        <v>1248</v>
       </c>
       <c r="E6" s="65" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:5" ht="15">
       <c r="A7" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12225,16 +12217,16 @@
         <v>1444</v>
       </c>
       <c r="C7" s="65" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D7" s="65" t="s">
         <v>1139</v>
-      </c>
-      <c r="D7" s="65" t="s">
-        <v>1249</v>
       </c>
       <c r="E7" s="65" t="s">
         <v>1335</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15">
+    <row r="8" spans="1:5" ht="15">
       <c r="A8" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12242,16 +12234,16 @@
         <v>1445</v>
       </c>
       <c r="C8" s="65" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D8" s="65" t="s">
         <v>1140</v>
-      </c>
-      <c r="D8" s="65" t="s">
-        <v>1250</v>
       </c>
       <c r="E8" s="65" t="s">
         <v>1337</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:5" ht="15">
       <c r="A9" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12259,16 +12251,16 @@
         <v>1446</v>
       </c>
       <c r="C9" s="65" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D9" s="65" t="s">
         <v>1141</v>
-      </c>
-      <c r="D9" s="65" t="s">
-        <v>1251</v>
       </c>
       <c r="E9" s="65" t="s">
         <v>1338</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:5" ht="15">
       <c r="A10" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12276,16 +12268,16 @@
         <v>1447</v>
       </c>
       <c r="C10" s="65" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D10" s="65" t="s">
         <v>1142</v>
-      </c>
-      <c r="D10" s="65" t="s">
-        <v>1252</v>
       </c>
       <c r="E10" s="65" t="s">
         <v>1339</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15">
+    <row r="11" spans="1:5" ht="15">
       <c r="A11" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12293,16 +12285,16 @@
         <v>1448</v>
       </c>
       <c r="C11" s="65" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D11" s="65" t="s">
         <v>1143</v>
-      </c>
-      <c r="D11" s="65" t="s">
-        <v>1253</v>
       </c>
       <c r="E11" s="65" t="s">
         <v>1340</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15">
+    <row r="12" spans="1:5" ht="15">
       <c r="A12" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12310,16 +12302,16 @@
         <v>1449</v>
       </c>
       <c r="C12" s="65" t="s">
+        <v>1254</v>
+      </c>
+      <c r="D12" s="65" t="s">
         <v>1144</v>
-      </c>
-      <c r="D12" s="65" t="s">
-        <v>1254</v>
       </c>
       <c r="E12" s="65" t="s">
         <v>1341</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15">
+    <row r="13" spans="1:5" ht="15">
       <c r="A13" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12327,16 +12319,16 @@
         <v>1450</v>
       </c>
       <c r="C13" s="65" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D13" s="65" t="s">
         <v>1145</v>
-      </c>
-      <c r="D13" s="65" t="s">
-        <v>1255</v>
       </c>
       <c r="E13" s="65" t="s">
         <v>1342</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15">
+    <row r="14" spans="1:5" ht="15">
       <c r="A14" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12344,16 +12336,16 @@
         <v>1451</v>
       </c>
       <c r="C14" s="65" t="s">
+        <v>1256</v>
+      </c>
+      <c r="D14" s="65" t="s">
         <v>1146</v>
-      </c>
-      <c r="D14" s="65" t="s">
-        <v>1256</v>
       </c>
       <c r="E14" s="65" t="s">
         <v>1343</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15">
+    <row r="15" spans="1:5" ht="15">
       <c r="A15" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12361,16 +12353,16 @@
         <v>1452</v>
       </c>
       <c r="C15" s="65" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D15" s="65" t="s">
         <v>1147</v>
-      </c>
-      <c r="D15" s="65" t="s">
-        <v>1257</v>
       </c>
       <c r="E15" s="65" t="s">
         <v>1344</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15">
+    <row r="16" spans="1:5" ht="15">
       <c r="A16" s="2" t="s">
         <v>1537</v>
       </c>
@@ -12378,10 +12370,10 @@
         <v>1453</v>
       </c>
       <c r="C16" s="65" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D16" s="65" t="s">
         <v>1148</v>
-      </c>
-      <c r="D16" s="65" t="s">
-        <v>1258</v>
       </c>
       <c r="E16" s="65" t="s">
         <v>1345</v>
@@ -12395,10 +12387,10 @@
         <v>1454</v>
       </c>
       <c r="C17" s="65" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D17" s="65" t="s">
         <v>1149</v>
-      </c>
-      <c r="D17" s="65" t="s">
-        <v>1259</v>
       </c>
       <c r="E17" s="65" t="s">
         <v>1346</v>
@@ -12412,10 +12404,10 @@
         <v>1455</v>
       </c>
       <c r="C18" s="65" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D18" s="65" t="s">
         <v>1150</v>
-      </c>
-      <c r="D18" s="65" t="s">
-        <v>1260</v>
       </c>
       <c r="E18" s="65" t="s">
         <v>1347</v>
@@ -12429,10 +12421,10 @@
         <v>1456</v>
       </c>
       <c r="C19" s="65" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D19" s="65" t="s">
         <v>1151</v>
-      </c>
-      <c r="D19" s="65" t="s">
-        <v>1261</v>
       </c>
       <c r="E19" s="65" t="s">
         <v>1348</v>
@@ -12446,10 +12438,10 @@
         <v>1457</v>
       </c>
       <c r="C20" s="65" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D20" s="65" t="s">
         <v>1152</v>
-      </c>
-      <c r="D20" s="65" t="s">
-        <v>1262</v>
       </c>
       <c r="E20" s="65" t="s">
         <v>1349</v>
@@ -12463,10 +12455,10 @@
         <v>1458</v>
       </c>
       <c r="C21" s="65" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D21" s="65" t="s">
         <v>1153</v>
-      </c>
-      <c r="D21" s="65" t="s">
-        <v>1263</v>
       </c>
       <c r="E21" s="65" t="s">
         <v>1350</v>
@@ -12480,10 +12472,10 @@
         <v>1459</v>
       </c>
       <c r="C22" s="65" t="s">
+        <v>1264</v>
+      </c>
+      <c r="D22" s="65" t="s">
         <v>1154</v>
-      </c>
-      <c r="D22" s="65" t="s">
-        <v>1264</v>
       </c>
       <c r="E22" s="65" t="s">
         <v>1351</v>
@@ -12497,10 +12489,10 @@
         <v>1460</v>
       </c>
       <c r="C23" s="65" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D23" s="65" t="s">
         <v>1155</v>
-      </c>
-      <c r="D23" s="65" t="s">
-        <v>1265</v>
       </c>
       <c r="E23" s="65" t="s">
         <v>1352</v>
@@ -12514,10 +12506,10 @@
         <v>1461</v>
       </c>
       <c r="C24" s="65" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D24" s="65" t="s">
         <v>1156</v>
-      </c>
-      <c r="D24" s="65" t="s">
-        <v>1266</v>
       </c>
       <c r="E24" s="65" t="s">
         <v>1353</v>
@@ -12531,10 +12523,10 @@
         <v>1462</v>
       </c>
       <c r="C25" s="65" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D25" s="65" t="s">
         <v>1157</v>
-      </c>
-      <c r="D25" s="65" t="s">
-        <v>1267</v>
       </c>
       <c r="E25" s="65" t="s">
         <v>1354</v>
@@ -12548,10 +12540,10 @@
         <v>1463</v>
       </c>
       <c r="C26" s="65" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D26" s="65" t="s">
         <v>1158</v>
-      </c>
-      <c r="D26" s="65" t="s">
-        <v>1268</v>
       </c>
       <c r="E26" s="65" t="s">
         <v>1355</v>
@@ -12565,10 +12557,10 @@
         <v>1464</v>
       </c>
       <c r="C27" s="65" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D27" s="65" t="s">
         <v>1159</v>
-      </c>
-      <c r="D27" s="65" t="s">
-        <v>1269</v>
       </c>
       <c r="E27" s="65" t="s">
         <v>1356</v>
@@ -12582,10 +12574,10 @@
         <v>1465</v>
       </c>
       <c r="C28" s="65" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D28" s="65" t="s">
         <v>1160</v>
-      </c>
-      <c r="D28" s="65" t="s">
-        <v>1270</v>
       </c>
       <c r="E28" s="65" t="s">
         <v>1357</v>
@@ -12599,10 +12591,10 @@
         <v>1466</v>
       </c>
       <c r="C29" s="65" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D29" s="65" t="s">
         <v>1161</v>
-      </c>
-      <c r="D29" s="65" t="s">
-        <v>1271</v>
       </c>
       <c r="E29" s="65" t="s">
         <v>1358</v>
@@ -12616,10 +12608,10 @@
         <v>1467</v>
       </c>
       <c r="C30" s="65" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D30" s="65" t="s">
         <v>1162</v>
-      </c>
-      <c r="D30" s="65" t="s">
-        <v>1272</v>
       </c>
       <c r="E30" s="65" t="s">
         <v>1359</v>
@@ -12633,10 +12625,10 @@
         <v>1468</v>
       </c>
       <c r="C31" s="65" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D31" s="65" t="s">
         <v>1163</v>
-      </c>
-      <c r="D31" s="65" t="s">
-        <v>1273</v>
       </c>
       <c r="E31" s="65" t="s">
         <v>1360</v>
@@ -12650,10 +12642,10 @@
         <v>1469</v>
       </c>
       <c r="C32" s="65" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D32" s="65" t="s">
         <v>1164</v>
-      </c>
-      <c r="D32" s="65" t="s">
-        <v>1274</v>
       </c>
       <c r="E32" s="65" t="s">
         <v>1361</v>
@@ -12667,10 +12659,10 @@
         <v>1470</v>
       </c>
       <c r="C33" s="65" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D33" s="65" t="s">
         <v>1165</v>
-      </c>
-      <c r="D33" s="65" t="s">
-        <v>1275</v>
       </c>
       <c r="E33" s="65" t="s">
         <v>1362</v>
@@ -12684,10 +12676,10 @@
         <v>1471</v>
       </c>
       <c r="C34" s="65" t="s">
+        <v>1276</v>
+      </c>
+      <c r="D34" s="65" t="s">
         <v>1166</v>
-      </c>
-      <c r="D34" s="65" t="s">
-        <v>1276</v>
       </c>
       <c r="E34" s="65" t="s">
         <v>1363</v>
@@ -12701,10 +12693,10 @@
         <v>1472</v>
       </c>
       <c r="C35" s="65" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D35" s="65" t="s">
         <v>1167</v>
-      </c>
-      <c r="D35" s="65" t="s">
-        <v>1277</v>
       </c>
       <c r="E35" s="65" t="s">
         <v>1364</v>
@@ -12718,10 +12710,10 @@
         <v>1168</v>
       </c>
       <c r="C36" s="65" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D36" s="65" t="s">
         <v>1169</v>
-      </c>
-      <c r="D36" s="65" t="s">
-        <v>1278</v>
       </c>
       <c r="E36" s="65" t="s">
         <v>1365</v>
@@ -12735,10 +12727,10 @@
         <v>1473</v>
       </c>
       <c r="C37" s="65" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D37" s="65" t="s">
         <v>1170</v>
-      </c>
-      <c r="D37" s="65" t="s">
-        <v>1279</v>
       </c>
       <c r="E37" s="65" t="s">
         <v>1366</v>
@@ -12752,10 +12744,10 @@
         <v>1474</v>
       </c>
       <c r="C38" s="65" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D38" s="65" t="s">
         <v>1171</v>
-      </c>
-      <c r="D38" s="65" t="s">
-        <v>1288</v>
       </c>
       <c r="E38" s="65" t="s">
         <v>1405</v>
@@ -12769,10 +12761,10 @@
         <v>1475</v>
       </c>
       <c r="C39" s="65" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D39" s="65" t="s">
         <v>1172</v>
-      </c>
-      <c r="D39" s="65" t="s">
-        <v>1281</v>
       </c>
       <c r="E39" s="65" t="s">
         <v>1368</v>
@@ -12786,10 +12778,10 @@
         <v>1476</v>
       </c>
       <c r="C40" s="65" t="s">
+        <v>1282</v>
+      </c>
+      <c r="D40" s="65" t="s">
         <v>1173</v>
-      </c>
-      <c r="D40" s="65" t="s">
-        <v>1282</v>
       </c>
       <c r="E40" s="65" t="s">
         <v>1369</v>
@@ -12803,10 +12795,10 @@
         <v>1477</v>
       </c>
       <c r="C41" s="65" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D41" s="65" t="s">
         <v>1174</v>
-      </c>
-      <c r="D41" s="65" t="s">
-        <v>1283</v>
       </c>
       <c r="E41" s="65" t="s">
         <v>1370</v>
@@ -12820,10 +12812,10 @@
         <v>1478</v>
       </c>
       <c r="C42" s="65" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D42" s="65" t="s">
         <v>1175</v>
-      </c>
-      <c r="D42" s="65" t="s">
-        <v>1280</v>
       </c>
       <c r="E42" s="65" t="s">
         <v>1367</v>
@@ -12837,10 +12829,10 @@
         <v>1479</v>
       </c>
       <c r="C43" s="65" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D43" s="65" t="s">
         <v>1176</v>
-      </c>
-      <c r="D43" s="65" t="s">
-        <v>1284</v>
       </c>
       <c r="E43" s="65" t="s">
         <v>1371</v>
@@ -12854,10 +12846,10 @@
         <v>1480</v>
       </c>
       <c r="C44" s="65" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D44" s="65" t="s">
         <v>1177</v>
-      </c>
-      <c r="D44" s="65" t="s">
-        <v>1285</v>
       </c>
       <c r="E44" s="65" t="s">
         <v>1372</v>
@@ -12871,10 +12863,10 @@
         <v>1481</v>
       </c>
       <c r="C45" s="65" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D45" s="65" t="s">
         <v>1178</v>
-      </c>
-      <c r="D45" s="65" t="s">
-        <v>1286</v>
       </c>
       <c r="E45" s="65" t="s">
         <v>1373</v>
@@ -12887,10 +12879,10 @@
       <c r="B46" s="26" t="s">
         <v>1482</v>
       </c>
-      <c r="C46" s="65" t="s">
+      <c r="C46" s="26"/>
+      <c r="D46" s="65" t="s">
         <v>1179</v>
       </c>
-      <c r="D46" s="26"/>
       <c r="E46" s="65" t="s">
         <v>1374</v>
       </c>
@@ -12902,10 +12894,10 @@
       <c r="B47" s="26" t="s">
         <v>1483</v>
       </c>
-      <c r="C47" s="65" t="s">
+      <c r="C47" s="26"/>
+      <c r="D47" s="65" t="s">
         <v>1180</v>
       </c>
-      <c r="D47" s="26"/>
       <c r="E47" s="65" t="s">
         <v>1375</v>
       </c>
@@ -12917,10 +12909,10 @@
       <c r="B48" s="26" t="s">
         <v>1484</v>
       </c>
-      <c r="C48" s="65" t="s">
+      <c r="C48" s="26"/>
+      <c r="D48" s="65" t="s">
         <v>1181</v>
       </c>
-      <c r="D48" s="26"/>
       <c r="E48" s="65" t="s">
         <v>1376</v>
       </c>
@@ -12932,10 +12924,10 @@
       <c r="B49" s="26" t="s">
         <v>1485</v>
       </c>
-      <c r="C49" s="65" t="s">
+      <c r="C49" s="26"/>
+      <c r="D49" s="65" t="s">
         <v>1182</v>
       </c>
-      <c r="D49" s="26"/>
       <c r="E49" s="65" t="s">
         <v>1377</v>
       </c>
@@ -12947,10 +12939,10 @@
       <c r="B50" s="26" t="s">
         <v>1486</v>
       </c>
-      <c r="C50" s="65" t="s">
+      <c r="C50" s="26"/>
+      <c r="D50" s="65" t="s">
         <v>1183</v>
       </c>
-      <c r="D50" s="26"/>
       <c r="E50" s="65" t="s">
         <v>1378</v>
       </c>
@@ -12962,10 +12954,10 @@
       <c r="B51" s="26" t="s">
         <v>1487</v>
       </c>
-      <c r="C51" s="65" t="s">
+      <c r="C51" s="26"/>
+      <c r="D51" s="65" t="s">
         <v>1184</v>
       </c>
-      <c r="D51" s="26"/>
       <c r="E51" s="65" t="s">
         <v>1379</v>
       </c>
@@ -12977,10 +12969,10 @@
       <c r="B52" s="26" t="s">
         <v>1488</v>
       </c>
-      <c r="C52" s="65" t="s">
+      <c r="C52" s="26"/>
+      <c r="D52" s="65" t="s">
         <v>1185</v>
       </c>
-      <c r="D52" s="26"/>
       <c r="E52" s="65" t="s">
         <v>1380</v>
       </c>
@@ -12992,10 +12984,10 @@
       <c r="B53" s="26" t="s">
         <v>1489</v>
       </c>
-      <c r="C53" s="65" t="s">
+      <c r="C53" s="26"/>
+      <c r="D53" s="65" t="s">
         <v>1186</v>
       </c>
-      <c r="D53" s="26"/>
       <c r="E53" s="65" t="s">
         <v>1381</v>
       </c>
@@ -13007,10 +12999,10 @@
       <c r="B54" s="26" t="s">
         <v>1490</v>
       </c>
-      <c r="C54" s="65" t="s">
+      <c r="C54" s="26"/>
+      <c r="D54" s="65" t="s">
         <v>1187</v>
       </c>
-      <c r="D54" s="26"/>
       <c r="E54" s="65" t="s">
         <v>1382</v>
       </c>
@@ -13022,10 +13014,10 @@
       <c r="B55" s="26" t="s">
         <v>1491</v>
       </c>
-      <c r="C55" s="65" t="s">
+      <c r="C55" s="26"/>
+      <c r="D55" s="65" t="s">
         <v>1188</v>
       </c>
-      <c r="D55" s="26"/>
       <c r="E55" s="65" t="s">
         <v>1383</v>
       </c>
@@ -13037,10 +13029,10 @@
       <c r="B56" s="26" t="s">
         <v>1492</v>
       </c>
-      <c r="C56" s="65" t="s">
+      <c r="C56" s="26"/>
+      <c r="D56" s="65" t="s">
         <v>1189</v>
       </c>
-      <c r="D56" s="26"/>
       <c r="E56" s="65" t="s">
         <v>1384</v>
       </c>
@@ -13052,10 +13044,10 @@
       <c r="B57" s="26" t="s">
         <v>1493</v>
       </c>
-      <c r="C57" s="65" t="s">
+      <c r="C57" s="26"/>
+      <c r="D57" s="65" t="s">
         <v>1190</v>
       </c>
-      <c r="D57" s="26"/>
       <c r="E57" s="65" t="s">
         <v>1385</v>
       </c>
@@ -13067,10 +13059,10 @@
       <c r="B58" s="26" t="s">
         <v>1494</v>
       </c>
-      <c r="C58" s="65" t="s">
+      <c r="C58" s="26"/>
+      <c r="D58" s="65" t="s">
         <v>1191</v>
       </c>
-      <c r="D58" s="26"/>
       <c r="E58" s="65" t="s">
         <v>1386</v>
       </c>
@@ -13082,10 +13074,10 @@
       <c r="B59" s="26" t="s">
         <v>1495</v>
       </c>
-      <c r="C59" s="65" t="s">
+      <c r="C59" s="26"/>
+      <c r="D59" s="65" t="s">
         <v>1192</v>
       </c>
-      <c r="D59" s="26"/>
       <c r="E59" s="65" t="s">
         <v>1387</v>
       </c>
@@ -13097,10 +13089,10 @@
       <c r="B60" s="26" t="s">
         <v>1496</v>
       </c>
-      <c r="C60" s="65" t="s">
+      <c r="C60" s="26"/>
+      <c r="D60" s="65" t="s">
         <v>1193</v>
       </c>
-      <c r="D60" s="26"/>
       <c r="E60" s="65" t="s">
         <v>1388</v>
       </c>
@@ -13112,10 +13104,10 @@
       <c r="B61" s="26" t="s">
         <v>1497</v>
       </c>
-      <c r="C61" s="65" t="s">
+      <c r="C61" s="26"/>
+      <c r="D61" s="65" t="s">
         <v>1194</v>
       </c>
-      <c r="D61" s="26"/>
       <c r="E61" s="65" t="s">
         <v>1389</v>
       </c>
@@ -13127,10 +13119,10 @@
       <c r="B62" s="26" t="s">
         <v>1498</v>
       </c>
-      <c r="C62" s="65" t="s">
+      <c r="C62" s="26"/>
+      <c r="D62" s="65" t="s">
         <v>1195</v>
       </c>
-      <c r="D62" s="26"/>
       <c r="E62" s="65" t="s">
         <v>1390</v>
       </c>
@@ -13142,10 +13134,10 @@
       <c r="B63" s="26" t="s">
         <v>1499</v>
       </c>
-      <c r="C63" s="65" t="s">
+      <c r="C63" s="26"/>
+      <c r="D63" s="65" t="s">
         <v>1196</v>
       </c>
-      <c r="D63" s="26"/>
       <c r="E63" s="65" t="s">
         <v>1391</v>
       </c>
@@ -13157,10 +13149,10 @@
       <c r="B64" s="26" t="s">
         <v>1500</v>
       </c>
-      <c r="C64" s="65" t="s">
+      <c r="C64" s="26"/>
+      <c r="D64" s="65" t="s">
         <v>1197</v>
       </c>
-      <c r="D64" s="26"/>
       <c r="E64" s="65" t="s">
         <v>1392</v>
       </c>
@@ -13172,10 +13164,10 @@
       <c r="B65" s="26" t="s">
         <v>1501</v>
       </c>
-      <c r="C65" s="65" t="s">
+      <c r="C65" s="26"/>
+      <c r="D65" s="65" t="s">
         <v>1198</v>
       </c>
-      <c r="D65" s="26"/>
       <c r="E65" s="65" t="s">
         <v>1393</v>
       </c>
@@ -13187,10 +13179,10 @@
       <c r="B66" s="26" t="s">
         <v>1109</v>
       </c>
-      <c r="C66" s="65" t="s">
+      <c r="C66" s="26"/>
+      <c r="D66" s="65" t="s">
         <v>1199</v>
       </c>
-      <c r="D66" s="26"/>
       <c r="E66" s="65" t="s">
         <v>1394</v>
       </c>
@@ -13202,10 +13194,10 @@
       <c r="B67" s="26" t="s">
         <v>1502</v>
       </c>
-      <c r="C67" s="65" t="s">
+      <c r="C67" s="26"/>
+      <c r="D67" s="65" t="s">
         <v>1201</v>
       </c>
-      <c r="D67" s="26"/>
       <c r="E67" s="65" t="s">
         <v>1395</v>
       </c>
@@ -13217,10 +13209,10 @@
       <c r="B68" s="26" t="s">
         <v>1503</v>
       </c>
-      <c r="C68" s="65" t="s">
+      <c r="C68" s="26"/>
+      <c r="D68" s="65" t="s">
         <v>1203</v>
       </c>
-      <c r="D68" s="26"/>
       <c r="E68" s="65" t="s">
         <v>1396</v>
       </c>
@@ -13232,10 +13224,10 @@
       <c r="B69" s="26" t="s">
         <v>1504</v>
       </c>
-      <c r="C69" s="65" t="s">
+      <c r="C69" s="26"/>
+      <c r="D69" s="65" t="s">
         <v>1205</v>
       </c>
-      <c r="D69" s="26"/>
       <c r="E69" s="65" t="s">
         <v>1397</v>
       </c>
@@ -13247,10 +13239,10 @@
       <c r="B70" s="26" t="s">
         <v>1505</v>
       </c>
-      <c r="C70" s="65" t="s">
+      <c r="C70" s="26"/>
+      <c r="D70" s="65" t="s">
         <v>1207</v>
       </c>
-      <c r="D70" s="26"/>
       <c r="E70" s="65" t="s">
         <v>1398</v>
       </c>
@@ -13262,10 +13254,10 @@
       <c r="B71" s="26" t="s">
         <v>1208</v>
       </c>
-      <c r="C71" s="65" t="s">
+      <c r="C71" s="26"/>
+      <c r="D71" s="65" t="s">
         <v>1209</v>
       </c>
-      <c r="D71" s="26"/>
       <c r="E71" s="65" t="s">
         <v>1399</v>
       </c>
@@ -13277,10 +13269,10 @@
       <c r="B72" s="26" t="s">
         <v>1506</v>
       </c>
-      <c r="C72" s="65" t="s">
+      <c r="C72" s="26"/>
+      <c r="D72" s="65" t="s">
         <v>1211</v>
       </c>
-      <c r="D72" s="26"/>
       <c r="E72" s="65" t="s">
         <v>1400</v>
       </c>
@@ -13292,10 +13284,10 @@
       <c r="B73" s="26" t="s">
         <v>1507</v>
       </c>
-      <c r="C73" s="65" t="s">
+      <c r="C73" s="26"/>
+      <c r="D73" s="65" t="s">
         <v>1213</v>
       </c>
-      <c r="D73" s="26"/>
       <c r="E73" s="65" t="s">
         <v>1401</v>
       </c>
@@ -13307,10 +13299,10 @@
       <c r="B74" s="26" t="s">
         <v>1508</v>
       </c>
-      <c r="C74" s="65" t="s">
+      <c r="C74" s="26"/>
+      <c r="D74" s="65" t="s">
         <v>1215</v>
       </c>
-      <c r="D74" s="26"/>
       <c r="E74" s="65" t="s">
         <v>1402</v>
       </c>
@@ -13322,10 +13314,10 @@
       <c r="B75" s="26" t="s">
         <v>1509</v>
       </c>
-      <c r="C75" s="65" t="s">
+      <c r="C75" s="26"/>
+      <c r="D75" s="65" t="s">
         <v>1217</v>
       </c>
-      <c r="D75" s="26"/>
       <c r="E75" s="65" t="s">
         <v>1403</v>
       </c>
@@ -13338,10 +13330,10 @@
         <v>1510</v>
       </c>
       <c r="C76" s="65" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D76" s="65" t="s">
         <v>1218</v>
-      </c>
-      <c r="D76" s="65" t="s">
-        <v>1289</v>
       </c>
       <c r="E76" s="65" t="s">
         <v>1406</v>
@@ -13355,10 +13347,10 @@
         <v>1511</v>
       </c>
       <c r="C77" s="65" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D77" s="65" t="s">
         <v>1219</v>
-      </c>
-      <c r="D77" s="65" t="s">
-        <v>1293</v>
       </c>
       <c r="E77" s="65" t="s">
         <v>1410</v>
@@ -13372,10 +13364,10 @@
         <v>1512</v>
       </c>
       <c r="C78" s="65" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D78" s="65" t="s">
         <v>1220</v>
-      </c>
-      <c r="D78" s="65" t="s">
-        <v>1294</v>
       </c>
       <c r="E78" s="65" t="s">
         <v>1411</v>
@@ -13389,10 +13381,10 @@
         <v>1513</v>
       </c>
       <c r="C79" s="65" t="s">
+        <v>1290</v>
+      </c>
+      <c r="D79" s="65" t="s">
         <v>1221</v>
-      </c>
-      <c r="D79" s="65" t="s">
-        <v>1290</v>
       </c>
       <c r="E79" s="65" t="s">
         <v>1407</v>
@@ -13406,10 +13398,10 @@
         <v>1514</v>
       </c>
       <c r="C80" s="65" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D80" s="65" t="s">
         <v>1222</v>
-      </c>
-      <c r="D80" s="65" t="s">
-        <v>1292</v>
       </c>
       <c r="E80" s="65" t="s">
         <v>1409</v>
@@ -13423,10 +13415,10 @@
         <v>1515</v>
       </c>
       <c r="C81" s="65" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D81" s="65" t="s">
         <v>1223</v>
-      </c>
-      <c r="D81" s="65" t="s">
-        <v>1295</v>
       </c>
       <c r="E81" s="65" t="s">
         <v>1412</v>
@@ -13440,10 +13432,10 @@
         <v>1516</v>
       </c>
       <c r="C82" s="65" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D82" s="65" t="s">
         <v>1224</v>
-      </c>
-      <c r="D82" s="65" t="s">
-        <v>1296</v>
       </c>
       <c r="E82" s="65" t="s">
         <v>1413</v>
@@ -13457,10 +13449,10 @@
         <v>1517</v>
       </c>
       <c r="C83" s="65" t="s">
+        <v>1297</v>
+      </c>
+      <c r="D83" s="65" t="s">
         <v>1225</v>
-      </c>
-      <c r="D83" s="65" t="s">
-        <v>1297</v>
       </c>
       <c r="E83" s="65" t="s">
         <v>1414</v>
@@ -13474,10 +13466,10 @@
         <v>1518</v>
       </c>
       <c r="C84" s="65" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D84" s="65" t="s">
         <v>1226</v>
-      </c>
-      <c r="D84" s="65" t="s">
-        <v>1298</v>
       </c>
       <c r="E84" s="65" t="s">
         <v>1415</v>
@@ -13491,10 +13483,10 @@
         <v>1519</v>
       </c>
       <c r="C85" s="65" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D85" s="65" t="s">
         <v>1227</v>
-      </c>
-      <c r="D85" s="65" t="s">
-        <v>1299</v>
       </c>
       <c r="E85" s="65" t="s">
         <v>1416</v>
@@ -13508,10 +13500,10 @@
         <v>1520</v>
       </c>
       <c r="C86" s="65" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D86" s="65" t="s">
         <v>1228</v>
-      </c>
-      <c r="D86" s="65" t="s">
-        <v>1300</v>
       </c>
       <c r="E86" s="65" t="s">
         <v>1417</v>
@@ -13525,10 +13517,10 @@
         <v>1521</v>
       </c>
       <c r="C87" s="65" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D87" s="65" t="s">
         <v>1229</v>
-      </c>
-      <c r="D87" s="65" t="s">
-        <v>1301</v>
       </c>
       <c r="E87" s="65" t="s">
         <v>1418</v>
@@ -13542,10 +13534,10 @@
         <v>1522</v>
       </c>
       <c r="C88" s="65" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D88" s="65" t="s">
         <v>1230</v>
-      </c>
-      <c r="D88" s="65" t="s">
-        <v>1302</v>
       </c>
       <c r="E88" s="65" t="s">
         <v>1419</v>
@@ -13559,10 +13551,10 @@
         <v>1523</v>
       </c>
       <c r="C89" s="65" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D89" s="65" t="s">
         <v>1231</v>
-      </c>
-      <c r="D89" s="65" t="s">
-        <v>1304</v>
       </c>
       <c r="E89" s="65" t="s">
         <v>1420</v>
@@ -13576,10 +13568,10 @@
         <v>1524</v>
       </c>
       <c r="C90" s="65" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D90" s="65" t="s">
         <v>1232</v>
-      </c>
-      <c r="D90" s="65" t="s">
-        <v>1305</v>
       </c>
       <c r="E90" s="65" t="s">
         <v>1421</v>
@@ -13593,10 +13585,10 @@
         <v>1525</v>
       </c>
       <c r="C91" s="65" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D91" s="65" t="s">
         <v>1233</v>
-      </c>
-      <c r="D91" s="65" t="s">
-        <v>1306</v>
       </c>
       <c r="E91" s="65" t="s">
         <v>1422</v>
@@ -13610,10 +13602,10 @@
         <v>1526</v>
       </c>
       <c r="C92" s="65" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D92" s="65" t="s">
         <v>1234</v>
-      </c>
-      <c r="D92" s="65" t="s">
-        <v>1307</v>
       </c>
       <c r="E92" s="65" t="s">
         <v>1423</v>
@@ -13627,10 +13619,10 @@
         <v>1527</v>
       </c>
       <c r="C93" s="65" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D93" s="65" t="s">
         <v>1235</v>
-      </c>
-      <c r="D93" s="65" t="s">
-        <v>1308</v>
       </c>
       <c r="E93" s="65" t="s">
         <v>1424</v>
@@ -13644,10 +13636,10 @@
         <v>1528</v>
       </c>
       <c r="C94" s="65" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D94" s="65" t="s">
         <v>1236</v>
-      </c>
-      <c r="D94" s="65" t="s">
-        <v>1309</v>
       </c>
       <c r="E94" s="65" t="s">
         <v>1425</v>
@@ -13661,10 +13653,10 @@
         <v>1529</v>
       </c>
       <c r="C95" s="65" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D95" s="65" t="s">
         <v>1237</v>
-      </c>
-      <c r="D95" s="65" t="s">
-        <v>1310</v>
       </c>
       <c r="E95" s="65" t="s">
         <v>1426</v>
@@ -13678,10 +13670,10 @@
         <v>1530</v>
       </c>
       <c r="C96" s="65" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D96" s="65" t="s">
         <v>1238</v>
-      </c>
-      <c r="D96" s="65" t="s">
-        <v>1311</v>
       </c>
       <c r="E96" s="65" t="s">
         <v>1427</v>
@@ -13695,10 +13687,10 @@
         <v>1531</v>
       </c>
       <c r="C97" s="65" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D97" s="65" t="s">
         <v>1239</v>
-      </c>
-      <c r="D97" s="65" t="s">
-        <v>1312</v>
       </c>
       <c r="E97" s="65" t="s">
         <v>1428</v>
@@ -13711,10 +13703,10 @@
       <c r="B98" s="26" t="s">
         <v>1240</v>
       </c>
-      <c r="C98" s="65" t="s">
+      <c r="C98" s="26"/>
+      <c r="D98" s="65" t="s">
         <v>1241</v>
       </c>
-      <c r="D98" s="26"/>
       <c r="E98" s="65" t="s">
         <v>1429</v>
       </c>
@@ -13727,10 +13719,10 @@
         <v>1532</v>
       </c>
       <c r="C99" s="65" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D99" s="65" t="s">
         <v>1242</v>
-      </c>
-      <c r="D99" s="65" t="s">
-        <v>1320</v>
       </c>
       <c r="E99" s="65" t="s">
         <v>1436</v>
@@ -13744,10 +13736,10 @@
         <v>1120</v>
       </c>
       <c r="C100" s="65" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D100" s="65" t="s">
         <v>1243</v>
-      </c>
-      <c r="D100" s="65" t="s">
-        <v>1108</v>
       </c>
       <c r="E100" s="65" t="s">
         <v>1437</v>
@@ -13760,10 +13752,10 @@
       <c r="B101" s="26" t="s">
         <v>1533</v>
       </c>
-      <c r="C101" s="26"/>
-      <c r="D101" s="65" t="s">
+      <c r="C101" s="65" t="s">
         <v>1303</v>
       </c>
+      <c r="D101" s="26"/>
       <c r="E101" s="67"/>
     </row>
     <row r="102" spans="1:5" ht="15">
@@ -13773,10 +13765,10 @@
       <c r="B102" s="26" t="s">
         <v>1534</v>
       </c>
-      <c r="C102" s="26"/>
-      <c r="D102" s="65" t="s">
+      <c r="C102" s="65" t="s">
         <v>1287</v>
       </c>
+      <c r="D102" s="26"/>
       <c r="E102" s="65" t="s">
         <v>1404</v>
       </c>
@@ -13788,10 +13780,10 @@
       <c r="B103" s="26" t="s">
         <v>1535</v>
       </c>
-      <c r="C103" s="26"/>
-      <c r="D103" s="65" t="s">
+      <c r="C103" s="65" t="s">
         <v>1291</v>
       </c>
+      <c r="D103" s="26"/>
       <c r="E103" s="65" t="s">
         <v>1408</v>
       </c>
@@ -13803,10 +13795,10 @@
       <c r="B104" s="26" t="s">
         <v>1323</v>
       </c>
-      <c r="C104" s="26"/>
-      <c r="D104" s="65" t="s">
+      <c r="C104" s="65" t="s">
         <v>1313</v>
       </c>
+      <c r="D104" s="26"/>
       <c r="E104" s="65" t="s">
         <v>1430</v>
       </c>
@@ -13818,10 +13810,10 @@
       <c r="B105" s="26" t="s">
         <v>1324</v>
       </c>
-      <c r="C105" s="26"/>
-      <c r="D105" s="65" t="s">
+      <c r="C105" s="65" t="s">
         <v>1314</v>
       </c>
+      <c r="D105" s="26"/>
       <c r="E105" s="67"/>
     </row>
     <row r="106" spans="1:5" ht="15">
@@ -13831,10 +13823,10 @@
       <c r="B106" s="26" t="s">
         <v>1325</v>
       </c>
-      <c r="C106" s="26"/>
-      <c r="D106" s="65" t="s">
+      <c r="C106" s="65" t="s">
         <v>1315</v>
       </c>
+      <c r="D106" s="26"/>
       <c r="E106" s="65" t="s">
         <v>1431</v>
       </c>
@@ -13846,10 +13838,10 @@
       <c r="B107" s="26" t="s">
         <v>1326</v>
       </c>
-      <c r="C107" s="26"/>
-      <c r="D107" s="65" t="s">
+      <c r="C107" s="65" t="s">
         <v>1316</v>
       </c>
+      <c r="D107" s="26"/>
       <c r="E107" s="65" t="s">
         <v>1432</v>
       </c>
@@ -13861,10 +13853,10 @@
       <c r="B108" s="26" t="s">
         <v>1327</v>
       </c>
-      <c r="C108" s="26"/>
-      <c r="D108" s="65" t="s">
+      <c r="C108" s="65" t="s">
         <v>1317</v>
       </c>
+      <c r="D108" s="26"/>
       <c r="E108" s="65" t="s">
         <v>1433</v>
       </c>
@@ -13876,10 +13868,10 @@
       <c r="B109" s="26" t="s">
         <v>1328</v>
       </c>
-      <c r="C109" s="26"/>
-      <c r="D109" s="65" t="s">
+      <c r="C109" s="65" t="s">
         <v>1318</v>
       </c>
+      <c r="D109" s="26"/>
       <c r="E109" s="65" t="s">
         <v>1434</v>
       </c>
@@ -13891,10 +13883,10 @@
       <c r="B110" s="26" t="s">
         <v>1329</v>
       </c>
-      <c r="C110" s="26"/>
-      <c r="D110" s="65" t="s">
+      <c r="C110" s="65" t="s">
         <v>1319</v>
       </c>
+      <c r="D110" s="26"/>
       <c r="E110" s="65" t="s">
         <v>1435</v>
       </c>
@@ -13915,1170 +13907,1169 @@
       <c r="B112" s="65" t="s">
         <v>1672</v>
       </c>
-      <c r="C112" s="65" t="s">
+      <c r="D112" s="65" t="s">
         <v>1539</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="15">
+    <row r="113" spans="1:4" ht="15">
       <c r="A113" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B113" s="65" t="s">
         <v>1673</v>
       </c>
-      <c r="C113" s="65" t="s">
+      <c r="D113" s="65" t="s">
         <v>1540</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="15">
+    <row r="114" spans="1:4" ht="15">
       <c r="A114" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B114" s="65" t="s">
         <v>1674</v>
       </c>
-      <c r="C114" s="65" t="s">
+      <c r="D114" s="65" t="s">
         <v>1541</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="15">
+    <row r="115" spans="1:4" ht="15">
       <c r="A115" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B115" s="65" t="s">
         <v>1675</v>
       </c>
-      <c r="C115" s="65" t="s">
+      <c r="D115" s="65" t="s">
         <v>1542</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="15">
+    <row r="116" spans="1:4" ht="15">
       <c r="A116" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B116" s="65" t="s">
         <v>1676</v>
       </c>
-      <c r="C116" s="65" t="s">
+      <c r="D116" s="65" t="s">
         <v>1543</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="15">
+    <row r="117" spans="1:4" ht="15">
       <c r="A117" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B117" s="65" t="s">
         <v>1677</v>
       </c>
-      <c r="C117" s="65" t="s">
+      <c r="D117" s="65" t="s">
         <v>1544</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="15">
+    <row r="118" spans="1:4" ht="15">
       <c r="A118" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B118" s="65" t="s">
         <v>1678</v>
       </c>
-      <c r="C118" s="65" t="s">
+      <c r="D118" s="65" t="s">
         <v>1545</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="15">
+    <row r="119" spans="1:4" ht="15">
       <c r="A119" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B119" s="65" t="s">
         <v>1679</v>
       </c>
-      <c r="C119" s="65" t="s">
+      <c r="D119" s="65" t="s">
         <v>1546</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="15">
+    <row r="120" spans="1:4" ht="15">
       <c r="A120" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B120" s="65" t="s">
         <v>1680</v>
       </c>
-      <c r="C120" s="65" t="s">
+      <c r="D120" s="65" t="s">
         <v>1547</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="15">
+    <row r="121" spans="1:4" ht="15">
       <c r="A121" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B121" s="65" t="s">
         <v>1681</v>
       </c>
-      <c r="C121" s="65" t="s">
+      <c r="D121" s="65" t="s">
         <v>1548</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="15">
+    <row r="122" spans="1:4" ht="15">
       <c r="A122" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B122" s="65" t="s">
         <v>1682</v>
       </c>
-      <c r="C122" s="65" t="s">
+      <c r="D122" s="65" t="s">
         <v>1549</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="15">
+    <row r="123" spans="1:4" ht="15">
       <c r="A123" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B123" s="65" t="s">
         <v>1683</v>
       </c>
-      <c r="C123" s="65" t="s">
+      <c r="D123" s="65" t="s">
         <v>1550</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="15">
+    <row r="124" spans="1:4" ht="15">
       <c r="A124" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B124" s="65" t="s">
         <v>1684</v>
       </c>
-      <c r="C124" s="65" t="s">
+      <c r="D124" s="65" t="s">
         <v>1551</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="15">
+    <row r="125" spans="1:4" ht="15">
       <c r="A125" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B125" s="65" t="s">
         <v>1685</v>
       </c>
-      <c r="C125" s="65" t="s">
+      <c r="D125" s="65" t="s">
         <v>1552</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="15">
+    <row r="126" spans="1:4" ht="15">
       <c r="A126" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B126" s="65" t="s">
         <v>1686</v>
       </c>
-      <c r="C126" s="65" t="s">
+      <c r="D126" s="65" t="s">
         <v>1553</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="15">
+    <row r="127" spans="1:4" ht="15">
       <c r="A127" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B127" s="65" t="s">
         <v>1687</v>
       </c>
-      <c r="C127" s="65" t="s">
+      <c r="D127" s="65" t="s">
         <v>1554</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="15">
+    <row r="128" spans="1:4" ht="15">
       <c r="A128" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B128" s="65" t="s">
         <v>1688</v>
       </c>
-      <c r="C128" s="65" t="s">
+      <c r="D128" s="65" t="s">
         <v>1555</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="15">
+    <row r="129" spans="1:4" ht="15">
       <c r="A129" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B129" s="65" t="s">
         <v>1689</v>
       </c>
-      <c r="C129" s="65" t="s">
+      <c r="D129" s="65" t="s">
         <v>1556</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="15">
+    <row r="130" spans="1:4" ht="15">
       <c r="A130" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B130" s="65" t="s">
         <v>1690</v>
       </c>
-      <c r="C130" s="65" t="s">
+      <c r="D130" s="65" t="s">
         <v>1557</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="15">
+    <row r="131" spans="1:4" ht="15">
       <c r="A131" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B131" s="65" t="s">
         <v>1691</v>
       </c>
-      <c r="C131" s="65" t="s">
+      <c r="D131" s="65" t="s">
         <v>1558</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="15">
+    <row r="132" spans="1:4" ht="15">
       <c r="A132" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B132" s="65" t="s">
         <v>1692</v>
       </c>
-      <c r="C132" s="65" t="s">
+      <c r="D132" s="65" t="s">
         <v>1559</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="15">
+    <row r="133" spans="1:4" ht="15">
       <c r="A133" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B133" s="65" t="s">
         <v>1693</v>
       </c>
-      <c r="C133" s="65" t="s">
+      <c r="D133" s="65" t="s">
         <v>1560</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="15">
+    <row r="134" spans="1:4" ht="15">
       <c r="A134" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B134" s="65" t="s">
         <v>1694</v>
       </c>
-      <c r="C134" s="65" t="s">
+      <c r="D134" s="65" t="s">
         <v>1561</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="15">
+    <row r="135" spans="1:4" ht="15">
       <c r="A135" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B135" s="65" t="s">
         <v>1695</v>
       </c>
-      <c r="C135" s="65" t="s">
+      <c r="D135" s="65" t="s">
         <v>1562</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="15">
+    <row r="136" spans="1:4" ht="15">
       <c r="A136" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B136" s="65" t="s">
         <v>1696</v>
       </c>
-      <c r="C136" s="65" t="s">
+      <c r="D136" s="65" t="s">
         <v>1563</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="15">
+    <row r="137" spans="1:4" ht="15">
       <c r="A137" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B137" s="65" t="s">
         <v>1697</v>
       </c>
-      <c r="C137" s="65" t="s">
+      <c r="D137" s="65" t="s">
         <v>1564</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="15">
+    <row r="138" spans="1:4" ht="15">
       <c r="A138" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B138" s="65" t="s">
         <v>1698</v>
       </c>
-      <c r="C138" s="65" t="s">
+      <c r="D138" s="65" t="s">
         <v>1565</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="15">
+    <row r="139" spans="1:4" ht="15">
       <c r="A139" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B139" s="65" t="s">
         <v>1699</v>
       </c>
-      <c r="C139" s="65" t="s">
+      <c r="D139" s="65" t="s">
         <v>1566</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="15">
+    <row r="140" spans="1:4" ht="15">
       <c r="A140" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B140" s="65" t="s">
         <v>1700</v>
       </c>
-      <c r="C140" s="65" t="s">
+      <c r="D140" s="65" t="s">
         <v>1567</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="15">
+    <row r="141" spans="1:4" ht="15">
       <c r="A141" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B141" s="65" t="s">
         <v>1701</v>
       </c>
-      <c r="C141" s="65" t="s">
+      <c r="D141" s="65" t="s">
         <v>1568</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="15">
+    <row r="142" spans="1:4" ht="15">
       <c r="A142" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B142" s="65" t="s">
         <v>1702</v>
       </c>
-      <c r="C142" s="65" t="s">
+      <c r="D142" s="65" t="s">
         <v>1569</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="15">
+    <row r="143" spans="1:4" ht="15">
       <c r="A143" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B143" s="65" t="s">
         <v>1675</v>
       </c>
-      <c r="C143" s="65" t="s">
+      <c r="D143" s="65" t="s">
         <v>1542</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="15">
+    <row r="144" spans="1:4" ht="15">
       <c r="A144" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B144" s="65" t="s">
         <v>1703</v>
       </c>
-      <c r="C144" s="65" t="s">
+      <c r="D144" s="65" t="s">
         <v>1570</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="15">
+    <row r="145" spans="1:4" ht="15">
       <c r="A145" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B145" s="65" t="s">
         <v>1704</v>
       </c>
-      <c r="C145" s="65" t="s">
+      <c r="D145" s="65" t="s">
         <v>1571</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="15">
+    <row r="146" spans="1:4" ht="15">
       <c r="A146" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B146" s="65" t="s">
         <v>1705</v>
       </c>
-      <c r="C146" s="65" t="s">
+      <c r="D146" s="65" t="s">
         <v>1572</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="15">
+    <row r="147" spans="1:4" ht="15">
       <c r="A147" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B147" s="65" t="s">
         <v>1706</v>
       </c>
-      <c r="C147" s="65" t="s">
+      <c r="D147" s="65" t="s">
         <v>1573</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="15">
+    <row r="148" spans="1:4" ht="15">
       <c r="A148" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B148" s="65" t="s">
         <v>1574</v>
       </c>
-      <c r="C148" s="65" t="s">
+      <c r="D148" s="65" t="s">
         <v>1575</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="15">
+    <row r="149" spans="1:4" ht="15">
       <c r="A149" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B149" s="65" t="s">
         <v>1576</v>
       </c>
-      <c r="C149" s="65" t="s">
+      <c r="D149" s="65" t="s">
         <v>1577</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="15">
+    <row r="150" spans="1:4" ht="15">
       <c r="A150" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B150" s="65" t="s">
         <v>1707</v>
       </c>
-      <c r="C150" s="65" t="s">
+      <c r="D150" s="65" t="s">
         <v>1578</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="15">
+    <row r="151" spans="1:4" ht="15">
       <c r="A151" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B151" s="65" t="s">
         <v>1708</v>
       </c>
-      <c r="C151" s="65" t="s">
+      <c r="D151" s="65" t="s">
         <v>1579</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="15">
+    <row r="152" spans="1:4" ht="15">
       <c r="A152" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B152" s="65" t="s">
         <v>1709</v>
       </c>
-      <c r="C152" s="65" t="s">
+      <c r="D152" s="65" t="s">
         <v>1580</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="15">
+    <row r="153" spans="1:4" ht="15">
       <c r="A153" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B153" s="65" t="s">
         <v>1581</v>
       </c>
-      <c r="C153" s="65" t="s">
+      <c r="D153" s="65" t="s">
         <v>1582</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="15">
+    <row r="154" spans="1:4" ht="15">
       <c r="A154" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B154" s="65" t="s">
         <v>1710</v>
       </c>
-      <c r="C154" s="65" t="s">
+      <c r="D154" s="65" t="s">
         <v>1583</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="15">
+    <row r="155" spans="1:4" ht="15">
       <c r="A155" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B155" s="65" t="s">
         <v>1711</v>
       </c>
-      <c r="C155" s="65" t="s">
+      <c r="D155" s="65" t="s">
         <v>1584</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="15">
+    <row r="156" spans="1:4" ht="15">
       <c r="A156" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B156" s="65" t="s">
         <v>1712</v>
       </c>
-      <c r="C156" s="65" t="s">
+      <c r="D156" s="65" t="s">
         <v>1585</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="15">
+    <row r="157" spans="1:4" ht="15">
       <c r="A157" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B157" s="65" t="s">
         <v>1713</v>
       </c>
-      <c r="C157" s="65" t="s">
+      <c r="D157" s="65" t="s">
         <v>1586</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="15">
+    <row r="158" spans="1:4" ht="15">
       <c r="A158" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B158" s="65" t="s">
         <v>1587</v>
       </c>
-      <c r="C158" s="65" t="s">
+      <c r="D158" s="65" t="s">
         <v>1588</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="15">
+    <row r="159" spans="1:4" ht="15">
       <c r="A159" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B159" s="65" t="s">
         <v>1714</v>
       </c>
-      <c r="C159" s="65" t="s">
+      <c r="D159" s="65" t="s">
         <v>1589</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="15">
+    <row r="160" spans="1:4" ht="15">
       <c r="A160" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B160" s="65" t="s">
         <v>1590</v>
       </c>
-      <c r="C160" s="65" t="s">
+      <c r="D160" s="65" t="s">
         <v>1591</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="15">
+    <row r="161" spans="1:4" ht="15">
       <c r="A161" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B161" s="65" t="s">
         <v>1715</v>
       </c>
-      <c r="C161" s="65" t="s">
+      <c r="D161" s="65" t="s">
         <v>1592</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="15">
+    <row r="162" spans="1:4" ht="15">
       <c r="A162" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B162" s="65" t="s">
         <v>1716</v>
       </c>
-      <c r="C162" s="65" t="s">
+      <c r="D162" s="65" t="s">
         <v>1593</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="15">
+    <row r="163" spans="1:4" ht="15">
       <c r="A163" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B163" s="65" t="s">
         <v>1210</v>
       </c>
-      <c r="C163" s="65" t="s">
+      <c r="D163" s="65" t="s">
         <v>1211</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="15">
+    <row r="164" spans="1:4" ht="15">
       <c r="A164" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B164" s="65" t="s">
         <v>1212</v>
       </c>
-      <c r="C164" s="65" t="s">
+      <c r="D164" s="65" t="s">
         <v>1213</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="15">
+    <row r="165" spans="1:4" ht="15">
       <c r="A165" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B165" s="65" t="s">
         <v>1214</v>
       </c>
-      <c r="C165" s="65" t="s">
+      <c r="D165" s="65" t="s">
         <v>1215</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="15">
+    <row r="166" spans="1:4" ht="15">
       <c r="A166" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B166" s="65" t="s">
         <v>1216</v>
       </c>
-      <c r="C166" s="65" t="s">
+      <c r="D166" s="65" t="s">
         <v>1217</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="15">
+    <row r="167" spans="1:4" ht="15">
       <c r="A167" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B167" s="65" t="s">
         <v>1200</v>
       </c>
-      <c r="C167" s="65" t="s">
+      <c r="D167" s="65" t="s">
         <v>1201</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="15">
+    <row r="168" spans="1:4" ht="15">
       <c r="A168" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B168" s="65" t="s">
         <v>1202</v>
       </c>
-      <c r="C168" s="65" t="s">
+      <c r="D168" s="65" t="s">
         <v>1203</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="15">
+    <row r="169" spans="1:4" ht="15">
       <c r="A169" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B169" s="65" t="s">
         <v>1204</v>
       </c>
-      <c r="C169" s="65" t="s">
+      <c r="D169" s="65" t="s">
         <v>1205</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="15">
+    <row r="170" spans="1:4" ht="15">
       <c r="A170" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B170" s="65" t="s">
         <v>1206</v>
       </c>
-      <c r="C170" s="65" t="s">
+      <c r="D170" s="65" t="s">
         <v>1207</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="15">
+    <row r="171" spans="1:4" ht="15">
       <c r="A171" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B171" s="65" t="s">
         <v>1717</v>
       </c>
-      <c r="C171" s="65" t="s">
+      <c r="D171" s="65" t="s">
         <v>1209</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="15">
+    <row r="172" spans="1:4" ht="15">
       <c r="A172" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B172" s="65" t="s">
         <v>1718</v>
       </c>
-      <c r="C172" s="65" t="s">
+      <c r="D172" s="65" t="s">
         <v>1594</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="15">
+    <row r="173" spans="1:4" ht="15">
       <c r="A173" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B173" s="65" t="s">
         <v>1719</v>
       </c>
-      <c r="C173" s="65" t="s">
+      <c r="D173" s="65" t="s">
         <v>1595</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="15">
+    <row r="174" spans="1:4" ht="15">
       <c r="A174" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B174" s="65" t="s">
         <v>1720</v>
       </c>
-      <c r="C174" s="65" t="s">
+      <c r="D174" s="65" t="s">
         <v>1596</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="15">
+    <row r="175" spans="1:4" ht="15">
       <c r="A175" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B175" s="65" t="s">
         <v>1597</v>
       </c>
-      <c r="C175" s="65" t="s">
+      <c r="D175" s="65" t="s">
         <v>1598</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="15">
+    <row r="176" spans="1:4" ht="15">
       <c r="A176" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B176" s="65" t="s">
         <v>1720</v>
       </c>
-      <c r="C176" s="65" t="s">
+      <c r="D176" s="65" t="s">
         <v>1596</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="15">
+    <row r="177" spans="1:4" ht="15">
       <c r="A177" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B177" s="65" t="s">
         <v>1599</v>
       </c>
-      <c r="C177" s="65" t="s">
+      <c r="D177" s="65" t="s">
         <v>1600</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="15">
+    <row r="178" spans="1:4" ht="15">
       <c r="A178" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B178" s="65" t="s">
         <v>1721</v>
       </c>
-      <c r="C178" s="65" t="s">
+      <c r="D178" s="65" t="s">
         <v>1601</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="15">
+    <row r="179" spans="1:4" ht="15">
       <c r="A179" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B179" s="65" t="s">
         <v>1602</v>
       </c>
-      <c r="C179" s="65" t="s">
+      <c r="D179" s="65" t="s">
         <v>1603</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="15">
+    <row r="180" spans="1:4" ht="15">
       <c r="A180" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B180" s="65" t="s">
         <v>1604</v>
       </c>
-      <c r="C180" s="65" t="s">
+      <c r="D180" s="65" t="s">
         <v>1605</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="15">
+    <row r="181" spans="1:4" ht="15">
       <c r="A181" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B181" s="65" t="s">
         <v>1722</v>
       </c>
-      <c r="C181" s="65" t="s">
+      <c r="D181" s="65" t="s">
         <v>1606</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="15">
+    <row r="182" spans="1:4" ht="15">
       <c r="A182" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B182" s="65" t="s">
         <v>1723</v>
       </c>
-      <c r="C182" s="65" t="s">
+      <c r="D182" s="65" t="s">
         <v>1607</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="15">
+    <row r="183" spans="1:4" ht="15">
       <c r="A183" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B183" s="65" t="s">
         <v>1724</v>
       </c>
-      <c r="C183" s="65" t="s">
+      <c r="D183" s="65" t="s">
         <v>1608</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="15">
+    <row r="184" spans="1:4" ht="15">
       <c r="A184" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B184" s="65" t="s">
         <v>1725</v>
       </c>
-      <c r="C184" s="65" t="s">
+      <c r="D184" s="65" t="s">
         <v>1609</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="15">
+    <row r="185" spans="1:4" ht="15">
       <c r="A185" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B185" s="65" t="s">
         <v>1726</v>
       </c>
-      <c r="C185" s="65" t="s">
+      <c r="D185" s="65" t="s">
         <v>1610</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="15">
+    <row r="186" spans="1:4" ht="15">
       <c r="A186" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B186" s="65" t="s">
         <v>1727</v>
       </c>
-      <c r="C186" s="65" t="s">
+      <c r="D186" s="65" t="s">
         <v>1611</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="15">
+    <row r="187" spans="1:4" ht="15">
       <c r="A187" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B187" s="65" t="s">
         <v>1728</v>
       </c>
-      <c r="C187" s="65" t="s">
+      <c r="D187" s="65" t="s">
         <v>1612</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="15">
+    <row r="188" spans="1:4" ht="15">
       <c r="A188" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B188" s="65" t="s">
         <v>1729</v>
       </c>
-      <c r="C188" s="65" t="s">
+      <c r="D188" s="65" t="s">
         <v>1613</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="15">
+    <row r="189" spans="1:4" ht="15">
       <c r="A189" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B189" s="65" t="s">
         <v>1730</v>
       </c>
-      <c r="C189" s="65" t="s">
+      <c r="D189" s="65" t="s">
         <v>1614</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="15">
+    <row r="190" spans="1:4" ht="15">
       <c r="A190" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B190" s="65" t="s">
         <v>1731</v>
       </c>
-      <c r="C190" s="65" t="s">
+      <c r="D190" s="65" t="s">
         <v>1615</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="15">
+    <row r="191" spans="1:4" ht="15">
       <c r="A191" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B191" s="65" t="s">
         <v>1732</v>
       </c>
-      <c r="C191" s="65" t="s">
+      <c r="D191" s="65" t="s">
         <v>1616</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="15">
+    <row r="192" spans="1:4" ht="15">
       <c r="A192" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B192" s="65" t="s">
         <v>1617</v>
       </c>
-      <c r="C192" s="65" t="s">
+      <c r="D192" s="65" t="s">
         <v>1618</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="15">
+    <row r="193" spans="1:4" ht="15">
       <c r="A193" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B193" s="65" t="s">
         <v>1619</v>
       </c>
-      <c r="C193" s="65" t="s">
+      <c r="D193" s="65" t="s">
         <v>1620</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="15">
+    <row r="194" spans="1:4" ht="15">
       <c r="A194" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B194" s="65" t="s">
         <v>1621</v>
       </c>
-      <c r="C194" s="65" t="s">
+      <c r="D194" s="65" t="s">
         <v>1622</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="15">
+    <row r="195" spans="1:4" ht="15">
       <c r="A195" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B195" s="65" t="s">
         <v>1623</v>
       </c>
-      <c r="C195" s="65" t="s">
+      <c r="D195" s="65" t="s">
         <v>1624</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="15">
+    <row r="196" spans="1:4" ht="15">
       <c r="A196" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B196" s="65" t="s">
         <v>1625</v>
       </c>
-      <c r="C196" s="65" t="s">
+      <c r="D196" s="65" t="s">
         <v>1626</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="15">
+    <row r="197" spans="1:4" ht="15">
       <c r="A197" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B197" s="65" t="s">
         <v>1627</v>
       </c>
-      <c r="C197" s="65" t="s">
+      <c r="D197" s="65" t="s">
         <v>1628</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="15">
+    <row r="198" spans="1:4" ht="15">
       <c r="A198" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B198" s="65" t="s">
         <v>1629</v>
       </c>
-      <c r="C198" s="65" t="s">
+      <c r="D198" s="65" t="s">
         <v>1630</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="15">
+    <row r="199" spans="1:4" ht="15">
       <c r="A199" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B199" s="65" t="s">
         <v>1631</v>
       </c>
-      <c r="C199" s="65" t="s">
+      <c r="D199" s="65" t="s">
         <v>1632</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="15">
+    <row r="200" spans="1:4" ht="15">
       <c r="A200" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B200" s="65" t="s">
         <v>1633</v>
       </c>
-      <c r="C200" s="65" t="s">
+      <c r="D200" s="65" t="s">
         <v>1634</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="15">
+    <row r="201" spans="1:4" ht="15">
       <c r="A201" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B201" s="65" t="s">
         <v>1635</v>
       </c>
-      <c r="C201" s="65" t="s">
+      <c r="D201" s="65" t="s">
         <v>1636</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="15">
+    <row r="202" spans="1:4" ht="15">
       <c r="A202" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B202" s="65" t="s">
         <v>1637</v>
       </c>
-      <c r="C202" s="65" t="s">
+      <c r="D202" s="65" t="s">
         <v>1638</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="15">
+    <row r="203" spans="1:4" ht="15">
       <c r="A203" s="2" t="s">
         <v>1538</v>
       </c>
       <c r="B203" s="65" t="s">
         <v>1639</v>
       </c>
-      <c r="C203" s="65" t="s">
+      <c r="D203" s="65" t="s">
         <v>1640</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="15">
+    <row r="204" spans="1:4" ht="15">
       <c r="A204" s="2" t="s">
         <v>1667</v>
       </c>
       <c r="B204" s="70" t="s">
         <v>1641</v>
       </c>
-      <c r="C204" s="65" t="s">
+      <c r="D204" s="65" t="s">
         <v>1642</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="15">
+    <row r="205" spans="1:4" ht="15">
       <c r="A205" s="2" t="s">
         <v>1667</v>
       </c>
       <c r="B205" s="70" t="s">
         <v>1643</v>
       </c>
-      <c r="C205" s="65" t="s">
+      <c r="D205" s="65" t="s">
         <v>1644</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="15">
+    <row r="206" spans="1:4" ht="15">
       <c r="A206" s="2" t="s">
         <v>1667</v>
       </c>
       <c r="B206" s="70" t="s">
         <v>1645</v>
       </c>
-      <c r="C206" s="65" t="s">
+      <c r="D206" s="65" t="s">
         <v>1646</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="15">
+    <row r="207" spans="1:4" ht="15">
       <c r="A207" s="2" t="s">
         <v>1667</v>
       </c>
       <c r="B207" s="70" t="s">
         <v>1647</v>
       </c>
-      <c r="C207" s="65" t="s">
+      <c r="D207" s="65" t="s">
         <v>1648</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="15">
+    <row r="208" spans="1:4" ht="15">
       <c r="A208" s="2" t="s">
         <v>1667</v>
       </c>
       <c r="B208" s="70" t="s">
         <v>1649</v>
       </c>
-      <c r="C208" s="65" t="s">
+      <c r="D208" s="65" t="s">
         <v>1650</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="15">
+    <row r="209" spans="1:4" ht="15">
       <c r="A209" s="2" t="s">
         <v>1667</v>
       </c>
       <c r="B209" s="70" t="s">
         <v>1651</v>
       </c>
-      <c r="C209" s="65" t="s">
+      <c r="D209" s="65" t="s">
         <v>1652</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="15">
+    <row r="210" spans="1:4" ht="15">
       <c r="A210" s="2" t="s">
         <v>1667</v>
       </c>
       <c r="B210" s="70" t="s">
         <v>1653</v>
       </c>
-      <c r="C210" s="65" t="s">
+      <c r="D210" s="65" t="s">
         <v>1654</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="15">
+    <row r="211" spans="1:4" ht="15">
       <c r="A211" s="2" t="s">
         <v>1667</v>
       </c>
       <c r="B211" s="70" t="s">
         <v>1655</v>
       </c>
-      <c r="C211" s="65" t="s">
+      <c r="D211" s="65" t="s">
         <v>1656</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="15">
+    <row r="212" spans="1:4" ht="15">
       <c r="A212" s="2" t="s">
         <v>1667</v>
       </c>
       <c r="B212" s="70" t="s">
         <v>1657</v>
       </c>
-      <c r="C212" s="65" t="s">
+      <c r="D212" s="65" t="s">
         <v>1658</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="15">
+    <row r="213" spans="1:4" ht="15">
       <c r="A213" s="2" t="s">
         <v>1667</v>
       </c>
       <c r="B213" s="70" t="s">
         <v>1659</v>
       </c>
-      <c r="C213" s="65" t="s">
+      <c r="D213" s="65" t="s">
         <v>1660</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="15">
+    <row r="214" spans="1:4" ht="15">
       <c r="A214" s="2" t="s">
         <v>1667</v>
       </c>
       <c r="B214" s="70" t="s">
         <v>1661</v>
       </c>
-      <c r="C214" s="65" t="s">
+      <c r="D214" s="65" t="s">
         <v>1662</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="15">
+    <row r="215" spans="1:4" ht="15">
       <c r="A215" s="2" t="s">
         <v>1667</v>
       </c>
       <c r="B215" s="70" t="s">
         <v>1663</v>
       </c>
-      <c r="C215" s="65" t="s">
+      <c r="D215" s="65" t="s">
         <v>1664</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="15">
+    <row r="216" spans="1:4" ht="15">
       <c r="A216" s="2" t="s">
         <v>1667</v>
       </c>
       <c r="B216" s="70" t="s">
         <v>1627</v>
       </c>
-      <c r="C216" s="65" t="s">
+      <c r="D216" s="65" t="s">
         <v>1628</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="15">
+    <row r="217" spans="1:4" ht="15">
       <c r="A217" s="2" t="s">
         <v>1667</v>
       </c>
       <c r="B217" s="70" t="s">
         <v>1665</v>
       </c>
-      <c r="C217" s="65" t="s">
+      <c r="D217" s="65" t="s">
         <v>1666</v>
       </c>
     </row>
-    <row r="218" spans="1:3">
+    <row r="218" spans="1:4">
       <c r="A218" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -15111,7 +15102,7 @@
       <c r="B3" s="28" t="s">
         <v>1669</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="81" t="s">
         <v>1670</v>
       </c>
     </row>
@@ -16717,21 +16708,21 @@
       <c r="C4" s="43"/>
       <c r="D4" s="37"/>
     </row>
-    <row r="5" spans="1:10" s="79" customFormat="1" ht="64">
-      <c r="A5" s="72"/>
-      <c r="B5" s="73"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="81" t="s">
+    <row r="5" spans="1:10" s="78" customFormat="1" ht="64">
+      <c r="A5" s="71"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="80" t="s">
         <v>1120</v>
       </c>
-      <c r="E5" s="75"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="80" t="s">
+      <c r="E5" s="74"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="79" t="s">
         <v>1121</v>
       </c>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="78"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="77"/>
     </row>
     <row r="6" spans="1:10" ht="32">
       <c r="A6" s="4" t="s">
@@ -16791,7 +16782,7 @@
     </row>
     <row r="9" spans="1:10" ht="17" customHeight="1">
       <c r="A9" s="58" t="str">
-        <f>IF(B9="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B9,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B9,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B9,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B9="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B9,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B9,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B9,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B9" s="16"/>
@@ -16812,7 +16803,7 @@
     </row>
     <row r="10" spans="1:10" ht="15">
       <c r="A10" s="6" t="str">
-        <f>IF(B10="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B10,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B10,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B10,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B10="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B10,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B10,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B10,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B10" s="16"/>
@@ -16833,7 +16824,7 @@
     </row>
     <row r="11" spans="1:10" ht="15">
       <c r="A11" s="6" t="str">
-        <f>IF(B11="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B11,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B11,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B11,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B11="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B11,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B11,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B11,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B11" s="16"/>
@@ -16854,7 +16845,7 @@
     </row>
     <row r="12" spans="1:10" ht="15">
       <c r="A12" s="6" t="str">
-        <f>IF(B12="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B12,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B12,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B12,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B12="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B12,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B12,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B12,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B12" s="16"/>
@@ -16875,7 +16866,7 @@
     </row>
     <row r="13" spans="1:10" ht="15">
       <c r="A13" s="6" t="str">
-        <f>IF(B13="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B13,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B13,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B13,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B13="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B13,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B13,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B13,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B13" s="16"/>
@@ -16896,7 +16887,7 @@
     </row>
     <row r="14" spans="1:10" ht="15">
       <c r="A14" s="6" t="str">
-        <f>IF(B14="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B14,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B14,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B14,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B14="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B14,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B14,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B14,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B14" s="16"/>
@@ -16917,7 +16908,7 @@
     </row>
     <row r="15" spans="1:10" ht="15">
       <c r="A15" s="6" t="str">
-        <f>IF(B15="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B15,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B15,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B15,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B15="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B15,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B15,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B15,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B15" s="16"/>
@@ -16938,7 +16929,7 @@
     </row>
     <row r="16" spans="1:10" ht="15">
       <c r="A16" s="6" t="str">
-        <f>IF(B16="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B16,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B16,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B16,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B16="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B16,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B16,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B16,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B16" s="16"/>
@@ -16959,7 +16950,7 @@
     </row>
     <row r="17" spans="1:10" ht="15">
       <c r="A17" s="6" t="str">
-        <f>IF(B17="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B17,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B17,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B17,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B17="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B17,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B17,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B17,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B17" s="16"/>
@@ -16980,7 +16971,7 @@
     </row>
     <row r="18" spans="1:10" ht="15" hidden="1">
       <c r="A18" s="6" t="str">
-        <f>IF(B18="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B18,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B18,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B18,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B18="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B18,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B18,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B18,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B18" s="16"/>
@@ -17001,7 +16992,7 @@
     </row>
     <row r="19" spans="1:10" ht="15" hidden="1">
       <c r="A19" s="6" t="str">
-        <f>IF(B19="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B19,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B19,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B19,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B19="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B19,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B19,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B19,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B19" s="16"/>
@@ -17022,7 +17013,7 @@
     </row>
     <row r="20" spans="1:10" ht="15" hidden="1">
       <c r="A20" s="6" t="str">
-        <f>IF(B20="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B20,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B20,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B20,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B20="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B20,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B20,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B20,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B20" s="16"/>
@@ -17043,7 +17034,7 @@
     </row>
     <row r="21" spans="1:10" ht="15" hidden="1">
       <c r="A21" s="6" t="str">
-        <f>IF(B21="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B21,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B21,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B21,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B21="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B21,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B21,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B21,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B21" s="16"/>
@@ -17064,7 +17055,7 @@
     </row>
     <row r="22" spans="1:10" ht="15">
       <c r="A22" s="6" t="str">
-        <f>IF(B22="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B22,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B22,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B22,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B22="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B22,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B22,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B22,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B22" s="16"/>
@@ -17128,7 +17119,7 @@
     </row>
     <row r="25" spans="1:10" ht="15">
       <c r="A25" s="6" t="str">
-        <f>IF(B25="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B25,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B25,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B25,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B25="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B25,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B25,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B25,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B25" s="16"/>
@@ -17149,7 +17140,7 @@
     </row>
     <row r="26" spans="1:10" ht="15">
       <c r="A26" s="6" t="str">
-        <f>IF(B26="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B26,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B26,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B26,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B26="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B26,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B26,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B26,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B26" s="16"/>
@@ -17170,7 +17161,7 @@
     </row>
     <row r="27" spans="1:10" ht="15">
       <c r="A27" s="6" t="str">
-        <f>IF(B27="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B27,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B27,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B27,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B27="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B27,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B27,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B27,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B27" s="16"/>
@@ -17191,7 +17182,7 @@
     </row>
     <row r="28" spans="1:10" ht="15">
       <c r="A28" s="6" t="str">
-        <f>IF(B28="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B28,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B28,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B28,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B28="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B28,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B28,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B28,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B28" s="16"/>
@@ -17212,7 +17203,7 @@
     </row>
     <row r="29" spans="1:10" ht="15">
       <c r="A29" s="6" t="str">
-        <f>IF(B29="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B29,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B29,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B29,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B29="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B29,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B29,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B29,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B29" s="16"/>
@@ -17233,7 +17224,7 @@
     </row>
     <row r="30" spans="1:10" ht="15">
       <c r="A30" s="6" t="str">
-        <f>IF(B30="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B30,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B30,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B30,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B30="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B30,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B30,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B30,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B30" s="16"/>
@@ -17254,7 +17245,7 @@
     </row>
     <row r="31" spans="1:10" ht="15">
       <c r="A31" s="6" t="str">
-        <f>IF(B31="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B31,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B31,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B31,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B31="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B31,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B31,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B31,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B31" s="16"/>
@@ -17275,7 +17266,7 @@
     </row>
     <row r="32" spans="1:10" ht="15" hidden="1">
       <c r="A32" s="6" t="str">
-        <f>IF(B32="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B32,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B32,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B32,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B32="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B32,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B32,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B32,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B32" s="16"/>
@@ -17296,7 +17287,7 @@
     </row>
     <row r="33" spans="1:10" ht="15" hidden="1">
       <c r="A33" s="6" t="str">
-        <f>IF(B33="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B33,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B33,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B33,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B33="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B33,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B33,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B33,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B33" s="16"/>
@@ -17317,7 +17308,7 @@
     </row>
     <row r="34" spans="1:10" ht="15" hidden="1">
       <c r="A34" s="6" t="str">
-        <f>IF(B34="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B34,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B34,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B34,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B34="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B34,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B34,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B34,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B34" s="16"/>
@@ -17338,7 +17329,7 @@
     </row>
     <row r="35" spans="1:10" ht="15" hidden="1">
       <c r="A35" s="6" t="str">
-        <f>IF(B35="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B35,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B35,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B35,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B35="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B35,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B35,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B35,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B35" s="16"/>
@@ -17359,7 +17350,7 @@
     </row>
     <row r="36" spans="1:10" ht="15">
       <c r="A36" s="6" t="str">
-        <f>IF(B36="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B36,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B36,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B36,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B36="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B36,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B36,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B36,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B36" s="16"/>
@@ -17472,7 +17463,7 @@
     </row>
     <row r="41" spans="1:10" ht="15">
       <c r="A41" s="6" t="str">
-        <f>IF(B41="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B41,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B41,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B41,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B41="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B41,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B41,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B41,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B41" s="16"/>
@@ -17499,7 +17490,7 @@
     </row>
     <row r="42" spans="1:10" ht="15">
       <c r="A42" s="6" t="str">
-        <f>IF(B42="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B42,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B42,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B42,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B42="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B42,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B42,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B42,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B42" s="16"/>
@@ -17526,7 +17517,7 @@
     </row>
     <row r="43" spans="1:10" ht="15">
       <c r="A43" s="6" t="str">
-        <f>IF(B43="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B43,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B43,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B43,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B43="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B43,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B43,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B43,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B43" s="16"/>
@@ -17553,7 +17544,7 @@
     </row>
     <row r="44" spans="1:10" ht="15">
       <c r="A44" s="6" t="str">
-        <f>IF(B44="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B44,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B44,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B44,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B44="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B44,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B44,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B44,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B44" s="16"/>
@@ -17580,7 +17571,7 @@
     </row>
     <row r="45" spans="1:10" ht="15">
       <c r="A45" s="6" t="str">
-        <f>IF(B45="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B45,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B45,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B45,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B45="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B45,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B45,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B45,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B45" s="16"/>
@@ -17607,7 +17598,7 @@
     </row>
     <row r="46" spans="1:10" ht="15" hidden="1">
       <c r="A46" s="6" t="str">
-        <f>IF(B46="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B46,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B46,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B46,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B46="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B46,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B46,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B46,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B46" s="16"/>
@@ -17634,7 +17625,7 @@
     </row>
     <row r="47" spans="1:10" ht="15" hidden="1">
       <c r="A47" s="6" t="str">
-        <f>IF(B47="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B47,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B47,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B47,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B47="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B47,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B47,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B47,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B47" s="16"/>
@@ -17661,7 +17652,7 @@
     </row>
     <row r="48" spans="1:10" ht="15" hidden="1">
       <c r="A48" s="6" t="str">
-        <f>IF(B48="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B48,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B48,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B48,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B48="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B48,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B48,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B48,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B48" s="16"/>
@@ -17688,7 +17679,7 @@
     </row>
     <row r="49" spans="1:10" ht="15">
       <c r="A49" s="6" t="str">
-        <f>IF(B49="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B49,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C),",",_xlfn.XLOOKUP(B49,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D), ",",_xlfn.XLOOKUP(B49,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
+        <f>IF(B49="", "Choose from drop-down --&gt;", _xlfn.CONCAT(_xlfn.XLOOKUP(B49,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D),",",_xlfn.XLOOKUP(B49,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C), ",",_xlfn.XLOOKUP(B49,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$E:$E)))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B49" s="16"/>
@@ -17785,14 +17776,14 @@
     </row>
     <row r="54" spans="1:10" ht="15">
       <c r="A54" s="6" t="str">
-        <f>IF(B54="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B54,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B54="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B54,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B54" s="16"/>
-      <c r="C54" s="84"/>
-      <c r="D54" s="85"/>
-      <c r="E54" s="85"/>
-      <c r="F54" s="85"/>
+      <c r="C54" s="83"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="84"/>
+      <c r="F54" s="84"/>
       <c r="G54" s="18"/>
       <c r="H54" s="18"/>
       <c r="I54" s="15" t="str">
@@ -17803,14 +17794,14 @@
     </row>
     <row r="55" spans="1:10" ht="15">
       <c r="A55" s="6" t="str">
-        <f>IF(B55="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B55,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B55="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B55,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B55" s="16"/>
-      <c r="C55" s="84"/>
-      <c r="D55" s="85"/>
-      <c r="E55" s="85"/>
-      <c r="F55" s="85"/>
+      <c r="C55" s="83"/>
+      <c r="D55" s="84"/>
+      <c r="E55" s="84"/>
+      <c r="F55" s="84"/>
       <c r="G55" s="18"/>
       <c r="H55" s="18"/>
       <c r="I55" s="15" t="str">
@@ -17821,14 +17812,14 @@
     </row>
     <row r="56" spans="1:10" ht="15">
       <c r="A56" s="6" t="str">
-        <f>IF(B56="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B56,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B56="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B56,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B56" s="16"/>
-      <c r="C56" s="84"/>
-      <c r="D56" s="85"/>
-      <c r="E56" s="85"/>
-      <c r="F56" s="85"/>
+      <c r="C56" s="83"/>
+      <c r="D56" s="84"/>
+      <c r="E56" s="84"/>
+      <c r="F56" s="84"/>
       <c r="G56" s="18"/>
       <c r="H56" s="18"/>
       <c r="I56" s="15" t="str">
@@ -17839,14 +17830,14 @@
     </row>
     <row r="57" spans="1:10" ht="15">
       <c r="A57" s="6" t="str">
-        <f>IF(B57="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B57,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B57="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B57,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B57" s="16"/>
-      <c r="C57" s="84"/>
-      <c r="D57" s="85"/>
-      <c r="E57" s="85"/>
-      <c r="F57" s="85"/>
+      <c r="C57" s="83"/>
+      <c r="D57" s="84"/>
+      <c r="E57" s="84"/>
+      <c r="F57" s="84"/>
       <c r="G57" s="18"/>
       <c r="H57" s="18"/>
       <c r="I57" s="15" t="str">
@@ -17857,14 +17848,14 @@
     </row>
     <row r="58" spans="1:10" ht="15">
       <c r="A58" s="6" t="str">
-        <f>IF(B58="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B58,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B58="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B58,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B58" s="16"/>
-      <c r="C58" s="84"/>
-      <c r="D58" s="85"/>
-      <c r="E58" s="85"/>
-      <c r="F58" s="85"/>
+      <c r="C58" s="83"/>
+      <c r="D58" s="84"/>
+      <c r="E58" s="84"/>
+      <c r="F58" s="84"/>
       <c r="G58" s="18"/>
       <c r="H58" s="18"/>
       <c r="I58" s="15" t="str">
@@ -17875,14 +17866,14 @@
     </row>
     <row r="59" spans="1:10" ht="15">
       <c r="A59" s="6" t="str">
-        <f>IF(B59="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B59,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B59="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B59,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B59" s="16"/>
-      <c r="C59" s="84"/>
-      <c r="D59" s="85"/>
-      <c r="E59" s="85"/>
-      <c r="F59" s="85"/>
+      <c r="C59" s="83"/>
+      <c r="D59" s="84"/>
+      <c r="E59" s="84"/>
+      <c r="F59" s="84"/>
       <c r="G59" s="18"/>
       <c r="H59" s="18"/>
       <c r="I59" s="15" t="str">
@@ -17893,14 +17884,14 @@
     </row>
     <row r="60" spans="1:10" ht="15">
       <c r="A60" s="6" t="str">
-        <f>IF(B60="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B60,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B60="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B60,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B60" s="16"/>
-      <c r="C60" s="84"/>
-      <c r="D60" s="85"/>
-      <c r="E60" s="85"/>
-      <c r="F60" s="85"/>
+      <c r="C60" s="83"/>
+      <c r="D60" s="84"/>
+      <c r="E60" s="84"/>
+      <c r="F60" s="84"/>
       <c r="G60" s="18"/>
       <c r="H60" s="18"/>
       <c r="I60" s="15" t="str">
@@ -17911,14 +17902,14 @@
     </row>
     <row r="61" spans="1:10" ht="15">
       <c r="A61" s="6" t="str">
-        <f>IF(B61="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B61,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B61="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B61,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B61" s="16"/>
-      <c r="C61" s="84"/>
-      <c r="D61" s="85"/>
-      <c r="E61" s="85"/>
-      <c r="F61" s="85"/>
+      <c r="C61" s="83"/>
+      <c r="D61" s="84"/>
+      <c r="E61" s="84"/>
+      <c r="F61" s="84"/>
       <c r="G61" s="18"/>
       <c r="H61" s="18"/>
       <c r="I61" s="15" t="str">
@@ -17929,14 +17920,14 @@
     </row>
     <row r="62" spans="1:10" ht="15">
       <c r="A62" s="6" t="str">
-        <f>IF(B62="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B62,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B62="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B62,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B62" s="16"/>
-      <c r="C62" s="84"/>
-      <c r="D62" s="85"/>
-      <c r="E62" s="85"/>
-      <c r="F62" s="85"/>
+      <c r="C62" s="83"/>
+      <c r="D62" s="84"/>
+      <c r="E62" s="84"/>
+      <c r="F62" s="84"/>
       <c r="G62" s="18"/>
       <c r="H62" s="18"/>
       <c r="I62" s="15" t="str">
@@ -17947,14 +17938,14 @@
     </row>
     <row r="63" spans="1:10" ht="15">
       <c r="A63" s="6" t="str">
-        <f>IF(B63="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B63,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B63="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B63,'Statement of activities labels'!$B:$B, 'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B63" s="16"/>
-      <c r="C63" s="84"/>
-      <c r="D63" s="85"/>
-      <c r="E63" s="85"/>
-      <c r="F63" s="85"/>
+      <c r="C63" s="83"/>
+      <c r="D63" s="84"/>
+      <c r="E63" s="84"/>
+      <c r="F63" s="84"/>
       <c r="G63" s="18"/>
       <c r="H63" s="18"/>
       <c r="I63" s="15" t="str">
@@ -17996,20 +17987,20 @@
       <c r="B65" s="13" t="s">
         <v>1133</v>
       </c>
-      <c r="C65" s="86"/>
-      <c r="D65" s="86"/>
+      <c r="C65" s="85"/>
+      <c r="D65" s="85"/>
       <c r="I65" s="13"/>
     </row>
     <row r="66" spans="1:10" ht="15">
       <c r="A66" s="6" t="str">
-        <f>IF(B66="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B66,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B66="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B66,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B66" s="16"/>
-      <c r="C66" s="84"/>
-      <c r="D66" s="85"/>
-      <c r="E66" s="85"/>
-      <c r="F66" s="85"/>
+      <c r="C66" s="83"/>
+      <c r="D66" s="84"/>
+      <c r="E66" s="84"/>
+      <c r="F66" s="84"/>
       <c r="G66" s="18"/>
       <c r="H66" s="18"/>
       <c r="I66" s="15" t="str">
@@ -18020,14 +18011,14 @@
     </row>
     <row r="67" spans="1:10" ht="15">
       <c r="A67" s="6" t="str">
-        <f>IF(B67="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B67,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B67="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B67,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B67" s="16"/>
-      <c r="C67" s="84"/>
-      <c r="D67" s="85"/>
-      <c r="E67" s="85"/>
-      <c r="F67" s="85"/>
+      <c r="C67" s="83"/>
+      <c r="D67" s="84"/>
+      <c r="E67" s="84"/>
+      <c r="F67" s="84"/>
       <c r="G67" s="18"/>
       <c r="H67" s="18"/>
       <c r="I67" s="15" t="str">
@@ -18038,14 +18029,14 @@
     </row>
     <row r="68" spans="1:10" ht="15">
       <c r="A68" s="6" t="str">
-        <f>IF(B68="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B68,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B68="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B68,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B68" s="16"/>
-      <c r="C68" s="84"/>
-      <c r="D68" s="85"/>
-      <c r="E68" s="85"/>
-      <c r="F68" s="85"/>
+      <c r="C68" s="83"/>
+      <c r="D68" s="84"/>
+      <c r="E68" s="84"/>
+      <c r="F68" s="84"/>
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
       <c r="I68" s="15" t="str">
@@ -18056,14 +18047,14 @@
     </row>
     <row r="69" spans="1:10" ht="15">
       <c r="A69" s="6" t="str">
-        <f>IF(B69="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B69,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B69="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B69,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B69" s="16"/>
-      <c r="C69" s="84"/>
-      <c r="D69" s="85"/>
-      <c r="E69" s="85"/>
-      <c r="F69" s="85"/>
+      <c r="C69" s="83"/>
+      <c r="D69" s="84"/>
+      <c r="E69" s="84"/>
+      <c r="F69" s="84"/>
       <c r="G69" s="18"/>
       <c r="H69" s="18"/>
       <c r="I69" s="15" t="str">
@@ -18074,14 +18065,14 @@
     </row>
     <row r="70" spans="1:10" ht="15">
       <c r="A70" s="6" t="str">
-        <f>IF(B70="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B70,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$C:$C))</f>
+        <f>IF(B70="", "Choose from drop-down --&gt;", _xlfn.XLOOKUP(B70,'Statement of activities labels'!$B:$B,'Statement of activities labels'!$D:$D))</f>
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B70" s="16"/>
-      <c r="C70" s="84"/>
-      <c r="D70" s="85"/>
-      <c r="E70" s="85"/>
-      <c r="F70" s="85"/>
+      <c r="C70" s="83"/>
+      <c r="D70" s="84"/>
+      <c r="E70" s="84"/>
+      <c r="F70" s="84"/>
       <c r="G70" s="18"/>
       <c r="H70" s="18"/>
       <c r="I70" s="15" t="str">
@@ -18167,10 +18158,10 @@
       <c r="B75" s="8" t="s">
         <v>1124</v>
       </c>
-      <c r="C75" s="84"/>
-      <c r="D75" s="85"/>
-      <c r="E75" s="85"/>
-      <c r="F75" s="85"/>
+      <c r="C75" s="83"/>
+      <c r="D75" s="84"/>
+      <c r="E75" s="84"/>
+      <c r="F75" s="84"/>
       <c r="G75" s="18"/>
       <c r="H75" s="18"/>
       <c r="I75" s="15">
@@ -18186,10 +18177,10 @@
       <c r="B76" s="8" t="s">
         <v>1125</v>
       </c>
-      <c r="C76" s="84"/>
-      <c r="D76" s="85"/>
-      <c r="E76" s="85"/>
-      <c r="F76" s="85"/>
+      <c r="C76" s="83"/>
+      <c r="D76" s="84"/>
+      <c r="E76" s="84"/>
+      <c r="F76" s="84"/>
       <c r="G76" s="18"/>
       <c r="H76" s="18"/>
       <c r="I76" s="15">
@@ -18205,10 +18196,10 @@
       <c r="B77" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="C77" s="84"/>
-      <c r="D77" s="85"/>
-      <c r="E77" s="85"/>
-      <c r="F77" s="85"/>
+      <c r="C77" s="83"/>
+      <c r="D77" s="84"/>
+      <c r="E77" s="84"/>
+      <c r="F77" s="84"/>
       <c r="G77" s="18"/>
       <c r="H77" s="18"/>
       <c r="I77" s="15">
@@ -18368,8 +18359,8 @@
   </sheetPr>
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -18390,7 +18381,7 @@
       <c r="A1" s="33" t="s">
         <v>1073</v>
       </c>
-      <c r="B1" s="83" t="s">
+      <c r="B1" s="82" t="s">
         <v>1671</v>
       </c>
       <c r="C1" s="43"/>
@@ -18483,32 +18474,32 @@
       <c r="J6" s="56"/>
     </row>
     <row r="7" spans="1:10" s="54" customFormat="1" ht="43">
-      <c r="A7" s="88" t="s">
+      <c r="A7" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="89"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="50" t="s">
         <v>1081</v>
       </c>
-      <c r="D7" s="87" t="s">
+      <c r="D7" s="86" t="s">
         <v>1106</v>
       </c>
-      <c r="E7" s="87" t="s">
+      <c r="E7" s="86" t="s">
         <v>1106</v>
       </c>
-      <c r="F7" s="87" t="s">
+      <c r="F7" s="86" t="s">
         <v>1106</v>
       </c>
-      <c r="G7" s="87" t="s">
+      <c r="G7" s="86" t="s">
         <v>1106</v>
       </c>
-      <c r="H7" s="87" t="s">
+      <c r="H7" s="86" t="s">
         <v>1106</v>
       </c>
-      <c r="I7" s="87" t="s">
+      <c r="I7" s="86" t="s">
         <v>1106</v>
       </c>
-      <c r="J7" s="90" t="s">
+      <c r="J7" s="89" t="s">
         <v>1734</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates from 04/09, need to do new col checks
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/byflow/Documents/Research/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50502D83-3266-434F-A97C-D51BC639959B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A16A9F4-CED8-0C48-A512-DEBE978050A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3162" uniqueCount="2280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3163" uniqueCount="2281">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -5371,9 +5371,6 @@
     <t>acfr:AccountsReceivableModifiedAccrual</t>
   </si>
   <si>
-    <t>XBRL Modified Label</t>
-  </si>
-  <si>
     <t>xblri:item from Taxonomy spreadsheet</t>
   </si>
   <si>
@@ -6367,9 +6364,6 @@
     <t>LiabilitiesAndDeferredInflowsOfResourcesAndFundBalancesModifiedAccrual</t>
   </si>
   <si>
-    <t>with acfr: added</t>
-  </si>
-  <si>
     <t>Does col D exist in col F?</t>
   </si>
   <si>
@@ -6920,6 +6914,15 @@
   </si>
   <si>
     <t>acfr:NetPensionLiabilityModifiedAccrual</t>
+  </si>
+  <si>
+    <t>with acfr: added from Taxonomy spreadsheet</t>
+  </si>
+  <si>
+    <t>exist in F but not in D?</t>
+  </si>
+  <si>
+    <t>XBRL Label (col C) with string 'ModifiedAccrual' appended</t>
   </si>
 </sst>
 </file>
@@ -8305,10 +8308,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE09D81-CE0E-407C-B6C2-C3432BAC9950}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J2380"/>
+  <dimension ref="A1:K2380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H44" zoomScale="108" workbookViewId="0">
-      <selection activeCell="J64" sqref="J64"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -8317,15 +8320,16 @@
     <col min="2" max="2" width="91.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="92.83203125" customWidth="1"/>
-    <col min="5" max="5" width="40" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
     <col min="6" max="6" width="70" customWidth="1"/>
     <col min="7" max="7" width="22.33203125" customWidth="1"/>
     <col min="8" max="8" width="67.6640625" style="116" customWidth="1"/>
     <col min="9" max="9" width="67.5" customWidth="1"/>
     <col min="10" max="10" width="70.33203125" customWidth="1"/>
+    <col min="11" max="11" width="36.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15">
+    <row r="1" spans="1:11" ht="15">
       <c r="A1" s="1" t="s">
         <v>58</v>
       </c>
@@ -8336,28 +8340,31 @@
         <v>1073</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2280</v>
+      </c>
+      <c r="E1" s="128" t="s">
         <v>1763</v>
       </c>
-      <c r="E1" s="128" t="s">
-        <v>1764</v>
-      </c>
       <c r="F1" s="128" t="s">
+        <v>2278</v>
+      </c>
+      <c r="G1" s="128" t="s">
+        <v>2094</v>
+      </c>
+      <c r="H1" s="129" t="s">
         <v>2095</v>
       </c>
-      <c r="G1" s="128" t="s">
-        <v>2096</v>
-      </c>
-      <c r="H1" s="129" t="s">
-        <v>2097</v>
-      </c>
       <c r="I1" s="128" t="s">
-        <v>2121</v>
+        <v>2119</v>
       </c>
       <c r="J1" s="128" t="s">
-        <v>2120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>2118</v>
+      </c>
+      <c r="K1" s="128" t="s">
+        <v>2279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -8371,7 +8378,7 @@
         <v>1762</v>
       </c>
       <c r="E2" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="F2" t="str">
         <f>"acfr:"&amp;E2</f>
@@ -8393,7 +8400,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -8408,7 +8415,7 @@
         <v>acfr:AccountsReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E3" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F66" si="0">"acfr:"&amp;E3</f>
@@ -8426,10 +8433,10 @@
         <v>acfr:AccountsReceivableModifiedAccrual</v>
       </c>
       <c r="J3" t="s">
-        <v>2098</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>2096</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -8444,7 +8451,7 @@
         <v>acfr:AccountsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E4" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -8462,10 +8469,10 @@
         <v>acfr:AccountsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="J4" t="s">
-        <v>2099</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -8480,7 +8487,7 @@
         <v>acfr:AccountsReceivableUnbilledModifiedAccrual</v>
       </c>
       <c r="E5" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -8498,10 +8505,10 @@
         <v>acfr:AccruedInterestReceivableModifiedAccrual</v>
       </c>
       <c r="J5" t="s">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -8516,7 +8523,7 @@
         <v>acfr:AccountsReceivableUnbilledAllowanceModifiedAccrual</v>
       </c>
       <c r="E6" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -8534,10 +8541,10 @@
         <v>acfr:AccruedInterestReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="J6" t="s">
-        <v>2101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -8552,7 +8559,7 @@
         <v>acfr:AccountsReceivableUnbilledNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E7" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -8570,10 +8577,10 @@
         <v>acfr:AssetsHeldForSaleModifiedAccrual</v>
       </c>
       <c r="J7" t="s">
-        <v>2102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -8588,7 +8595,7 @@
         <v>acfr:AccruedInterestReceivableModifiedAccrual</v>
       </c>
       <c r="E8" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
@@ -8606,10 +8613,10 @@
         <v>acfr:CashModifiedAccrual</v>
       </c>
       <c r="J8" t="s">
-        <v>2103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>2101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -8624,7 +8631,7 @@
         <v>acfr:AccruedInterestReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E9" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -8642,10 +8649,10 @@
         <v>acfr:CashAndCashEquivalentsModifiedAccrual</v>
       </c>
       <c r="J9" t="s">
-        <v>2104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -8660,7 +8667,7 @@
         <v>acfr:AdvancesReceivableModifiedAccrual</v>
       </c>
       <c r="E10" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -8678,10 +8685,10 @@
         <v>acfr:CashAndCashEquivalentsAndInvestmentsModifiedAccrual</v>
       </c>
       <c r="J10" t="s">
-        <v>2105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -8696,7 +8703,7 @@
         <v>acfr:AdvancesToDevelopersModifiedAccrual</v>
       </c>
       <c r="E11" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -8714,10 +8721,10 @@
         <v>acfr:CashAndCashEquivalentsWithFiscalAndEscrowAndOtherAgentsModifiedAccrual</v>
       </c>
       <c r="J11" t="s">
-        <v>2106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>2104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -8732,7 +8739,7 @@
         <v>acfr:AllowanceForReceivablesModifiedAccrual</v>
       </c>
       <c r="E12" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -8750,10 +8757,10 @@
         <v>acfr:CashAndCashEquivalentsWithTreasurerModifiedAccrual</v>
       </c>
       <c r="J12" t="s">
-        <v>2107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -8768,7 +8775,7 @@
         <v>acfr:AssessmentsReceivableModifiedAccrual</v>
       </c>
       <c r="E13" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
@@ -8786,10 +8793,10 @@
         <v>acfr:CashAndCashEquivalentsWithTrusteeModifiedAccrual</v>
       </c>
       <c r="J13" t="s">
-        <v>2108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -8804,7 +8811,7 @@
         <v>acfr:AssessmentsReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E14" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
@@ -8822,10 +8829,10 @@
         <v>acfr:CashCheckingModifiedAccrual</v>
       </c>
       <c r="J14" t="s">
-        <v>2109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>2107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -8840,7 +8847,7 @@
         <v>acfr:AssessmentsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E15" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
@@ -8858,10 +8865,10 @@
         <v>acfr:CashOnHandModifiedAccrual</v>
       </c>
       <c r="J15" t="s">
-        <v>2110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -8876,7 +8883,7 @@
         <v>acfr:AssetRetirementObligationsPrincipalDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E16" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
@@ -8894,7 +8901,7 @@
         <v>acfr:CashPayrollBankAccountModifiedAccrual</v>
       </c>
       <c r="J16" t="s">
-        <v>2111</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -8912,7 +8919,7 @@
         <v>acfr:AssetsHeldForSaleModifiedAccrual</v>
       </c>
       <c r="E17" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
@@ -8930,7 +8937,7 @@
         <v>acfr:CashSavingsModifiedAccrual</v>
       </c>
       <c r="J17" t="s">
-        <v>2112</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -8948,7 +8955,7 @@
         <v>acfr:BondPremiumPrincipalDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E18" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
@@ -8966,7 +8973,7 @@
         <v>acfr:CertificatesOfDepositModifiedAccrual</v>
       </c>
       <c r="J18" t="s">
-        <v>2113</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -8984,7 +8991,7 @@
         <v>acfr:BondsPayableDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E19" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
@@ -9002,7 +9009,7 @@
         <v>acfr:ClaimsAndJudgmentsReceivableModifiedAccrual</v>
       </c>
       <c r="J19" t="s">
-        <v>2114</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -9020,7 +9027,7 @@
         <v>acfr:CashModifiedAccrual</v>
       </c>
       <c r="E20" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
@@ -9038,7 +9045,7 @@
         <v>acfr:ClaimsAndJudgmentsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="J20" t="s">
-        <v>2115</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -9056,7 +9063,7 @@
         <v>acfr:CashAndCashEquivalentsModifiedAccrual</v>
       </c>
       <c r="E21" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
@@ -9074,7 +9081,7 @@
         <v>acfr:ContractsPayableDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="J21" t="s">
-        <v>2116</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -9092,7 +9099,7 @@
         <v>acfr:CashAndCashEquivalentsAndInvestmentsModifiedAccrual</v>
       </c>
       <c r="E22" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
@@ -9110,7 +9117,7 @@
         <v>acfr:CourtOrdersReceivableModifiedAccrual</v>
       </c>
       <c r="J22" t="s">
-        <v>2117</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -9128,7 +9135,7 @@
         <v>acfr:CashAndCashEquivalentsAndInvestmentsAbtract_1ModifiedAccrual</v>
       </c>
       <c r="E23" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
@@ -9146,7 +9153,7 @@
         <v>acfr:DelinquentTaxesReceivableModifiedAccrual</v>
       </c>
       <c r="J23" t="s">
-        <v>2118</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -9164,7 +9171,7 @@
         <v>acfr:CashAndCashEquivalentsOthersModifiedAccrual</v>
       </c>
       <c r="E24" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
@@ -9182,7 +9189,7 @@
         <v>acfr:DelinquentUtilityBillsReceivableModifiedAccrual</v>
       </c>
       <c r="J24" t="s">
-        <v>2119</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -9200,7 +9207,7 @@
         <v>acfr:CashAndCashEquivalentsWithFiscalAndEscrowAndOtherAgentsModifiedAccrual</v>
       </c>
       <c r="E25" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
@@ -9218,7 +9225,7 @@
         <v>acfr:DepositsReceivableModifiedAccrual</v>
       </c>
       <c r="J25" t="s">
-        <v>2122</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -9236,7 +9243,7 @@
         <v>acfr:CashAndCashEquivalentsWithTreasurerModifiedAccrual</v>
       </c>
       <c r="E26" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
@@ -9254,7 +9261,7 @@
         <v>acfr:DepositsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="J26" t="s">
-        <v>2123</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -9272,7 +9279,7 @@
         <v>acfr:CashAndCashEquivalentsWithTrusteeModifiedAccrual</v>
       </c>
       <c r="E27" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
@@ -9290,7 +9297,7 @@
         <v>acfr:DepositsWithFiscalAgentsModifiedAccrual</v>
       </c>
       <c r="J27" t="s">
-        <v>2124</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -9308,7 +9315,7 @@
         <v>acfr:CashCheckingModifiedAccrual</v>
       </c>
       <c r="E28" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
@@ -9326,7 +9333,7 @@
         <v>acfr:DueFromCitiesModifiedAccrual</v>
       </c>
       <c r="J28" t="s">
-        <v>2125</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -9344,7 +9351,7 @@
         <v>acfr:CashEquivalentsModifiedAccrual</v>
       </c>
       <c r="E29" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
@@ -9362,7 +9369,7 @@
         <v>acfr:DueFromComponentUnitModifiedAccrual</v>
       </c>
       <c r="J29" t="s">
-        <v>2126</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -9380,7 +9387,7 @@
         <v>acfr:CashInBankModifiedAccrual</v>
       </c>
       <c r="E30" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
@@ -9398,7 +9405,7 @@
         <v>acfr:DueFromCountiesModifiedAccrual</v>
       </c>
       <c r="J30" t="s">
-        <v>2127</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -9416,7 +9423,7 @@
         <v>acfr:CashOnHandModifiedAccrual</v>
       </c>
       <c r="E31" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
@@ -9434,7 +9441,7 @@
         <v>acfr:DueFromEmployeesModifiedAccrual</v>
       </c>
       <c r="J31" t="s">
-        <v>2128</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -9452,7 +9459,7 @@
         <v>acfr:CashPayrollBankAccountModifiedAccrual</v>
       </c>
       <c r="E32" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
@@ -9470,7 +9477,7 @@
         <v>acfr:DueFromEnterpriseFundsModifiedAccrual</v>
       </c>
       <c r="J32" t="s">
-        <v>2129</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -9488,7 +9495,7 @@
         <v>acfr:CashSavingsModifiedAccrual</v>
       </c>
       <c r="E33" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
@@ -9506,7 +9513,7 @@
         <v>acfr:DueFromFederalGovernmentModifiedAccrual</v>
       </c>
       <c r="J33" t="s">
-        <v>2130</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -9524,7 +9531,7 @@
         <v>acfr:CertificatesOfDepositModifiedAccrual</v>
       </c>
       <c r="E34" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
@@ -9542,7 +9549,7 @@
         <v>acfr:DueFromFiduciaryFundsModifiedAccrual</v>
       </c>
       <c r="J34" t="s">
-        <v>2131</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -9560,7 +9567,7 @@
         <v>acfr:ClaimsAndJudgmentsPayableDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E35" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
@@ -9578,7 +9585,7 @@
         <v>acfr:DueFromLibrariesModifiedAccrual</v>
       </c>
       <c r="J35" t="s">
-        <v>2132</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -9596,7 +9603,7 @@
         <v>acfr:ClaimsAndJudgmentsReceivableModifiedAccrual</v>
       </c>
       <c r="E36" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
@@ -9614,7 +9621,7 @@
         <v>acfr:DueFromOtherFundsModifiedAccrual</v>
       </c>
       <c r="J36" t="s">
-        <v>2133</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -9632,7 +9639,7 @@
         <v>acfr:ClaimsAndJudgmentsReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E37" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
@@ -9650,7 +9657,7 @@
         <v>acfr:DueFromRoadCommissionsModifiedAccrual</v>
       </c>
       <c r="J37" t="s">
-        <v>2134</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -9668,7 +9675,7 @@
         <v>acfr:ClaimsAndJudgmentsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E38" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
@@ -9686,7 +9693,7 @@
         <v>acfr:DueFromSchoolsModifiedAccrual</v>
       </c>
       <c r="J38" t="s">
-        <v>2135</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -9704,7 +9711,7 @@
         <v>acfr:ComputerSoftwareModifiedAccrual</v>
       </c>
       <c r="E39" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
@@ -9722,7 +9729,7 @@
         <v>acfr:DueFromStateGovernmentModifiedAccrual</v>
       </c>
       <c r="J39" t="s">
-        <v>2136</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -9740,7 +9747,7 @@
         <v>acfr:ConnectionFeesReceivableModifiedAccrual</v>
       </c>
       <c r="E40" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
@@ -9758,7 +9765,7 @@
         <v>acfr:DueFromTownshipsExceptRoadAgreementsModifiedAccrual</v>
       </c>
       <c r="J40" t="s">
-        <v>2137</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -9776,7 +9783,7 @@
         <v>acfr:ConnectionFeesReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E41" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
@@ -9794,7 +9801,7 @@
         <v>acfr:DueFromTownshipsRoadAgreementsModifiedAccrual</v>
       </c>
       <c r="J41" t="s">
-        <v>2138</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -9812,7 +9819,7 @@
         <v>acfr:ConnectionFeesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E42" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
@@ -9830,7 +9837,7 @@
         <v>acfr:DueFromVillagesModifiedAccrual</v>
       </c>
       <c r="J42" t="s">
-        <v>2139</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -9848,7 +9855,7 @@
         <v>acfr:ContractorsAdvancesModifiedAccrual</v>
       </c>
       <c r="E43" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
@@ -9866,7 +9873,7 @@
         <v>acfr:ForfeitureCertificateRecordingFeesReceivableModifiedAccrual</v>
       </c>
       <c r="J43" t="s">
-        <v>2140</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -9884,7 +9891,7 @@
         <v>acfr:ContractsPayableDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E44" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
@@ -9902,7 +9909,7 @@
         <v>acfr:GrantsAndContractsReceivableModifiedAccrual</v>
       </c>
       <c r="J44" t="s">
-        <v>2141</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -9920,7 +9927,7 @@
         <v>acfr:CourtOrdersReceivableModifiedAccrual</v>
       </c>
       <c r="E45" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
@@ -9938,7 +9945,7 @@
         <v>acfr:GrantsAndContractsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="J45" t="s">
-        <v>2142</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -9956,7 +9963,7 @@
         <v>acfr:CurrentAssetsModifiedAccrual</v>
       </c>
       <c r="E46" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
@@ -9974,7 +9981,7 @@
         <v>acfr:IncomeTaxReceivableModifiedAccrual</v>
       </c>
       <c r="J46" t="s">
-        <v>2143</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -9992,7 +9999,7 @@
         <v>acfr:CurrentAssetsCustomModifiedAccrual</v>
       </c>
       <c r="E47" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
@@ -10010,7 +10017,7 @@
         <v>acfr:InterGovernmentalReceivableModifiedAccrual</v>
       </c>
       <c r="J47" t="s">
-        <v>2144</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -10028,7 +10035,7 @@
         <v>acfr:CustomerAndOtherGovernmentReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E48" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
@@ -10046,7 +10053,7 @@
         <v>acfr:InterGovernmentalReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="J48" t="s">
-        <v>2145</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -10064,7 +10071,7 @@
         <v>acfr:CustomerAndOtherGovernmentReceivablesModifiedAccrual</v>
       </c>
       <c r="E49" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
@@ -10082,7 +10089,7 @@
         <v>acfr:InterestAndPenaltiesReceivableOnTaxesModifiedAccrual</v>
       </c>
       <c r="J49" t="s">
-        <v>2146</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -10100,7 +10107,7 @@
         <v>acfr:CustomerAndOtherGovernmentReceivablesNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E50" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
@@ -10118,7 +10125,7 @@
         <v>acfr:InventoryModifiedAccrual</v>
       </c>
       <c r="J50" t="s">
-        <v>2147</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -10136,7 +10143,7 @@
         <v>acfr:DelinquentTaxesReceivableModifiedAccrual</v>
       </c>
       <c r="E51" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
@@ -10154,7 +10161,7 @@
         <v>acfr:InventoryEquipmentMaterialsAndPartsModifiedAccrual</v>
       </c>
       <c r="J51" t="s">
-        <v>2148</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -10172,7 +10179,7 @@
         <v>acfr:DelinquentUtilityBillsReceivableModifiedAccrual</v>
       </c>
       <c r="E52" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
@@ -10190,7 +10197,7 @@
         <v>acfr:InventoryRoadMaterialsModifiedAccrual</v>
       </c>
       <c r="J52" t="s">
-        <v>2149</v>
+        <v>2147</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -10208,7 +10215,7 @@
         <v>acfr:DepositsReceivableModifiedAccrual</v>
       </c>
       <c r="E53" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
@@ -10226,7 +10233,7 @@
         <v>acfr:InvestmentsWithFiscalAgentsModifiedAccrual</v>
       </c>
       <c r="J53" t="s">
-        <v>2150</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -10244,7 +10251,7 @@
         <v>acfr:DepositsReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E54" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
@@ -10262,7 +10269,7 @@
         <v>acfr:InvestmentsWithStateTreasuryModifiedAccrual</v>
       </c>
       <c r="J54" t="s">
-        <v>2151</v>
+        <v>2149</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -10280,7 +10287,7 @@
         <v>acfr:DepositsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E55" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
@@ -10298,7 +10305,7 @@
         <v>acfr:LandContractsPayableModifiedAccrual</v>
       </c>
       <c r="J55" t="s">
-        <v>2152</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -10316,7 +10323,7 @@
         <v>acfr:DepositsWithFiscalAgentsModifiedAccrual</v>
       </c>
       <c r="E56" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
@@ -10334,7 +10341,7 @@
         <v>acfr:LandContractsReceivableModifiedAccrual</v>
       </c>
       <c r="J56" t="s">
-        <v>2153</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -10352,7 +10359,7 @@
         <v>acfr:DerivativeInstrumentsAssetsCurrentModifiedAccrual</v>
       </c>
       <c r="E57" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
@@ -10370,7 +10377,7 @@
         <v>acfr:LandContractsReceivablesAllowanceModifiedAccrual</v>
       </c>
       <c r="J57" t="s">
-        <v>2154</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -10388,7 +10395,7 @@
         <v>acfr:DerivativeInstrumentsLiabilityCurrentModifiedAccrual</v>
       </c>
       <c r="E58" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
@@ -10406,7 +10413,7 @@
         <v>acfr:LandContractsReceivablesNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="J58" t="s">
-        <v>2155</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -10424,7 +10431,7 @@
         <v>acfr:DueFromCitiesModifiedAccrual</v>
       </c>
       <c r="E59" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
@@ -10442,7 +10449,7 @@
         <v>acfr:LeaseAssetsRightOfUseModifiedAccrual</v>
       </c>
       <c r="J59" t="s">
-        <v>2156</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -10460,7 +10467,7 @@
         <v>acfr:DueFromComponentUnitModifiedAccrual</v>
       </c>
       <c r="E60" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
@@ -10478,7 +10485,7 @@
         <v>acfr:LeasesReceivableModifiedAccrual</v>
       </c>
       <c r="J60" t="s">
-        <v>2157</v>
+        <v>2155</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -10496,7 +10503,7 @@
         <v>acfr:DueFromCountiesModifiedAccrual</v>
       </c>
       <c r="E61" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
@@ -10514,7 +10521,7 @@
         <v>acfr:LeasesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="J61" t="s">
-        <v>2158</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -10532,7 +10539,7 @@
         <v>acfr:DueFromCustodialFundsModifiedAccrual</v>
       </c>
       <c r="E62" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
@@ -10550,7 +10557,7 @@
         <v>acfr:LoansAndNotesReceivableModifiedAccrual</v>
       </c>
       <c r="J62" t="s">
-        <v>2159</v>
+        <v>2157</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -10568,7 +10575,7 @@
         <v>acfr:DueFromEmployeesModifiedAccrual</v>
       </c>
       <c r="E63" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
@@ -10586,7 +10593,7 @@
         <v>acfr:LoansAndNotesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="J63" t="s">
-        <v>2160</v>
+        <v>2158</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -10604,7 +10611,7 @@
         <v>acfr:DueFromEnterpriseFundsModifiedAccrual</v>
       </c>
       <c r="E64" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
@@ -10622,7 +10629,7 @@
         <v>acfr:LoansReceivableModifiedAccrual</v>
       </c>
       <c r="J64" t="s">
-        <v>2161</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -10640,7 +10647,7 @@
         <v>acfr:DueFromFederalGovernmentModifiedAccrual</v>
       </c>
       <c r="E65" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="F65" t="str">
         <f t="shared" si="0"/>
@@ -10658,7 +10665,7 @@
         <v>acfr:LoansReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="J65" t="s">
-        <v>2162</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -10676,7 +10683,7 @@
         <v>acfr:DueFromFiduciaryFundsModifiedAccrual</v>
       </c>
       <c r="E66" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="F66" t="str">
         <f t="shared" si="0"/>
@@ -10694,7 +10701,7 @@
         <v>acfr:LoansReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="J66" t="s">
-        <v>2163</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -10712,7 +10719,7 @@
         <v>acfr:DueFromGovernmentModifiedAccrual</v>
       </c>
       <c r="E67" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="F67" t="str">
         <f t="shared" ref="F67:F130" si="4">"acfr:"&amp;E67</f>
@@ -10730,7 +10737,7 @@
         <v>acfr:LocalUnitShareOfAssessmentImprovementCostsReceivableModifiedAccrual</v>
       </c>
       <c r="J67" t="s">
-        <v>2164</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -10748,7 +10755,7 @@
         <v>acfr:DueFromLibrariesModifiedAccrual</v>
       </c>
       <c r="E68" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="F68" t="str">
         <f t="shared" si="4"/>
@@ -10766,7 +10773,7 @@
         <v>acfr:NotesReceivableModifiedAccrual</v>
       </c>
       <c r="J68" t="s">
-        <v>2165</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -10784,7 +10791,7 @@
         <v>acfr:DueFromOtherFundsModifiedAccrual</v>
       </c>
       <c r="E69" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="F69" t="str">
         <f t="shared" si="4"/>
@@ -10802,7 +10809,7 @@
         <v>acfr:NotesReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="J69" t="s">
-        <v>2166</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -10820,7 +10827,7 @@
         <v>acfr:DueFromOtherGovernmentsModifiedAccrual</v>
       </c>
       <c r="E70" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="F70" t="str">
         <f t="shared" si="4"/>
@@ -10838,7 +10845,7 @@
         <v>acfr:NotesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="J70" t="s">
-        <v>2167</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -10856,7 +10863,7 @@
         <v>acfr:DueFromPrimaryGovernmentModifiedAccrual</v>
       </c>
       <c r="E71" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="F71" t="str">
         <f t="shared" si="4"/>
@@ -10874,7 +10881,7 @@
         <v>acfr:OtherAccountsReceivableModifiedAccrual</v>
       </c>
       <c r="J71" t="s">
-        <v>2168</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -10892,7 +10899,7 @@
         <v>acfr:DueFromRelatedPartiesModifiedAccrual</v>
       </c>
       <c r="E72" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" si="4"/>
@@ -10910,7 +10917,7 @@
         <v>acfr:OtherReceivablesModifiedAccrual</v>
       </c>
       <c r="J72" t="s">
-        <v>2169</v>
+        <v>2167</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -10928,7 +10935,7 @@
         <v>acfr:DueFromRetirementSystemModifiedAccrual</v>
       </c>
       <c r="E73" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="F73" t="str">
         <f t="shared" si="4"/>
@@ -10946,7 +10953,7 @@
         <v>acfr:OtherRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="J73" t="s">
-        <v>2170</v>
+        <v>2168</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -10964,7 +10971,7 @@
         <v>acfr:DueFromRoadCommissionsModifiedAccrual</v>
       </c>
       <c r="E74" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="F74" t="str">
         <f t="shared" si="4"/>
@@ -10982,7 +10989,7 @@
         <v>acfr:OtherTaxesReceivableModifiedAccrual</v>
       </c>
       <c r="J74" t="s">
-        <v>2171</v>
+        <v>2169</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -11000,7 +11007,7 @@
         <v>acfr:DueFromSchoolsModifiedAccrual</v>
       </c>
       <c r="E75" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="F75" t="str">
         <f t="shared" si="4"/>
@@ -11018,7 +11025,7 @@
         <v>acfr:PaymentsInLieuOfTaxesReceivableModifiedAccrual</v>
       </c>
       <c r="J75" t="s">
-        <v>2172</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -11036,7 +11043,7 @@
         <v>acfr:DueFromStateGovernmentModifiedAccrual</v>
       </c>
       <c r="E76" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="F76" t="str">
         <f t="shared" si="4"/>
@@ -11054,7 +11061,7 @@
         <v>acfr:PenaltiesReceivableModifiedAccrual</v>
       </c>
       <c r="J76" t="s">
-        <v>2173</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -11072,7 +11079,7 @@
         <v>acfr:DueFromTaxCollectionFundsModifiedAccrual</v>
       </c>
       <c r="E77" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="F77" t="str">
         <f t="shared" si="4"/>
@@ -11090,7 +11097,7 @@
         <v>acfr:PenaltiesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="J77" t="s">
-        <v>2174</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -11108,7 +11115,7 @@
         <v>acfr:DueFromTownshipsExceptRoadAgreementsModifiedAccrual</v>
       </c>
       <c r="E78" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="F78" t="str">
         <f t="shared" si="4"/>
@@ -11126,7 +11133,7 @@
         <v>acfr:PooledCashAndInvestmentsModifiedAccrual</v>
       </c>
       <c r="J78" t="s">
-        <v>2175</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -11144,7 +11151,7 @@
         <v>acfr:DueFromTownshipsRoadAgreementsModifiedAccrual</v>
       </c>
       <c r="E79" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="F79" t="str">
         <f t="shared" si="4"/>
@@ -11162,7 +11169,7 @@
         <v>acfr:PrepaidDepositsModifiedAccrual</v>
       </c>
       <c r="J79" t="s">
-        <v>2176</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -11180,7 +11187,7 @@
         <v>acfr:DueFromVillagesModifiedAccrual</v>
       </c>
       <c r="E80" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="F80" t="str">
         <f t="shared" si="4"/>
@@ -11198,7 +11205,7 @@
         <v>acfr:PrepaidExpensesModifiedAccrual</v>
       </c>
       <c r="J80" t="s">
-        <v>2177</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -11216,7 +11223,7 @@
         <v>acfr:EasementsRightOfWayModifiedAccrual</v>
       </c>
       <c r="E81" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="F81" t="str">
         <f t="shared" si="4"/>
@@ -11234,7 +11241,7 @@
         <v>acfr:PropertyTaxesReceivableModifiedAccrual</v>
       </c>
       <c r="J81" t="s">
-        <v>2178</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -11252,7 +11259,7 @@
         <v>acfr:ForfeitureCertificateRecordingFeesReceivableModifiedAccrual</v>
       </c>
       <c r="E82" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="F82" t="str">
         <f t="shared" si="4"/>
@@ -11270,7 +11277,7 @@
         <v>acfr:PropertyTaxesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="J82" t="s">
-        <v>2179</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -11288,7 +11295,7 @@
         <v>acfr:GeneralObligationBondsPayableDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E83" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="4"/>
@@ -11306,7 +11313,7 @@
         <v>acfr:ReceivablesModifiedAccrual</v>
       </c>
       <c r="J83" t="s">
-        <v>2180</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -11324,7 +11331,7 @@
         <v>acfr:GovernmentClaimsReceivableModifiedAccrual</v>
       </c>
       <c r="E84" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="F84" t="str">
         <f t="shared" si="4"/>
@@ -11342,7 +11349,7 @@
         <v>acfr:RestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="J84" t="s">
-        <v>2181</v>
+        <v>2179</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -11360,7 +11367,7 @@
         <v>acfr:GovernmentClaimsReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E85" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="F85" t="str">
         <f t="shared" si="4"/>
@@ -11378,7 +11385,7 @@
         <v>acfr:RestrictedCashModifiedAccrual</v>
       </c>
       <c r="J85" t="s">
-        <v>2182</v>
+        <v>2180</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -11396,7 +11403,7 @@
         <v>acfr:GovernmentClaimsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E86" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="F86" t="str">
         <f t="shared" si="4"/>
@@ -11414,7 +11421,7 @@
         <v>acfr:RestrictedCashAndCashEquivalentsModifiedAccrual</v>
       </c>
       <c r="J86" t="s">
-        <v>2183</v>
+        <v>2181</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -11432,7 +11439,7 @@
         <v>acfr:GrantsAndContractsReceivableModifiedAccrual</v>
       </c>
       <c r="E87" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="F87" t="str">
         <f t="shared" si="4"/>
@@ -11450,7 +11457,7 @@
         <v>acfr:RestrictedCashAndInvestmentsModifiedAccrual</v>
       </c>
       <c r="J87" t="s">
-        <v>2184</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -11468,7 +11475,7 @@
         <v>acfr:GrantsAndContractsReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E88" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="F88" t="str">
         <f t="shared" si="4"/>
@@ -11486,7 +11493,7 @@
         <v>acfr:SalesTaxReceivableModifiedAccrual</v>
       </c>
       <c r="J88" t="s">
-        <v>2185</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -11504,7 +11511,7 @@
         <v>acfr:GrantsAndContractsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E89" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="F89" t="str">
         <f t="shared" si="4"/>
@@ -11522,7 +11529,7 @@
         <v>acfr:SecuritiesLendingCollateralAssetsModifiedAccrual</v>
       </c>
       <c r="J89" t="s">
-        <v>2186</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -11540,7 +11547,7 @@
         <v>acfr:IncomeTaxReceivableModifiedAccrual</v>
       </c>
       <c r="E90" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="F90" t="str">
         <f t="shared" si="4"/>
@@ -11558,7 +11565,7 @@
         <v>acfr:SecuritiesLendingObligationsLiabilityModifiedAccrual</v>
       </c>
       <c r="J90" t="s">
-        <v>2187</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -11576,7 +11583,7 @@
         <v>acfr:InstallmentDebtPrincipalDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E91" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="F91" t="str">
         <f t="shared" si="4"/>
@@ -11594,7 +11601,7 @@
         <v>acfr:ServiceFeesReceivableModifiedAccrual</v>
       </c>
       <c r="J91" t="s">
-        <v>2188</v>
+        <v>2186</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -11612,7 +11619,7 @@
         <v>acfr:IntangibleAssetsModifiedAccrual</v>
       </c>
       <c r="E92" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="F92" t="str">
         <f t="shared" si="4"/>
@@ -11630,7 +11637,7 @@
         <v>acfr:SpecialAssessmentTaxesReceivableModifiedAccrual</v>
       </c>
       <c r="J92" t="s">
-        <v>2189</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -11648,7 +11655,7 @@
         <v>acfr:IntangibleAssetsNetOfAccumulatedAmortizationModifiedAccrual</v>
       </c>
       <c r="E93" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="F93" t="str">
         <f t="shared" si="4"/>
@@ -11666,7 +11673,7 @@
         <v>acfr:SpecialAssessmentTaxesReceivableUnavailableModifiedAccrual</v>
       </c>
       <c r="J93" t="s">
-        <v>2190</v>
+        <v>2188</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -11684,7 +11691,7 @@
         <v>acfr:InterGovernmentalReceivableModifiedAccrual</v>
       </c>
       <c r="E94" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="F94" t="str">
         <f t="shared" si="4"/>
@@ -11702,7 +11709,7 @@
         <v>acfr:SpecialAssessmentsReceivableDelinquentModifiedAccrual</v>
       </c>
       <c r="J94" t="s">
-        <v>2191</v>
+        <v>2189</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -11720,7 +11727,7 @@
         <v>acfr:InterGovernmentalReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E95" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="F95" t="str">
         <f t="shared" si="4"/>
@@ -11738,7 +11745,7 @@
         <v>acfr:TaxesReceivableModifiedAccrual</v>
       </c>
       <c r="J95" t="s">
-        <v>2192</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -11756,7 +11763,7 @@
         <v>acfr:InterGovernmentalReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E96" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="F96" t="str">
         <f t="shared" si="4"/>
@@ -11774,7 +11781,7 @@
         <v>acfr:TaxesReceivableDelinquentPersonalPropertyModifiedAccrual</v>
       </c>
       <c r="J96" t="s">
-        <v>2193</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -11792,7 +11799,7 @@
         <v>acfr:InterestAndPenaltiesReceivableOnTaxesModifiedAccrual</v>
       </c>
       <c r="E97" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="F97" t="str">
         <f t="shared" si="4"/>
@@ -11810,7 +11817,7 @@
         <v>acfr:TaxesReceivableDelinquentRealPropertyModifiedAccrual</v>
       </c>
       <c r="J97" t="s">
-        <v>2194</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -11828,7 +11835,7 @@
         <v>acfr:InterestReceivableAllowancesModifiedAccrual</v>
       </c>
       <c r="E98" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="F98" t="str">
         <f t="shared" si="4"/>
@@ -11846,7 +11853,7 @@
         <v>acfr:TaxesReceivablePersonalPropertyCurrentLevyModifiedAccrual</v>
       </c>
       <c r="J98" t="s">
-        <v>2195</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -11864,7 +11871,7 @@
         <v>acfr:IntergovernmentalAgreementPayablePrincipalDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E99" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="F99" t="str">
         <f t="shared" si="4"/>
@@ -11882,7 +11889,7 @@
         <v>acfr:TaxesReceivableRealPropertyCurrentLevyModifiedAccrual</v>
       </c>
       <c r="J99" t="s">
-        <v>2196</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -11900,7 +11907,7 @@
         <v>acfr:InternalBalanceModifiedAccrual</v>
       </c>
       <c r="E100" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="F100" t="str">
         <f t="shared" si="4"/>
@@ -11918,7 +11925,7 @@
         <v>acfr:TuitionAndFeesAllowancesModifiedAccrual</v>
       </c>
       <c r="J100" t="s">
-        <v>2197</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -11936,7 +11943,7 @@
         <v>acfr:InventoryModifiedAccrual</v>
       </c>
       <c r="E101" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="F101" t="str">
         <f t="shared" si="4"/>
@@ -11954,7 +11961,7 @@
         <v>acfr:TuitionAndFeesReceivableModifiedAccrual</v>
       </c>
       <c r="J101" t="s">
-        <v>2198</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="102" spans="1:10">
@@ -11972,7 +11979,7 @@
         <v>acfr:InventoryEquipmentMaterialsAndPartsModifiedAccrual</v>
       </c>
       <c r="E102" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="F102" t="str">
         <f t="shared" si="4"/>
@@ -11990,7 +11997,7 @@
         <v>acfr:TuitionAndFeesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="J102" t="s">
-        <v>2199</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="103" spans="1:10">
@@ -12008,7 +12015,7 @@
         <v>acfr:InventoryRoadMaterialsModifiedAccrual</v>
       </c>
       <c r="E103" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="F103" t="str">
         <f t="shared" si="4"/>
@@ -12026,7 +12033,7 @@
         <v>acfr:AccountsPayableModifiedAccrual</v>
       </c>
       <c r="J103" t="s">
-        <v>2200</v>
+        <v>2198</v>
       </c>
     </row>
     <row r="104" spans="1:10">
@@ -12044,7 +12051,7 @@
         <v>acfr:InvestmentsAbtractModifiedAccrual</v>
       </c>
       <c r="E104" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="F104" t="str">
         <f t="shared" si="4"/>
@@ -12062,7 +12069,7 @@
         <v>acfr:AccruedExpensesPayableModifiedAccrual</v>
       </c>
       <c r="J104" t="s">
-        <v>2201</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="105" spans="1:10">
@@ -12080,7 +12087,7 @@
         <v>acfr:InvestmentsCurrentModifiedAccrual</v>
       </c>
       <c r="E105" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="F105" t="str">
         <f t="shared" si="4"/>
@@ -12098,7 +12105,7 @@
         <v>acfr:AccruedInterestPayableModifiedAccrual</v>
       </c>
       <c r="J105" t="s">
-        <v>2202</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="106" spans="1:10">
@@ -12116,7 +12123,7 @@
         <v>acfr:InvestmentsHeldByThirdPartiesModifiedAccrual</v>
       </c>
       <c r="E106" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="F106" t="str">
         <f t="shared" si="4"/>
@@ -12134,7 +12141,7 @@
         <v>acfr:AccruedLiabilitiesModifiedAccrual</v>
       </c>
       <c r="J106" t="s">
-        <v>2203</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="107" spans="1:10">
@@ -12152,7 +12159,7 @@
         <v>acfr:InvestmentsRestrictedModifiedAccrual</v>
       </c>
       <c r="E107" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="F107" t="str">
         <f t="shared" si="4"/>
@@ -12170,7 +12177,7 @@
         <v>acfr:AccruedTuitionAndFeesModifiedAccrual</v>
       </c>
       <c r="J107" t="s">
-        <v>2204</v>
+        <v>2202</v>
       </c>
     </row>
     <row r="108" spans="1:10">
@@ -12188,7 +12195,7 @@
         <v>acfr:InvestmentsWithFiscalAgentsModifiedAccrual</v>
       </c>
       <c r="E108" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="F108" t="str">
         <f t="shared" si="4"/>
@@ -12206,7 +12213,7 @@
         <v>acfr:AccruedVacationPayableModifiedAccrual</v>
       </c>
       <c r="J108" t="s">
-        <v>2205</v>
+        <v>2203</v>
       </c>
     </row>
     <row r="109" spans="1:10">
@@ -12224,7 +12231,7 @@
         <v>acfr:InvestmentsWithStateTreasuryModifiedAccrual</v>
       </c>
       <c r="E109" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="F109" t="str">
         <f t="shared" si="4"/>
@@ -12242,7 +12249,7 @@
         <v>acfr:AccruedWagesAndRelatedLiabilitiesPayableModifiedAccrual</v>
       </c>
       <c r="J109" t="s">
-        <v>2206</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="110" spans="1:10">
@@ -12260,7 +12267,7 @@
         <v>acfr:LandContractsPayableModifiedAccrual</v>
       </c>
       <c r="E110" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="F110" t="str">
         <f t="shared" si="4"/>
@@ -12278,7 +12285,7 @@
         <v>acfr:AccruedWagesPayableModifiedAccrual</v>
       </c>
       <c r="J110" t="s">
-        <v>2207</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="111" spans="1:10">
@@ -12296,7 +12303,7 @@
         <v>acfr:LandContractsReceivableModifiedAccrual</v>
       </c>
       <c r="E111" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="F111" t="str">
         <f t="shared" si="4"/>
@@ -12314,7 +12321,7 @@
         <v>acfr:AdvancesFromFederalGovernmentNoncurrentModifiedAccrual</v>
       </c>
       <c r="J111" t="s">
-        <v>2208</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="112" spans="1:10">
@@ -12332,7 +12339,7 @@
         <v>acfr:LandContractsReceivablesAllowanceModifiedAccrual</v>
       </c>
       <c r="E112" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="F112" t="str">
         <f t="shared" si="4"/>
@@ -12350,7 +12357,7 @@
         <v>acfr:AdvancesFromGrantorsModifiedAccrual</v>
       </c>
       <c r="J112" t="s">
-        <v>2209</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="113" spans="1:10">
@@ -12368,7 +12375,7 @@
         <v>acfr:LandContractsReceivablesNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E113" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="F113" t="str">
         <f t="shared" si="4"/>
@@ -12386,7 +12393,7 @@
         <v>acfr:AdvancesFromOtherFundsModifiedAccrual</v>
       </c>
       <c r="J113" t="s">
-        <v>2210</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="114" spans="1:10">
@@ -12404,7 +12411,7 @@
         <v>acfr:LeaseAssetsRightOfUseModifiedAccrual</v>
       </c>
       <c r="E114" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="F114" t="str">
         <f t="shared" si="4"/>
@@ -12422,7 +12429,7 @@
         <v>acfr:AdvancesFromOtherGovernmentsNoncurrentModifiedAccrual</v>
       </c>
       <c r="J114" t="s">
-        <v>2211</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="115" spans="1:10">
@@ -12440,7 +12447,7 @@
         <v>acfr:LeasesPayableDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E115" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="F115" t="str">
         <f t="shared" si="4"/>
@@ -12458,7 +12465,7 @@
         <v>acfr:AdvancesFromStateNoncurrentModifiedAccrual</v>
       </c>
       <c r="J115" t="s">
-        <v>2212</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="116" spans="1:10">
@@ -12476,7 +12483,7 @@
         <v>acfr:LeasesReceivableModifiedAccrual</v>
       </c>
       <c r="E116" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="F116" t="str">
         <f t="shared" si="4"/>
@@ -12494,7 +12501,7 @@
         <v>acfr:AdvancesSpecialAssessmentDistrictsModifiedAccrual</v>
       </c>
       <c r="J116" t="s">
-        <v>2213</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="117" spans="1:10">
@@ -12512,7 +12519,7 @@
         <v>acfr:LeasesReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E117" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="F117" t="str">
         <f t="shared" si="4"/>
@@ -12530,7 +12537,7 @@
         <v>acfr:AnnuitiesPayableModifiedAccrual</v>
       </c>
       <c r="J117" t="s">
-        <v>2214</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="118" spans="1:10">
@@ -12548,7 +12555,7 @@
         <v>acfr:LeasesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E118" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="F118" t="str">
         <f t="shared" si="4"/>
@@ -12566,7 +12573,7 @@
         <v>acfr:CashBondsPayableModifiedAccrual</v>
       </c>
       <c r="J118" t="s">
-        <v>2215</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="119" spans="1:10">
@@ -12584,7 +12591,7 @@
         <v>acfr:LimitedTaxBondsPrincipalDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E119" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="F119" t="str">
         <f t="shared" si="4"/>
@@ -12602,7 +12609,7 @@
         <v>acfr:CourtOrdersPayableModifiedAccrual</v>
       </c>
       <c r="J119" t="s">
-        <v>2216</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="120" spans="1:10">
@@ -12620,7 +12627,7 @@
         <v>acfr:LoansAndNotesReceivableModifiedAccrual</v>
       </c>
       <c r="E120" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="F120" t="str">
         <f t="shared" si="4"/>
@@ -12638,7 +12645,7 @@
         <v>acfr:CustomerDepositsModifiedAccrual</v>
       </c>
       <c r="J120" t="s">
-        <v>2217</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="121" spans="1:10">
@@ -12656,7 +12663,7 @@
         <v>acfr:LoansAndNotesReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E121" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="F121" t="str">
         <f t="shared" si="4"/>
@@ -12674,7 +12681,7 @@
         <v>acfr:DepositsHeldforOthersModifiedAccrual</v>
       </c>
       <c r="J121" t="s">
-        <v>2218</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="122" spans="1:10">
@@ -12692,7 +12699,7 @@
         <v>acfr:LoansAndNotesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E122" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="F122" t="str">
         <f t="shared" si="4"/>
@@ -12710,7 +12717,7 @@
         <v>acfr:DrainOrdersPayableModifiedAccrual</v>
       </c>
       <c r="J122" t="s">
-        <v>2219</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="123" spans="1:10">
@@ -12728,7 +12735,7 @@
         <v>acfr:LoansPayableDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E123" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="F123" t="str">
         <f t="shared" si="4"/>
@@ -12746,7 +12753,7 @@
         <v>acfr:DueToCitiesModifiedAccrual</v>
       </c>
       <c r="J123" t="s">
-        <v>2220</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="124" spans="1:10">
@@ -12764,7 +12771,7 @@
         <v>acfr:LoansReceivableModifiedAccrual</v>
       </c>
       <c r="E124" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="F124" t="str">
         <f t="shared" si="4"/>
@@ -12782,7 +12789,7 @@
         <v>acfr:DueToCommunityCollegeModifiedAccrual</v>
       </c>
       <c r="J124" t="s">
-        <v>2221</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="125" spans="1:10">
@@ -12800,7 +12807,7 @@
         <v>acfr:LoansReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E125" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="F125" t="str">
         <f t="shared" si="4"/>
@@ -12818,7 +12825,7 @@
         <v>acfr:DueToComponentUnitModifiedAccrual</v>
       </c>
       <c r="J125" t="s">
-        <v>2222</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="126" spans="1:10">
@@ -12836,7 +12843,7 @@
         <v>acfr:LoansReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E126" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="F126" t="str">
         <f t="shared" si="4"/>
@@ -12854,7 +12861,7 @@
         <v>acfr:DueToCountiesModifiedAccrual</v>
       </c>
       <c r="J126" t="s">
-        <v>2223</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="127" spans="1:10">
@@ -12872,7 +12879,7 @@
         <v>acfr:LocalUnitShareOfAssessmentImprovementCostsReceivableModifiedAccrual</v>
       </c>
       <c r="E127" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="F127" t="str">
         <f t="shared" si="4"/>
@@ -12890,7 +12897,7 @@
         <v>acfr:DueToCourtWardsModifiedAccrual</v>
       </c>
       <c r="J127" t="s">
-        <v>2224</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="128" spans="1:10">
@@ -12908,7 +12915,7 @@
         <v>acfr:LongTermDebtDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E128" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="F128" t="str">
         <f t="shared" si="4"/>
@@ -12926,7 +12933,7 @@
         <v>acfr:DueToEmployeesModifiedAccrual</v>
       </c>
       <c r="J128" t="s">
-        <v>2225</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="129" spans="1:10">
@@ -12944,7 +12951,7 @@
         <v>acfr:LotteryTicketInventoriesModifiedAccrual</v>
       </c>
       <c r="E129" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="F129" t="str">
         <f t="shared" si="4"/>
@@ -12962,7 +12969,7 @@
         <v>acfr:DueToFederalGovernmentModifiedAccrual</v>
       </c>
       <c r="J129" t="s">
-        <v>2226</v>
+        <v>2224</v>
       </c>
     </row>
     <row r="130" spans="1:10">
@@ -12980,7 +12987,7 @@
         <v>acfr:NotesPayableDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E130" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="F130" t="str">
         <f t="shared" si="4"/>
@@ -12998,7 +13005,7 @@
         <v>acfr:DueToFiduciaryFundsModifiedAccrual</v>
       </c>
       <c r="J130" t="s">
-        <v>2227</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="131" spans="1:10">
@@ -13016,7 +13023,7 @@
         <v>acfr:NotesReceivableModifiedAccrual</v>
       </c>
       <c r="E131" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="F131" t="str">
         <f t="shared" ref="F131:F194" si="8">"acfr:"&amp;E131</f>
@@ -13034,7 +13041,7 @@
         <v>acfr:DueToFiscalAgentModifiedAccrual</v>
       </c>
       <c r="J131" t="s">
-        <v>2228</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="132" spans="1:10">
@@ -13052,7 +13059,7 @@
         <v>acfr:NotesReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E132" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="F132" t="str">
         <f t="shared" si="8"/>
@@ -13070,7 +13077,7 @@
         <v>acfr:DueToFormerEmployeesModifiedAccrual</v>
       </c>
       <c r="J132" t="s">
-        <v>2229</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="133" spans="1:10">
@@ -13088,7 +13095,7 @@
         <v>acfr:NotesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E133" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="F133" t="str">
         <f t="shared" si="8"/>
@@ -13106,7 +13113,7 @@
         <v>acfr:DueToIntermediateSchoolDistrictsModifiedAccrual</v>
       </c>
       <c r="J133" t="s">
-        <v>2230</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="134" spans="1:10">
@@ -13124,7 +13131,7 @@
         <v>acfr:OtherAccountsReceivableModifiedAccrual</v>
       </c>
       <c r="E134" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="F134" t="str">
         <f t="shared" si="8"/>
@@ -13142,7 +13149,7 @@
         <v>acfr:DueToLibrariesModifiedAccrual</v>
       </c>
       <c r="J134" t="s">
-        <v>2231</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="135" spans="1:10">
@@ -13160,7 +13167,7 @@
         <v>acfr:OtherAccountsReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E135" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="F135" t="str">
         <f t="shared" si="8"/>
@@ -13178,7 +13185,7 @@
         <v>acfr:DueToOtherFundsModifiedAccrual</v>
       </c>
       <c r="J135" t="s">
-        <v>2232</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="136" spans="1:10">
@@ -13196,7 +13203,7 @@
         <v>acfr:OtherAccountsReceivableNetModifiedAccrual</v>
       </c>
       <c r="E136" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="F136" t="str">
         <f t="shared" si="8"/>
@@ -13214,7 +13221,7 @@
         <v>acfr:DueToOtherGovernmentsModifiedAccrual</v>
       </c>
       <c r="J136" t="s">
-        <v>2233</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="137" spans="1:10">
@@ -13232,7 +13239,7 @@
         <v>acfr:OtherCurrentAssetsModifiedAccrual</v>
       </c>
       <c r="E137" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="F137" t="str">
         <f t="shared" si="8"/>
@@ -13250,7 +13257,7 @@
         <v>acfr:DueToOthersModifiedAccrual</v>
       </c>
       <c r="J137" t="s">
-        <v>2234</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="138" spans="1:10">
@@ -13268,7 +13275,7 @@
         <v>acfr:OtherCurrentInvestmentsModifiedAccrual</v>
       </c>
       <c r="E138" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="F138" t="str">
         <f t="shared" si="8"/>
@@ -13286,7 +13293,7 @@
         <v>acfr:DueToPrimaryGovernmentModifiedAccrual</v>
       </c>
       <c r="J138" t="s">
-        <v>2235</v>
+        <v>2233</v>
       </c>
     </row>
     <row r="139" spans="1:10">
@@ -13304,7 +13311,7 @@
         <v>acfr:OtherReceivablesModifiedAccrual</v>
       </c>
       <c r="E139" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="F139" t="str">
         <f t="shared" si="8"/>
@@ -13322,7 +13329,7 @@
         <v>acfr:DueToRoadCommissionsModifiedAccrual</v>
       </c>
       <c r="J139" t="s">
-        <v>2236</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="140" spans="1:10">
@@ -13340,7 +13347,7 @@
         <v>acfr:OtherRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E140" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="F140" t="str">
         <f t="shared" si="8"/>
@@ -13358,7 +13365,7 @@
         <v>acfr:DueToSchoolsModifiedAccrual</v>
       </c>
       <c r="J140" t="s">
-        <v>2237</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="141" spans="1:10">
@@ -13376,7 +13383,7 @@
         <v>acfr:OtherTaxesReceivableModifiedAccrual</v>
       </c>
       <c r="E141" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="F141" t="str">
         <f t="shared" si="8"/>
@@ -13394,7 +13401,7 @@
         <v>acfr:DueToSpecialEducationModifiedAccrual</v>
       </c>
       <c r="J141" t="s">
-        <v>2238</v>
+        <v>2236</v>
       </c>
     </row>
     <row r="142" spans="1:10">
@@ -13412,7 +13419,7 @@
         <v>acfr:PatentsModifiedAccrual</v>
       </c>
       <c r="E142" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="F142" t="str">
         <f t="shared" si="8"/>
@@ -13430,7 +13437,7 @@
         <v>acfr:DueToStateGovernmentModifiedAccrual</v>
       </c>
       <c r="J142" t="s">
-        <v>2239</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="143" spans="1:10">
@@ -13448,7 +13455,7 @@
         <v>acfr:PaymentsInLieuOfTaxesReceivableModifiedAccrual</v>
       </c>
       <c r="E143" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="F143" t="str">
         <f t="shared" si="8"/>
@@ -13466,7 +13473,7 @@
         <v>acfr:DueToTaxpayersTaxOverpaymentsAndDuplicatePaymentsModifiedAccrual</v>
       </c>
       <c r="J143" t="s">
-        <v>2240</v>
+        <v>2238</v>
       </c>
     </row>
     <row r="144" spans="1:10">
@@ -13484,7 +13491,7 @@
         <v>acfr:PenaltiesReceivableModifiedAccrual</v>
       </c>
       <c r="E144" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="F144" t="str">
         <f t="shared" si="8"/>
@@ -13502,7 +13509,7 @@
         <v>acfr:DueToTownshipsModifiedAccrual</v>
       </c>
       <c r="J144" t="s">
-        <v>2241</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="145" spans="1:10">
@@ -13520,7 +13527,7 @@
         <v>acfr:PenaltiesReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E145" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="F145" t="str">
         <f t="shared" si="8"/>
@@ -13538,7 +13545,7 @@
         <v>acfr:DueToVillagesModifiedAccrual</v>
       </c>
       <c r="J145" t="s">
-        <v>2242</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="146" spans="1:10">
@@ -13556,7 +13563,7 @@
         <v>acfr:PenaltiesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E146" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="F146" t="str">
         <f t="shared" si="8"/>
@@ -13574,7 +13581,7 @@
         <v>acfr:GarnishmentsPayableModifiedAccrual</v>
       </c>
       <c r="J146" t="s">
-        <v>2243</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="147" spans="1:10">
@@ -13592,7 +13599,7 @@
         <v>acfr:PerformanceBondsPayableDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E147" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="F147" t="str">
         <f t="shared" si="8"/>
@@ -13610,7 +13617,7 @@
         <v>acfr:GrantsPayableModifiedAccrual</v>
       </c>
       <c r="J147" t="s">
-        <v>2244</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="148" spans="1:10">
@@ -13628,7 +13635,7 @@
         <v>acfr:PooledCashAndInvestmentsModifiedAccrual</v>
       </c>
       <c r="E148" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="F148" t="str">
         <f t="shared" si="8"/>
@@ -13646,7 +13653,7 @@
         <v>acfr:OtherAdvancesModifiedAccrual</v>
       </c>
       <c r="J148" t="s">
-        <v>2245</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="149" spans="1:10">
@@ -13664,7 +13671,7 @@
         <v>acfr:PrepaidDepositsModifiedAccrual</v>
       </c>
       <c r="E149" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="F149" t="str">
         <f t="shared" si="8"/>
@@ -13682,7 +13689,7 @@
         <v>acfr:PatientsOrInmatesTrustMoneyPayableModifiedAccrual</v>
       </c>
       <c r="J149" t="s">
-        <v>2246</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="150" spans="1:10">
@@ -13700,7 +13707,7 @@
         <v>acfr:PrepaidExpensesModifiedAccrual</v>
       </c>
       <c r="E150" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="F150" t="str">
         <f t="shared" si="8"/>
@@ -13718,7 +13725,7 @@
         <v>acfr:PayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="J150" t="s">
-        <v>2247</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="151" spans="1:10">
@@ -13736,7 +13743,7 @@
         <v>acfr:PrepaidsAndOtherAssetsModifiedAccrual</v>
       </c>
       <c r="E151" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="F151" t="str">
         <f t="shared" si="8"/>
@@ -13754,7 +13761,7 @@
         <v>acfr:PayrollDeductionsPayableModifiedAccrual</v>
       </c>
       <c r="J151" t="s">
-        <v>2248</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="152" spans="1:10">
@@ -13772,7 +13779,7 @@
         <v>acfr:PropertyTaxesReceivableModifiedAccrual</v>
       </c>
       <c r="E152" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="F152" t="str">
         <f t="shared" si="8"/>
@@ -13790,7 +13797,7 @@
         <v>acfr:PenaltiesPayableModifiedAccrual</v>
       </c>
       <c r="J152" t="s">
-        <v>2249</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="153" spans="1:10">
@@ -13808,7 +13815,7 @@
         <v>acfr:PropertyTaxesReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E153" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="F153" t="str">
         <f t="shared" si="8"/>
@@ -13826,7 +13833,7 @@
         <v>acfr:PerformanceDepositsPayableModifiedAccrual</v>
       </c>
       <c r="J153" t="s">
-        <v>2250</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="154" spans="1:10">
@@ -13844,7 +13851,7 @@
         <v>acfr:PropertyTaxesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E154" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="F154" t="str">
         <f t="shared" si="8"/>
@@ -13862,7 +13869,7 @@
         <v>acfr:ReceiptsRefundableModifiedAccrual</v>
       </c>
       <c r="J154" t="s">
-        <v>2251</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="155" spans="1:10">
@@ -13880,7 +13887,7 @@
         <v>acfr:ReceivableModifiedAccrual</v>
       </c>
       <c r="E155" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="F155" t="str">
         <f t="shared" si="8"/>
@@ -13898,7 +13905,7 @@
         <v>acfr:RegulatoryLiabilityCurrentModifiedAccrual</v>
       </c>
       <c r="J155" t="s">
-        <v>2252</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="156" spans="1:10">
@@ -13916,7 +13923,7 @@
         <v>acfr:ReceivablesModifiedAccrual</v>
       </c>
       <c r="E156" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="F156" t="str">
         <f t="shared" si="8"/>
@@ -13934,7 +13941,7 @@
         <v>acfr:RestitutionsPayableModifiedAccrual</v>
       </c>
       <c r="J156" t="s">
-        <v>2253</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="157" spans="1:10">
@@ -13952,7 +13959,7 @@
         <v>acfr:RegulatoryAssetsCurrentModifiedAccrual</v>
       </c>
       <c r="E157" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="F157" t="str">
         <f t="shared" si="8"/>
@@ -13970,7 +13977,7 @@
         <v>acfr:RetainagePayableModifiedAccrual</v>
       </c>
       <c r="J157" t="s">
-        <v>2254</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="158" spans="1:10">
@@ -13988,7 +13995,7 @@
         <v>acfr:RestrictedAccountsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E158" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="F158" t="str">
         <f t="shared" si="8"/>
@@ -14006,7 +14013,7 @@
         <v>acfr:TaxesPayableModifiedAccrual</v>
       </c>
       <c r="J158" t="s">
-        <v>2255</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="159" spans="1:10">
@@ -14024,7 +14031,7 @@
         <v>acfr:RestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E159" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="F159" t="str">
         <f t="shared" si="8"/>
@@ -14042,7 +14049,7 @@
         <v>acfr:UnclaimedMoneyModifiedAccrual</v>
       </c>
       <c r="J159" t="s">
-        <v>2256</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="160" spans="1:10">
@@ -14060,7 +14067,7 @@
         <v>acfr:RestrictedAssetsCustomModifiedAccrual</v>
       </c>
       <c r="E160" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="F160" t="str">
         <f t="shared" si="8"/>
@@ -14078,7 +14085,7 @@
         <v>acfr:UndistributedReceiptsModifiedAccrual</v>
       </c>
       <c r="J160" t="s">
-        <v>2257</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="161" spans="1:10">
@@ -14096,7 +14103,7 @@
         <v>acfr:RestrictedBondAndInterestRedemptionModifiedAccrual</v>
       </c>
       <c r="E161" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="F161" t="str">
         <f t="shared" si="8"/>
@@ -14114,7 +14121,7 @@
         <v>acfr:UndistributedTaxCollectionsModifiedAccrual</v>
       </c>
       <c r="J161" t="s">
-        <v>2258</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="162" spans="1:10">
@@ -14132,7 +14139,7 @@
         <v>acfr:RestrictedBondReserveModifiedAccrual</v>
       </c>
       <c r="E162" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="F162" t="str">
         <f t="shared" si="8"/>
@@ -14150,7 +14157,7 @@
         <v>acfr:UnearnedRevenueModifiedAccrual</v>
       </c>
       <c r="J162" t="s">
-        <v>2259</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="163" spans="1:10">
@@ -14168,7 +14175,7 @@
         <v>acfr:RestrictedCashModifiedAccrual</v>
       </c>
       <c r="E163" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="F163" t="str">
         <f t="shared" si="8"/>
@@ -14204,7 +14211,7 @@
         <v>acfr:RestrictedCashAndCashEquivalentsModifiedAccrual</v>
       </c>
       <c r="E164" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="F164" t="str">
         <f t="shared" si="8"/>
@@ -14222,7 +14229,7 @@
         <v>acfr:DeferredInflowsOfResourcesModifiedAccrual</v>
       </c>
       <c r="J164" t="s">
-        <v>2260</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="165" spans="1:10">
@@ -14240,7 +14247,7 @@
         <v>acfr:RestrictedCashAndInvestmentsModifiedAccrual</v>
       </c>
       <c r="E165" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="F165" t="str">
         <f t="shared" si="8"/>
@@ -14258,7 +14265,7 @@
         <v>acfr:DeferredInflowsOfResourcesPropertyTaxesModifiedAccrual</v>
       </c>
       <c r="J165" t="s">
-        <v>2261</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="166" spans="1:10">
@@ -14276,7 +14283,7 @@
         <v>acfr:RestrictedCashDebtRetirementModifiedAccrual</v>
       </c>
       <c r="E166" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="F166" t="str">
         <f t="shared" si="8"/>
@@ -14294,7 +14301,7 @@
         <v>acfr:DeferredInflowsOfResourcesTaxesLeviedForASubsequentPeriodModifiedAccrual</v>
       </c>
       <c r="J166" t="s">
-        <v>2262</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="167" spans="1:10">
@@ -14312,7 +14319,7 @@
         <v>acfr:RestrictedCashDebtServiceModifiedAccrual</v>
       </c>
       <c r="E167" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="F167" t="str">
         <f t="shared" si="8"/>
@@ -14330,7 +14337,7 @@
         <v>acfr:OtherDeferredInflowsOfResourcesModifiedAccrual</v>
       </c>
       <c r="J167" t="s">
-        <v>2263</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="168" spans="1:10">
@@ -14348,7 +14355,7 @@
         <v>acfr:RestrictedCashRepairsReplacementAndImprovementsReserveModifiedAccrual</v>
       </c>
       <c r="E168" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="F168" t="str">
         <f t="shared" si="8"/>
@@ -14366,7 +14373,7 @@
         <v>acfr:DeferredOutflowsOfResourcesModifiedAccrual</v>
       </c>
       <c r="J168" t="s">
-        <v>2264</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="169" spans="1:10">
@@ -14384,7 +14391,7 @@
         <v>acfr:RestrictedCertificatesOfDepositModifiedAccrual</v>
       </c>
       <c r="E169" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="F169" t="str">
         <f t="shared" si="8"/>
@@ -14402,7 +14409,7 @@
         <v>acfr:OtherDeferredOutflowsOfResourcesModifiedAccrual</v>
       </c>
       <c r="J169" t="s">
-        <v>2265</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="170" spans="1:10">
@@ -14420,7 +14427,7 @@
         <v>acfr:RestrictedReceivablesAndDepositsModifiedAccrual</v>
       </c>
       <c r="E170" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="F170" t="str">
         <f t="shared" si="8"/>
@@ -14438,7 +14445,7 @@
         <v>acfr:ConstructionInProgressModifiedAccrual</v>
       </c>
       <c r="J170" t="s">
-        <v>2266</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="171" spans="1:10">
@@ -14456,7 +14463,7 @@
         <v>acfr:RevenueBondsPayableDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E171" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="F171" t="str">
         <f t="shared" si="8"/>
@@ -14474,7 +14481,7 @@
         <v>acfr:InvestmentsInJointVenturesModifiedAccrual</v>
       </c>
       <c r="J171" t="s">
-        <v>2267</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="172" spans="1:10">
@@ -14492,7 +14499,7 @@
         <v>acfr:SalesTaxReceivableModifiedAccrual</v>
       </c>
       <c r="E172" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="F172" t="str">
         <f t="shared" si="8"/>
@@ -14510,7 +14517,7 @@
         <v>acfr:InvestmentsOfSurplusFundsModifiedAccrual</v>
       </c>
       <c r="J172" t="s">
-        <v>2268</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="173" spans="1:10">
@@ -14528,7 +14535,7 @@
         <v>acfr:SecuritiesLendingCollateralAssetsModifiedAccrual</v>
       </c>
       <c r="E173" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="F173" t="str">
         <f t="shared" si="8"/>
@@ -14546,7 +14553,7 @@
         <v>acfr:LeasesAccumulatedAmortizationModifiedAccrual</v>
       </c>
       <c r="J173" t="s">
-        <v>2269</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="174" spans="1:10">
@@ -14564,7 +14571,7 @@
         <v>acfr:SecuritiesLendingObligationsLiabilityModifiedAccrual</v>
       </c>
       <c r="E174" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="F174" t="str">
         <f t="shared" si="8"/>
@@ -14582,7 +14589,7 @@
         <v>acfr:LongTermContractsReceivableModifiedAccrual</v>
       </c>
       <c r="J174" t="s">
-        <v>2270</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="175" spans="1:10">
@@ -14600,7 +14607,7 @@
         <v>acfr:SelfInsuranceLiabilitiesCurrentPortionModifiedAccrual</v>
       </c>
       <c r="E175" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="F175" t="str">
         <f t="shared" si="8"/>
@@ -14618,7 +14625,7 @@
         <v>acfr:LongTermInvestmentsModifiedAccrual</v>
       </c>
       <c r="J175" t="s">
-        <v>2271</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="176" spans="1:10">
@@ -14636,7 +14643,7 @@
         <v>acfr:ServiceFeesReceivableModifiedAccrual</v>
       </c>
       <c r="E176" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="F176" t="str">
         <f t="shared" si="8"/>
@@ -14654,7 +14661,7 @@
         <v>acfr:NetOPEBAssetModifiedAccrual</v>
       </c>
       <c r="J176" t="s">
-        <v>2272</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="177" spans="1:10">
@@ -14672,7 +14679,7 @@
         <v>acfr:SpecialAssessmentTaxesReceivableModifiedAccrual</v>
       </c>
       <c r="E177" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="F177" t="str">
         <f t="shared" si="8"/>
@@ -14690,7 +14697,7 @@
         <v>acfr:NetPensionAssetModifiedAccrual</v>
       </c>
       <c r="J177" t="s">
-        <v>2273</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="178" spans="1:10">
@@ -14708,7 +14715,7 @@
         <v>acfr:SpecialAssessmentTaxesReceivableUnavailableModifiedAccrual</v>
       </c>
       <c r="E178" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="F178" t="str">
         <f t="shared" si="8"/>
@@ -14726,7 +14733,7 @@
         <v>acfr:OtherAssetsModifiedAccrual</v>
       </c>
       <c r="J178" t="s">
-        <v>2274</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="179" spans="1:10">
@@ -14744,7 +14751,7 @@
         <v>acfr:SpecialAssessmentsReceivableDelinquentModifiedAccrual</v>
       </c>
       <c r="E179" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="F179" t="str">
         <f t="shared" si="8"/>
@@ -14762,7 +14769,7 @@
         <v>acfr:OtherInvestmentsModifiedAccrual</v>
       </c>
       <c r="J179" t="s">
-        <v>2275</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="180" spans="1:10">
@@ -14780,7 +14787,7 @@
         <v>acfr:TaxesReceivableModifiedAccrual</v>
       </c>
       <c r="E180" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="F180" t="str">
         <f t="shared" si="8"/>
@@ -14798,7 +14805,7 @@
         <v>acfr:UnamortizedDiscountsOnBondsSoldByLocalUnitModifiedAccrual</v>
       </c>
       <c r="J180" t="s">
-        <v>2276</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="181" spans="1:10">
@@ -14816,7 +14823,7 @@
         <v>acfr:TaxesReceivableDelinquentPersonalPropertyModifiedAccrual</v>
       </c>
       <c r="E181" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="F181" t="str">
         <f t="shared" si="8"/>
@@ -14834,7 +14841,7 @@
         <v>acfr:AdvancesToComponentUnitModifiedAccrual</v>
       </c>
       <c r="J181" t="s">
-        <v>2277</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="182" spans="1:10">
@@ -14852,7 +14859,7 @@
         <v>acfr:TaxesReceivableDelinquentRealPropertyModifiedAccrual</v>
       </c>
       <c r="E182" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="F182" t="str">
         <f t="shared" si="8"/>
@@ -14870,7 +14877,7 @@
         <v>acfr:AdvancesToOtherFundsModifiedAccrual</v>
       </c>
       <c r="J182" t="s">
-        <v>2278</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="183" spans="1:10">
@@ -14888,7 +14895,7 @@
         <v>acfr:TaxesReceivablePersonalPropertyCurrentLevyModifiedAccrual</v>
       </c>
       <c r="E183" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="F183" t="str">
         <f t="shared" si="8"/>
@@ -14906,7 +14913,7 @@
         <v>acfr:AdvancesToOtherGovernmentsModifiedAccrual</v>
       </c>
       <c r="J183" t="s">
-        <v>2279</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="184" spans="1:10">
@@ -14924,7 +14931,7 @@
         <v>acfr:TaxesReceivableRealPropertyCurrentLevyModifiedAccrual</v>
       </c>
       <c r="E184" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="F184" t="str">
         <f t="shared" si="8"/>
@@ -14957,7 +14964,7 @@
         <v>acfr:TenantAccountsReceivableModifiedAccrual</v>
       </c>
       <c r="E185" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="F185" t="str">
         <f t="shared" si="8"/>
@@ -14987,7 +14994,7 @@
         <v>acfr:TenantAccountsReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E186" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="F186" t="str">
         <f t="shared" si="8"/>
@@ -15017,7 +15024,7 @@
         <v>acfr:TenantAccountsReceivableNetOfAllowancesModifiedAccrual</v>
       </c>
       <c r="E187" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="F187" t="str">
         <f t="shared" si="8"/>
@@ -15047,7 +15054,7 @@
         <v>acfr:TimberRightsModifiedAccrual</v>
       </c>
       <c r="E188" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="F188" t="str">
         <f t="shared" si="8"/>
@@ -15077,7 +15084,7 @@
         <v>acfr:TradeReceivableModifiedAccrual</v>
       </c>
       <c r="E189" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="F189" t="str">
         <f t="shared" si="8"/>
@@ -15107,7 +15114,7 @@
         <v>acfr:TradeReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E190" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="F190" t="str">
         <f t="shared" si="8"/>
@@ -15137,7 +15144,7 @@
         <v>acfr:TradeReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E191" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="F191" t="str">
         <f t="shared" si="8"/>
@@ -15167,7 +15174,7 @@
         <v>acfr:TrademarksModifiedAccrual</v>
       </c>
       <c r="E192" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="F192" t="str">
         <f t="shared" si="8"/>
@@ -15197,7 +15204,7 @@
         <v>acfr:TuitionAndFeesAllowancesModifiedAccrual</v>
       </c>
       <c r="E193" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="F193" t="str">
         <f t="shared" si="8"/>
@@ -15227,7 +15234,7 @@
         <v>acfr:TuitionAndFeesReceivableModifiedAccrual</v>
       </c>
       <c r="E194" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="F194" t="str">
         <f t="shared" si="8"/>
@@ -15257,7 +15264,7 @@
         <v>acfr:TuitionAndFeesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E195" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="F195" t="str">
         <f t="shared" ref="F195:F258" si="12">"acfr:"&amp;E195</f>
@@ -15287,7 +15294,7 @@
         <v>acfr:UnamortizedPremiumOnBondsPrincipalDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E196" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="F196" t="str">
         <f t="shared" si="12"/>
@@ -15317,7 +15324,7 @@
         <v>acfr:UnbilledRevenueModifiedAccrual</v>
       </c>
       <c r="E197" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="F197" t="str">
         <f t="shared" si="12"/>
@@ -15347,7 +15354,7 @@
         <v>acfr:UninsuredClaimLiabilityCurrentPortionModifiedAccrual</v>
       </c>
       <c r="E198" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="F198" t="str">
         <f t="shared" si="12"/>
@@ -15377,7 +15384,7 @@
         <v>acfr:UnlimitedTaxBondsPrincipalDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E199" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="F199" t="str">
         <f t="shared" si="12"/>
@@ -15407,7 +15414,7 @@
         <v>acfr:UtilitiesAndWaterReceivableModifiedAccrual</v>
       </c>
       <c r="E200" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="F200" t="str">
         <f t="shared" si="12"/>
@@ -15437,7 +15444,7 @@
         <v>acfr:UtilitiesAndWaterReceivableAllowanceModifiedAccrual</v>
       </c>
       <c r="E201" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="F201" t="str">
         <f t="shared" si="12"/>
@@ -15467,7 +15474,7 @@
         <v>acfr:UtilitiesAndWaterReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
       <c r="E202" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="F202" t="str">
         <f t="shared" si="12"/>
@@ -15497,7 +15504,7 @@
         <v>acfr:VestedEmployeeBenefitsPayableDueWithinOneYearModifiedAccrual</v>
       </c>
       <c r="E203" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="F203" t="str">
         <f t="shared" si="12"/>
@@ -15527,7 +15534,7 @@
         <v>acfr:WaterRightsModifiedAccrual</v>
       </c>
       <c r="E204" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="F204" t="str">
         <f t="shared" si="12"/>
@@ -15557,7 +15564,7 @@
         <v>acfr:AccountsPayableModifiedAccrual</v>
       </c>
       <c r="E205" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="F205" t="str">
         <f t="shared" si="12"/>
@@ -15587,7 +15594,7 @@
         <v>acfr:AccountsPayableAndAccruedLiabilitiesModifiedAccrual</v>
       </c>
       <c r="E206" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="F206" t="str">
         <f t="shared" si="12"/>
@@ -15617,7 +15624,7 @@
         <v>acfr:AccountsPayableNoncurrentPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E207" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="F207" t="str">
         <f t="shared" si="12"/>
@@ -15647,7 +15654,7 @@
         <v>acfr:AccountsPayablePayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E208" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="F208" t="str">
         <f t="shared" si="12"/>
@@ -15677,7 +15684,7 @@
         <v>acfr:AccruedConnectionFeesModifiedAccrual</v>
       </c>
       <c r="E209" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="F209" t="str">
         <f t="shared" si="12"/>
@@ -15707,7 +15714,7 @@
         <v>acfr:AccruedExpensesPayableModifiedAccrual</v>
       </c>
       <c r="E210" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="F210" t="str">
         <f t="shared" si="12"/>
@@ -15737,7 +15744,7 @@
         <v>acfr:AccruedInterestAndPenaltiesModifiedAccrual</v>
       </c>
       <c r="E211" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="F211" t="str">
         <f t="shared" si="12"/>
@@ -15767,7 +15774,7 @@
         <v>acfr:AccruedInterestPayableModifiedAccrual</v>
       </c>
       <c r="E212" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="F212" t="str">
         <f t="shared" si="12"/>
@@ -15797,7 +15804,7 @@
         <v>acfr:AccruedInterestPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E213" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="F213" t="str">
         <f t="shared" si="12"/>
@@ -15827,7 +15834,7 @@
         <v>acfr:AccruedLiabilitiesModifiedAccrual</v>
       </c>
       <c r="E214" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="F214" t="str">
         <f t="shared" si="12"/>
@@ -15857,7 +15864,7 @@
         <v>acfr:AccruedSickLeavePayableModifiedAccrual</v>
       </c>
       <c r="E215" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="F215" t="str">
         <f t="shared" si="12"/>
@@ -15887,7 +15894,7 @@
         <v>acfr:AccruedTuitionAndFeesModifiedAccrual</v>
       </c>
       <c r="E216" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="F216" t="str">
         <f t="shared" si="12"/>
@@ -15917,7 +15924,7 @@
         <v>acfr:AccruedVacationPayableModifiedAccrual</v>
       </c>
       <c r="E217" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="F217" t="str">
         <f t="shared" si="12"/>
@@ -15947,7 +15954,7 @@
         <v>acfr:AccruedWagesAndRelatedLiabilitiesPayableModifiedAccrual</v>
       </c>
       <c r="E218" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="F218" t="str">
         <f t="shared" si="12"/>
@@ -15977,7 +15984,7 @@
         <v>acfr:AccruedWagesPayableModifiedAccrual</v>
       </c>
       <c r="E219" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="F219" t="str">
         <f t="shared" si="12"/>
@@ -16007,7 +16014,7 @@
         <v>acfr:AdvancesCurrentModifiedAccrual</v>
       </c>
       <c r="E220" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="F220" t="str">
         <f t="shared" si="12"/>
@@ -16037,7 +16044,7 @@
         <v>acfr:AdvancesFromFederalGovernmentNoncurrentModifiedAccrual</v>
       </c>
       <c r="E221" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="F221" t="str">
         <f t="shared" si="12"/>
@@ -16067,7 +16074,7 @@
         <v>acfr:AdvancesFromGrantorsModifiedAccrual</v>
       </c>
       <c r="E222" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="F222" t="str">
         <f t="shared" si="12"/>
@@ -16097,7 +16104,7 @@
         <v>acfr:AdvancesFromOtherFundsModifiedAccrual</v>
       </c>
       <c r="E223" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="F223" t="str">
         <f t="shared" si="12"/>
@@ -16127,7 +16134,7 @@
         <v>acfr:AdvancesFromOtherFundsNoncurrentModifiedAccrual</v>
       </c>
       <c r="E224" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="F224" t="str">
         <f t="shared" si="12"/>
@@ -16157,7 +16164,7 @@
         <v>acfr:AdvancesFromOtherFundsNoncurrentPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E225" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="F225" t="str">
         <f t="shared" si="12"/>
@@ -16187,7 +16194,7 @@
         <v>acfr:AdvancesFromOtherFundsPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E226" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="F226" t="str">
         <f t="shared" si="12"/>
@@ -16217,7 +16224,7 @@
         <v>acfr:AdvancesFromOtherGovernmentsModifiedAccrual</v>
       </c>
       <c r="E227" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="F227" t="str">
         <f t="shared" si="12"/>
@@ -16247,7 +16254,7 @@
         <v>acfr:AdvancesFromOtherGovernmentsNoncurrentModifiedAccrual</v>
       </c>
       <c r="E228" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="F228" t="str">
         <f t="shared" si="12"/>
@@ -16277,7 +16284,7 @@
         <v>acfr:AdvancesFromPrimaryGovernmentNoncurrentModifiedAccrual</v>
       </c>
       <c r="E229" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="F229" t="str">
         <f t="shared" si="12"/>
@@ -16307,7 +16314,7 @@
         <v>acfr:AdvancesFromStateNoncurrentModifiedAccrual</v>
       </c>
       <c r="E230" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="F230" t="str">
         <f t="shared" si="12"/>
@@ -16337,7 +16344,7 @@
         <v>acfr:AdvancesReceivedNoncurrentModifiedAccrual</v>
       </c>
       <c r="E231" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="F231" t="str">
         <f t="shared" si="12"/>
@@ -16367,7 +16374,7 @@
         <v>acfr:AdvancesSpecialAssessmentDistrictsModifiedAccrual</v>
       </c>
       <c r="E232" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="F232" t="str">
         <f t="shared" si="12"/>
@@ -16397,7 +16404,7 @@
         <v>acfr:AnnuitiesPayableModifiedAccrual</v>
       </c>
       <c r="E233" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="F233" t="str">
         <f t="shared" si="12"/>
@@ -16427,7 +16434,7 @@
         <v>acfr:BondInterestPayableModifiedAccrual</v>
       </c>
       <c r="E234" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="F234" t="str">
         <f t="shared" si="12"/>
@@ -16457,7 +16464,7 @@
         <v>acfr:BondsPayableDueInMoreThanOneYearPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E235" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="F235" t="str">
         <f t="shared" si="12"/>
@@ -16487,7 +16494,7 @@
         <v>acfr:BondsPayableDueWithinOneYearPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E236" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="F236" t="str">
         <f t="shared" si="12"/>
@@ -16517,7 +16524,7 @@
         <v>acfr:CashBondsPayableModifiedAccrual</v>
       </c>
       <c r="E237" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="F237" t="str">
         <f t="shared" si="12"/>
@@ -16547,7 +16554,7 @@
         <v>acfr:CashOverdraftsModifiedAccrual</v>
       </c>
       <c r="E238" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="F238" t="str">
         <f t="shared" si="12"/>
@@ -16577,7 +16584,7 @@
         <v>acfr:ChecksWrittenAgainstFutureDepositsModifiedAccrual</v>
       </c>
       <c r="E239" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="F239" t="str">
         <f t="shared" si="12"/>
@@ -16607,7 +16614,7 @@
         <v>acfr:CompensatedAbsencesPayableCurrentModifiedAccrual</v>
       </c>
       <c r="E240" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="F240" t="str">
         <f t="shared" si="12"/>
@@ -16637,7 +16644,7 @@
         <v>acfr:ContractsPayableDueWithinOneYearPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E241" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="F241" t="str">
         <f t="shared" si="12"/>
@@ -16667,7 +16674,7 @@
         <v>acfr:CourtOrdersPayableModifiedAccrual</v>
       </c>
       <c r="E242" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="F242" t="str">
         <f t="shared" si="12"/>
@@ -16697,7 +16704,7 @@
         <v>acfr:CurrentLiabilitiesModifiedAccrual</v>
       </c>
       <c r="E243" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="F243" t="str">
         <f t="shared" si="12"/>
@@ -16727,7 +16734,7 @@
         <v>acfr:CurrentLiabilitiesCustomModifiedAccrual</v>
       </c>
       <c r="E244" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="F244" t="str">
         <f t="shared" si="12"/>
@@ -16757,7 +16764,7 @@
         <v>acfr:CurrentLiabilitiesPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E245" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="F245" t="str">
         <f t="shared" si="12"/>
@@ -16787,7 +16794,7 @@
         <v>acfr:CustomerDepositsModifiedAccrual</v>
       </c>
       <c r="E246" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="F246" t="str">
         <f t="shared" si="12"/>
@@ -16817,7 +16824,7 @@
         <v>acfr:CustomerDepositsPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E247" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="F247" t="str">
         <f t="shared" si="12"/>
@@ -16847,7 +16854,7 @@
         <v>acfr:DepositsHeldforOthersModifiedAccrual</v>
       </c>
       <c r="E248" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="F248" t="str">
         <f t="shared" si="12"/>
@@ -16877,7 +16884,7 @@
         <v>acfr:DrainOrdersPayableModifiedAccrual</v>
       </c>
       <c r="E249" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="F249" t="str">
         <f t="shared" si="12"/>
@@ -16907,7 +16914,7 @@
         <v>acfr:DueToCitiesModifiedAccrual</v>
       </c>
       <c r="E250" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="F250" t="str">
         <f t="shared" si="12"/>
@@ -16937,7 +16944,7 @@
         <v>acfr:DueToCommunityCollegeModifiedAccrual</v>
       </c>
       <c r="E251" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="F251" t="str">
         <f t="shared" si="12"/>
@@ -16967,7 +16974,7 @@
         <v>acfr:DueToComponentUnitModifiedAccrual</v>
       </c>
       <c r="E252" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="F252" t="str">
         <f t="shared" si="12"/>
@@ -16997,7 +17004,7 @@
         <v>acfr:DueToCountiesModifiedAccrual</v>
       </c>
       <c r="E253" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="F253" t="str">
         <f t="shared" si="12"/>
@@ -17027,7 +17034,7 @@
         <v>acfr:DueToCourtWardsModifiedAccrual</v>
       </c>
       <c r="E254" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="F254" t="str">
         <f t="shared" si="12"/>
@@ -17057,7 +17064,7 @@
         <v>acfr:DueToEducationModifiedAccrual</v>
       </c>
       <c r="E255" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="F255" t="str">
         <f t="shared" si="12"/>
@@ -17087,7 +17094,7 @@
         <v>acfr:DueToEmployeesModifiedAccrual</v>
       </c>
       <c r="E256" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F256" t="str">
         <f t="shared" si="12"/>
@@ -17117,7 +17124,7 @@
         <v>acfr:DueToFederalGovernmentModifiedAccrual</v>
       </c>
       <c r="E257" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F257" t="str">
         <f t="shared" si="12"/>
@@ -17147,7 +17154,7 @@
         <v>acfr:DueToFiduciaryFundsModifiedAccrual</v>
       </c>
       <c r="E258" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="F258" t="str">
         <f t="shared" si="12"/>
@@ -17177,7 +17184,7 @@
         <v>acfr:DueToFiscalAgentModifiedAccrual</v>
       </c>
       <c r="E259" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="F259" t="str">
         <f t="shared" ref="F259:F322" si="17">"acfr:"&amp;E259</f>
@@ -17207,7 +17214,7 @@
         <v>acfr:DueToFormerEmployeesModifiedAccrual</v>
       </c>
       <c r="E260" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="F260" t="str">
         <f t="shared" si="17"/>
@@ -17237,7 +17244,7 @@
         <v>acfr:DueToGeneralFundModifiedAccrual</v>
       </c>
       <c r="E261" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="F261" t="str">
         <f t="shared" si="17"/>
@@ -17267,7 +17274,7 @@
         <v>acfr:DueToIntermediateSchoolDistrictsModifiedAccrual</v>
       </c>
       <c r="E262" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="F262" t="str">
         <f t="shared" si="17"/>
@@ -17297,7 +17304,7 @@
         <v>acfr:DueToLibrariesModifiedAccrual</v>
       </c>
       <c r="E263" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="F263" t="str">
         <f t="shared" si="17"/>
@@ -17327,7 +17334,7 @@
         <v>acfr:DueToOtherAgenciesPayableFromRestictedAssetsModifiedAccrual</v>
       </c>
       <c r="E264" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="F264" t="str">
         <f t="shared" si="17"/>
@@ -17357,7 +17364,7 @@
         <v>acfr:DueToOtherFundsModifiedAccrual</v>
       </c>
       <c r="E265" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="F265" t="str">
         <f t="shared" si="17"/>
@@ -17387,7 +17394,7 @@
         <v>acfr:DueToOtherGovernmentsModifiedAccrual</v>
       </c>
       <c r="E266" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="F266" t="str">
         <f t="shared" si="17"/>
@@ -17417,7 +17424,7 @@
         <v>acfr:DueToOthersModifiedAccrual</v>
       </c>
       <c r="E267" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="F267" t="str">
         <f t="shared" si="17"/>
@@ -17447,7 +17454,7 @@
         <v>acfr:DueToPrimaryGovernmentModifiedAccrual</v>
       </c>
       <c r="E268" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="F268" t="str">
         <f t="shared" si="17"/>
@@ -17477,7 +17484,7 @@
         <v>acfr:DueToProprietaryFundsModifiedAccrual</v>
       </c>
       <c r="E269" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="F269" t="str">
         <f t="shared" si="17"/>
@@ -17507,7 +17514,7 @@
         <v>acfr:DueToRelatedPartiesModifiedAccrual</v>
       </c>
       <c r="E270" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="F270" t="str">
         <f t="shared" si="17"/>
@@ -17537,7 +17544,7 @@
         <v>acfr:DueToRoadCommissionsModifiedAccrual</v>
       </c>
       <c r="E271" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="F271" t="str">
         <f t="shared" si="17"/>
@@ -17567,7 +17574,7 @@
         <v>acfr:DueToSchoolsModifiedAccrual</v>
       </c>
       <c r="E272" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="F272" t="str">
         <f t="shared" si="17"/>
@@ -17597,7 +17604,7 @@
         <v>acfr:DueToSpecialEducationModifiedAccrual</v>
       </c>
       <c r="E273" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="F273" t="str">
         <f t="shared" si="17"/>
@@ -17627,7 +17634,7 @@
         <v>acfr:DueToStateGovernmentModifiedAccrual</v>
       </c>
       <c r="E274" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="F274" t="str">
         <f t="shared" si="17"/>
@@ -17657,7 +17664,7 @@
         <v>acfr:DueToTaxpayersTaxOverpaymentsAndDuplicatePaymentsModifiedAccrual</v>
       </c>
       <c r="E275" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="F275" t="str">
         <f t="shared" si="17"/>
@@ -17687,7 +17694,7 @@
         <v>acfr:DueToTownshipsModifiedAccrual</v>
       </c>
       <c r="E276" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="F276" t="str">
         <f t="shared" si="17"/>
@@ -17717,7 +17724,7 @@
         <v>acfr:DueToVillagesModifiedAccrual</v>
       </c>
       <c r="E277" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="F277" t="str">
         <f t="shared" si="17"/>
@@ -17747,7 +17754,7 @@
         <v>acfr:Dup_1_DueToGovernmentsModifiedAccrual</v>
       </c>
       <c r="E278" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="F278" t="str">
         <f t="shared" si="17"/>
@@ -17777,7 +17784,7 @@
         <v>acfr:EscrowDepositsModifiedAccrual</v>
       </c>
       <c r="E279" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="F279" t="str">
         <f t="shared" si="17"/>
@@ -17807,7 +17814,7 @@
         <v>acfr:FamilySelfSuffciencyEscrowsModifiedAccrual</v>
       </c>
       <c r="E280" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="F280" t="str">
         <f t="shared" si="17"/>
@@ -17837,7 +17844,7 @@
         <v>acfr:GarnishmentsPayableModifiedAccrual</v>
       </c>
       <c r="E281" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="F281" t="str">
         <f t="shared" si="17"/>
@@ -17867,7 +17874,7 @@
         <v>acfr:GrantsPayableModifiedAccrual</v>
       </c>
       <c r="E282" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="F282" t="str">
         <f t="shared" si="17"/>
@@ -17897,7 +17904,7 @@
         <v>acfr:InternalBalancesPayableModifiedAccrual</v>
       </c>
       <c r="E283" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="F283" t="str">
         <f t="shared" si="17"/>
@@ -17927,7 +17934,7 @@
         <v>acfr:LongTermDebtDueInMoreThanOneYearPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E284" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="F284" t="str">
         <f t="shared" si="17"/>
@@ -17957,7 +17964,7 @@
         <v>acfr:LongTermDebtDueWithinOneYearPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E285" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="F285" t="str">
         <f t="shared" si="17"/>
@@ -17987,7 +17994,7 @@
         <v>acfr:LotteryPrizeLiabilityCurrentModifiedAccrual</v>
       </c>
       <c r="E286" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="F286" t="str">
         <f t="shared" si="17"/>
@@ -18017,7 +18024,7 @@
         <v>acfr:LotteryPrizesPayableModifiedAccrual</v>
       </c>
       <c r="E287" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="F287" t="str">
         <f t="shared" si="17"/>
@@ -18047,7 +18054,7 @@
         <v>acfr:NetPensionLiabilityPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E288" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="F288" t="str">
         <f t="shared" si="17"/>
@@ -18077,7 +18084,7 @@
         <v>acfr:NoncurrentLiabilitiesPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E289" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="F289" t="str">
         <f t="shared" si="17"/>
@@ -18107,7 +18114,7 @@
         <v>acfr:OtherAccountsPayableModifiedAccrual</v>
       </c>
       <c r="E290" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="F290" t="str">
         <f t="shared" si="17"/>
@@ -18137,7 +18144,7 @@
         <v>acfr:OtherAccountsPayableAndAccruedLiabilitiesModifiedAccrual</v>
       </c>
       <c r="E291" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="F291" t="str">
         <f t="shared" si="17"/>
@@ -18167,7 +18174,7 @@
         <v>acfr:OtherAccruedExpensesModifiedAccrual</v>
       </c>
       <c r="E292" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="F292" t="str">
         <f t="shared" si="17"/>
@@ -18197,7 +18204,7 @@
         <v>acfr:OtherAdvancesModifiedAccrual</v>
       </c>
       <c r="E293" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="F293" t="str">
         <f t="shared" si="17"/>
@@ -18227,7 +18234,7 @@
         <v>acfr:OtherCurrentLiabilitiesModifiedAccrual</v>
       </c>
       <c r="E294" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="F294" t="str">
         <f t="shared" si="17"/>
@@ -18257,7 +18264,7 @@
         <v>acfr:OtherCurrentLiabilitiesPayableFromRestictedAssetsModifiedAccrual</v>
       </c>
       <c r="E295" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="F295" t="str">
         <f t="shared" si="17"/>
@@ -18287,7 +18294,7 @@
         <v>acfr:OtherNoncurrentLiabilitiesPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E296" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="F296" t="str">
         <f t="shared" si="17"/>
@@ -18317,7 +18324,7 @@
         <v>acfr:PatientsOrInmatesTrustMoneyPayableModifiedAccrual</v>
       </c>
       <c r="E297" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F297" t="str">
         <f t="shared" si="17"/>
@@ -18347,7 +18354,7 @@
         <v>acfr:PayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E298" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="F298" t="str">
         <f t="shared" si="17"/>
@@ -18377,7 +18384,7 @@
         <v>acfr:PayableFromRestrictedAssetsCustomModifiedAccrual</v>
       </c>
       <c r="E299" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="F299" t="str">
         <f t="shared" si="17"/>
@@ -18407,7 +18414,7 @@
         <v>acfr:PayrollDeductionsPayableModifiedAccrual</v>
       </c>
       <c r="E300" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="F300" t="str">
         <f t="shared" si="17"/>
@@ -18437,7 +18444,7 @@
         <v>acfr:PayrollTaxesPayableModifiedAccrual</v>
       </c>
       <c r="E301" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="F301" t="str">
         <f t="shared" si="17"/>
@@ -18467,7 +18474,7 @@
         <v>acfr:PenaltiesPayableModifiedAccrual</v>
       </c>
       <c r="E302" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="F302" t="str">
         <f t="shared" si="17"/>
@@ -18497,7 +18504,7 @@
         <v>acfr:PerformanceDepositsPayableModifiedAccrual</v>
       </c>
       <c r="E303" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="F303" t="str">
         <f t="shared" si="17"/>
@@ -18527,7 +18534,7 @@
         <v>acfr:ReceiptsRefundableModifiedAccrual</v>
       </c>
       <c r="E304" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="F304" t="str">
         <f t="shared" si="17"/>
@@ -18557,7 +18564,7 @@
         <v>acfr:RefundableDepositsBondsModifiedAccrual</v>
       </c>
       <c r="E305" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="F305" t="str">
         <f t="shared" si="17"/>
@@ -18587,7 +18594,7 @@
         <v>acfr:RegulatoryLiabilityCurrentModifiedAccrual</v>
       </c>
       <c r="E306" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="F306" t="str">
         <f t="shared" si="17"/>
@@ -18617,7 +18624,7 @@
         <v>acfr:RestitutionsPayableModifiedAccrual</v>
       </c>
       <c r="E307" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="F307" t="str">
         <f t="shared" si="17"/>
@@ -18647,7 +18654,7 @@
         <v>acfr:RetainagePayableModifiedAccrual</v>
       </c>
       <c r="E308" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="F308" t="str">
         <f t="shared" si="17"/>
@@ -18677,7 +18684,7 @@
         <v>acfr:RevenueBondsPayableDueWithinOneYearPayableFromRestrictedAssetsModifiedAccrual</v>
       </c>
       <c r="E309" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="F309" t="str">
         <f t="shared" si="17"/>
@@ -18707,7 +18714,7 @@
         <v>acfr:ShortTermDebtPayableModifiedAccrual</v>
       </c>
       <c r="E310" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="F310" t="str">
         <f t="shared" si="17"/>
@@ -18737,7 +18744,7 @@
         <v>acfr:TaxesPayableModifiedAccrual</v>
       </c>
       <c r="E311" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="F311" t="str">
         <f t="shared" si="17"/>
@@ -18767,7 +18774,7 @@
         <v>acfr:TenantSecurityDepositsPayableFromRestictedAssetsModifiedAccrual</v>
       </c>
       <c r="E312" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="F312" t="str">
         <f t="shared" si="17"/>
@@ -18797,7 +18804,7 @@
         <v>acfr:UnclaimedMoneyModifiedAccrual</v>
       </c>
       <c r="E313" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="F313" t="str">
         <f t="shared" si="17"/>
@@ -18827,7 +18834,7 @@
         <v>acfr:UndistributedReceiptsModifiedAccrual</v>
       </c>
       <c r="E314" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="F314" t="str">
         <f t="shared" si="17"/>
@@ -18857,7 +18864,7 @@
         <v>acfr:UndistributedTaxCollectionsModifiedAccrual</v>
       </c>
       <c r="E315" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="F315" t="str">
         <f t="shared" si="17"/>
@@ -18887,7 +18894,7 @@
         <v>acfr:UnearnedRevenueModifiedAccrual</v>
       </c>
       <c r="E316" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="F316" t="str">
         <f t="shared" si="17"/>
@@ -18917,7 +18924,7 @@
         <v>acfr:UnearnedRevenuePayableFromRestictedAssetsModifiedAccrual</v>
       </c>
       <c r="E317" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="F317" t="str">
         <f t="shared" si="17"/>
@@ -18947,7 +18954,7 @@
         <v>acfr:UnearnedTicketSalesModifiedAccrual</v>
       </c>
       <c r="E318" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="F318" t="str">
         <f t="shared" si="17"/>
@@ -18977,7 +18984,7 @@
         <v>acfr:VouchersPayableModifiedAccrual</v>
       </c>
       <c r="E319" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="F319" t="str">
         <f t="shared" si="17"/>
@@ -19007,7 +19014,7 @@
         <v>acfr:DeferredInflowsFromDeferredAmountOnRefundingModifiedAccrual</v>
       </c>
       <c r="E320" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="F320" t="str">
         <f t="shared" si="17"/>
@@ -19037,7 +19044,7 @@
         <v>acfr:DeferredInflowsFromOPEBChangesInProportionModifiedAccrual</v>
       </c>
       <c r="E321" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="F321" t="str">
         <f t="shared" si="17"/>
@@ -19067,7 +19074,7 @@
         <v>acfr:DeferredInflowsFromPensionChangesInProportionModifiedAccrual</v>
       </c>
       <c r="E322" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="F322" t="str">
         <f t="shared" si="17"/>
@@ -19097,7 +19104,7 @@
         <v>acfr:DeferredInflowsOfResourcesModifiedAccrual</v>
       </c>
       <c r="E323" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="F323" t="str">
         <f t="shared" ref="F323:F331" si="21">"acfr:"&amp;E323</f>
@@ -19127,7 +19134,7 @@
         <v>acfr:DeferredInflowsOfResourcesCustomModifiedAccrual</v>
       </c>
       <c r="E324" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="F324" t="str">
         <f t="shared" si="21"/>
@@ -19157,7 +19164,7 @@
         <v>acfr:DeferredInflowsOfResourcesDebtModifiedAccrual</v>
       </c>
       <c r="E325" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="F325" t="str">
         <f t="shared" si="21"/>
@@ -19187,7 +19194,7 @@
         <v>acfr:DeferredInflowsOfResourcesDrainOrdersModifiedAccrual</v>
       </c>
       <c r="E326" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="F326" t="str">
         <f t="shared" si="21"/>
@@ -19217,7 +19224,7 @@
         <v>acfr:DeferredInflowsOfResourcesLeasesModifiedAccrual</v>
       </c>
       <c r="E327" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="F327" t="str">
         <f t="shared" si="21"/>
@@ -19247,7 +19254,7 @@
         <v>acfr:DeferredInflowsOfResourcesOPEBModifiedAccrual</v>
       </c>
       <c r="E328" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="F328" t="str">
         <f t="shared" si="21"/>
@@ -19277,7 +19284,7 @@
         <v>acfr:DeferredInflowsOfResourcesOPEBChangesInAssumptionsModifiedAccrual</v>
       </c>
       <c r="E329" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="F329" t="str">
         <f t="shared" si="21"/>
@@ -19307,7 +19314,7 @@
         <v>acfr:DeferredInflowsOfResourcesOPEBContributionsMadeAfterMeasurementDateModifiedAccrual</v>
       </c>
       <c r="E330" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="F330" t="str">
         <f t="shared" si="21"/>
@@ -19337,7 +19344,7 @@
         <v>acfr:DeferredInflowsOfResourcesPensionModifiedAccrual</v>
       </c>
       <c r="E331" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="F331" t="str">
         <f t="shared" si="21"/>
@@ -36957,7 +36964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62560919-E4A0-3A4F-9164-3F35B35B852C}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
removed 2 cols to clean up in label dropdowns
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/byflow/Documents/Research/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A16A9F4-CED8-0C48-A512-DEBE978050A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7664A1AC-643D-D94A-9BC4-8483A931E063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3163" uniqueCount="2281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2979" uniqueCount="2099">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -6368,552 +6368,6 @@
   </si>
   <si>
     <t>Keep cells in col D that are marked 'Exists'</t>
-  </si>
-  <si>
-    <t>acfr:AccountsReceivableNetOfAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AccruedInterestReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AccruedInterestReceivableNetOfAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AssetsHeldForSaleModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CashModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CashAndCashEquivalentsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CashAndCashEquivalentsAndInvestmentsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CashAndCashEquivalentsWithFiscalAndEscrowAndOtherAgentsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CashAndCashEquivalentsWithTreasurerModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CashAndCashEquivalentsWithTrusteeModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CashCheckingModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CashOnHandModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CashPayrollBankAccountModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CashSavingsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CertificatesOfDepositModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:ClaimsAndJudgmentsReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:ClaimsAndJudgmentsReceivableNetOfAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:ContractsPayableDueWithinOneYearModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CourtOrdersReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DelinquentTaxesReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DelinquentUtilityBillsReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DepositsReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>Actual Modified Labels</t>
-  </si>
-  <si>
-    <t>Filtered col H without spaces</t>
-  </si>
-  <si>
-    <t>acfr:DepositsReceivableNetOfAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DepositsWithFiscalAgentsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromCitiesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromComponentUnitModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromCountiesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromEmployeesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromEnterpriseFundsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromFederalGovernmentModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromFiduciaryFundsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromLibrariesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromOtherFundsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromRoadCommissionsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromSchoolsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromStateGovernmentModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromTownshipsExceptRoadAgreementsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromTownshipsRoadAgreementsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueFromVillagesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:ForfeitureCertificateRecordingFeesReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:GrantsAndContractsReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:GrantsAndContractsReceivableNetOfAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:IncomeTaxReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:InterGovernmentalReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:InterGovernmentalReceivableNetOfAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:InterestAndPenaltiesReceivableOnTaxesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:InventoryModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:InventoryEquipmentMaterialsAndPartsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:InventoryRoadMaterialsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:InvestmentsWithFiscalAgentsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:InvestmentsWithStateTreasuryModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LandContractsPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LandContractsReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LandContractsReceivablesAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LandContractsReceivablesNetOfAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LeaseAssetsRightOfUseModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LeasesReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LeasesReceivableNetOfAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LoansAndNotesReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LoansAndNotesReceivableNetOfAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LoansReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LoansReceivableAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LoansReceivableNetOfAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LocalUnitShareOfAssessmentImprovementCostsReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:NotesReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:NotesReceivableAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:NotesReceivableNetOfAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:OtherAccountsReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:OtherReceivablesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:OtherRestrictedAssetsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:OtherTaxesReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:PaymentsInLieuOfTaxesReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:PenaltiesReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:PenaltiesReceivableNetOfAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:PooledCashAndInvestmentsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:PrepaidDepositsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:PrepaidExpensesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:PropertyTaxesReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:PropertyTaxesReceivableNetOfAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:ReceivablesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:RestrictedAssetsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:RestrictedCashModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:RestrictedCashAndCashEquivalentsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:RestrictedCashAndInvestmentsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:SalesTaxReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:SecuritiesLendingCollateralAssetsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:SecuritiesLendingObligationsLiabilityModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:ServiceFeesReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:SpecialAssessmentTaxesReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:SpecialAssessmentTaxesReceivableUnavailableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:SpecialAssessmentsReceivableDelinquentModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:TaxesReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:TaxesReceivableDelinquentPersonalPropertyModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:TaxesReceivableDelinquentRealPropertyModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:TaxesReceivablePersonalPropertyCurrentLevyModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:TaxesReceivableRealPropertyCurrentLevyModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:TuitionAndFeesAllowancesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:TuitionAndFeesReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:TuitionAndFeesReceivableNetOfAllowanceModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AccountsPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AccruedExpensesPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AccruedInterestPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AccruedLiabilitiesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AccruedTuitionAndFeesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AccruedVacationPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AccruedWagesAndRelatedLiabilitiesPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AccruedWagesPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AdvancesFromFederalGovernmentNoncurrentModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AdvancesFromGrantorsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AdvancesFromOtherFundsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AdvancesFromOtherGovernmentsNoncurrentModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AdvancesFromStateNoncurrentModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AdvancesSpecialAssessmentDistrictsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AnnuitiesPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CashBondsPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CourtOrdersPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:CustomerDepositsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DepositsHeldforOthersModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DrainOrdersPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToCitiesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToCommunityCollegeModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToComponentUnitModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToCountiesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToCourtWardsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToEmployeesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToFederalGovernmentModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToFiduciaryFundsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToFiscalAgentModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToFormerEmployeesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToIntermediateSchoolDistrictsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToLibrariesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToOtherFundsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToOtherGovernmentsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToOthersModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToPrimaryGovernmentModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToRoadCommissionsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToSchoolsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToSpecialEducationModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToStateGovernmentModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToTaxpayersTaxOverpaymentsAndDuplicatePaymentsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToTownshipsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DueToVillagesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:GarnishmentsPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:GrantsPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:OtherAdvancesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:PatientsOrInmatesTrustMoneyPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:PayableFromRestrictedAssetsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:PayrollDeductionsPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:PenaltiesPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:PerformanceDepositsPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:ReceiptsRefundableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:RegulatoryLiabilityCurrentModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:RestitutionsPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:RetainagePayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:TaxesPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:UnclaimedMoneyModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:UndistributedReceiptsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:UndistributedTaxCollectionsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:UnearnedRevenueModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:VouchersPayableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DeferredInflowsOfResourcesPropertyTaxesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DeferredInflowsOfResourcesTaxesLeviedForASubsequentPeriodModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:OtherDeferredInflowsOfResourcesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:DeferredOutflowsOfResourcesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:OtherDeferredOutflowsOfResourcesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:ConstructionInProgressModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:InvestmentsInJointVenturesModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:InvestmentsOfSurplusFundsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LeasesAccumulatedAmortizationModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LongTermContractsReceivableModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:LongTermInvestmentsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:NetOPEBAssetModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:NetPensionAssetModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:OtherAssetsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:OtherInvestmentsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:UnamortizedDiscountsOnBondsSoldByLocalUnitModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AdvancesToComponentUnitModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AdvancesToOtherFundsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:AdvancesToOtherGovernmentsModifiedAccrual</t>
-  </si>
-  <si>
-    <t>acfr:NetPensionLiabilityModifiedAccrual</t>
   </si>
   <si>
     <t>with acfr: added from Taxonomy spreadsheet</t>
@@ -8308,10 +7762,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE09D81-CE0E-407C-B6C2-C3432BAC9950}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K2380"/>
+  <dimension ref="A1:I2380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -8324,12 +7778,10 @@
     <col min="6" max="6" width="70" customWidth="1"/>
     <col min="7" max="7" width="22.33203125" customWidth="1"/>
     <col min="8" max="8" width="67.6640625" style="116" customWidth="1"/>
-    <col min="9" max="9" width="67.5" customWidth="1"/>
-    <col min="10" max="10" width="70.33203125" customWidth="1"/>
-    <col min="11" max="11" width="36.83203125" customWidth="1"/>
+    <col min="9" max="9" width="36.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="1" t="s">
         <v>58</v>
       </c>
@@ -8340,13 +7792,13 @@
         <v>1073</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2280</v>
+        <v>2098</v>
       </c>
       <c r="E1" s="128" t="s">
         <v>1763</v>
       </c>
       <c r="F1" s="128" t="s">
-        <v>2278</v>
+        <v>2096</v>
       </c>
       <c r="G1" s="128" t="s">
         <v>2094</v>
@@ -8355,16 +7807,10 @@
         <v>2095</v>
       </c>
       <c r="I1" s="128" t="s">
-        <v>2119</v>
-      </c>
-      <c r="J1" s="128" t="s">
-        <v>2118</v>
-      </c>
-      <c r="K1" s="128" t="s">
-        <v>2279</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -8392,15 +7838,8 @@
         <f>IF(G2="Exists", D2, "")</f>
         <v>acfr:AccountsReceivableModifiedAccrual</v>
       </c>
-      <c r="I2" t="str" cm="1">
-        <f t="array" ref="I2:I184">_xlfn._xlws.FILTER(H:H, H:H&lt;&gt;"")</f>
-        <v>Keep cells in col D that are marked 'Exists'</v>
-      </c>
-      <c r="J2" t="s">
-        <v>1762</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -8429,14 +7868,8 @@
         <f t="shared" ref="H3:H66" si="2">IF(G3="Exists", D3, "")</f>
         <v/>
       </c>
-      <c r="I3" t="str">
-        <v>acfr:AccountsReceivableModifiedAccrual</v>
-      </c>
-      <c r="J3" t="s">
-        <v>2096</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -8465,14 +7898,8 @@
         <f t="shared" si="2"/>
         <v>acfr:AccountsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
-      <c r="I4" t="str">
-        <v>acfr:AccountsReceivableNetOfAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J4" t="s">
-        <v>2097</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -8501,14 +7928,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I5" t="str">
-        <v>acfr:AccruedInterestReceivableModifiedAccrual</v>
-      </c>
-      <c r="J5" t="s">
-        <v>2098</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -8537,14 +7958,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I6" t="str">
-        <v>acfr:AccruedInterestReceivableNetOfAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J6" t="s">
-        <v>2099</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -8573,14 +7988,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I7" t="str">
-        <v>acfr:AssetsHeldForSaleModifiedAccrual</v>
-      </c>
-      <c r="J7" t="s">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -8609,14 +8018,8 @@
         <f t="shared" si="2"/>
         <v>acfr:AccruedInterestReceivableModifiedAccrual</v>
       </c>
-      <c r="I8" t="str">
-        <v>acfr:CashModifiedAccrual</v>
-      </c>
-      <c r="J8" t="s">
-        <v>2101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -8645,14 +8048,8 @@
         <f t="shared" si="2"/>
         <v>acfr:AccruedInterestReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
-      <c r="I9" t="str">
-        <v>acfr:CashAndCashEquivalentsModifiedAccrual</v>
-      </c>
-      <c r="J9" t="s">
-        <v>2102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -8681,14 +8078,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I10" t="str">
-        <v>acfr:CashAndCashEquivalentsAndInvestmentsModifiedAccrual</v>
-      </c>
-      <c r="J10" t="s">
-        <v>2103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -8717,14 +8108,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I11" t="str">
-        <v>acfr:CashAndCashEquivalentsWithFiscalAndEscrowAndOtherAgentsModifiedAccrual</v>
-      </c>
-      <c r="J11" t="s">
-        <v>2104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -8753,14 +8138,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I12" t="str">
-        <v>acfr:CashAndCashEquivalentsWithTreasurerModifiedAccrual</v>
-      </c>
-      <c r="J12" t="s">
-        <v>2105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -8789,14 +8168,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I13" t="str">
-        <v>acfr:CashAndCashEquivalentsWithTrusteeModifiedAccrual</v>
-      </c>
-      <c r="J13" t="s">
-        <v>2106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -8825,14 +8198,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I14" t="str">
-        <v>acfr:CashCheckingModifiedAccrual</v>
-      </c>
-      <c r="J14" t="s">
-        <v>2107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -8861,14 +8228,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I15" t="str">
-        <v>acfr:CashOnHandModifiedAccrual</v>
-      </c>
-      <c r="J15" t="s">
-        <v>2108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -8897,14 +8258,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I16" t="str">
-        <v>acfr:CashPayrollBankAccountModifiedAccrual</v>
-      </c>
-      <c r="J16" t="s">
-        <v>2109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -8933,14 +8288,8 @@
         <f t="shared" si="2"/>
         <v>acfr:AssetsHeldForSaleModifiedAccrual</v>
       </c>
-      <c r="I17" t="str">
-        <v>acfr:CashSavingsModifiedAccrual</v>
-      </c>
-      <c r="J17" t="s">
-        <v>2110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -8969,14 +8318,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I18" t="str">
-        <v>acfr:CertificatesOfDepositModifiedAccrual</v>
-      </c>
-      <c r="J18" t="s">
-        <v>2111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -9005,14 +8348,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I19" t="str">
-        <v>acfr:ClaimsAndJudgmentsReceivableModifiedAccrual</v>
-      </c>
-      <c r="J19" t="s">
-        <v>2112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -9041,14 +8378,8 @@
         <f t="shared" si="2"/>
         <v>acfr:CashModifiedAccrual</v>
       </c>
-      <c r="I20" t="str">
-        <v>acfr:ClaimsAndJudgmentsReceivableNetOfAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J20" t="s">
-        <v>2113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -9077,14 +8408,8 @@
         <f t="shared" si="2"/>
         <v>acfr:CashAndCashEquivalentsModifiedAccrual</v>
       </c>
-      <c r="I21" t="str">
-        <v>acfr:ContractsPayableDueWithinOneYearModifiedAccrual</v>
-      </c>
-      <c r="J21" t="s">
-        <v>2114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -9113,14 +8438,8 @@
         <f t="shared" si="2"/>
         <v>acfr:CashAndCashEquivalentsAndInvestmentsModifiedAccrual</v>
       </c>
-      <c r="I22" t="str">
-        <v>acfr:CourtOrdersReceivableModifiedAccrual</v>
-      </c>
-      <c r="J22" t="s">
-        <v>2115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -9149,14 +8468,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I23" t="str">
-        <v>acfr:DelinquentTaxesReceivableModifiedAccrual</v>
-      </c>
-      <c r="J23" t="s">
-        <v>2116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -9185,14 +8498,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I24" t="str">
-        <v>acfr:DelinquentUtilityBillsReceivableModifiedAccrual</v>
-      </c>
-      <c r="J24" t="s">
-        <v>2117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -9221,14 +8528,8 @@
         <f t="shared" si="2"/>
         <v>acfr:CashAndCashEquivalentsWithFiscalAndEscrowAndOtherAgentsModifiedAccrual</v>
       </c>
-      <c r="I25" t="str">
-        <v>acfr:DepositsReceivableModifiedAccrual</v>
-      </c>
-      <c r="J25" t="s">
-        <v>2120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -9257,14 +8558,8 @@
         <f t="shared" si="2"/>
         <v>acfr:CashAndCashEquivalentsWithTreasurerModifiedAccrual</v>
       </c>
-      <c r="I26" t="str">
-        <v>acfr:DepositsReceivableNetOfAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J26" t="s">
-        <v>2121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -9293,14 +8588,8 @@
         <f t="shared" si="2"/>
         <v>acfr:CashAndCashEquivalentsWithTrusteeModifiedAccrual</v>
       </c>
-      <c r="I27" t="str">
-        <v>acfr:DepositsWithFiscalAgentsModifiedAccrual</v>
-      </c>
-      <c r="J27" t="s">
-        <v>2122</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -9329,14 +8618,8 @@
         <f t="shared" si="2"/>
         <v>acfr:CashCheckingModifiedAccrual</v>
       </c>
-      <c r="I28" t="str">
-        <v>acfr:DueFromCitiesModifiedAccrual</v>
-      </c>
-      <c r="J28" t="s">
-        <v>2123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -9365,14 +8648,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I29" t="str">
-        <v>acfr:DueFromComponentUnitModifiedAccrual</v>
-      </c>
-      <c r="J29" t="s">
-        <v>2124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -9401,14 +8678,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I30" t="str">
-        <v>acfr:DueFromCountiesModifiedAccrual</v>
-      </c>
-      <c r="J30" t="s">
-        <v>2125</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -9437,14 +8708,8 @@
         <f t="shared" si="2"/>
         <v>acfr:CashOnHandModifiedAccrual</v>
       </c>
-      <c r="I31" t="str">
-        <v>acfr:DueFromEmployeesModifiedAccrual</v>
-      </c>
-      <c r="J31" t="s">
-        <v>2126</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -9473,14 +8738,8 @@
         <f t="shared" si="2"/>
         <v>acfr:CashPayrollBankAccountModifiedAccrual</v>
       </c>
-      <c r="I32" t="str">
-        <v>acfr:DueFromEnterpriseFundsModifiedAccrual</v>
-      </c>
-      <c r="J32" t="s">
-        <v>2127</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -9509,14 +8768,8 @@
         <f t="shared" si="2"/>
         <v>acfr:CashSavingsModifiedAccrual</v>
       </c>
-      <c r="I33" t="str">
-        <v>acfr:DueFromFederalGovernmentModifiedAccrual</v>
-      </c>
-      <c r="J33" t="s">
-        <v>2128</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -9545,14 +8798,8 @@
         <f t="shared" si="2"/>
         <v>acfr:CertificatesOfDepositModifiedAccrual</v>
       </c>
-      <c r="I34" t="str">
-        <v>acfr:DueFromFiduciaryFundsModifiedAccrual</v>
-      </c>
-      <c r="J34" t="s">
-        <v>2129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -9581,14 +8828,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I35" t="str">
-        <v>acfr:DueFromLibrariesModifiedAccrual</v>
-      </c>
-      <c r="J35" t="s">
-        <v>2130</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -9617,14 +8858,8 @@
         <f t="shared" si="2"/>
         <v>acfr:ClaimsAndJudgmentsReceivableModifiedAccrual</v>
       </c>
-      <c r="I36" t="str">
-        <v>acfr:DueFromOtherFundsModifiedAccrual</v>
-      </c>
-      <c r="J36" t="s">
-        <v>2131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -9653,14 +8888,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I37" t="str">
-        <v>acfr:DueFromRoadCommissionsModifiedAccrual</v>
-      </c>
-      <c r="J37" t="s">
-        <v>2132</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>60</v>
       </c>
@@ -9689,14 +8918,8 @@
         <f t="shared" si="2"/>
         <v>acfr:ClaimsAndJudgmentsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
-      <c r="I38" t="str">
-        <v>acfr:DueFromSchoolsModifiedAccrual</v>
-      </c>
-      <c r="J38" t="s">
-        <v>2133</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -9725,14 +8948,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I39" t="str">
-        <v>acfr:DueFromStateGovernmentModifiedAccrual</v>
-      </c>
-      <c r="J39" t="s">
-        <v>2134</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>60</v>
       </c>
@@ -9761,14 +8978,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I40" t="str">
-        <v>acfr:DueFromTownshipsExceptRoadAgreementsModifiedAccrual</v>
-      </c>
-      <c r="J40" t="s">
-        <v>2135</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>60</v>
       </c>
@@ -9797,14 +9008,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I41" t="str">
-        <v>acfr:DueFromTownshipsRoadAgreementsModifiedAccrual</v>
-      </c>
-      <c r="J41" t="s">
-        <v>2136</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>60</v>
       </c>
@@ -9833,14 +9038,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I42" t="str">
-        <v>acfr:DueFromVillagesModifiedAccrual</v>
-      </c>
-      <c r="J42" t="s">
-        <v>2137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -9869,14 +9068,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I43" t="str">
-        <v>acfr:ForfeitureCertificateRecordingFeesReceivableModifiedAccrual</v>
-      </c>
-      <c r="J43" t="s">
-        <v>2138</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -9905,14 +9098,8 @@
         <f t="shared" si="2"/>
         <v>acfr:ContractsPayableDueWithinOneYearModifiedAccrual</v>
       </c>
-      <c r="I44" t="str">
-        <v>acfr:GrantsAndContractsReceivableModifiedAccrual</v>
-      </c>
-      <c r="J44" t="s">
-        <v>2139</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -9941,14 +9128,8 @@
         <f t="shared" si="2"/>
         <v>acfr:CourtOrdersReceivableModifiedAccrual</v>
       </c>
-      <c r="I45" t="str">
-        <v>acfr:GrantsAndContractsReceivableNetOfAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J45" t="s">
-        <v>2140</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -9977,14 +9158,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I46" t="str">
-        <v>acfr:IncomeTaxReceivableModifiedAccrual</v>
-      </c>
-      <c r="J46" t="s">
-        <v>2141</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -10013,14 +9188,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I47" t="str">
-        <v>acfr:InterGovernmentalReceivableModifiedAccrual</v>
-      </c>
-      <c r="J47" t="s">
-        <v>2142</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -10049,14 +9218,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I48" t="str">
-        <v>acfr:InterGovernmentalReceivableNetOfAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J48" t="s">
-        <v>2143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -10085,14 +9248,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I49" t="str">
-        <v>acfr:InterestAndPenaltiesReceivableOnTaxesModifiedAccrual</v>
-      </c>
-      <c r="J49" t="s">
-        <v>2144</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -10121,14 +9278,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I50" t="str">
-        <v>acfr:InventoryModifiedAccrual</v>
-      </c>
-      <c r="J50" t="s">
-        <v>2145</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -10157,14 +9308,8 @@
         <f t="shared" si="2"/>
         <v>acfr:DelinquentTaxesReceivableModifiedAccrual</v>
       </c>
-      <c r="I51" t="str">
-        <v>acfr:InventoryEquipmentMaterialsAndPartsModifiedAccrual</v>
-      </c>
-      <c r="J51" t="s">
-        <v>2146</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -10193,14 +9338,8 @@
         <f t="shared" si="2"/>
         <v>acfr:DelinquentUtilityBillsReceivableModifiedAccrual</v>
       </c>
-      <c r="I52" t="str">
-        <v>acfr:InventoryRoadMaterialsModifiedAccrual</v>
-      </c>
-      <c r="J52" t="s">
-        <v>2147</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -10229,14 +9368,8 @@
         <f t="shared" si="2"/>
         <v>acfr:DepositsReceivableModifiedAccrual</v>
       </c>
-      <c r="I53" t="str">
-        <v>acfr:InvestmentsWithFiscalAgentsModifiedAccrual</v>
-      </c>
-      <c r="J53" t="s">
-        <v>2148</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -10265,14 +9398,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I54" t="str">
-        <v>acfr:InvestmentsWithStateTreasuryModifiedAccrual</v>
-      </c>
-      <c r="J54" t="s">
-        <v>2149</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -10301,14 +9428,8 @@
         <f t="shared" si="2"/>
         <v>acfr:DepositsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
-      <c r="I55" t="str">
-        <v>acfr:LandContractsPayableModifiedAccrual</v>
-      </c>
-      <c r="J55" t="s">
-        <v>2150</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -10337,14 +9458,8 @@
         <f t="shared" si="2"/>
         <v>acfr:DepositsWithFiscalAgentsModifiedAccrual</v>
       </c>
-      <c r="I56" t="str">
-        <v>acfr:LandContractsReceivableModifiedAccrual</v>
-      </c>
-      <c r="J56" t="s">
-        <v>2151</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -10373,14 +9488,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I57" t="str">
-        <v>acfr:LandContractsReceivablesAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J57" t="s">
-        <v>2152</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -10409,14 +9518,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I58" t="str">
-        <v>acfr:LandContractsReceivablesNetOfAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J58" t="s">
-        <v>2153</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -10445,14 +9548,8 @@
         <f t="shared" si="2"/>
         <v>acfr:DueFromCitiesModifiedAccrual</v>
       </c>
-      <c r="I59" t="str">
-        <v>acfr:LeaseAssetsRightOfUseModifiedAccrual</v>
-      </c>
-      <c r="J59" t="s">
-        <v>2154</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -10481,14 +9578,8 @@
         <f t="shared" si="2"/>
         <v>acfr:DueFromComponentUnitModifiedAccrual</v>
       </c>
-      <c r="I60" t="str">
-        <v>acfr:LeasesReceivableModifiedAccrual</v>
-      </c>
-      <c r="J60" t="s">
-        <v>2155</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -10517,14 +9608,8 @@
         <f t="shared" si="2"/>
         <v>acfr:DueFromCountiesModifiedAccrual</v>
       </c>
-      <c r="I61" t="str">
-        <v>acfr:LeasesReceivableNetOfAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J61" t="s">
-        <v>2156</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -10553,14 +9638,8 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I62" t="str">
-        <v>acfr:LoansAndNotesReceivableModifiedAccrual</v>
-      </c>
-      <c r="J62" t="s">
-        <v>2157</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -10589,14 +9668,8 @@
         <f t="shared" si="2"/>
         <v>acfr:DueFromEmployeesModifiedAccrual</v>
       </c>
-      <c r="I63" t="str">
-        <v>acfr:LoansAndNotesReceivableNetOfAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J63" t="s">
-        <v>2158</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>60</v>
       </c>
@@ -10625,14 +9698,8 @@
         <f t="shared" si="2"/>
         <v>acfr:DueFromEnterpriseFundsModifiedAccrual</v>
       </c>
-      <c r="I64" t="str">
-        <v>acfr:LoansReceivableModifiedAccrual</v>
-      </c>
-      <c r="J64" t="s">
-        <v>2159</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>60</v>
       </c>
@@ -10661,14 +9728,8 @@
         <f t="shared" si="2"/>
         <v>acfr:DueFromFederalGovernmentModifiedAccrual</v>
       </c>
-      <c r="I65" t="str">
-        <v>acfr:LoansReceivableAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J65" t="s">
-        <v>2160</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>60</v>
       </c>
@@ -10697,14 +9758,8 @@
         <f t="shared" si="2"/>
         <v>acfr:DueFromFiduciaryFundsModifiedAccrual</v>
       </c>
-      <c r="I66" t="str">
-        <v>acfr:LoansReceivableNetOfAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J66" t="s">
-        <v>2161</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>60</v>
       </c>
@@ -10733,14 +9788,8 @@
         <f t="shared" ref="H67:H130" si="6">IF(G67="Exists", D67, "")</f>
         <v/>
       </c>
-      <c r="I67" t="str">
-        <v>acfr:LocalUnitShareOfAssessmentImprovementCostsReceivableModifiedAccrual</v>
-      </c>
-      <c r="J67" t="s">
-        <v>2162</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>60</v>
       </c>
@@ -10769,14 +9818,8 @@
         <f t="shared" si="6"/>
         <v>acfr:DueFromLibrariesModifiedAccrual</v>
       </c>
-      <c r="I68" t="str">
-        <v>acfr:NotesReceivableModifiedAccrual</v>
-      </c>
-      <c r="J68" t="s">
-        <v>2163</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>60</v>
       </c>
@@ -10805,14 +9848,8 @@
         <f t="shared" si="6"/>
         <v>acfr:DueFromOtherFundsModifiedAccrual</v>
       </c>
-      <c r="I69" t="str">
-        <v>acfr:NotesReceivableAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J69" t="s">
-        <v>2164</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>60</v>
       </c>
@@ -10841,14 +9878,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I70" t="str">
-        <v>acfr:NotesReceivableNetOfAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J70" t="s">
-        <v>2165</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>60</v>
       </c>
@@ -10877,14 +9908,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I71" t="str">
-        <v>acfr:OtherAccountsReceivableModifiedAccrual</v>
-      </c>
-      <c r="J71" t="s">
-        <v>2166</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10">
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>60</v>
       </c>
@@ -10913,14 +9938,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I72" t="str">
-        <v>acfr:OtherReceivablesModifiedAccrual</v>
-      </c>
-      <c r="J72" t="s">
-        <v>2167</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10">
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>60</v>
       </c>
@@ -10949,14 +9968,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I73" t="str">
-        <v>acfr:OtherRestrictedAssetsModifiedAccrual</v>
-      </c>
-      <c r="J73" t="s">
-        <v>2168</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>60</v>
       </c>
@@ -10985,14 +9998,8 @@
         <f t="shared" si="6"/>
         <v>acfr:DueFromRoadCommissionsModifiedAccrual</v>
       </c>
-      <c r="I74" t="str">
-        <v>acfr:OtherTaxesReceivableModifiedAccrual</v>
-      </c>
-      <c r="J74" t="s">
-        <v>2169</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>60</v>
       </c>
@@ -11021,14 +10028,8 @@
         <f t="shared" si="6"/>
         <v>acfr:DueFromSchoolsModifiedAccrual</v>
       </c>
-      <c r="I75" t="str">
-        <v>acfr:PaymentsInLieuOfTaxesReceivableModifiedAccrual</v>
-      </c>
-      <c r="J75" t="s">
-        <v>2170</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>60</v>
       </c>
@@ -11057,14 +10058,8 @@
         <f t="shared" si="6"/>
         <v>acfr:DueFromStateGovernmentModifiedAccrual</v>
       </c>
-      <c r="I76" t="str">
-        <v>acfr:PenaltiesReceivableModifiedAccrual</v>
-      </c>
-      <c r="J76" t="s">
-        <v>2171</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10">
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>60</v>
       </c>
@@ -11093,14 +10088,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I77" t="str">
-        <v>acfr:PenaltiesReceivableNetOfAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J77" t="s">
-        <v>2172</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>60</v>
       </c>
@@ -11129,14 +10118,8 @@
         <f t="shared" si="6"/>
         <v>acfr:DueFromTownshipsExceptRoadAgreementsModifiedAccrual</v>
       </c>
-      <c r="I78" t="str">
-        <v>acfr:PooledCashAndInvestmentsModifiedAccrual</v>
-      </c>
-      <c r="J78" t="s">
-        <v>2173</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10">
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>60</v>
       </c>
@@ -11165,14 +10148,8 @@
         <f t="shared" si="6"/>
         <v>acfr:DueFromTownshipsRoadAgreementsModifiedAccrual</v>
       </c>
-      <c r="I79" t="str">
-        <v>acfr:PrepaidDepositsModifiedAccrual</v>
-      </c>
-      <c r="J79" t="s">
-        <v>2174</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>60</v>
       </c>
@@ -11201,14 +10178,8 @@
         <f t="shared" si="6"/>
         <v>acfr:DueFromVillagesModifiedAccrual</v>
       </c>
-      <c r="I80" t="str">
-        <v>acfr:PrepaidExpensesModifiedAccrual</v>
-      </c>
-      <c r="J80" t="s">
-        <v>2175</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10">
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>60</v>
       </c>
@@ -11237,14 +10208,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I81" t="str">
-        <v>acfr:PropertyTaxesReceivableModifiedAccrual</v>
-      </c>
-      <c r="J81" t="s">
-        <v>2176</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10">
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>60</v>
       </c>
@@ -11273,14 +10238,8 @@
         <f t="shared" si="6"/>
         <v>acfr:ForfeitureCertificateRecordingFeesReceivableModifiedAccrual</v>
       </c>
-      <c r="I82" t="str">
-        <v>acfr:PropertyTaxesReceivableNetOfAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J82" t="s">
-        <v>2177</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10">
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>60</v>
       </c>
@@ -11309,14 +10268,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I83" t="str">
-        <v>acfr:ReceivablesModifiedAccrual</v>
-      </c>
-      <c r="J83" t="s">
-        <v>2178</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10">
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>60</v>
       </c>
@@ -11345,14 +10298,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I84" t="str">
-        <v>acfr:RestrictedAssetsModifiedAccrual</v>
-      </c>
-      <c r="J84" t="s">
-        <v>2179</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>60</v>
       </c>
@@ -11381,14 +10328,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I85" t="str">
-        <v>acfr:RestrictedCashModifiedAccrual</v>
-      </c>
-      <c r="J85" t="s">
-        <v>2180</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10">
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>60</v>
       </c>
@@ -11417,14 +10358,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I86" t="str">
-        <v>acfr:RestrictedCashAndCashEquivalentsModifiedAccrual</v>
-      </c>
-      <c r="J86" t="s">
-        <v>2181</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10">
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>60</v>
       </c>
@@ -11453,14 +10388,8 @@
         <f t="shared" si="6"/>
         <v>acfr:GrantsAndContractsReceivableModifiedAccrual</v>
       </c>
-      <c r="I87" t="str">
-        <v>acfr:RestrictedCashAndInvestmentsModifiedAccrual</v>
-      </c>
-      <c r="J87" t="s">
-        <v>2182</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10">
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>60</v>
       </c>
@@ -11489,14 +10418,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I88" t="str">
-        <v>acfr:SalesTaxReceivableModifiedAccrual</v>
-      </c>
-      <c r="J88" t="s">
-        <v>2183</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10">
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>60</v>
       </c>
@@ -11525,14 +10448,8 @@
         <f t="shared" si="6"/>
         <v>acfr:GrantsAndContractsReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
-      <c r="I89" t="str">
-        <v>acfr:SecuritiesLendingCollateralAssetsModifiedAccrual</v>
-      </c>
-      <c r="J89" t="s">
-        <v>2184</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10">
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90" t="s">
         <v>60</v>
       </c>
@@ -11561,14 +10478,8 @@
         <f t="shared" si="6"/>
         <v>acfr:IncomeTaxReceivableModifiedAccrual</v>
       </c>
-      <c r="I90" t="str">
-        <v>acfr:SecuritiesLendingObligationsLiabilityModifiedAccrual</v>
-      </c>
-      <c r="J90" t="s">
-        <v>2185</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10">
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
         <v>60</v>
       </c>
@@ -11597,14 +10508,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I91" t="str">
-        <v>acfr:ServiceFeesReceivableModifiedAccrual</v>
-      </c>
-      <c r="J91" t="s">
-        <v>2186</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10">
+    </row>
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
         <v>60</v>
       </c>
@@ -11633,14 +10538,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I92" t="str">
-        <v>acfr:SpecialAssessmentTaxesReceivableModifiedAccrual</v>
-      </c>
-      <c r="J92" t="s">
-        <v>2187</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10">
+    </row>
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
         <v>60</v>
       </c>
@@ -11669,14 +10568,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I93" t="str">
-        <v>acfr:SpecialAssessmentTaxesReceivableUnavailableModifiedAccrual</v>
-      </c>
-      <c r="J93" t="s">
-        <v>2188</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10">
+    </row>
+    <row r="94" spans="1:8">
       <c r="A94" t="s">
         <v>60</v>
       </c>
@@ -11705,14 +10598,8 @@
         <f t="shared" si="6"/>
         <v>acfr:InterGovernmentalReceivableModifiedAccrual</v>
       </c>
-      <c r="I94" t="str">
-        <v>acfr:SpecialAssessmentsReceivableDelinquentModifiedAccrual</v>
-      </c>
-      <c r="J94" t="s">
-        <v>2189</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10">
+    </row>
+    <row r="95" spans="1:8">
       <c r="A95" t="s">
         <v>60</v>
       </c>
@@ -11741,14 +10628,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I95" t="str">
-        <v>acfr:TaxesReceivableModifiedAccrual</v>
-      </c>
-      <c r="J95" t="s">
-        <v>2190</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10">
+    </row>
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
         <v>60</v>
       </c>
@@ -11777,14 +10658,8 @@
         <f t="shared" si="6"/>
         <v>acfr:InterGovernmentalReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
-      <c r="I96" t="str">
-        <v>acfr:TaxesReceivableDelinquentPersonalPropertyModifiedAccrual</v>
-      </c>
-      <c r="J96" t="s">
-        <v>2191</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10">
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
         <v>60</v>
       </c>
@@ -11813,14 +10688,8 @@
         <f t="shared" si="6"/>
         <v>acfr:InterestAndPenaltiesReceivableOnTaxesModifiedAccrual</v>
       </c>
-      <c r="I97" t="str">
-        <v>acfr:TaxesReceivableDelinquentRealPropertyModifiedAccrual</v>
-      </c>
-      <c r="J97" t="s">
-        <v>2192</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10">
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
         <v>60</v>
       </c>
@@ -11849,14 +10718,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I98" t="str">
-        <v>acfr:TaxesReceivablePersonalPropertyCurrentLevyModifiedAccrual</v>
-      </c>
-      <c r="J98" t="s">
-        <v>2193</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10">
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
         <v>60</v>
       </c>
@@ -11885,14 +10748,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I99" t="str">
-        <v>acfr:TaxesReceivableRealPropertyCurrentLevyModifiedAccrual</v>
-      </c>
-      <c r="J99" t="s">
-        <v>2194</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10">
+    </row>
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
         <v>60</v>
       </c>
@@ -11921,14 +10778,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I100" t="str">
-        <v>acfr:TuitionAndFeesAllowancesModifiedAccrual</v>
-      </c>
-      <c r="J100" t="s">
-        <v>2195</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10">
+    </row>
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
         <v>60</v>
       </c>
@@ -11957,14 +10808,8 @@
         <f t="shared" si="6"/>
         <v>acfr:InventoryModifiedAccrual</v>
       </c>
-      <c r="I101" t="str">
-        <v>acfr:TuitionAndFeesReceivableModifiedAccrual</v>
-      </c>
-      <c r="J101" t="s">
-        <v>2196</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10">
+    </row>
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
         <v>60</v>
       </c>
@@ -11993,14 +10838,8 @@
         <f t="shared" si="6"/>
         <v>acfr:InventoryEquipmentMaterialsAndPartsModifiedAccrual</v>
       </c>
-      <c r="I102" t="str">
-        <v>acfr:TuitionAndFeesReceivableNetOfAllowanceModifiedAccrual</v>
-      </c>
-      <c r="J102" t="s">
-        <v>2197</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10">
+    </row>
+    <row r="103" spans="1:8">
       <c r="A103" t="s">
         <v>60</v>
       </c>
@@ -12029,14 +10868,8 @@
         <f t="shared" si="6"/>
         <v>acfr:InventoryRoadMaterialsModifiedAccrual</v>
       </c>
-      <c r="I103" t="str">
-        <v>acfr:AccountsPayableModifiedAccrual</v>
-      </c>
-      <c r="J103" t="s">
-        <v>2198</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10">
+    </row>
+    <row r="104" spans="1:8">
       <c r="A104" t="s">
         <v>60</v>
       </c>
@@ -12065,14 +10898,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I104" t="str">
-        <v>acfr:AccruedExpensesPayableModifiedAccrual</v>
-      </c>
-      <c r="J104" t="s">
-        <v>2199</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10">
+    </row>
+    <row r="105" spans="1:8">
       <c r="A105" t="s">
         <v>60</v>
       </c>
@@ -12101,14 +10928,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I105" t="str">
-        <v>acfr:AccruedInterestPayableModifiedAccrual</v>
-      </c>
-      <c r="J105" t="s">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10">
+    </row>
+    <row r="106" spans="1:8">
       <c r="A106" t="s">
         <v>60</v>
       </c>
@@ -12137,14 +10958,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I106" t="str">
-        <v>acfr:AccruedLiabilitiesModifiedAccrual</v>
-      </c>
-      <c r="J106" t="s">
-        <v>2201</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10">
+    </row>
+    <row r="107" spans="1:8">
       <c r="A107" t="s">
         <v>60</v>
       </c>
@@ -12173,14 +10988,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I107" t="str">
-        <v>acfr:AccruedTuitionAndFeesModifiedAccrual</v>
-      </c>
-      <c r="J107" t="s">
-        <v>2202</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10">
+    </row>
+    <row r="108" spans="1:8">
       <c r="A108" t="s">
         <v>60</v>
       </c>
@@ -12209,14 +11018,8 @@
         <f t="shared" si="6"/>
         <v>acfr:InvestmentsWithFiscalAgentsModifiedAccrual</v>
       </c>
-      <c r="I108" t="str">
-        <v>acfr:AccruedVacationPayableModifiedAccrual</v>
-      </c>
-      <c r="J108" t="s">
-        <v>2203</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10">
+    </row>
+    <row r="109" spans="1:8">
       <c r="A109" t="s">
         <v>60</v>
       </c>
@@ -12245,14 +11048,8 @@
         <f t="shared" si="6"/>
         <v>acfr:InvestmentsWithStateTreasuryModifiedAccrual</v>
       </c>
-      <c r="I109" t="str">
-        <v>acfr:AccruedWagesAndRelatedLiabilitiesPayableModifiedAccrual</v>
-      </c>
-      <c r="J109" t="s">
-        <v>2204</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10">
+    </row>
+    <row r="110" spans="1:8">
       <c r="A110" t="s">
         <v>60</v>
       </c>
@@ -12281,14 +11078,8 @@
         <f t="shared" si="6"/>
         <v>acfr:LandContractsPayableModifiedAccrual</v>
       </c>
-      <c r="I110" t="str">
-        <v>acfr:AccruedWagesPayableModifiedAccrual</v>
-      </c>
-      <c r="J110" t="s">
-        <v>2205</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10">
+    </row>
+    <row r="111" spans="1:8">
       <c r="A111" t="s">
         <v>60</v>
       </c>
@@ -12317,14 +11108,8 @@
         <f t="shared" si="6"/>
         <v>acfr:LandContractsReceivableModifiedAccrual</v>
       </c>
-      <c r="I111" t="str">
-        <v>acfr:AdvancesFromFederalGovernmentNoncurrentModifiedAccrual</v>
-      </c>
-      <c r="J111" t="s">
-        <v>2206</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10">
+    </row>
+    <row r="112" spans="1:8">
       <c r="A112" t="s">
         <v>60</v>
       </c>
@@ -12353,14 +11138,8 @@
         <f t="shared" si="6"/>
         <v>acfr:LandContractsReceivablesAllowanceModifiedAccrual</v>
       </c>
-      <c r="I112" t="str">
-        <v>acfr:AdvancesFromGrantorsModifiedAccrual</v>
-      </c>
-      <c r="J112" t="s">
-        <v>2207</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10">
+    </row>
+    <row r="113" spans="1:8">
       <c r="A113" t="s">
         <v>60</v>
       </c>
@@ -12389,14 +11168,8 @@
         <f t="shared" si="6"/>
         <v>acfr:LandContractsReceivablesNetOfAllowanceModifiedAccrual</v>
       </c>
-      <c r="I113" t="str">
-        <v>acfr:AdvancesFromOtherFundsModifiedAccrual</v>
-      </c>
-      <c r="J113" t="s">
-        <v>2208</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10">
+    </row>
+    <row r="114" spans="1:8">
       <c r="A114" t="s">
         <v>60</v>
       </c>
@@ -12425,14 +11198,8 @@
         <f t="shared" si="6"/>
         <v>acfr:LeaseAssetsRightOfUseModifiedAccrual</v>
       </c>
-      <c r="I114" t="str">
-        <v>acfr:AdvancesFromOtherGovernmentsNoncurrentModifiedAccrual</v>
-      </c>
-      <c r="J114" t="s">
-        <v>2209</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10">
+    </row>
+    <row r="115" spans="1:8">
       <c r="A115" t="s">
         <v>60</v>
       </c>
@@ -12461,14 +11228,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I115" t="str">
-        <v>acfr:AdvancesFromStateNoncurrentModifiedAccrual</v>
-      </c>
-      <c r="J115" t="s">
-        <v>2210</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10">
+    </row>
+    <row r="116" spans="1:8">
       <c r="A116" t="s">
         <v>60</v>
       </c>
@@ -12497,14 +11258,8 @@
         <f t="shared" si="6"/>
         <v>acfr:LeasesReceivableModifiedAccrual</v>
       </c>
-      <c r="I116" t="str">
-        <v>acfr:AdvancesSpecialAssessmentDistrictsModifiedAccrual</v>
-      </c>
-      <c r="J116" t="s">
-        <v>2211</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10">
+    </row>
+    <row r="117" spans="1:8">
       <c r="A117" t="s">
         <v>60</v>
       </c>
@@ -12533,14 +11288,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I117" t="str">
-        <v>acfr:AnnuitiesPayableModifiedAccrual</v>
-      </c>
-      <c r="J117" t="s">
-        <v>2212</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10">
+    </row>
+    <row r="118" spans="1:8">
       <c r="A118" t="s">
         <v>60</v>
       </c>
@@ -12569,14 +11318,8 @@
         <f t="shared" si="6"/>
         <v>acfr:LeasesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
-      <c r="I118" t="str">
-        <v>acfr:CashBondsPayableModifiedAccrual</v>
-      </c>
-      <c r="J118" t="s">
-        <v>2213</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10">
+    </row>
+    <row r="119" spans="1:8">
       <c r="A119" t="s">
         <v>60</v>
       </c>
@@ -12605,14 +11348,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I119" t="str">
-        <v>acfr:CourtOrdersPayableModifiedAccrual</v>
-      </c>
-      <c r="J119" t="s">
-        <v>2214</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10">
+    </row>
+    <row r="120" spans="1:8">
       <c r="A120" t="s">
         <v>60</v>
       </c>
@@ -12641,14 +11378,8 @@
         <f t="shared" si="6"/>
         <v>acfr:LoansAndNotesReceivableModifiedAccrual</v>
       </c>
-      <c r="I120" t="str">
-        <v>acfr:CustomerDepositsModifiedAccrual</v>
-      </c>
-      <c r="J120" t="s">
-        <v>2215</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10">
+    </row>
+    <row r="121" spans="1:8">
       <c r="A121" t="s">
         <v>60</v>
       </c>
@@ -12677,14 +11408,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I121" t="str">
-        <v>acfr:DepositsHeldforOthersModifiedAccrual</v>
-      </c>
-      <c r="J121" t="s">
-        <v>2216</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10">
+    </row>
+    <row r="122" spans="1:8">
       <c r="A122" t="s">
         <v>60</v>
       </c>
@@ -12713,14 +11438,8 @@
         <f t="shared" si="6"/>
         <v>acfr:LoansAndNotesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
-      <c r="I122" t="str">
-        <v>acfr:DrainOrdersPayableModifiedAccrual</v>
-      </c>
-      <c r="J122" t="s">
-        <v>2217</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10">
+    </row>
+    <row r="123" spans="1:8">
       <c r="A123" t="s">
         <v>60</v>
       </c>
@@ -12749,14 +11468,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I123" t="str">
-        <v>acfr:DueToCitiesModifiedAccrual</v>
-      </c>
-      <c r="J123" t="s">
-        <v>2218</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10">
+    </row>
+    <row r="124" spans="1:8">
       <c r="A124" t="s">
         <v>60</v>
       </c>
@@ -12785,14 +11498,8 @@
         <f t="shared" si="6"/>
         <v>acfr:LoansReceivableModifiedAccrual</v>
       </c>
-      <c r="I124" t="str">
-        <v>acfr:DueToCommunityCollegeModifiedAccrual</v>
-      </c>
-      <c r="J124" t="s">
-        <v>2219</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10">
+    </row>
+    <row r="125" spans="1:8">
       <c r="A125" t="s">
         <v>60</v>
       </c>
@@ -12821,14 +11528,8 @@
         <f t="shared" si="6"/>
         <v>acfr:LoansReceivableAllowanceModifiedAccrual</v>
       </c>
-      <c r="I125" t="str">
-        <v>acfr:DueToComponentUnitModifiedAccrual</v>
-      </c>
-      <c r="J125" t="s">
-        <v>2220</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10">
+    </row>
+    <row r="126" spans="1:8">
       <c r="A126" t="s">
         <v>60</v>
       </c>
@@ -12857,14 +11558,8 @@
         <f t="shared" si="6"/>
         <v>acfr:LoansReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
-      <c r="I126" t="str">
-        <v>acfr:DueToCountiesModifiedAccrual</v>
-      </c>
-      <c r="J126" t="s">
-        <v>2221</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10">
+    </row>
+    <row r="127" spans="1:8">
       <c r="A127" t="s">
         <v>60</v>
       </c>
@@ -12893,14 +11588,8 @@
         <f t="shared" si="6"/>
         <v>acfr:LocalUnitShareOfAssessmentImprovementCostsReceivableModifiedAccrual</v>
       </c>
-      <c r="I127" t="str">
-        <v>acfr:DueToCourtWardsModifiedAccrual</v>
-      </c>
-      <c r="J127" t="s">
-        <v>2222</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10">
+    </row>
+    <row r="128" spans="1:8">
       <c r="A128" t="s">
         <v>60</v>
       </c>
@@ -12929,14 +11618,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I128" t="str">
-        <v>acfr:DueToEmployeesModifiedAccrual</v>
-      </c>
-      <c r="J128" t="s">
-        <v>2223</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10">
+    </row>
+    <row r="129" spans="1:8">
       <c r="A129" t="s">
         <v>60</v>
       </c>
@@ -12965,14 +11648,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I129" t="str">
-        <v>acfr:DueToFederalGovernmentModifiedAccrual</v>
-      </c>
-      <c r="J129" t="s">
-        <v>2224</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10">
+    </row>
+    <row r="130" spans="1:8">
       <c r="A130" t="s">
         <v>60</v>
       </c>
@@ -13001,14 +11678,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I130" t="str">
-        <v>acfr:DueToFiduciaryFundsModifiedAccrual</v>
-      </c>
-      <c r="J130" t="s">
-        <v>2225</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10">
+    </row>
+    <row r="131" spans="1:8">
       <c r="A131" t="s">
         <v>60</v>
       </c>
@@ -13037,14 +11708,8 @@
         <f t="shared" ref="H131:H194" si="10">IF(G131="Exists", D131, "")</f>
         <v>acfr:NotesReceivableModifiedAccrual</v>
       </c>
-      <c r="I131" t="str">
-        <v>acfr:DueToFiscalAgentModifiedAccrual</v>
-      </c>
-      <c r="J131" t="s">
-        <v>2226</v>
-      </c>
-    </row>
-    <row r="132" spans="1:10">
+    </row>
+    <row r="132" spans="1:8">
       <c r="A132" t="s">
         <v>60</v>
       </c>
@@ -13073,14 +11738,8 @@
         <f t="shared" si="10"/>
         <v>acfr:NotesReceivableAllowanceModifiedAccrual</v>
       </c>
-      <c r="I132" t="str">
-        <v>acfr:DueToFormerEmployeesModifiedAccrual</v>
-      </c>
-      <c r="J132" t="s">
-        <v>2227</v>
-      </c>
-    </row>
-    <row r="133" spans="1:10">
+    </row>
+    <row r="133" spans="1:8">
       <c r="A133" t="s">
         <v>60</v>
       </c>
@@ -13109,14 +11768,8 @@
         <f t="shared" si="10"/>
         <v>acfr:NotesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
-      <c r="I133" t="str">
-        <v>acfr:DueToIntermediateSchoolDistrictsModifiedAccrual</v>
-      </c>
-      <c r="J133" t="s">
-        <v>2228</v>
-      </c>
-    </row>
-    <row r="134" spans="1:10">
+    </row>
+    <row r="134" spans="1:8">
       <c r="A134" t="s">
         <v>60</v>
       </c>
@@ -13145,14 +11798,8 @@
         <f t="shared" si="10"/>
         <v>acfr:OtherAccountsReceivableModifiedAccrual</v>
       </c>
-      <c r="I134" t="str">
-        <v>acfr:DueToLibrariesModifiedAccrual</v>
-      </c>
-      <c r="J134" t="s">
-        <v>2229</v>
-      </c>
-    </row>
-    <row r="135" spans="1:10">
+    </row>
+    <row r="135" spans="1:8">
       <c r="A135" t="s">
         <v>60</v>
       </c>
@@ -13181,14 +11828,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I135" t="str">
-        <v>acfr:DueToOtherFundsModifiedAccrual</v>
-      </c>
-      <c r="J135" t="s">
-        <v>2230</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10">
+    </row>
+    <row r="136" spans="1:8">
       <c r="A136" t="s">
         <v>60</v>
       </c>
@@ -13217,14 +11858,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I136" t="str">
-        <v>acfr:DueToOtherGovernmentsModifiedAccrual</v>
-      </c>
-      <c r="J136" t="s">
-        <v>2231</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10">
+    </row>
+    <row r="137" spans="1:8">
       <c r="A137" t="s">
         <v>60</v>
       </c>
@@ -13253,14 +11888,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I137" t="str">
-        <v>acfr:DueToOthersModifiedAccrual</v>
-      </c>
-      <c r="J137" t="s">
-        <v>2232</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10">
+    </row>
+    <row r="138" spans="1:8">
       <c r="A138" t="s">
         <v>60</v>
       </c>
@@ -13289,14 +11918,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I138" t="str">
-        <v>acfr:DueToPrimaryGovernmentModifiedAccrual</v>
-      </c>
-      <c r="J138" t="s">
-        <v>2233</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10">
+    </row>
+    <row r="139" spans="1:8">
       <c r="A139" t="s">
         <v>60</v>
       </c>
@@ -13325,14 +11948,8 @@
         <f t="shared" si="10"/>
         <v>acfr:OtherReceivablesModifiedAccrual</v>
       </c>
-      <c r="I139" t="str">
-        <v>acfr:DueToRoadCommissionsModifiedAccrual</v>
-      </c>
-      <c r="J139" t="s">
-        <v>2234</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10">
+    </row>
+    <row r="140" spans="1:8">
       <c r="A140" t="s">
         <v>60</v>
       </c>
@@ -13361,14 +11978,8 @@
         <f t="shared" si="10"/>
         <v>acfr:OtherRestrictedAssetsModifiedAccrual</v>
       </c>
-      <c r="I140" t="str">
-        <v>acfr:DueToSchoolsModifiedAccrual</v>
-      </c>
-      <c r="J140" t="s">
-        <v>2235</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10">
+    </row>
+    <row r="141" spans="1:8">
       <c r="A141" t="s">
         <v>60</v>
       </c>
@@ -13397,14 +12008,8 @@
         <f t="shared" si="10"/>
         <v>acfr:OtherTaxesReceivableModifiedAccrual</v>
       </c>
-      <c r="I141" t="str">
-        <v>acfr:DueToSpecialEducationModifiedAccrual</v>
-      </c>
-      <c r="J141" t="s">
-        <v>2236</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10">
+    </row>
+    <row r="142" spans="1:8">
       <c r="A142" t="s">
         <v>60</v>
       </c>
@@ -13433,14 +12038,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I142" t="str">
-        <v>acfr:DueToStateGovernmentModifiedAccrual</v>
-      </c>
-      <c r="J142" t="s">
-        <v>2237</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10">
+    </row>
+    <row r="143" spans="1:8">
       <c r="A143" t="s">
         <v>60</v>
       </c>
@@ -13469,14 +12068,8 @@
         <f t="shared" si="10"/>
         <v>acfr:PaymentsInLieuOfTaxesReceivableModifiedAccrual</v>
       </c>
-      <c r="I143" t="str">
-        <v>acfr:DueToTaxpayersTaxOverpaymentsAndDuplicatePaymentsModifiedAccrual</v>
-      </c>
-      <c r="J143" t="s">
-        <v>2238</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10">
+    </row>
+    <row r="144" spans="1:8">
       <c r="A144" t="s">
         <v>60</v>
       </c>
@@ -13505,14 +12098,8 @@
         <f t="shared" si="10"/>
         <v>acfr:PenaltiesReceivableModifiedAccrual</v>
       </c>
-      <c r="I144" t="str">
-        <v>acfr:DueToTownshipsModifiedAccrual</v>
-      </c>
-      <c r="J144" t="s">
-        <v>2239</v>
-      </c>
-    </row>
-    <row r="145" spans="1:10">
+    </row>
+    <row r="145" spans="1:8">
       <c r="A145" t="s">
         <v>60</v>
       </c>
@@ -13541,14 +12128,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I145" t="str">
-        <v>acfr:DueToVillagesModifiedAccrual</v>
-      </c>
-      <c r="J145" t="s">
-        <v>2240</v>
-      </c>
-    </row>
-    <row r="146" spans="1:10">
+    </row>
+    <row r="146" spans="1:8">
       <c r="A146" t="s">
         <v>60</v>
       </c>
@@ -13577,14 +12158,8 @@
         <f t="shared" si="10"/>
         <v>acfr:PenaltiesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
-      <c r="I146" t="str">
-        <v>acfr:GarnishmentsPayableModifiedAccrual</v>
-      </c>
-      <c r="J146" t="s">
-        <v>2241</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10">
+    </row>
+    <row r="147" spans="1:8">
       <c r="A147" t="s">
         <v>60</v>
       </c>
@@ -13613,14 +12188,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I147" t="str">
-        <v>acfr:GrantsPayableModifiedAccrual</v>
-      </c>
-      <c r="J147" t="s">
-        <v>2242</v>
-      </c>
-    </row>
-    <row r="148" spans="1:10">
+    </row>
+    <row r="148" spans="1:8">
       <c r="A148" t="s">
         <v>60</v>
       </c>
@@ -13649,14 +12218,8 @@
         <f t="shared" si="10"/>
         <v>acfr:PooledCashAndInvestmentsModifiedAccrual</v>
       </c>
-      <c r="I148" t="str">
-        <v>acfr:OtherAdvancesModifiedAccrual</v>
-      </c>
-      <c r="J148" t="s">
-        <v>2243</v>
-      </c>
-    </row>
-    <row r="149" spans="1:10">
+    </row>
+    <row r="149" spans="1:8">
       <c r="A149" t="s">
         <v>60</v>
       </c>
@@ -13685,14 +12248,8 @@
         <f t="shared" si="10"/>
         <v>acfr:PrepaidDepositsModifiedAccrual</v>
       </c>
-      <c r="I149" t="str">
-        <v>acfr:PatientsOrInmatesTrustMoneyPayableModifiedAccrual</v>
-      </c>
-      <c r="J149" t="s">
-        <v>2244</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10">
+    </row>
+    <row r="150" spans="1:8">
       <c r="A150" t="s">
         <v>60</v>
       </c>
@@ -13721,14 +12278,8 @@
         <f t="shared" si="10"/>
         <v>acfr:PrepaidExpensesModifiedAccrual</v>
       </c>
-      <c r="I150" t="str">
-        <v>acfr:PayableFromRestrictedAssetsModifiedAccrual</v>
-      </c>
-      <c r="J150" t="s">
-        <v>2245</v>
-      </c>
-    </row>
-    <row r="151" spans="1:10">
+    </row>
+    <row r="151" spans="1:8">
       <c r="A151" t="s">
         <v>60</v>
       </c>
@@ -13757,14 +12308,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I151" t="str">
-        <v>acfr:PayrollDeductionsPayableModifiedAccrual</v>
-      </c>
-      <c r="J151" t="s">
-        <v>2246</v>
-      </c>
-    </row>
-    <row r="152" spans="1:10">
+    </row>
+    <row r="152" spans="1:8">
       <c r="A152" t="s">
         <v>60</v>
       </c>
@@ -13793,14 +12338,8 @@
         <f t="shared" si="10"/>
         <v>acfr:PropertyTaxesReceivableModifiedAccrual</v>
       </c>
-      <c r="I152" t="str">
-        <v>acfr:PenaltiesPayableModifiedAccrual</v>
-      </c>
-      <c r="J152" t="s">
-        <v>2247</v>
-      </c>
-    </row>
-    <row r="153" spans="1:10">
+    </row>
+    <row r="153" spans="1:8">
       <c r="A153" t="s">
         <v>60</v>
       </c>
@@ -13829,14 +12368,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I153" t="str">
-        <v>acfr:PerformanceDepositsPayableModifiedAccrual</v>
-      </c>
-      <c r="J153" t="s">
-        <v>2248</v>
-      </c>
-    </row>
-    <row r="154" spans="1:10">
+    </row>
+    <row r="154" spans="1:8">
       <c r="A154" t="s">
         <v>60</v>
       </c>
@@ -13865,14 +12398,8 @@
         <f t="shared" si="10"/>
         <v>acfr:PropertyTaxesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
-      <c r="I154" t="str">
-        <v>acfr:ReceiptsRefundableModifiedAccrual</v>
-      </c>
-      <c r="J154" t="s">
-        <v>2249</v>
-      </c>
-    </row>
-    <row r="155" spans="1:10">
+    </row>
+    <row r="155" spans="1:8">
       <c r="A155" t="s">
         <v>60</v>
       </c>
@@ -13901,14 +12428,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I155" t="str">
-        <v>acfr:RegulatoryLiabilityCurrentModifiedAccrual</v>
-      </c>
-      <c r="J155" t="s">
-        <v>2250</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10">
+    </row>
+    <row r="156" spans="1:8">
       <c r="A156" t="s">
         <v>60</v>
       </c>
@@ -13937,14 +12458,8 @@
         <f t="shared" si="10"/>
         <v>acfr:ReceivablesModifiedAccrual</v>
       </c>
-      <c r="I156" t="str">
-        <v>acfr:RestitutionsPayableModifiedAccrual</v>
-      </c>
-      <c r="J156" t="s">
-        <v>2251</v>
-      </c>
-    </row>
-    <row r="157" spans="1:10">
+    </row>
+    <row r="157" spans="1:8">
       <c r="A157" t="s">
         <v>60</v>
       </c>
@@ -13973,14 +12488,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I157" t="str">
-        <v>acfr:RetainagePayableModifiedAccrual</v>
-      </c>
-      <c r="J157" t="s">
-        <v>2252</v>
-      </c>
-    </row>
-    <row r="158" spans="1:10">
+    </row>
+    <row r="158" spans="1:8">
       <c r="A158" t="s">
         <v>60</v>
       </c>
@@ -14009,14 +12518,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I158" t="str">
-        <v>acfr:TaxesPayableModifiedAccrual</v>
-      </c>
-      <c r="J158" t="s">
-        <v>2253</v>
-      </c>
-    </row>
-    <row r="159" spans="1:10">
+    </row>
+    <row r="159" spans="1:8">
       <c r="A159" t="s">
         <v>60</v>
       </c>
@@ -14045,14 +12548,8 @@
         <f t="shared" si="10"/>
         <v>acfr:RestrictedAssetsModifiedAccrual</v>
       </c>
-      <c r="I159" t="str">
-        <v>acfr:UnclaimedMoneyModifiedAccrual</v>
-      </c>
-      <c r="J159" t="s">
-        <v>2254</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10">
+    </row>
+    <row r="160" spans="1:8">
       <c r="A160" t="s">
         <v>60</v>
       </c>
@@ -14081,14 +12578,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I160" t="str">
-        <v>acfr:UndistributedReceiptsModifiedAccrual</v>
-      </c>
-      <c r="J160" t="s">
-        <v>2255</v>
-      </c>
-    </row>
-    <row r="161" spans="1:10">
+    </row>
+    <row r="161" spans="1:8">
       <c r="A161" t="s">
         <v>60</v>
       </c>
@@ -14117,14 +12608,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I161" t="str">
-        <v>acfr:UndistributedTaxCollectionsModifiedAccrual</v>
-      </c>
-      <c r="J161" t="s">
-        <v>2256</v>
-      </c>
-    </row>
-    <row r="162" spans="1:10">
+    </row>
+    <row r="162" spans="1:8">
       <c r="A162" t="s">
         <v>60</v>
       </c>
@@ -14153,14 +12638,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I162" t="str">
-        <v>acfr:UnearnedRevenueModifiedAccrual</v>
-      </c>
-      <c r="J162" t="s">
-        <v>2257</v>
-      </c>
-    </row>
-    <row r="163" spans="1:10">
+    </row>
+    <row r="163" spans="1:8">
       <c r="A163" t="s">
         <v>60</v>
       </c>
@@ -14189,14 +12668,8 @@
         <f t="shared" si="10"/>
         <v>acfr:RestrictedCashModifiedAccrual</v>
       </c>
-      <c r="I163" t="str">
-        <v>acfr:VouchersPayableModifiedAccrual</v>
-      </c>
-      <c r="J163" t="s">
-        <v>1752</v>
-      </c>
-    </row>
-    <row r="164" spans="1:10">
+    </row>
+    <row r="164" spans="1:8">
       <c r="A164" t="s">
         <v>60</v>
       </c>
@@ -14225,14 +12698,8 @@
         <f t="shared" si="10"/>
         <v>acfr:RestrictedCashAndCashEquivalentsModifiedAccrual</v>
       </c>
-      <c r="I164" t="str">
-        <v>acfr:DeferredInflowsOfResourcesModifiedAccrual</v>
-      </c>
-      <c r="J164" t="s">
-        <v>2258</v>
-      </c>
-    </row>
-    <row r="165" spans="1:10">
+    </row>
+    <row r="165" spans="1:8">
       <c r="A165" t="s">
         <v>60</v>
       </c>
@@ -14261,14 +12728,8 @@
         <f t="shared" si="10"/>
         <v>acfr:RestrictedCashAndInvestmentsModifiedAccrual</v>
       </c>
-      <c r="I165" t="str">
-        <v>acfr:DeferredInflowsOfResourcesPropertyTaxesModifiedAccrual</v>
-      </c>
-      <c r="J165" t="s">
-        <v>2259</v>
-      </c>
-    </row>
-    <row r="166" spans="1:10">
+    </row>
+    <row r="166" spans="1:8">
       <c r="A166" t="s">
         <v>60</v>
       </c>
@@ -14297,14 +12758,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I166" t="str">
-        <v>acfr:DeferredInflowsOfResourcesTaxesLeviedForASubsequentPeriodModifiedAccrual</v>
-      </c>
-      <c r="J166" t="s">
-        <v>2260</v>
-      </c>
-    </row>
-    <row r="167" spans="1:10">
+    </row>
+    <row r="167" spans="1:8">
       <c r="A167" t="s">
         <v>60</v>
       </c>
@@ -14333,14 +12788,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I167" t="str">
-        <v>acfr:OtherDeferredInflowsOfResourcesModifiedAccrual</v>
-      </c>
-      <c r="J167" t="s">
-        <v>2261</v>
-      </c>
-    </row>
-    <row r="168" spans="1:10">
+    </row>
+    <row r="168" spans="1:8">
       <c r="A168" t="s">
         <v>60</v>
       </c>
@@ -14369,14 +12818,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I168" t="str">
-        <v>acfr:DeferredOutflowsOfResourcesModifiedAccrual</v>
-      </c>
-      <c r="J168" t="s">
-        <v>2262</v>
-      </c>
-    </row>
-    <row r="169" spans="1:10">
+    </row>
+    <row r="169" spans="1:8">
       <c r="A169" t="s">
         <v>60</v>
       </c>
@@ -14405,14 +12848,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I169" t="str">
-        <v>acfr:OtherDeferredOutflowsOfResourcesModifiedAccrual</v>
-      </c>
-      <c r="J169" t="s">
-        <v>2263</v>
-      </c>
-    </row>
-    <row r="170" spans="1:10">
+    </row>
+    <row r="170" spans="1:8">
       <c r="A170" t="s">
         <v>60</v>
       </c>
@@ -14441,14 +12878,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I170" t="str">
-        <v>acfr:ConstructionInProgressModifiedAccrual</v>
-      </c>
-      <c r="J170" t="s">
-        <v>2264</v>
-      </c>
-    </row>
-    <row r="171" spans="1:10">
+    </row>
+    <row r="171" spans="1:8">
       <c r="A171" t="s">
         <v>60</v>
       </c>
@@ -14477,14 +12908,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I171" t="str">
-        <v>acfr:InvestmentsInJointVenturesModifiedAccrual</v>
-      </c>
-      <c r="J171" t="s">
-        <v>2265</v>
-      </c>
-    </row>
-    <row r="172" spans="1:10">
+    </row>
+    <row r="172" spans="1:8">
       <c r="A172" t="s">
         <v>60</v>
       </c>
@@ -14513,14 +12938,8 @@
         <f t="shared" si="10"/>
         <v>acfr:SalesTaxReceivableModifiedAccrual</v>
       </c>
-      <c r="I172" t="str">
-        <v>acfr:InvestmentsOfSurplusFundsModifiedAccrual</v>
-      </c>
-      <c r="J172" t="s">
-        <v>2266</v>
-      </c>
-    </row>
-    <row r="173" spans="1:10">
+    </row>
+    <row r="173" spans="1:8">
       <c r="A173" t="s">
         <v>60</v>
       </c>
@@ -14549,14 +12968,8 @@
         <f t="shared" si="10"/>
         <v>acfr:SecuritiesLendingCollateralAssetsModifiedAccrual</v>
       </c>
-      <c r="I173" t="str">
-        <v>acfr:LeasesAccumulatedAmortizationModifiedAccrual</v>
-      </c>
-      <c r="J173" t="s">
-        <v>2267</v>
-      </c>
-    </row>
-    <row r="174" spans="1:10">
+    </row>
+    <row r="174" spans="1:8">
       <c r="A174" t="s">
         <v>60</v>
       </c>
@@ -14585,14 +12998,8 @@
         <f t="shared" si="10"/>
         <v>acfr:SecuritiesLendingObligationsLiabilityModifiedAccrual</v>
       </c>
-      <c r="I174" t="str">
-        <v>acfr:LongTermContractsReceivableModifiedAccrual</v>
-      </c>
-      <c r="J174" t="s">
-        <v>2268</v>
-      </c>
-    </row>
-    <row r="175" spans="1:10">
+    </row>
+    <row r="175" spans="1:8">
       <c r="A175" t="s">
         <v>60</v>
       </c>
@@ -14621,14 +13028,8 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="I175" t="str">
-        <v>acfr:LongTermInvestmentsModifiedAccrual</v>
-      </c>
-      <c r="J175" t="s">
-        <v>2269</v>
-      </c>
-    </row>
-    <row r="176" spans="1:10">
+    </row>
+    <row r="176" spans="1:8">
       <c r="A176" t="s">
         <v>60</v>
       </c>
@@ -14657,14 +13058,8 @@
         <f t="shared" si="10"/>
         <v>acfr:ServiceFeesReceivableModifiedAccrual</v>
       </c>
-      <c r="I176" t="str">
-        <v>acfr:NetOPEBAssetModifiedAccrual</v>
-      </c>
-      <c r="J176" t="s">
-        <v>2270</v>
-      </c>
-    </row>
-    <row r="177" spans="1:10">
+    </row>
+    <row r="177" spans="1:8">
       <c r="A177" t="s">
         <v>60</v>
       </c>
@@ -14693,14 +13088,8 @@
         <f t="shared" si="10"/>
         <v>acfr:SpecialAssessmentTaxesReceivableModifiedAccrual</v>
       </c>
-      <c r="I177" t="str">
-        <v>acfr:NetPensionAssetModifiedAccrual</v>
-      </c>
-      <c r="J177" t="s">
-        <v>2271</v>
-      </c>
-    </row>
-    <row r="178" spans="1:10">
+    </row>
+    <row r="178" spans="1:8">
       <c r="A178" t="s">
         <v>60</v>
       </c>
@@ -14729,14 +13118,8 @@
         <f t="shared" si="10"/>
         <v>acfr:SpecialAssessmentTaxesReceivableUnavailableModifiedAccrual</v>
       </c>
-      <c r="I178" t="str">
-        <v>acfr:OtherAssetsModifiedAccrual</v>
-      </c>
-      <c r="J178" t="s">
-        <v>2272</v>
-      </c>
-    </row>
-    <row r="179" spans="1:10">
+    </row>
+    <row r="179" spans="1:8">
       <c r="A179" t="s">
         <v>60</v>
       </c>
@@ -14765,14 +13148,8 @@
         <f t="shared" si="10"/>
         <v>acfr:SpecialAssessmentsReceivableDelinquentModifiedAccrual</v>
       </c>
-      <c r="I179" t="str">
-        <v>acfr:OtherInvestmentsModifiedAccrual</v>
-      </c>
-      <c r="J179" t="s">
-        <v>2273</v>
-      </c>
-    </row>
-    <row r="180" spans="1:10">
+    </row>
+    <row r="180" spans="1:8">
       <c r="A180" t="s">
         <v>60</v>
       </c>
@@ -14801,14 +13178,8 @@
         <f t="shared" si="10"/>
         <v>acfr:TaxesReceivableModifiedAccrual</v>
       </c>
-      <c r="I180" t="str">
-        <v>acfr:UnamortizedDiscountsOnBondsSoldByLocalUnitModifiedAccrual</v>
-      </c>
-      <c r="J180" t="s">
-        <v>2274</v>
-      </c>
-    </row>
-    <row r="181" spans="1:10">
+    </row>
+    <row r="181" spans="1:8">
       <c r="A181" t="s">
         <v>60</v>
       </c>
@@ -14837,14 +13208,8 @@
         <f t="shared" si="10"/>
         <v>acfr:TaxesReceivableDelinquentPersonalPropertyModifiedAccrual</v>
       </c>
-      <c r="I181" t="str">
-        <v>acfr:AdvancesToComponentUnitModifiedAccrual</v>
-      </c>
-      <c r="J181" t="s">
-        <v>2275</v>
-      </c>
-    </row>
-    <row r="182" spans="1:10">
+    </row>
+    <row r="182" spans="1:8">
       <c r="A182" t="s">
         <v>60</v>
       </c>
@@ -14873,14 +13238,8 @@
         <f t="shared" si="10"/>
         <v>acfr:TaxesReceivableDelinquentRealPropertyModifiedAccrual</v>
       </c>
-      <c r="I182" t="str">
-        <v>acfr:AdvancesToOtherFundsModifiedAccrual</v>
-      </c>
-      <c r="J182" t="s">
-        <v>2276</v>
-      </c>
-    </row>
-    <row r="183" spans="1:10">
+    </row>
+    <row r="183" spans="1:8">
       <c r="A183" t="s">
         <v>60</v>
       </c>
@@ -14909,14 +13268,8 @@
         <f t="shared" si="10"/>
         <v>acfr:TaxesReceivablePersonalPropertyCurrentLevyModifiedAccrual</v>
       </c>
-      <c r="I183" t="str">
-        <v>acfr:AdvancesToOtherGovernmentsModifiedAccrual</v>
-      </c>
-      <c r="J183" t="s">
-        <v>2277</v>
-      </c>
-    </row>
-    <row r="184" spans="1:10">
+    </row>
+    <row r="184" spans="1:8">
       <c r="A184" t="s">
         <v>60</v>
       </c>
@@ -14945,11 +13298,8 @@
         <f t="shared" si="10"/>
         <v>acfr:TaxesReceivableRealPropertyCurrentLevyModifiedAccrual</v>
       </c>
-      <c r="I184" t="str">
-        <v>acfr:NetPensionLiabilityModifiedAccrual</v>
-      </c>
-    </row>
-    <row r="185" spans="1:10">
+    </row>
+    <row r="185" spans="1:8">
       <c r="A185" t="s">
         <v>60</v>
       </c>
@@ -14979,7 +13329,7 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:8">
       <c r="A186" t="s">
         <v>60</v>
       </c>
@@ -15009,7 +13359,7 @@
         <v/>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:8">
       <c r="A187" t="s">
         <v>60</v>
       </c>
@@ -15039,7 +13389,7 @@
         <v/>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:8">
       <c r="A188" t="s">
         <v>60</v>
       </c>
@@ -15069,7 +13419,7 @@
         <v/>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:8">
       <c r="A189" t="s">
         <v>60</v>
       </c>
@@ -15099,7 +13449,7 @@
         <v/>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:8">
       <c r="A190" t="s">
         <v>60</v>
       </c>
@@ -15129,7 +13479,7 @@
         <v/>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:8">
       <c r="A191" t="s">
         <v>60</v>
       </c>
@@ -15159,7 +13509,7 @@
         <v/>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:8">
       <c r="A192" t="s">
         <v>60</v>
       </c>
@@ -36964,7 +35314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62560919-E4A0-3A4F-9164-3F35B35B852C}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -38109,8 +36459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAF299C-3D3B-8F47-AA92-8FD95A662E81}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
issue 9- template created
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarrahahmed/Desktop/CLOSUP/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3F0F51-2748-BC4D-B213-20D11DE781AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3B43F2-DDFC-784A-9BB4-9F6EF624716E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="14580" windowHeight="18400" tabRatio="834" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" tabRatio="834" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Label Dropdowns" sheetId="8" r:id="rId1"/>
@@ -22401,7 +22401,7 @@
   </sheetPr>
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
issue 9- final edits complete
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarrahahmed/Desktop/CLOSUP/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3B43F2-DDFC-784A-9BB4-9F6EF624716E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51EDB25-5535-A748-966D-E06E3C1B5539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" tabRatio="834" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14820" yWindow="720" windowWidth="14580" windowHeight="18400" tabRatio="834" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Label Dropdowns" sheetId="8" r:id="rId1"/>
@@ -6111,6 +6111,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6120,151 +6129,13 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
   </cellStyles>
-  <dxfs count="55">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="47">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -6396,6 +6267,64 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13979,31 +13908,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C101">
-    <cfRule type="cellIs" dxfId="21" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="equal">
       <formula>$C$101</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>$C$101</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:E101">
-    <cfRule type="cellIs" dxfId="19" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D101">
-    <cfRule type="cellIs" dxfId="18" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
       <formula>$D$101</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="notEqual">
       <formula>$D$101</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E101">
-    <cfRule type="cellIs" dxfId="16" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>$E$101</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
       <formula>$E$101</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18545,18 +18474,18 @@
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <conditionalFormatting sqref="C101:F101">
-    <cfRule type="cellIs" dxfId="54" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="18" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="19" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="20" operator="notEqual">
+    <cfRule type="cellIs" dxfId="44" priority="20" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F101 C23 C37 C50 C65 C76:C77 C89 C101">
-    <cfRule type="expression" dxfId="51" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="2" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20230,62 +20159,62 @@
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <conditionalFormatting sqref="C23 C37 C50 D53:G63 D74:H77 J74:J77">
-    <cfRule type="expression" dxfId="50" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="49" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:J64">
-    <cfRule type="expression" dxfId="49" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="34" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:J72">
-    <cfRule type="expression" dxfId="48" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="10" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:F6 D52:F52">
-    <cfRule type="expression" dxfId="47" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="46" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:G51">
-    <cfRule type="expression" dxfId="46" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="6" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D65:J70">
-    <cfRule type="expression" dxfId="45" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="2" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39:H50">
-    <cfRule type="expression" dxfId="44" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="5" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38:I38">
-    <cfRule type="expression" dxfId="43" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="43" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:J6 D7:I37 I39:I51">
-    <cfRule type="expression" dxfId="42" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="39" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52:J63">
-    <cfRule type="expression" dxfId="41" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="3" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I74:I99">
-    <cfRule type="expression" dxfId="40" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="1" stopIfTrue="1">
       <formula>I$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:J50">
-    <cfRule type="expression" dxfId="39" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="4" stopIfTrue="1">
       <formula>J$6=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20943,47 +20872,47 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C35:G35">
-    <cfRule type="expression" dxfId="38" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="10" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:H25">
-    <cfRule type="expression" dxfId="37" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="16" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:I28">
-    <cfRule type="expression" dxfId="36" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="11" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="35" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:G16">
-    <cfRule type="expression" dxfId="34" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="3" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:G18">
-    <cfRule type="expression" dxfId="33" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="20" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:G24">
-    <cfRule type="expression" dxfId="32" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="2" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:G27">
-    <cfRule type="expression" dxfId="31" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="14" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:G34">
-    <cfRule type="expression" dxfId="30" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="1" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22362,7 +22291,7 @@
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="D7:I7 D8:J23 C23 D25:J36 C36 C37:J37 D38:J71 C60:J60 C70">
-    <cfRule type="expression" dxfId="29" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="17" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22401,8 +22330,8 @@
   </sheetPr>
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="O42" sqref="O42"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -22435,7 +22364,7 @@
         <v>1105</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="C2" s="55"/>
       <c r="D2" s="55"/>
@@ -22499,16 +22428,16 @@
       <c r="C6" s="12" t="s">
         <v>1756</v>
       </c>
-      <c r="D6" s="122" t="str">
+      <c r="D6" s="119" t="str">
         <f>IF(AND('Master Info'!C5="N",'Master Info'!C6="N"), "",  IF('Master Info'!C5="N", "Component Units", "Business-Type Activities - Enterprise Funds"))</f>
         <v>Business-Type Activities - Enterprise Funds</v>
       </c>
-      <c r="E6" s="123"/>
-      <c r="F6" s="123"/>
-      <c r="G6" s="123"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="123"/>
-      <c r="J6" s="124"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
+      <c r="G6" s="120"/>
+      <c r="H6" s="120"/>
+      <c r="I6" s="120"/>
+      <c r="J6" s="121"/>
     </row>
     <row r="7" spans="1:10" ht="15">
       <c r="A7" s="7"/>
@@ -22553,7 +22482,10 @@
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
+      <c r="J9" s="20">
+        <f>SUM(D9:I9)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="15">
       <c r="A10" s="8" t="str">
@@ -22568,7 +22500,10 @@
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
-      <c r="J10" s="20"/>
+      <c r="J10" s="20">
+        <f>SUM(D10:I10)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="15">
       <c r="A11" s="8" t="str">
@@ -22583,7 +22518,10 @@
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
+      <c r="J11" s="20">
+        <f>SUM(D11:I11)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="15">
       <c r="A12" s="8" t="str">
@@ -22598,7 +22536,10 @@
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
+      <c r="J12" s="20">
+        <f>SUM(D12:I12)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="15">
       <c r="A13" s="8" t="str">
@@ -22613,7 +22554,10 @@
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
+      <c r="J13" s="20">
+        <f>SUM(D13:I13)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="15">
       <c r="A14" s="8" t="str">
@@ -22628,7 +22572,10 @@
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
       <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
+      <c r="J14" s="20">
+        <f>SUM(D14:I14)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="15">
       <c r="A15" s="8" t="str">
@@ -22643,7 +22590,10 @@
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
-      <c r="J15" s="20"/>
+      <c r="J15" s="20">
+        <f>SUM(D15:I15)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="15">
       <c r="A16" s="8" t="str">
@@ -22658,7 +22608,10 @@
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
+      <c r="J16" s="20">
+        <f>SUM(D16:I16)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="15">
       <c r="A17" s="8" t="str">
@@ -22673,7 +22626,10 @@
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
-      <c r="J17" s="20"/>
+      <c r="J17" s="20">
+        <f>SUM(D17:I17)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="15" hidden="1">
       <c r="A18" s="8" t="str">
@@ -22688,7 +22644,10 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
+      <c r="J18" s="20">
+        <f t="shared" ref="J18:J22" si="0">SUM(D18:I18)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="15" hidden="1">
       <c r="A19" s="8" t="str">
@@ -22703,7 +22662,10 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
-      <c r="J19" s="20"/>
+      <c r="J19" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="15" hidden="1">
       <c r="A20" s="8" t="str">
@@ -22718,7 +22680,10 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
-      <c r="J20" s="20"/>
+      <c r="J20" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:10" ht="15" hidden="1">
       <c r="A21" s="8" t="str">
@@ -22733,7 +22698,10 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
-      <c r="J21" s="20"/>
+      <c r="J21" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:10" ht="15">
       <c r="A22" s="8" t="str">
@@ -22748,7 +22716,10 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
-      <c r="J22" s="20"/>
+      <c r="J22" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:10" ht="15">
       <c r="A23" s="8" t="s">
@@ -22974,7 +22945,7 @@
         <v>18</v>
       </c>
       <c r="C37" s="17">
-        <f>IF(C6="","",SUM(C25:C36))</f>
+        <f ca="1">SUM(_xlfn.XLOOKUP("Total Noncurrent Assets",$B:$B,C:C))</f>
         <v>0</v>
       </c>
       <c r="D37" s="17"/>
@@ -22996,7 +22967,7 @@
         <v>20</v>
       </c>
       <c r="C38" s="23">
-        <f>SUM(_xlfn.XLOOKUP("Total Current Assets",$B:$B,C:C),(_xlfn.XLOOKUP("Total Noncurrent Assets",$B:$B,C:C)))</f>
+        <f ca="1">SUM(_xlfn.XLOOKUP("Total Current Assets",$B:$B,C:C),(_xlfn.XLOOKUP("Total Noncurrent Assets",$B:$B,C:C)))</f>
         <v>0</v>
       </c>
       <c r="D38" s="23"/>
@@ -23394,7 +23365,7 @@
         <v>39</v>
       </c>
       <c r="C64" s="17">
-        <f>IF(C6="","",SUM(C55:C63))</f>
+        <f ca="1">SUM(_xlfn.XLOOKUP("Total Noncurrent Liabilities",$B:$B,C:C))</f>
         <v>0</v>
       </c>
       <c r="D64" s="17"/>
@@ -23416,7 +23387,7 @@
         <v>41</v>
       </c>
       <c r="C65" s="23">
-        <f>SUM(_xlfn.XLOOKUP("Total Current Liabilities",$B:$B,C:C),(_xlfn.XLOOKUP("Total Noncurrent Liabilities",$B:$B,C:C)))</f>
+        <f ca="1">SUM(_xlfn.XLOOKUP("Total Current Liabilities",$B:$B,C:C),(_xlfn.XLOOKUP("Total Noncurrent Liabilities",$B:$B,C:C)))</f>
         <v>0</v>
       </c>
       <c r="D65" s="23"/>
@@ -23629,34 +23600,34 @@
     <mergeCell ref="D6:J6"/>
   </mergeCells>
   <conditionalFormatting sqref="C77:J77">
-    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="notEqual">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="notEqual">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23 E23:I23 C37 E37:I37 C53 E53:I53 C64:C65 E64:I65 C77 E77:I77 D6">
-    <cfRule type="expression" dxfId="11" priority="2" stopIfTrue="1">
+  <conditionalFormatting sqref="D6 C23 E23:I23 C37 E37:I37 C53 E53:I53 C64:C65 E64:I65 C77 E77:I77">
+    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D23 D37 D53 D64:D65 D77">
-    <cfRule type="expression" dxfId="10" priority="52" stopIfTrue="1">
+  <conditionalFormatting sqref="D77 D23 D37 D53 D64:D65">
+    <cfRule type="expression" dxfId="16" priority="52" stopIfTrue="1">
       <formula>#REF!=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7:J77">
-    <cfRule type="expression" dxfId="9" priority="63" stopIfTrue="1">
-      <formula>D$6=""</formula>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
+      <formula>COUNTA(D2:I2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
-      <formula>COUNTA(D2:I2)=1</formula>
+  <conditionalFormatting sqref="J7:J77">
+    <cfRule type="expression" dxfId="14" priority="63" stopIfTrue="1">
+      <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
@@ -23977,12 +23948,12 @@
     </row>
     <row r="25" spans="1:5" ht="15">
       <c r="A25" s="7"/>
-      <c r="B25" s="119" t="s">
+      <c r="B25" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="120"/>
-      <c r="D25" s="120"/>
-      <c r="E25" s="121"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="123"/>
+      <c r="E25" s="124"/>
     </row>
     <row r="26" spans="1:5" ht="15">
       <c r="A26" s="8" t="str">
@@ -24999,31 +24970,31 @@
     <mergeCell ref="B25:E25"/>
   </mergeCells>
   <conditionalFormatting sqref="C102">
-    <cfRule type="cellIs" dxfId="28" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="equal">
       <formula>$C$102</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>$C$102</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C102:E102">
-    <cfRule type="cellIs" dxfId="26" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D102">
-    <cfRule type="cellIs" dxfId="25" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" stopIfTrue="1" operator="equal">
       <formula>$D$102</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="notEqual">
       <formula>$D$102</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E102">
-    <cfRule type="cellIs" dxfId="23" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>$E$102</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>$E$102</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added 1 nice label
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/byflow/Documents/Research/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9817F2-53D5-D64E-B073-6D1FEE1127F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1641DF-EE81-2740-AB0D-1EE563DC47B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3244" uniqueCount="2021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3245" uniqueCount="2022">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -6143,6 +6143,9 @@
   </si>
   <si>
     <t>Modified Accrual XBRL Tag</t>
+  </si>
+  <si>
+    <t>Other Cash and Cash Equivalents, Modified Accrual</t>
   </si>
 </sst>
 </file>
@@ -7527,8 +7530,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E602"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D512" zoomScale="108" workbookViewId="0">
-      <selection activeCell="F537" sqref="F537"/>
+    <sheetView tabSelected="1" topLeftCell="A514" zoomScale="108" workbookViewId="0">
+      <selection activeCell="B528" sqref="B528"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -14849,6 +14852,9 @@
       </c>
     </row>
     <row r="523" spans="1:5">
+      <c r="B523" t="s">
+        <v>2021</v>
+      </c>
       <c r="D523" t="s">
         <v>1763</v>
       </c>

</xml_diff>

<commit_message>
#10 added pretty names, done i think
</commit_message>
<xml_diff>
--- a/static/input_files/ACFR_template.xlsx
+++ b/static/input_files/ACFR_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/byflow/Documents/Research/process-xbrl/static/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1641DF-EE81-2740-AB0D-1EE563DC47B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B97CF5-9ADE-EF4F-BB45-FF715BF42DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Label Dropdowns" sheetId="8" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3245" uniqueCount="2022">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3324" uniqueCount="2101">
   <si>
     <t>Statement of Net Position</t>
   </si>
@@ -6146,6 +6146,243 @@
   </si>
   <si>
     <t>Other Cash and Cash Equivalents, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Cash and Cash Equivalents and Investments, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Restricted Investments, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Pooled Investments, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Investments, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Investments Held by Third Parties Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Uncollectible Receivables, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Customer Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Customer Receivables, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Customer Receivable, Net of Allowance, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Uncollectible Interest, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Utility Bills Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Property Taxes, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Income Taxes, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Income Taxes Receivable, Net of Allowance, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Special Assessment Taxes, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Special Assessment Taxes Receivable, Net of Allowance, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Sales Taxes, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Sales Taxes Receivable, Net of Allowance, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Other Taxes Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Other Taxes Receivable, Net of Allowance, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Taxes, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Taxes Receivable, Net of Allowance, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Penalties Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Leases Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Grants and Contracts Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Deposits Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Loans and Notes Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Claims and Judgments Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Inter Governmental Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Receivables (Net of Allowance), Modified Accrual</t>
+  </si>
+  <si>
+    <t>Restricted Receivables, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Restricted Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Receivables, Restricted (Net of Allowance), Modified Accrual</t>
+  </si>
+  <si>
+    <t>Investment Income Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Investment Income Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Investment Income Receivable, Net of Allowance, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Allowance for Other Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Other Receivables, (Net of Allowance), Modified Accrual</t>
+  </si>
+  <si>
+    <t>Receivables from Contracts, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Due from Other Government, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Due from Others, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Prepaid Insurance, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Other Prepaid Assets, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Prepaid Expenses and Other Assets, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Inventory and Prepaid Items, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Travel Advances Receivable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Derivative Instruments, Assets, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Regulatory Assets, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Assets, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Assets and Deferred Outflows of Resources, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Cash Overdraft, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Benefits Payable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Inter Governmental Payable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Claims and Judgments Payable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Payables for Others, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Accrued Payroll Taxes, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Accrued Benefits and Compensation Long Term, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Compensated Absences Payable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>All Other Accounts Payable and Accrued Liabilities, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Due to Enterprise Funds, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Advances from Component Unit, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Provision for Property Tax Refunds, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Unamortized Premium on Bonds, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Leases Payable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Bonds Payable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Loans Payable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Notes Payable, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Notes Payable, Due in More Than One Year, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Regulatory Liability, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Derivative Instruments, Liability, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Other Liabilities, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Liabilities, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Deferred Inflows of Resources, Drain Fund, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Deferred Inflows of Resources, Special Assessments, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Deferred Inflows of Resources, Unavailable Revenue, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Liabilities and Deferred Inflows of Resources, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Investment in Capital Assets, Modified Accrual</t>
+  </si>
+  <si>
+    <t>Liabilities and Deferred Inflows of Resources and Fund Balances, Modified Accrual</t>
   </si>
 </sst>
 </file>
@@ -6156,7 +6393,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -6301,6 +6538,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -6658,7 +6901,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6913,6 +7156,7 @@
     </xf>
     <xf numFmtId="44" fontId="13" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="44" fontId="23" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6922,7 +7166,7 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -7530,15 +7774,15 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E602"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A514" zoomScale="108" workbookViewId="0">
-      <selection activeCell="B528" sqref="B528"/>
+    <sheetView tabSelected="1" topLeftCell="A518" zoomScale="108" workbookViewId="0">
+      <selection activeCell="A544" sqref="A544"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.83203125" customWidth="1"/>
-    <col min="3" max="3" width="63.1640625" customWidth="1"/>
+    <col min="2" max="2" width="43.83203125" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" customWidth="1"/>
     <col min="4" max="4" width="67.1640625" customWidth="1"/>
     <col min="5" max="10" width="79.1640625" customWidth="1"/>
   </cols>
@@ -7553,7 +7797,7 @@
       <c r="C1" s="1" t="s">
         <v>1762</v>
       </c>
-      <c r="D1" s="131" t="s">
+      <c r="D1" s="128" t="s">
         <v>2020</v>
       </c>
     </row>
@@ -14852,7 +15096,7 @@
       </c>
     </row>
     <row r="523" spans="1:5">
-      <c r="B523" t="s">
+      <c r="B523" s="2" t="s">
         <v>2021</v>
       </c>
       <c r="D523" t="s">
@@ -14864,6 +15108,9 @@
       </c>
     </row>
     <row r="524" spans="1:5">
+      <c r="B524" s="132" t="s">
+        <v>2022</v>
+      </c>
       <c r="D524" t="s">
         <v>1764</v>
       </c>
@@ -14873,6 +15120,9 @@
       </c>
     </row>
     <row r="525" spans="1:5">
+      <c r="B525" s="132" t="s">
+        <v>2023</v>
+      </c>
       <c r="D525" t="s">
         <v>1765</v>
       </c>
@@ -14882,6 +15132,9 @@
       </c>
     </row>
     <row r="526" spans="1:5">
+      <c r="B526" s="2" t="s">
+        <v>2024</v>
+      </c>
       <c r="D526" t="s">
         <v>1766</v>
       </c>
@@ -14891,6 +15144,9 @@
       </c>
     </row>
     <row r="527" spans="1:5">
+      <c r="B527" s="132" t="s">
+        <v>2025</v>
+      </c>
       <c r="D527" t="s">
         <v>1767</v>
       </c>
@@ -14900,6 +15156,9 @@
       </c>
     </row>
     <row r="528" spans="1:5">
+      <c r="B528" s="2" t="s">
+        <v>2026</v>
+      </c>
       <c r="D528" t="s">
         <v>1768</v>
       </c>
@@ -14908,7 +15167,10 @@
         <v>Dup_1_InvestmentsHeldByThirdPartiesModifiedAccrual</v>
       </c>
     </row>
-    <row r="529" spans="4:5">
+    <row r="529" spans="2:5">
+      <c r="B529" s="2" t="s">
+        <v>2027</v>
+      </c>
       <c r="D529" t="s">
         <v>1769</v>
       </c>
@@ -14917,7 +15179,10 @@
         <v>AllowanceForUncollectibleReceivablesModifiedAccrual</v>
       </c>
     </row>
-    <row r="530" spans="4:5">
+    <row r="530" spans="2:5">
+      <c r="B530" s="2" t="s">
+        <v>2028</v>
+      </c>
       <c r="D530" t="s">
         <v>1770</v>
       </c>
@@ -14926,7 +15191,10 @@
         <v>CustomerReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="531" spans="4:5">
+    <row r="531" spans="2:5">
+      <c r="B531" s="2" t="s">
+        <v>2029</v>
+      </c>
       <c r="D531" t="s">
         <v>1771</v>
       </c>
@@ -14935,7 +15203,10 @@
         <v>AllowanceForCustomerReceivablesModifiedAccrual</v>
       </c>
     </row>
-    <row r="532" spans="4:5">
+    <row r="532" spans="2:5">
+      <c r="B532" s="2" t="s">
+        <v>2030</v>
+      </c>
       <c r="D532" t="s">
         <v>1772</v>
       </c>
@@ -14944,7 +15215,10 @@
         <v>CustomerReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
     </row>
-    <row r="533" spans="4:5">
+    <row r="533" spans="2:5">
+      <c r="B533" s="2" t="s">
+        <v>2031</v>
+      </c>
       <c r="D533" t="s">
         <v>1773</v>
       </c>
@@ -14953,7 +15227,10 @@
         <v>AllowanceForUncollectibleInterestModifiedAccrual</v>
       </c>
     </row>
-    <row r="534" spans="4:5">
+    <row r="534" spans="2:5">
+      <c r="B534" s="2" t="s">
+        <v>2032</v>
+      </c>
       <c r="D534" t="s">
         <v>1774</v>
       </c>
@@ -14962,7 +15239,10 @@
         <v>UtilityBillsReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="535" spans="4:5">
+    <row r="535" spans="2:5">
+      <c r="B535" s="2" t="s">
+        <v>2033</v>
+      </c>
       <c r="D535" t="s">
         <v>1775</v>
       </c>
@@ -14971,7 +15251,10 @@
         <v>AllowanceForPropertyTaxesModifiedAccrual</v>
       </c>
     </row>
-    <row r="536" spans="4:5">
+    <row r="536" spans="2:5">
+      <c r="B536" t="s">
+        <v>2034</v>
+      </c>
       <c r="D536" t="s">
         <v>1776</v>
       </c>
@@ -14980,7 +15263,10 @@
         <v>AllowanceForIncomeTaxesModifiedAccrual</v>
       </c>
     </row>
-    <row r="537" spans="4:5">
+    <row r="537" spans="2:5">
+      <c r="B537" t="s">
+        <v>2035</v>
+      </c>
       <c r="D537" t="s">
         <v>1777</v>
       </c>
@@ -14989,7 +15275,10 @@
         <v>IncomeTaxesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
     </row>
-    <row r="538" spans="4:5">
+    <row r="538" spans="2:5">
+      <c r="B538" t="s">
+        <v>2036</v>
+      </c>
       <c r="D538" t="s">
         <v>1778</v>
       </c>
@@ -14998,7 +15287,10 @@
         <v>AllowanceForSpecialAssessmentTaxesModifiedAccrual</v>
       </c>
     </row>
-    <row r="539" spans="4:5">
+    <row r="539" spans="2:5">
+      <c r="B539" t="s">
+        <v>2037</v>
+      </c>
       <c r="D539" t="s">
         <v>1779</v>
       </c>
@@ -15007,7 +15299,10 @@
         <v>SpecialAssessmentTaxesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
     </row>
-    <row r="540" spans="4:5">
+    <row r="540" spans="2:5">
+      <c r="B540" t="s">
+        <v>2038</v>
+      </c>
       <c r="D540" t="s">
         <v>1780</v>
       </c>
@@ -15016,7 +15311,10 @@
         <v>AllowanceForSalesTaxesModifiedAccrual</v>
       </c>
     </row>
-    <row r="541" spans="4:5">
+    <row r="541" spans="2:5">
+      <c r="B541" t="s">
+        <v>2039</v>
+      </c>
       <c r="D541" t="s">
         <v>1781</v>
       </c>
@@ -15025,7 +15323,10 @@
         <v>SalesTaxesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
     </row>
-    <row r="542" spans="4:5">
+    <row r="542" spans="2:5">
+      <c r="B542" t="s">
+        <v>2040</v>
+      </c>
       <c r="D542" t="s">
         <v>1782</v>
       </c>
@@ -15034,7 +15335,10 @@
         <v>AllowanceForOtherTaxesReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="543" spans="4:5">
+    <row r="543" spans="2:5">
+      <c r="B543" t="s">
+        <v>2041</v>
+      </c>
       <c r="D543" t="s">
         <v>1783</v>
       </c>
@@ -15043,7 +15347,10 @@
         <v>OtherTaxesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
     </row>
-    <row r="544" spans="4:5">
+    <row r="544" spans="2:5">
+      <c r="B544" t="s">
+        <v>2042</v>
+      </c>
       <c r="D544" t="s">
         <v>1784</v>
       </c>
@@ -15052,7 +15359,10 @@
         <v>AllowanceForTaxesModifiedAccrual</v>
       </c>
     </row>
-    <row r="545" spans="4:5">
+    <row r="545" spans="2:5">
+      <c r="B545" t="s">
+        <v>2043</v>
+      </c>
       <c r="D545" t="s">
         <v>1785</v>
       </c>
@@ -15061,7 +15371,10 @@
         <v>TaxesReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
     </row>
-    <row r="546" spans="4:5">
+    <row r="546" spans="2:5">
+      <c r="B546" t="s">
+        <v>2044</v>
+      </c>
       <c r="D546" t="s">
         <v>1786</v>
       </c>
@@ -15070,7 +15383,10 @@
         <v>AllowanceForPenaltiesReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="547" spans="4:5">
+    <row r="547" spans="2:5">
+      <c r="B547" t="s">
+        <v>2045</v>
+      </c>
       <c r="D547" t="s">
         <v>1787</v>
       </c>
@@ -15079,7 +15395,10 @@
         <v>AllowanceForLeasesReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="548" spans="4:5">
+    <row r="548" spans="2:5">
+      <c r="B548" t="s">
+        <v>2046</v>
+      </c>
       <c r="D548" t="s">
         <v>1788</v>
       </c>
@@ -15088,7 +15407,10 @@
         <v>AllowanceForGrantsAndContractsReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="549" spans="4:5">
+    <row r="549" spans="2:5">
+      <c r="B549" t="s">
+        <v>2047</v>
+      </c>
       <c r="D549" t="s">
         <v>1789</v>
       </c>
@@ -15097,7 +15419,10 @@
         <v>AllowanceForDepositsReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="550" spans="4:5">
+    <row r="550" spans="2:5">
+      <c r="B550" t="s">
+        <v>2048</v>
+      </c>
       <c r="D550" t="s">
         <v>1790</v>
       </c>
@@ -15106,7 +15431,10 @@
         <v>AllowanceForLoansAndNotesReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="551" spans="4:5">
+    <row r="551" spans="2:5">
+      <c r="B551" t="s">
+        <v>2049</v>
+      </c>
       <c r="D551" t="s">
         <v>1791</v>
       </c>
@@ -15115,7 +15443,10 @@
         <v>AllowanceForClaimsAndJudgmentsReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="552" spans="4:5">
+    <row r="552" spans="2:5">
+      <c r="B552" t="s">
+        <v>2050</v>
+      </c>
       <c r="D552" t="s">
         <v>1792</v>
       </c>
@@ -15124,7 +15455,10 @@
         <v>AllowanceForInterGovernmentalReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="553" spans="4:5">
+    <row r="553" spans="2:5">
+      <c r="B553" t="s">
+        <v>2051</v>
+      </c>
       <c r="D553" t="s">
         <v>1793</v>
       </c>
@@ -15133,7 +15467,10 @@
         <v>AllowanceForReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="554" spans="4:5">
+    <row r="554" spans="2:5">
+      <c r="B554" t="s">
+        <v>2052</v>
+      </c>
       <c r="D554" t="s">
         <v>1794</v>
       </c>
@@ -15142,7 +15479,10 @@
         <v>ReceivablesNetOfAllowanceModifiedAccrual</v>
       </c>
     </row>
-    <row r="555" spans="4:5">
+    <row r="555" spans="2:5">
+      <c r="B555" t="s">
+        <v>2053</v>
+      </c>
       <c r="D555" t="s">
         <v>1795</v>
       </c>
@@ -15151,7 +15491,10 @@
         <v>RestrictedReceivablesModifiedAccrual</v>
       </c>
     </row>
-    <row r="556" spans="4:5">
+    <row r="556" spans="2:5">
+      <c r="B556" t="s">
+        <v>2054</v>
+      </c>
       <c r="D556" t="s">
         <v>1796</v>
       </c>
@@ -15160,7 +15503,10 @@
         <v>AllowanceForRestrictedReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="557" spans="4:5">
+    <row r="557" spans="2:5">
+      <c r="B557" t="s">
+        <v>2055</v>
+      </c>
       <c r="D557" t="s">
         <v>1797</v>
       </c>
@@ -15169,7 +15515,10 @@
         <v>ReceivablesRestrictedNetOfAllowanceModifiedAccrual</v>
       </c>
     </row>
-    <row r="558" spans="4:5">
+    <row r="558" spans="2:5">
+      <c r="B558" t="s">
+        <v>2056</v>
+      </c>
       <c r="D558" t="s">
         <v>1798</v>
       </c>
@@ -15178,7 +15527,10 @@
         <v>InvestmentIncomeReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="559" spans="4:5">
+    <row r="559" spans="2:5">
+      <c r="B559" t="s">
+        <v>2057</v>
+      </c>
       <c r="D559" t="s">
         <v>1799</v>
       </c>
@@ -15187,7 +15539,10 @@
         <v>AllowanceForInvestmentIncomeReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="560" spans="4:5">
+    <row r="560" spans="2:5">
+      <c r="B560" t="s">
+        <v>2058</v>
+      </c>
       <c r="D560" t="s">
         <v>1800</v>
       </c>
@@ -15196,7 +15551,10 @@
         <v>InvestmentIncomeReceivableNetOfAllowanceModifiedAccrual</v>
       </c>
     </row>
-    <row r="561" spans="4:5">
+    <row r="561" spans="2:5">
+      <c r="B561" t="s">
+        <v>2059</v>
+      </c>
       <c r="D561" t="s">
         <v>1801</v>
       </c>
@@ -15205,7 +15563,10 @@
         <v>AllowanceForOtherReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="562" spans="4:5">
+    <row r="562" spans="2:5">
+      <c r="B562" t="s">
+        <v>2060</v>
+      </c>
       <c r="D562" t="s">
         <v>1802</v>
       </c>
@@ -15214,7 +15575,10 @@
         <v>OtherReceivablesNetOfAllowanceModifiedAccrual</v>
       </c>
     </row>
-    <row r="563" spans="4:5">
+    <row r="563" spans="2:5">
+      <c r="B563" t="s">
+        <v>2061</v>
+      </c>
       <c r="D563" t="s">
         <v>1803</v>
       </c>
@@ -15223,7 +15587,10 @@
         <v>ReceivablesFromContractsModifiedAccrual</v>
       </c>
     </row>
-    <row r="564" spans="4:5">
+    <row r="564" spans="2:5">
+      <c r="B564" t="s">
+        <v>2062</v>
+      </c>
       <c r="D564" t="s">
         <v>1804</v>
       </c>
@@ -15232,7 +15599,10 @@
         <v>DueFromOtherGovernmentModifiedAccrual</v>
       </c>
     </row>
-    <row r="565" spans="4:5">
+    <row r="565" spans="2:5">
+      <c r="B565" t="s">
+        <v>2063</v>
+      </c>
       <c r="D565" t="s">
         <v>1805</v>
       </c>
@@ -15241,7 +15611,10 @@
         <v>DueFromOthersModifiedAccrual</v>
       </c>
     </row>
-    <row r="566" spans="4:5">
+    <row r="566" spans="2:5">
+      <c r="B566" t="s">
+        <v>2064</v>
+      </c>
       <c r="D566" t="s">
         <v>1806</v>
       </c>
@@ -15250,7 +15623,10 @@
         <v>PrepaidInsuranceModifiedAccrual</v>
       </c>
     </row>
-    <row r="567" spans="4:5">
+    <row r="567" spans="2:5">
+      <c r="B567" t="s">
+        <v>2065</v>
+      </c>
       <c r="D567" t="s">
         <v>1807</v>
       </c>
@@ -15259,7 +15635,10 @@
         <v>OtherPrepaidAssetsModifiedAccrual</v>
       </c>
     </row>
-    <row r="568" spans="4:5">
+    <row r="568" spans="2:5">
+      <c r="B568" t="s">
+        <v>2066</v>
+      </c>
       <c r="D568" t="s">
         <v>1808</v>
       </c>
@@ -15268,7 +15647,10 @@
         <v>PrepaidExpensesAndOtherAssetsModifiedAccrual</v>
       </c>
     </row>
-    <row r="569" spans="4:5">
+    <row r="569" spans="2:5">
+      <c r="B569" t="s">
+        <v>2067</v>
+      </c>
       <c r="D569" t="s">
         <v>1809</v>
       </c>
@@ -15277,7 +15659,10 @@
         <v>InventoryAndPrepaidItemsModifiedAccrual</v>
       </c>
     </row>
-    <row r="570" spans="4:5">
+    <row r="570" spans="2:5">
+      <c r="B570" t="s">
+        <v>2068</v>
+      </c>
       <c r="D570" t="s">
         <v>1810</v>
       </c>
@@ -15286,7 +15671,10 @@
         <v>TravelAdvancesReceivableModifiedAccrual</v>
       </c>
     </row>
-    <row r="571" spans="4:5">
+    <row r="571" spans="2:5">
+      <c r="B571" t="s">
+        <v>2069</v>
+      </c>
       <c r="D571" t="s">
         <v>1811</v>
       </c>
@@ -15295,7 +15683,10 @@
         <v>DerivativeInstrumentsAssetsModifiedAccrual</v>
       </c>
     </row>
-    <row r="572" spans="4:5">
+    <row r="572" spans="2:5">
+      <c r="B572" t="s">
+        <v>2070</v>
+      </c>
       <c r="D572" t="s">
         <v>1812</v>
       </c>
@@ -15304,7 +15695,10 @@
         <v>RegulatoryAssetsModifiedAccrual</v>
       </c>
     </row>
-    <row r="573" spans="4:5">
+    <row r="573" spans="2:5">
+      <c r="B573" t="s">
+        <v>2071</v>
+      </c>
       <c r="D573" t="s">
         <v>1753</v>
       </c>
@@ -15313,7 +15707,10 @@
         <v>AssetsModifiedAccrual</v>
       </c>
     </row>
-    <row r="574" spans="4:5">
+    <row r="574" spans="2:5">
+      <c r="B574" t="s">
+        <v>2072</v>
+      </c>
       <c r="D574" t="s">
         <v>1813</v>
       </c>
@@ -15322,7 +15719,10 @@
         <v>AssetsAndDeferredOutflowsOfResourcesModifiedAccrual</v>
       </c>
     </row>
-    <row r="575" spans="4:5">
+    <row r="575" spans="2:5">
+      <c r="B575" t="s">
+        <v>2073</v>
+      </c>
       <c r="D575" t="s">
         <v>1814</v>
       </c>
@@ -15331,7 +15731,10 @@
         <v>CashOverdraftModifiedAccrual</v>
       </c>
     </row>
-    <row r="576" spans="4:5">
+    <row r="576" spans="2:5">
+      <c r="B576" t="s">
+        <v>2074</v>
+      </c>
       <c r="D576" t="s">
         <v>1815</v>
       </c>
@@ -15340,7 +15743,10 @@
         <v>BenefitsPayableModifiedAccrual</v>
       </c>
     </row>
-    <row r="577" spans="4:5">
+    <row r="577" spans="2:5">
+      <c r="B577" t="s">
+        <v>2075</v>
+      </c>
       <c r="D577" t="s">
         <v>1816</v>
       </c>
@@ -15349,7 +15755,10 @@
         <v>InterGovernmentalPayableModifiedAccrual</v>
       </c>
     </row>
-    <row r="578" spans="4:5">
+    <row r="578" spans="2:5">
+      <c r="B578" t="s">
+        <v>2076</v>
+      </c>
       <c r="D578" t="s">
         <v>1817</v>
       </c>
@@ -15358,7 +15767,10 @@
         <v>ClaimsAndJudgmentsPayableModifiedAccrual</v>
       </c>
     </row>
-    <row r="579" spans="4:5">
+    <row r="579" spans="2:5">
+      <c r="B579" t="s">
+        <v>2077</v>
+      </c>
       <c r="D579" t="s">
         <v>1818</v>
       </c>
@@ -15367,7 +15779,10 @@
         <v>PayablesForOthersModifiedAccrual</v>
       </c>
     </row>
-    <row r="580" spans="4:5">
+    <row r="580" spans="2:5">
+      <c r="B580" t="s">
+        <v>2078</v>
+      </c>
       <c r="D580" t="s">
         <v>1819</v>
       </c>
@@ -15376,7 +15791,10 @@
         <v>AccruedPayrollTaxesModifiedAccrual</v>
       </c>
     </row>
-    <row r="581" spans="4:5">
+    <row r="581" spans="2:5">
+      <c r="B581" t="s">
+        <v>2079</v>
+      </c>
       <c r="D581" t="s">
         <v>1820</v>
       </c>
@@ -15385,7 +15803,10 @@
         <v>AccruedBenefitsAndCompensationLongTermModifiedAccrual</v>
       </c>
     </row>
-    <row r="582" spans="4:5">
+    <row r="582" spans="2:5">
+      <c r="B582" t="s">
+        <v>2080</v>
+      </c>
       <c r="D582" t="s">
         <v>1821</v>
       </c>
@@ -15394,7 +15815,10 @@
         <v>CompensatedAbsencesPayableModifiedAccrual</v>
       </c>
     </row>
-    <row r="583" spans="4:5">
+    <row r="583" spans="2:5">
+      <c r="B583" t="s">
+        <v>2081</v>
+      </c>
       <c r="D583" t="s">
         <v>1822</v>
       </c>
@@ -15403,7 +15827,10 @@
         <v>AllOtherAccountsPayableAndAccruedLiabilitiesModifiedAccrual</v>
       </c>
     </row>
-    <row r="584" spans="4:5">
+    <row r="584" spans="2:5">
+      <c r="B584" t="s">
+        <v>2082</v>
+      </c>
       <c r="D584" t="s">
         <v>1823</v>
       </c>
@@ -15412,7 +15839,10 @@
         <v>DueToEnterpriseFundsModifiedAccrual</v>
       </c>
     </row>
-    <row r="585" spans="4:5">
+    <row r="585" spans="2:5">
+      <c r="B585" t="s">
+        <v>2083</v>
+      </c>
       <c r="D585" t="s">
         <v>1824</v>
       </c>
@@ -15421,7 +15851,10 @@
         <v>AdvancesFromComponentUnitModifiedAccrual</v>
       </c>
     </row>
-    <row r="586" spans="4:5">
+    <row r="586" spans="2:5">
+      <c r="B586" t="s">
+        <v>2084</v>
+      </c>
       <c r="D586" t="s">
         <v>1825</v>
       </c>
@@ -15430,7 +15863,10 @@
         <v>ProvisionForPropertyTaxRefundsModifiedAccrual</v>
       </c>
     </row>
-    <row r="587" spans="4:5">
+    <row r="587" spans="2:5">
+      <c r="B587" t="s">
+        <v>2085</v>
+      </c>
       <c r="D587" t="s">
         <v>1826</v>
       </c>
@@ -15439,7 +15875,10 @@
         <v>UnamortizedPremiumOnBondsModifiedAccrual</v>
       </c>
     </row>
-    <row r="588" spans="4:5">
+    <row r="588" spans="2:5">
+      <c r="B588" t="s">
+        <v>2086</v>
+      </c>
       <c r="D588" t="s">
         <v>1827</v>
       </c>
@@ -15448,7 +15887,10 @@
         <v>LeasesPayableModifiedAccrual</v>
       </c>
     </row>
-    <row r="589" spans="4:5">
+    <row r="589" spans="2:5">
+      <c r="B589" t="s">
+        <v>2087</v>
+      </c>
       <c r="D589" t="s">
         <v>1828</v>
       </c>
@@ -15457,7 +15899,10 @@
         <v>BondsPayableModifiedAccrual</v>
       </c>
     </row>
-    <row r="590" spans="4:5">
+    <row r="590" spans="2:5">
+      <c r="B590" t="s">
+        <v>2088</v>
+      </c>
       <c r="D590" t="s">
         <v>1829</v>
       </c>
@@ -15466,7 +15911,10 @@
         <v>LoansPayableModifiedAccrual</v>
       </c>
     </row>
-    <row r="591" spans="4:5">
+    <row r="591" spans="2:5">
+      <c r="B591" t="s">
+        <v>2089</v>
+      </c>
       <c r="D591" t="s">
         <v>1830</v>
       </c>
@@ -15475,7 +15923,10 @@
         <v>NotesPayableModifiedAccrual</v>
       </c>
     </row>
-    <row r="592" spans="4:5">
+    <row r="592" spans="2:5">
+      <c r="B592" t="s">
+        <v>2090</v>
+      </c>
       <c r="D592" t="s">
         <v>1831</v>
       </c>
@@ -15484,7 +15935,10 @@
         <v>NotesAndLoansPayableDueWithinOneYearModifiedAccrual</v>
       </c>
     </row>
-    <row r="593" spans="4:5">
+    <row r="593" spans="2:5">
+      <c r="B593" t="s">
+        <v>2091</v>
+      </c>
       <c r="D593" t="s">
         <v>1832</v>
       </c>
@@ -15493,7 +15947,10 @@
         <v>RegulatoryLiabilityModifiedAccrual</v>
       </c>
     </row>
-    <row r="594" spans="4:5">
+    <row r="594" spans="2:5">
+      <c r="B594" t="s">
+        <v>2092</v>
+      </c>
       <c r="D594" t="s">
         <v>1833</v>
       </c>
@@ -15502,7 +15959,10 @@
         <v>DerivativeInstrumentsLiabilityModifiedAccrual</v>
       </c>
     </row>
-    <row r="595" spans="4:5">
+    <row r="595" spans="2:5">
+      <c r="B595" t="s">
+        <v>2093</v>
+      </c>
       <c r="D595" t="s">
         <v>1834</v>
       </c>
@@ -15511,7 +15971,10 @@
         <v>OtherLiabilitiesModifiedAccrual</v>
       </c>
     </row>
-    <row r="596" spans="4:5">
+    <row r="596" spans="2:5">
+      <c r="B596" t="s">
+        <v>2094</v>
+      </c>
       <c r="D596" t="s">
         <v>1752</v>
       </c>
@@ -15520,7 +15983,10 @@
         <v>LiabilitiesModifiedAccrual</v>
       </c>
     </row>
-    <row r="597" spans="4:5">
+    <row r="597" spans="2:5">
+      <c r="B597" t="s">
+        <v>2095</v>
+      </c>
       <c r="D597" t="s">
         <v>1835</v>
       </c>
@@ -15529,7 +15995,10 @@
         <v>DeferredInflowsOfResourcesDrainFundModifiedAccrual</v>
       </c>
     </row>
-    <row r="598" spans="4:5">
+    <row r="598" spans="2:5">
+      <c r="B598" t="s">
+        <v>2096</v>
+      </c>
       <c r="D598" t="s">
         <v>1836</v>
       </c>
@@ -15538,7 +16007,10 @@
         <v>DeferredInflowsOfResourcesSpecialAssessmentsModifiedAccrual</v>
       </c>
     </row>
-    <row r="599" spans="4:5">
+    <row r="599" spans="2:5">
+      <c r="B599" t="s">
+        <v>2097</v>
+      </c>
       <c r="D599" t="s">
         <v>1837</v>
       </c>
@@ -15547,7 +16019,10 @@
         <v>DeferredInflowsOfResourcesUnavailableRevenueModifiedAccrual</v>
       </c>
     </row>
-    <row r="600" spans="4:5">
+    <row r="600" spans="2:5">
+      <c r="B600" t="s">
+        <v>2098</v>
+      </c>
       <c r="D600" t="s">
         <v>1838</v>
       </c>
@@ -15556,7 +16031,10 @@
         <v>LiabilitiesAndDeferredInflowsOfResourcesModifiedAccrual</v>
       </c>
     </row>
-    <row r="601" spans="4:5">
+    <row r="601" spans="2:5">
+      <c r="B601" t="s">
+        <v>2099</v>
+      </c>
       <c r="D601" t="s">
         <v>1839</v>
       </c>
@@ -15565,7 +16043,10 @@
         <v>InvestmentInCapitalAssetsModifiedAccrual</v>
       </c>
     </row>
-    <row r="602" spans="4:5">
+    <row r="602" spans="2:5">
+      <c r="B602" t="s">
+        <v>2100</v>
+      </c>
       <c r="D602" t="s">
         <v>1750</v>
       </c>
@@ -26223,12 +26704,12 @@
     </row>
     <row r="25" spans="1:5" ht="15">
       <c r="A25" s="7"/>
-      <c r="B25" s="128" t="s">
+      <c r="B25" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="129"/>
-      <c r="D25" s="129"/>
-      <c r="E25" s="130"/>
+      <c r="C25" s="130"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="131"/>
     </row>
     <row r="26" spans="1:5" ht="15">
       <c r="A26" s="8" t="str">

</xml_diff>